<commit_message>
Update niche-generation prompt and remove offer/rating logic
</commit_message>
<xml_diff>
--- a/output/master.xlsx
+++ b/output/master.xlsx
@@ -453,31 +453,40 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>UCYyel9YAgwvs07rz5kugU7g</t>
+          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ricky Impey</t>
+          <t>itsbasicbible</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">This channel exists to help you with your 3d printing. From selecting the right products to fixing problems and tuning for great results, it's all here. My ethos is to explain complicated things in simple, easy to understand terms that anyone can understand and learn from. 
-I strive to have you enjoying 3d printing, whatever your experience.
-If you'd like to show your appreciation for any of the free information provided here, then why not buy me a coffee?  
-https://www.buymeacoffee.com/rickyimpey
+          <t xml:space="preserve">Welcome to the channel.
+I help young men build lives of purpose, clarity, confidence, and conviction through biblical truth and practical leadership teaching.
+Most men feel stuck because they lack three things: Bible clarity, purpose clarity, and calling clarity.
+This channel gives you all three.
+Here, you’ll learn how to:
+• Understand Scripture with simplicity and truth
+• Discover your God-given purpose and calling
+• Renew your mind and rebuild your identity
+• Grow in biblical masculinity, strength, and discipline
+• Lead your life with confidence and conviction
+• Overcome insecurity, confusion, and internal limitations
+• Become a man of impact, influence, and Kingdom leadership without limitations
+If you're ready to stop drifting and make an impact, subscribe and join a community of men becoming who God created them to be.
 </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>72000</t>
+          <t>17200</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>168</t>
+          <t>868</t>
         </is>
       </c>
     </row>
@@ -570,74 +579,78 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>UCYyel9YAgwvs07rz5kugU7g</t>
+          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Ricky Impey</t>
+          <t>itsbasicbible</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>paltsNeM6Y0</t>
+          <t>TO_COKkK6Pw</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>New 3D Printer? Watch This First</t>
+          <t>Is Your Faith SABOTAGING Your IMPACT? | Middle Ground Christian</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://brilliant.org/rickyimpey
-Try Brilliant free for 30 days + get 20% off an annual subscription.
-If you’ve just bought your first 3D printer — or you’re about to open the box — this is the video you should watch first.
-This beginner-friendly guide walks you through the most important things you need to know before you even turn your 3D printer on. It’s designed to help first-time users avoid the most common (and frustrating) mistakes that can ruin your first print or even damage your printer.
-I’m not going to tell you to buy loads of extra tools or read hundreds of pages of instructions. Instead, I’ll show you the simple, practical steps that actually matter, using the experience I’ve gained from setting up and using countless 3D printers over the years.
-*Affiliate links (If you purchase something after clicking any of the below links I may earn a small commission at no cost to you. This is a great way to support the channel)*
-*Budget Filament*
-*Sunlu*
-https://amzn.to/4qkj8II
-*Geeetech*
-https://amzn.to/4s4Zy4I
-*eSun*
-https://amzn.to/48Iepuq
-*Tinmorry*
-https://amzn.to/4i9fKNX
-*Overture*
-https://amzn.to/4pLSZmc
-This video was sponsored by Brilliant
-..............................................................................................................................................................
-BUY ME A COFFEE
-If you're enjoying my content, why not consider supporting the channel by buying me a coffee? 
-Even very small amounts are greatly appreciated and re-invested into bringing you better content.
-https://www.buymeacoffee.com/rickyimpey
-You can also use the YouTube 'Thanks' button above if you prefer.</t>
+          <t>The problem with lukewarm Christianity is that you blend in with everyone and you impact no one." Are you following Jesus just enough to be called a disciple, but still betraying Him with your lifestyle? As we move into 2026, it’s time to stop repping the "Christian jersey" on the sidelines and actually get on the field. Remember: You may be the only Bible someone ever reads.
+In this powerful message, we dive deep into the spiritual danger of the "middle ground." Using the warning to the church of Laodicea in Revelation 3, we explore how becoming "comfortable" makes us ineffective for the Kingdom of God.
+Just like the lukewarm water in the ancient aqueducts of Laodicea, a faith without heat is worthless to a world in need of a savior. We break down the betrayal of Judas, the choice of Joshua (Joshua 24:15), and the sobering reality of Titus 1:16—where people claim to know God but deny Him by the way they live.
+If you feel like your impact has been sabotaged by compromise, this video is your wake-up call to stop looking back like Lot's wife and start pursuing your purpose with undivided attention. Don't waste 2026 like you did 2025. It’s time to choose: Christ or Culture?
+00:00 The Problem with Lukewarm Christianity
+00:47 A Message from God
+00:53 Understanding Revelation 3
+02:02 The Call to Make a Difference
+02:20 Reflecting on 2025 and Looking Ahead
+03:00 Living a Committed Christian Life
+03:46 The Consequences of Lukewarm Faith
+05:57 Choosing to Follow Christ Fully
+08:33 The Importance of Loving God and Others
+11:40 A Prayer for Dedication
+13:08 Final Encouragement and Farewell
+Connect 
+https://linktr.ee/itsbasicbible
+MALTA APPAREL LINK 
+https://malta-apparel.com/?ref=BBAZ16 
+FOR 15% OFF: basicbible15 
+FREE 10 DAY DEVO BOOK 
+https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
+I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
+https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
+I WANT TO FOLLOW JESUS CHRIST
+https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
+Get vidIQ to grow your channel faster! 🚀
+https://vidiq.com/itsbasicbible</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2025-12-22T17:01:34Z</t>
+          <t>2026-01-03T00:00:39Z</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>7925</t>
+          <t>46</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>271</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.035331</v>
+        <v>0.173913</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -646,91 +659,78 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>If you've just received your first 3D printer, stop. Pausing to watch this video will save you a lot of frustration on day one. I'm not going to take any of the fun out of getting started. I just want to show you a few simple things that will help you get it working properly the first time. I've set up a lot of 3D printers over the years, and I've pretty much made every beginner mistake there is. This video is here to help you avoid those mistakes and get your first print done right without panicking if something goes wrong. This video is sponsored by Brilliant. So, first things first, whatever type of 3D printer you've got, there will be a couple of things to do before plugging it in and turning it on. Start by finding yourself a bit of space. Ideally, you want a clear tabletop, but wherever you're going to set up your printer, make sure it's clear of any clutter or mess. There can sometimes be some small parts to assemble, and you don't want to lose anything in the excitement of getting started. Take all of the parts out of the box and then lay them all out in a way that makes it easy to see everything. Remove all of the packing materials and double check that there's nothing left in the box before moving it out of the way somewhere. With every modern 3D printer, there will be a manual quick start guide or a QR code that you can scan to access a quick start guide. I'm not going to go into model specifics here, but I do have a lot of setup and review videos on my channel if you do need something more specific for your printer. This is not one of those occasions where you can bluff through without opening the manual. It's very important that you follow the first couple of steps in the guide that comes with your particular printer. With some machines, it will be cutting or removing transport fixings. With others, there may be some minimal assembly, but please don't skip this part. It won't take long, and it's very important to follow the specific instructions for your model up until the point where you turn it on. Once you've reached the part where your printer is built and it seems like you're ready to turn it on, stop. There is one last very important thing to check that could really ruin your day if you miss it. That thing is the voltage setting. This is probably one of the most important parts of the whole setup. So, don't rush it. These 3D printers are shipped all over the world, so they have to work with different countries voltages. Many 3D printers now sense the voltage automatically, but many also need setting manually. And if the setting is wrong, you could seriously damage your printer. If you do need to set the voltage manually on your printer, there'll be a switch that looks a lot like this one somewhere obvious, usually on the back or side of the printer. It should also be very obvious in the manual or quick start guide, too. What setting you need to use will depend on where you live. Most of the world uses 220 to 240 volt, while many areas of North and South America and Japan use 110 to 120 volt. If you don't know what to use, check and be sure before turning your printer on. If there's no mention of a voltage setting in your manual and no obvious switch, then it is very likely that your printer senses voltage automatically. This is very common now on new 3D printers. Have one last final check that every stage of setup from the manual has been completed and that all of the packing materials and fixings have been removed. Then plug your printer in using the provided lead only and turn it on. Most 3D printers will now take you through a short setup procedure where you select your language, enter your Wi-Fi details if you want to, and then they run through some form of automatic calibration. This can be quite quick and simple or it can be more involved. However long it takes, it's important that you let it complete fully for the very best first print experience. Before it starts, make sure your printer is on a level, flat surface, ideally in the place where you plan to use it. Modern 3D printers sense things like how much they're going to move when printing. So, if you move the printer after the calibration phase, you should really get it to do the calibration again afterwards for best results. If you made it to this point, you're doing great so far. While the printer is getting itself ready, it's time to get your filament open and ready to use. Filament is what the string-like material that 3D printers use is called. It comes supplied on rolls, and you need to handle it a little bit carefully to avoid headaches. The single most important thing to do when handling 3D printer filament is to keep hold of the end. Filament needs to unwind cleanly as your printer pulls it, and letting go of the end will very likely allow the filament to tangle. Any tangles in the filament will stop the print from completing successfully. So when you hold the filament, always hold on to the end or make sure it's tucked into the holes on the side of the spool in a way where it can't get loose. Generally, I always leave it tucked into these holes right up until the point where I'm about to feed it into the printer. So hopefully by now your printer has completed its setup and it's now time to load your filament. Every 3D printer should have a place for the filament spool to sit and rotate. Some have a horizontal post, some have rollers and bearings, and some have multifilament holders that allow multiolor printing. If you do have a multifilament printer, just load one single spool of filament for your first print. If this is your first time printing, the filament you want to be using is PLA. There are other options that allow you to do all types of things, but PLA is the most common and it's the one to start with. If you receive some filament with your printer, it will be PLA. If you don't have any filament and you need to order some, buy PLA. You don't have to spend a lot of money. Buy 1 kilogram of simple PLA. Nothing fancy, just something like black or white. And it also needs to be 1.75 mm, which most of them are. There are many different brands to choose from, and you don't need to buy anything expensive. I'll put some links in the description to budget brands I trust if you want them. Loading the filament is done slightly differently on each machine, but the basics are the same. The nozzle of the printer needs to get hot and the printer's motors need to pull the filament through. Usually after you've manually fed it in to a certain point before you feed the end of the filament into the printer, cut any kinks or bends off of the end with either some cutters or even just some scissors if you don't have cutters. This is to make sure it feeds in cleanly without snagging. One way or another, you will likely have to tell your printer that you want to load filament, except if you have a multifilament feeding unit, in which case it's often just a case of feeding the end in one at a time, and the printer will automatically heat the nozzle and load the one it wants when the print starts. Filament loading options are usually pretty obvious in your printer's screen menus, and most manuals and guides supplied with your printer cover it well. If you notice any smells or hear motor noises while loading filament, it's all very normal. Don't worry. Once your filament is loaded, you're very nearly there. The hard part's done. We're now going to find something to print. If your printer came with a USB stick or SD card, insert it and look for an option in your printer screen for print or USB or something similar. We're trying to find preloaded print files that your 3D printer manufacturer has supplied to get you started. You may have a lot of files to choose from, but pick something small. All we're doing is getting a simple first print complete. Maybe save the Flexi Dragons for later. Now, before you hit print, just some final checks. Did you load filament? Is your print surface fitted correctly? And is it clean? And have you checked that there are no obstructions on the bed or print surface? If everything's good, hit print. The printer will now heat the bed and the nozzle and probably run through a few minutes of its own checks before starting to print. Hopefully, your first print will start and complete without any issue. However, if things don't go to plan, don't panic. It's very likely to be something simple, and I'll give you a few things to check. If the filament doesn't stick to the bed and gets pulled around on the nozzle, or if anything else is obviously wrong, cancel the print on the printer's screen. This is really common on first prints, so don't worry. Ideally, with something like a pair of tweezers, remove any lumps of filament from the nozzle after it stopped moving. The reason we use tweezers is that the nozzle is still hot and you don't want to burn yourself. If there are any lines of filament, these are called purge lines, on the bed, gently remove them or let the bed cool and then remove them. Now try the same print again and carefully watch the first layer of the print going down as this is where 99% of all 3D printing problems occur. What we're going to do is to try and quickly understand what's not quite working right before we fix it. Now what we're doing here, stopping observing what's happening and figuring out what needs changing, that's problem solving. And that's exactly the reason why this video is sponsored by Brilliant. Brilliant is built around the idea that you already can figure things out. You just need the right way of learning. Instead of passively watching lessons, you work through real problems step by step using visuals and interaction until the ideas actually make sense, just like you're doing with this video. What I like about Brilliant is that it doesn't assume you're bad at math or science. It treats you like a thinker and helps you build that intuition properly. You're not memorizing formulas. You're understanding why things work. I've been using Brilliant to sharpen my own problem solving skills, especially around logical thinking and cause and effect. The exact same kind of thinking you're using when setting up and troubleshooting something like a 3D printer. Brilliant personalizes what you see based on where you're at, so you're always being challenged at the right level. And you can really feel yourself making progress as things start to click. If you want to try it out, you can learn for free at brilliant.org/ickyimpy org/riickympi or scan the QR code on screen. Brilliant also giving you 20% off an annual premium subscription which gives you unlimited access to everything on the platform. Right now, let's get back to the printer. For a 3D print to be successful, the first layer has to stick to the bed. For this to happen, a few things have to be right. The surface of the bed needs to be clean and the melted material needs to be pushed into the surface just the right amount for it to stay stuck. If the nozzle is too far away, then the filament won't be pushed into the surface enough. And if it's too close, then the nozzle will scrape on the print surface and stop the filament coming out at all. Nowadays, printers should set the nozzle position automatically. But if it's wrong, you'll see it by the way the filament that's pushed out or extruded behaves. If your printer doesn't fix this issue by running through the calibration process again, then the setting you're looking for is called Z or Z offset. If everything looks right, but the filament is just not sticking, then your print surface may be dirty. The easiest thing to clean it with is IPA or rubbing alcohol. But if you don't have any and your print surface is removable, simply wash it with soap and water and then try to only touch it on the edges afterwards. Your fingers have oils that can make it hard for prints to stick. So, you don't want to touch the print surface if you can avoid it. This should solve the vast majority of first print problems, but I've got some far more detailed deep dives on this kind of thing on my channel, and more specifically in this playlist. Once your successful first print is finished, don't try and yank it straight off the bed. It will likely be stuck quite well while everything is hot. Just leave it to cool down for a few minutes and it will likely pop right off or at least be much easier to remove. If you really can't wait and you've got a magnetic bed, then remove your print surface and put it somewhere to cool as it will release much quicker this way than leaving it on the printer. Once your removed print surface is cooled down, you can flex it which will make the print pop straight off. You can leave your printer switched on between prints. It won't use much power, but if you're not going to print anytime soon, don't switch it off straight after the print finishes. Let it cool down for 5 minutes first. This just lets everything get cooled down quicker by the fans and avoids something called heat soak. You can leave the filament loaded ready for next time, or you can use the printer screen to unload it if you don't want it sitting on the printer. Just remember to keep hold of the end if you do. Well done. You've now well and truly started your 3D printing journey. And with a successful first print done, you know that your printer is ready for all those crazy projects you actually wanted it for. When you want to print things that didn't come supplied with your printer, have a look at one of these videos for how to set up your own prints using Slicer software. Check out the top one if you've got a Bamboo Lab printer, and if not, check out the other one. Hit subscribe if you want to see more from me about 3D printing, and I'll see you in the next one.</t>
+          <t>The problem with lukewarm Christianity is that you blend [music] in with everyone and you impact no one. And also another problem with lukewarm Christianity is that you can follow [music] Christ enough to be called a disciple but then still betray Jesus. And that's what [music] Judas did. He followed Jesus enough to be counted as one of the 12, but then when [music] the time came to it, when his life was on the line, when he was desperate, where his commitment [music] was there, his choice, he betrayed Jesus. And that's what happens with lukewarm Christianity is that you end up betraying Jesus. You don't have [music] time to be a lukewarm Christian. And ultimately, God doesn't have time for you to be a lukewarm Christian. You know, people's lives mistake because of the way that [music] we live because you may be literally the only Bible that someone reads. Hear that? You literally may be the only Bible that someone reads. Hey guys, I truly believe that God is speaking to you right now and he wants you to hear this. Today as I was reading the Bible, this particular verse stuck out to me. And it's not the first time that I read it, but it's something that just hit me a little differently, if that makes sense. And that was in Revelations chapter 3 where God was talking to the church of Leodysia. And he was talking about how I don't want you to be lukewarm. You're neither hot nor cold. And he's like, I just wish that you would choose one or the other. And as I began to think about that, I did some research just to get a better understanding of what that particular Bible verse was saying. And in case you didn't know that the church of Philadelphia, that city had an aqueduct that was six miles long and it was taking in water from a hot spring. So whenever it reached the city, it was lukewarm and people just got used to it. And I think that as believers, if we're not careful, the more we are hanging hanging around with the world or hanging out with believers who are not pursuing their purpose and really living the life that God has called them to, we can we can become comfortable. And because of that, we become ineffective for the kingdom of God. And I believe that Jesus wants us to make a difference in this world around us. He doesn't want us just to have the label Christian and really not make an impact. Instead, he wants us to live the Christian life so that we can actually make a difference. And I just began to think about how many of us, including myself, a little bit in 2025, we wasted time because we wasn't pursuing our purpose or we lived in compromise and we wasn't fully dedicated and being in alignment with what God has for us. And it just got me thinking that guys, God doesn't want you to waste your 2026 like you did in 2025. He doesn't want you to be the Christian that has the label Christian, but your life doesn't reflect Christ. Come on. You know what I'm talking about, right? You have Christian all over your Instagram bio. You you you you call yourself a believer. You go to church, but then on Saturdays and Friday nights, you're not really living for the Lord. Or even in the things that you're watching or even listening to, you know, it's not good for your soul, but you're still listening to it. And I believe that God is really trying to help the church, help the believers to really draw a separation because honestly guys, the time for middle Christianity being in the middle ground, those days are over. And to be honest, that should have never been a time, but it has been a time. And really, I believe God is really trying to extract and draw out people and believers who are truly committed to following the Lord. Because Jesus even said it that if you are a lukewarm person, you are worthless to me. I'm going to spit you out my mouth. And that's what's happening to some of us because we are not committed to God. Because we are not desperately dedicating our life to God. We're worthless to God. We can't even make an impact. We can't even make a difference in the world around us. And maybe that could be the reason why some of our family members are not saved still or even some of our friends or even our co-workers. Maybe that could be one of the reasons why we actually don't see transformation in our life is because we're not fully de dedicated and submitted to God. And because of that, God is just going to spit us out. You know what's so interesting? When Jesus said, "I I I wish you was just hot or cold." It made me think about being allin, right? Jesus is looking for committed followers of Christ. He's looking for people who are truly seeking after him and not just playing the middle ground or just happy that they're on the team and they got the jersey, but they really don't want to get in. They don't really want to get on the field and play. And guys, Jesus will spit you out his mouth. The person that is lukewarm, you see, I I would say this, the problem with lukewarm Christianity is that is that you blend in with everyone and you impact no one. Think about that for a moment. Lukewarm Christianity, you blend in with everyone, but you impact no one. That means your life looks the same as everyone else. Your speech looks the same. Your lifestyle, your your dress, the way you carry yourself, the way you even treat other people. It looks like the world around you, but you impact no one. You're not being a light. You look just like the darkness. And also, another problem with lukewarm Christianity is that you can follow Christ enough to be called a disciple, but then still betray Jesus. And that's what Judas did. He followed Jesus enough to be counted as one of the 12. But then when the time came to it, when his life was on the line, when he was desperate, where his commitment was there, his choice, he betrayed Jesus. And that's what happens with lukewarm Christianity is that you end up betraying Jesus. Even though you follow Jesus, you end up betraying Jesus in your commitments, your values, your theology, your your beliefs, your ideology, and all these different things. how you raise your family, the the type of people that you vote for in office, the the ways that you conduct your business, the way that you treat other people, your friendships, all these different things, your personal life. Lukewarm Christianity will eventually cause you to betray Jesus. And Jesus doesn't want that. Jesus wants you to be fully committed. That's why in Joshua 24:15, Joshua looks at the people and says, "Look, you can follow the people across the Euphrates River. You can follow these guides. you can follow these people, but he said, "As for me in my house, I will serve the Lord. As for me in my house, I will follow God in." And guys, as believers, some of you haven't made a commitment yet on who you're going to follow. You want to follow Jesus because you like what he gives, but then you still tampering around and playing with the world. You still want to drink a little bit. You still want to get drunk. You still want to smoke weed. You still want to watch seductive movies. You still want to uh read books that that spur the desire of lust in your life. You think it's all okay, but what you really don't know is that because you became comfortable with it, you don't realize that is toxic to your life. See, the issue with lukewarm Christianity as well is that you can get so used to toxicity that you are unfamiliar with what health looks like. And guys, God doesn't want that for you in 2026. He wants you to be a man and a woman that's fully passionate, that's fully surrendered, and that's fully committed to him. He doesn't want you to pursue the other things. He doesn't want you to be like Lot's wife who was running away from danger. But because she loved the cities of of Sodom and Gomorrah so much, she turned and she she looked back at the city and became a pillar of salt. Guys, God doesn't want you to look back anymore. He wants you to let go. That's why he says just uh the person who follows me and puts the hand to the plow and then looks back is is unfit for my kingdom. God doesn't want people who's constantly looking back and looking at what they missed out. Instead, God wants you to focus on the things that you can get for him from him because you are pursuing his his purpose that he has for you, you are pursuing the kingdom. And guys, I just believe that if you really want to make an impact in the world around you, if you really want to make a difference in this world that Jesus Christ has for you, guys, you got to be committed. You got to be fully surrendered and committed to God. Because even in Titus 1:16, man, guys, this verse always hits at home and and and to be honest, it always checks me. It says this, "People claim that they know God, but by the way that they live, they deny him. And because of that, they are detestable and they are disobedient and worthless for doing anything good." hear that people claim that they know God, but by the way that they live, they deny Jesus. And because of that, they are detestable and disobedient before God and they are worthless to him. Guys, that's the Bible. That's strong. That's not Renee Mallet. That is the Bible. That's what Jesus is saying is that you have to ensure that you're not just a person that has the label of Christianity, but your life actually reflects Christ. Does your lifestyle, does your deeds, does your thoughts, does your actions, does the way you treat people? Because Jesus also said this when they asked him, "What is the greatest commandment?" And he said, "Love the Lord your God with all your heart, mind, soul, and strength. And then love your neighbor as yourself." He says, "This sums up the law and all the ten commandments." Says, "Loving God with everything and then love your neighbor as yourself." You got to love your neighbor. You got to love people. You got to love God ultimately because the way that you love God reflects how you're going to love people. And the way that you love people is a reflection on how you love yourself and also God. And guys, I just believe that God is stirring up the church. He is stirring up the believers say, "Look, there's no time for lukewarm Christianity anymore. There's no more time to be on the sidelines and not on the field playing it. there. There's no more time just to say you have the Christian jersey on just so that you can be part of the team, but you don't want to contribute to the team. And Jesus is saying if you want to be that, if you want to be that type of follower, if you want to be a fan of Christ, but not a follower, then I'm going to spit you out my mouth. See, what I noticed whenever I played football is that the players who played and who who got reps and everything was the ones that were good, right? It was the ones that were really good. But this is what I've noticed through the the training and offseason is that you had a lot of people that wanted the jersey of the football team, but they didn't really want the commitment. They they always looked nice. They always had their bands, the sleeves, and all the gloves. They always looked pretty, right? They always looked pretty cuz they were part of the team, but they never really played. And it was because some of them just wanted the jersey so much that they didn't really care if they played or not. They were just happy that they rep the jersey. And Jesus doesn't want that. He doesn't just want you to rep the jersey of Christ. He wants you to be on the field playing the plays that he's given you, the assignments that he's called you to so that you can go out and really make a difference. And guys, I just want to say that God does not want lukewarm Christianity. You have to choose today whom you're going to serve. Is it going to be God? Are you going to follow Christ? Are you going to follow culture? Are you going to follow your carnal nature and your flesh? But guys, that that day of Christianity, that time is over. God doesn't want you to do that anymore. That day of Christianity is over because your family is counting on it. Your children, your businesses, the industry that you're in, the schools that you're in, the people around you don't have time for you to be a lukewarm Christian. And ultimately, God doesn't have time for you to be a lukewarm Christian. You know, people's lives are at stake because of the way that we live. Because you may be literally the only Bible that someone reads. Hear that? You literally may be the only Bible that someone reads. And if you're not living out the life how God has for you, man, you're giving them a false narrative of the gospel. And God doesn't want that. So, look, I just want to pray for you. If you just feel like this really touched home for you and you really want to submit and you just want to get back in alignment with Christ so that you can be fully dedicated to him, then I want to pray this prayer for you so that you can start off 2026 on the right foot. You can start off strong so that you can also end well. So let me pray for you real quick. All right. Lord, I thank you for my friend right now that's watching this video. And I just pray that as they are just [music] seeking your face. I pray that my friend would just repent from all of their sins right now. [music] Repent from being lukewarm and instead, God, that they would choose [music] to be fully dedicated to you. I pray that you forgive my friend right now. And Lord, as they are surrendering their mind and their heart back to you to get in alignment to you, [music] that you're just flooding their heart and their mind with peace and that they would just feel that you are closer than a [music] brother. God, you're closer than anyone else, God, because your word says that you're [music] standing at the door and knock. And God, you're knocking right now. And I pray that they will let you in. I pray for my friends right now [music] that they will just start off strong, God, and that they will end well and be the light and salt of the earth, God. That they won't compromise. instead that they will [music] emit your rays, God. They will be your lighthouse, God. And when people [music] look at them, they know, man, that man and that woman is a Christ follower in Jesus name. [music] Amen. Well, guys, hope this video really blessed you. Um, thank you so [music] much for tuning in and I just pray that, man, why don't you just encourage somebody with this video as well? If you're not a subscriber, man, [music] please consider subscribing because, man, I would love for you to be a part of the family here so that we can continue to grow [music] together. But ultimately, man, I love y'all. Thank y'all so much for tuning in and y'all have a great day. Peace.</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>https://brilliant.org/rickyimpey
-Try Brilliant free for 30 days + get 20% off an annual subscription. || I`ve been printing for several years, but this video is one of the best and pleasurable one on YT for entry-level enthusiasts. Thank you for such a guide and good luck! || In my experience, soap and water is *much* better than IPA. Evaporating IPA can leave a residue on a build plate that can actually make adhesion worse.
-Even if I have something on my build plate that needs IPA to help remove it, I always wash it with soap and water afterwards. This fully removes both residual IPA and any deposits that soap is better at removing than IPA.
-Also, I would highly recommend drying washed plates using lint free wipes, rather than a towel or paper towel. Cotton towels can shed cotton fibres onto the build plate, while paper towels can shed paper fibres. Fresh lint free cloths don't leave fibres of any kind behind, and prepare the print surface in a way that results in maximum first layer adhesion.
-* IPA=Isopropyl Alcohol/Isopropanol, not India Pale Ale, International Phonetic Alphabet or Institute of Practitioners in Advertising || I’m about to buy a 3d printer, either A1 or A1 mini which one would you chose? || My first 2 prints failed but I relocated the spool and it works perfectly || Useful stuff || Just got a P2S. This is like the best video out there by a margin. Thanks! || @rickyimpey I've used numerous amounts of your guides and videos over the years and to this day still find myself appreciating your patience and revisiting for introductory users. Cheers! || Brazil uses 127V and 220V depending on the region</t>
+          <t>❤   Amen  🙏 
+        ALL  IN
+        💯    ❤ || Yes!</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>UCYyel9YAgwvs07rz5kugU7g</t>
+          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Ricky Impey</t>
+          <t>itsbasicbible</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>i3VycY5v-Tg</t>
+          <t>hb9G_3dqr9I</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Is It FINALLY Time To Buy A Desktop CNC? - Makera Carvera Air</t>
+          <t>Men Don't LEAVE 2025 WITHOUT HEARING This</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>I never wanted a 3D printer, I wanted a machine that allowed me to make the parts I needed. Is that machine now finally available for desktop use? The Makera Carvera Air certainly make a good case!
-*This video is sponsored by PCBWay*
-Custom PCBs, 3D printing, and CNC machining! New users can get projects started by saving $5 at PCBWay here: https://pcbway.com/g/0IW9ST
-*PCB Way Christmas Big Sales now on*
-https://www.pcbway.com/activity/christmas2025.html
-*Affiliate links (If you purchase something after clicking any of the below links I may earn a small commission at no cost to you. This is a great way to support the channel)*
-*Big Holiday discounts available for a limited time!*
-*Makera Carvera Air*
-https://makerainc.sjv.io/o42qDW
-Discount Code for $100 off - ricky100OFF
-*Makera Carvera*
-https://makerainc.sjv.io/OeNr0P
-Discount Code for $100 off - ricky100OFF
-*Dewalt Stealthsonic*
-https://amzn.to/4iCcnza
-*Makera Wiki*
-https://wiki.makera.com/en/home
-*Vacuum adaptor*
-https://makerworld.com/en/models/1054438-carvera-air-vacuum-45mm-adapter#profileId-1258778
-..............................................................................................................................................................
-BUY ME A COFFEE
-If you're enjoying my content, why not consider supporting the channel by buying me a coffee? 
-Even very small amounts are greatly appreciated and re-invested into bringing you better content.
-https://www.buymeacoffee.com/rickyimpey
-You can also use the YouTube 'Thanks' button above if you prefer.</t>
+          <t>This Video delves into the core issues holding many men back: a flawed identity rooted in fear, insecurity, confusion, and hesitation. These symptoms arise when one's identity is not anchored in Jesus Christ. The Bible teaches that God has given us a spirit of power, love, and a sound mind, not of fear. When a man is unsure of his identity in God, he hesitates and operates in delayed obedience, waiting for confidence. This hinders his potential and purpose. The key to overcoming these internal battles is not trying harder but standing firm in one's identity in God. When this identity is rebuilt, it transforms the mind, leading to shifts in confidence, clarity, and courage. Every man is created on purpose, for a purpose, and action must stem from a strong sense of identity in Christ.
+Connect 
+https://linktr.ee/itsbasicbible
+MALTA APPAREL LINK 
+https://malta-apparel.com/?ref=BBAZ16 
+FOR 15% OFF: basicbible15 
+FREE 10 DAY DEVO BOOK 
+https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
+I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
+https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
+I WANT TO FOLLOW JESUS CHRIST
+https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
+Get vidIQ to grow your channel faster! 🚀
+https://vidiq.com/itsbasicbible</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-12-07T17:01:18Z</t>
+          <t>2025-12-30T00:01:01Z</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>199792</t>
+          <t>28</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>3934</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>275</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>0.021067</v>
+        <v>0.142857</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -739,217 +739,83 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>What if the machine you really wanted when you bought a 3D printer finally exists? Now, I live 3D printers, but years ago when I first started looking for a machine to bring my CAD designs to life, I didn't actually want a 3D printer. What I really wanted was the ability to make functional parts, real solid components that could take load, survive in the real world, and ideally be made from metal. But desktop CNCs just weren't an option back then. There were huge, messy industrial machines that needed a dedicated workshop, and I couldn't afford them anyway. So, like a lot of people, I settled for a 3D printer. Not because it was what I truly wanted, but because it was the closest thing that existed at the time. And yes, 3D printers have come a long way. Today, you can make genuinely strong, functional parts out of advanced materials, but at the end of the day, it's still plastic. And for more than a decade, we've all been waiting for affordable metal 3D printing at home to finally become a thing. But maybe we've been looking in the wrong direction. Because the capability we've been waiting for, the ability to make real, precise, functional parts at home, might already exist. It's just called a desktop CNC. And if they do everything they claim, modern machines like the Mara Carvera Air might finally make functional part production at home a realistic option for normal people. This video is sponsored by PCBway. This Carva Air was sent to me by Makeer. I didn't buy it. However, Makea don't have any influence over what I say in the video. Now, before we go any further, I want to make something clear. I haven't just spent a week with this machine machining the sample projects and calling it a review. I've had the Car Bear Air for over 3 months and I've put hundreds of hours into it. I don't have a way to know exactly how many, but it's way more than I've ever done on any review before by a long way. I've broken tools. I've crashed jobs. I've pushed the for axis way past what it was designed for. And I've found every single place where this machine struggles and where it absolutely shines. And because I came into this with no CNC experience, I've hit every problem from a beginner perspective. So, if you want a video that shows you the real limitations, the bits the marketing doesn't mention, and the things other reviewers haven't run into yet, that's exactly what you're about to see. Because this machine is fantastic, but it isn't perfect. And I've pushed it far enough to know exactly where the line is. So, let me show you exactly what happened when I put this machine to work. The first thing I was concerned about when I agreed to try out the Carva Air was how much other stuff I'd have to buy just to get it set up and working. When I tried my first laser engraver, I was annoyed that they didn't send me any laser safe goggles. I had to not only buy my own, but I had to research what I even needed to keep my eyes safe. Maya assured me that almost everything would be supplied in the box, but to keep the price down on the air, there was no compressor and no vacuum for cleaning machine material. Whilst I'd never used a CNC machine before, I did know that tooling can get expensive. And the last thing I wanted to be doing on day one was researching what tooling I needed to buy just to make my first thing. I didn't have worried though, as the version I was sent came with a huge selection of tool bits, far more than I knew what to do with, and many of which I still don't know what to do with. The ones I use for almost all of the jobs I've run are the ones you receive in even the most stripped down, lowest price package. So, I don't believe you need to invest in the full milling bit package straight away. Save that for when you know you need more varied tooling down the line. What you also get is a comprehensive pack of material that allows you to make all of the example projects and a guide to show you how to make all of those example projects. You also get a manual for the machine itself. After looking through everything I've been sent, I realized that the Carba Air comes 99% complete and there's actually very little you need to do before starting your first job. I was a little stumped by the manual's instruction to check that the power supply switch was in the correct voltage setting as I couldn't find a switch anywhere. It turns out that my model didn't have one, but I only found this out by removing panels and peering through vents. Once I was sure that the voltage was right, though, I switched it on and it immediately moved all the axis to their home positions, ready to start, just like a 3D printer does really. I followed the guide which said to fit the arm to the side of the machine, but I never actually used it. The arm's there so that you can run the machine from an Android device if you have one. I don't, so I just used a laptop instead. Now, this is the first difference I found to something like a 3D printer. Nowadays, with 3D printer, you have an in-built controller with a screen that lets you run all of the functions on the machine. With the carba and I believe most desktop CNCs, it's a bit different. The machine has a similar control board to run everything locally, but other than one button, there are no controls on the machine itself. Everything is controlled by software that you run on a separate Windows laptop, Mac or Android device. This device initially needs to connect via USB, but after giving it your network details, you can use your Wi-Fi network to connect them wirelessly. In this way, the CNC machine is a lot more similar to a laser engraver than a 3D printer. I didn't mind it, but if I didn't have a laptop, Mac, or Android device that I was prepared to leave next to my CNC for hours on end, I might have found this a problem. Once you install the controller software on whatever device you plan to use and connect it to your Carva Air, is very simple to upload and run prepared G-code files. The example files come ready to go, and once you start the job, it runs locally. You aren't relying on your Wi-Fi network being active the whole time to prevent the machine from stopping. If you do want to stop a job in a hurry, there's an emergency stop button that you need to put somewhere obvious. And of course, one hit of the button and everything stops immediately. As I said, there is one button on the machine which is at the top and it's used for telling the machine when you've completed a task like fitting a probe or changing a tool. The Carva Air relies on manual tool changes unfortunately, but its bigger brother, the Carva, is able to complete automatic changes to the next tool you want to run when one operation is finished. When it comes to setting up the first example jobs, first you need to fit what's called spoil board to the bed, which is a sacrificial layer that you slightly cut into, which allows you to cut all the way through materials that are sitting flat. Unlike a 3D printer with a CNC machine, you need to secure the material to the bed with some kind of clamp or fixture. And the Carver Air comes with a number of these and other fixings and guides to line everything up. What I really liked about the example jobs that I started with was that the guide book actually shows you exactly what clamps to use and where, so that there's no room for error while you're learning the basics. The example job guide also tells you what tooling to use. So, all you have to do is find what you need in the supplied tool kit and have it ready. I started with a 3D relief that's machined out of epoxy board. So, after fitting it down as shown and getting my tooling ready, I was able to select the cutting file as shown in the book. Once you have the file load in the controller software, you can run through the tool path on screen to see what it plans to do before you hit start. But before you hit start, you have to tell it whereabouts on the bed you want it to start, just like a laser engraver. You then hit run and you're told to load the probe. The probe is a combination of something very similar to a 3D printer's touch probe and a laser pointer. After probing a calibration post on the back of the bed, it then draws a box around the area it will start machining. With the example jobs, you're given all of the correct offsets to use. But when you come to aligning your own jobs, this is very useful to make sure you've not got something wrong. The probe also then, just like a 3D printer, probes the material you're about to machine, so it knows where the top surface is for when the tool is fitted. It then returns to its starting position, and you're instructed to fit the first tool. As I said, tool changes on the Cera Air are manual, but they're also very quick. All you have to do is pull down the lever on the side, and one tool drops out. You then insert the next tool and lift the lever back up, and it's done. All you have to do then is press the button on the top to say that you've changed the tool and after probing the post on the back of the bed to set the tool height, the spindle starts and your job starts to run. It's best to close the cover before hitting the button for safety and to prevent any of the machine material from coming out and making a mess. I was actually surprised how well the cover works at keeping the mess inside the enclosure. Whilst the cover feels a little flimsy when it's up, when it's down, magnets hold it in place and there are brushed strips along all the joints that work really well at containing everything. For this job, I just let it run without any kind of vacuum or compressor as I didn't have either, which meant quite a lot of buildup of material as it's removed but not moved away. I couldn't really see what was going on. So, I went and got a portable vacuum we use in the house and tried putting it up to the port on the side of the machine. There's a vacuum shield around the cutting area, which works really well at providing a contained area for the vacuum. Even this small portable Hoover just pushed up to the port did a really good job of removing most of the waste. Once the roughing's done, you get a beep to tell you it's time to change the tool to a finishing bit. And then off it goes again. This time taking a different path to pick out all of the detail of the design. You then switch back to the first tool so that it can cut your piece out, leaving only a few tabs in place that you remove by hand afterwards. With a little bit of clean up with the supplied sanding block, you're done and you've completed your first CNC job, which I have to say is of a very high quality. When you're used to 3D printed parts with their layer lines and Minecraft looking steps on curves, seeing these super smooth surfaces from a desktop machine is very impressive. And for three axis jobs at least, that's it. That's the whole process that you basically just repeat for each job. The only thing that changes is the way you set up the tool paths in the CAM or computed aided manufacturing software, which I will get to in a minute. Next, rather than just running through all the example jobs, I wanted to learn more. So, I decided to change the design on the LED lamp job. With this job, you machine an acrylic base that houses a supplied PCB board and an aluminium button that you machine yourself into this. You slot a clear acrylic panel that you also machine. But I wanted to change the design and add my logo. Now, firstly, not only did everything go exactly as shown in the guide book, but I was very impressed to see the absolute precision with which everything fitted together. I keep coming back to 3D printing analogies, but I feel like so many people have 3D printers now. It's the most relatable comparison. With the melted plastic in 3D printing, this kind of precision is unthinkable. If you want something to fit together this well, then it either takes some trial and error with changing tolerances or you simply have to finish the part yourself with a file or a knife. It was at this stage that I also treated myself to a new shop fact. Not because it was absolutely necessary, but because I needed one anyway, and this made a good excuse to get the one I wanted. I bought the DeWalt supersonic which I can highly recommend if you need a shopvac. The sound of the air going down the hose is actually louder than the motor noise and it has an extremely good amount of suction. I 3D printed a fitting that bolts to the side of the cara. So anytime I want extraction, I just plug it in. As I say, you don't need to go out and buy a new shop fact just for this machine. But for threeaxis or flat jobs, some kind of vacuum helps. But you can use anything for this, even a household vacuum. For modifying the standard design of the lamp, I needed to learn how to use mayer's cam software, which is very cleverly named Mara Cam. Make cam doesn't have to run on the same machine that you use to control your cara if it isn't on the same machine. You just have to transfer the output file in the same way that you do with a 3D printer or a laser engraver. I've come to find that maker cam is relatively simple to use. But just like any new software like this, I was a bit lost the first time I fired it up. You don't have to worry though as unlike a lot of 3D printing manufacturers, Mayera have put a lot of effort into providing resources to help you understand every stage of using their machines. They have an extremely comprehensive series of videos on their YouTube channel and a wiki page where you can read about anything to do with using one of their machines. This really impressed me and even after months of using this machine, I still refer to the wiki and Makeer's YouTube channel to this day. It didn't take long for me to find the right video that guided me through what I needed to do to add the logo to the lamp design. Once this was done, I also needed to choose what tools to use to actually machine it. Again, this does have a steep learning curve that is helped massively by a make error. Within make error cam, there's a tool library. You do need to know some basics about what you're trying to achieve with a tool and what material you're trying to cut. But once you've selected a couple of simple details, default values are pulled through into the tool path window so that you don't have to sit and calculate things like chip loading, feeds and speeds, and any of the other headacheinducing jargon that turns most people off of CNC machining. All of the complicated stuff is handled so that you only need to make a couple of decisions. It's not quite as automated as using a 3D printer slicer, but it's similar to setting up a laser engraving job, which is pretty simple once you've done it a few times. I was fully expecting my first bespoke job to be a complete failure, but to my surprise, it turned out perfect and better than I ever could have imagined. I'd avoided CNC machining for years because it seemed so complicated. But with the way Maker have everything set up, it wasn't anywhere near as daunting as I'd thought. And actually, this is a good moment to talk about today's sponsor, PCB Way. If you want to get something CNC machined, but aren't yet able to invest in a desktop CNC like the Carvera Air, then PCB Way is the place to go. Alongside their well-known PCB fabrication and assembly services, PCB way also offer full CNC machining in aluminium, brass, copper, steel, and engineering plastics. And the entire ordering process happens directly on their website. If you go to the CNC machining section, you can upload a step file, choose your material, surface finish, tolerances, threads, and you get an instant quote right there on the page. It's extremely straightforward, especially if you're coming from the 3D printing world. And if you're working on electronics projects too, they make PCB manufacturing just as simple. Upload your gerbers, pick your board thickness and solder mask color, and you can preview the price before ordering. It pairs really nicely with what this desktop CNC can already do. You can prototype PCBs at home and then get a full production version made properly. So whether you want precision machine metal parts or professionallymade circuit boards, the whole process on PCBway's website is very intuitive. Check out PCBway.com for more information. Now that I had a couple of successful CNC jobs under my belt, I moved on to the part that I was most excited about, which was fourth axis machining. Three-axis machining, surprisingly just uses three axes, X, Y, and Zed, or Z. What the fourth axis does is introduce another axis that rotates your material, allowing you to machine shapes that don't have to sit flat on the bed. This means that you can machine all sorts of different shapes that you otherwise can't. The fourth axis just bolts down to the bed and is precisely aligned with locating pins. The stated maximum stock size is 92 mm diameter and 200 mm long, but I'll tell you in a bit why I found that to not quite be true, and I did thoroughly test it. You can't run the dust shoe around the spindle when you use the fourth axis, which basically rules out using any kind of vacuum. Instead, especially with materials like aluminium, you're advised to run some kind of compressed air to clear machine material away from the cutting area. I didn't have a compressor to use for this, but I did have an air assist pump from a laser engraver, which is actually pretty perfect for this job, and you can pick these up for around $20. And they provide just enough of an airirstream to do the job. And they're quiet and small, unlike most shop compressors. There is a fourth axis example job using epoxy board again. So, I followed the instructions and set it running. I was beginning to trust the Carbara Air a little now, so I dared to do some other stuff while periodically checking in on it. When I returned, I found that the air assist and lack of extraction had meant that all of the cut material had been blasted all around the inside of the machine, which looked like it was going to take ages to clean up. However, I was really happy to see that as it was all dry, it vacuumed up really easily, especially with my new DeWalt machine. So, just like with three axis jobs, after roughing the shape out, you change the tool bit to a finishing bit and let it do its thing. Again, the result is beautiful with every tiny detail picked out. For anyone used to making small figurines with an FDM 3D printer, this kind of quality is pretty staggering and only usually possible with resin printing, which unfortunately also comes with a lot of mess. It was at this point where I'd had enough with the example jobs and decided to learn how to use make error cam to create my own tool path from scratch. So I found a chest piece STL file and imported it. Make error cam can work with a number of file types. You can import 2D files like SVG, DXF, JPEG, PNG and bitmap. Also Gerber files for PCB layouts if you want to make PCBs with your cara air which you absolutely can do. You can also import 3D files in the form of STL, OBJ, and step files. The chest piece was an STL, which I believe I found on Maker World. I tried to keep things simple by using the same single flute endmill that Maker seem to use for roughing out all of their example jobs, and then finishing up with the same 0.3 mm 30° engraving bit. All I did was select hardwood when selecting the tool. As I was making this part from oak, and again, default values were pulled through. I was curious as to when I might need to start looking into how these different settings affect the way the tools work. And you can absolutely dive head first into all of that information, but with Mara Cam, you don't really have to. I actually being the curious fellow that I am asked chat PT about what all of the settings meant. And whilst I learned quite a lot, I was happy to continue using the default settings, at least for now. To get the material ready, I cut it roughly to the right length and then drilled a hole in the middle for the tailtock to locate in. Very much like the example fourfaxis job. This went really well. But I did actually run it again as the piece of oak dal I used had a split in it which I hadn't noticed. I was really keen to machine metal though and happened to have the same diameter piece of brass which I prepped and set up the same way. Unfortunately, this was the first point where my inexperience showed. As soon as the longer tool touched the stock, it shattered. This, I learned, was a combination of a longer tool that needed different settings and me not understanding that it's pretty important how the tool enters the material, especially with harder stuff like metals. What I should have done was enabled ramping, which gently moves the tool from side to side while plunging or moving down to avoid overstressing the tool. I also used a shorter tool bit to reduce stress. All it took was watching another video or two to learn this, but I was too impatient to get started with making shiny bits. Whilst it takes a bit longer as you have to machine material away in smaller steps, machining things out of metal follows the same process as any softer materials. Another lesson I learned on this job was that when creating a roughing tool path, it's best to leave a little bit of material rather than machining all the way down to the model surface. Also, this is where I believe I found one issue with the way Maker Cam handles fourth axis jobs. You see, you can set what's called a depth allowance when creating a tool path, but from what I can see, it only adds an allowance to the Z axis. It doesn't leave an allowance all over the model. To do this, it would also have to add an allowance on the X-axis, which it doesn't. What this means is if you have any vertical or nearly vertical surfaces, the roughing tool will machine right up to the model surface. When you try to follow this up with a tool with a smaller end, because of the tool geometry, it can't get in as close to the vertical surface to clean it up. This may be a common thing with this type of machining, but it seems that allowing an offset in X as well as zed would leave a cleaner final surface, even if it might not technically be as dimensionally accurate. Anyway, I made it work, and with a bit of cleanup, I'm really pleased with the result. From here, I tried to use the Carvera Air to machine some polyurethane skateboard wheels, which meant 3D printing a fixture to be able to hold it in the chuck, as the external diameter was larger than the chuck would go to, and there was no internal diameter that the chuck could grip. This job was also where I discovered the limitation on stock diameter with the fourth axis. 92 mm is indeed the size of material that technically fits in the fourth axis if you find a way to hold it with the chuck as the jaws don't go that big. And technically, if you use a very short bit, the spindle will clear the material and be able to machine it. However, firstly, if you try to use the probe on anything over about 76 mil in diameter to line the job up, it will crash into the stop and break it. You can turn this off though, which gets you around that problem, but if you forget, it's bye-bye probe. However, the bigger problem is that no matter what settings you use for safe positions and clearance height, with stock this big, make cam will try to move the tool to a Z position that triggers the Carva Air's soft limits. These are firmware axis limits that keep the machine from moving to the actual axis physical limits and triggers a tool path ending error when it reaches that section in the G-code. There's no reason to try and move this far either. I found that trying to move to anything over about 39 millimeters on the X-axis triggers the soft limit which actually gives you 78 mm of usable stock diameter without triggering the limits. However, even when your stock is smaller, make still tries to move the tool above the 39 mm limit. You can turn the soft limits off in the controller firmware, but I wasn't comfortable doing this. So, what I did instead was manually modify the G-code. This was only a case of using Notepad++ to search for any Z coordinate above 39 mm and reduce it to 39 mm and then the job runs with no issue. I was happy to do this as to a degree I understand the G-code, but how many others will want to do this? I imagine not many, and I'm sure it's something that could be fixed in the software. Knowing about this bug, I decided to see if I could make something that used a full usable fourthaxis capacity on the Makeer Carva Air. So, I designed a trophy using a CAD file from a crash helmet I found online and then a support that I modeled myself. The idea was to make a trophy for a fantasy Formula 1 league that I'm part of and incidentally have no chance of winning. Setup was a lot more difficult as I don't have any kind of band saw or chopsaw to cut through 3-in of solid aluminium. So, I had to do it with a hacksaw which took ages. I actually did it over a few days, cutting until my arm gave out and then coming back later to try again. I did it though and I also had to 3D print a step down end cap which I drilled, tap, bolted, and glued to the end of the stock. Everything started well and after quite a few hours of machining, the shapes were starting to appear. Unfortunately, it was at this point that I ran into the first drama with this job. I had a power cut. And unlike a lot of 3D printers, there's no default way to restart a job once it stopped with the cara. I really didn't want to start the G-code from scratch and leave the job air cutting for hours on end until it caught up to where it got to. Whilst figuring out what I was going to do, I tried to open the job up again in Make Heracam, only to discover that whilst there was a save file, it was empty. I'd lost all of the information about model position, scale, everything. I still had the G-code from the roughing tool path, but I hadn't yet created any other tool paths, so I had no way to finish the job once the roughing was done. This was almost a disaster for me as I didn't have it in me to cut through another 3 in of material by hand or repeat all of the other work done so far. After a lot of measuring and after hours of work, I managed to approximate the position of the main section, which was the main part I was worried about. It took a lot of trial and error with small changes and lots of saves. But I discovered that if you try and work on a model this complicated and of this size, the resulting tool paths create such huge G-code files that saving after creating a tool path causes makeanam to crash and not save. The workaround is to save a backup before creating tool paths. So at least you don't lose everything if it falls over like it did with me. So, the only way I could continue the job roughly from where I left off without air cutting for hours and hours was to again manually modify the G-code by chopping out all of the completed code and then hacking what was left to trick the machine into thinking it had already completed. Well, it hadn't. It worked, but it wasn't pretty. We don't have time here to go into all of the issues I found with this job. But by this point, I felt it was time to talk to make error and ask them why I was having all of the problems that I was encountering. Expecting the usual response of either not really understanding the problems I was having or somehow implying that I was doing something wrong. I was pleasantly surprised to get a very open receptive response. I was asked to provide details of the issues and I also sent over all of the information about the job I was trying to run so that they could try to see if they experienced the same problems. After confirming that there were some issues with Mera Cam when using the fourth axis section, Mera said that they were working to iron out the bugs. They explained to me that they began as a machine manufacturer and that they used to advise that users use other CAM software. However, they realized that these other software options could be overwhelming and complicated. So, they decided to try and create their own with the aim of making it userfriendly. They admit that Maceram isn't perfect for all applications. And after I sent them all of the details of what I was trying to do, they advised that most of the issues I was having was because of the size of the part I was trying to machine and the level of detail I was trying to achieve, which I have to agree with. The smaller foraxis jobs had very few issues. Maker actually encouraged me to share all of the issues I'd had with my viewers. They didn't shy away from them, and they also pointed to their GitHub report page where users can leave their issues so that they can be fixed in later versions. Once this video is finished, I will do that and then all of my findings can go into improving what could be very useful free software once all of the bugs are ironed out. So, eventually I did get the trophy job finished, but not before I messed up one stage of G-code hacks, which meant that I sliced out a section that shouldn't have been machined, which I then filled with epoxy to try and hide it. It didn't work. After some clean up with some files, wet and dry, and my fantic rotary tool, I've eventually ended up with a piece that isn't perfect, but I'm very happy with the result, especially with all the drama I had to go through to get it. Just for fun, I 3D printed the same file on my Bamboo Lab P2S. And while the 3D printing took a fraction of the time, I know which one I would rather have sitting on my mantle piece. So, what I learned from this mammoth job was that if you want to machine larger diameter hard materials with a lot of detail, make cam is not going to be the best software to use until it's improved further. However, for slightly smaller diameters and all three axis jobs, it's very good. And with all of this said, all of the problems I had were softwarebased. The Carva Air has never missed a beat. It's awesome. When the software catches up, this will be one hell of a package. So, let's quickly go through some of the things I haven't covered, but you will want to know. With threeaxis machining, you have a work area of 300 by 200 mm and a stock tooling height of 130 mm, unless you need to use longer tooling, in which case that height is reduced so that you don't have the tooling crash into the stock. As we discovered, the fourth axis size limitations are more softwarebased, and if you want to avoid all the issues I found, you probably need to keep the stock diameter below about 60 mm. Once all of the bugs are worked out though, larger diameters should be less hassle. The spindle is 200 W and is spec to 13,000 RPM. However, the hard limit is actually 15,000, which I tested quite a bit. The standard collet size is 1/8 of an inch or 3.175 mm, but you can change these to 1/4 in and 6 mm versions if you want to use other tooling. Cooling is by air alone, which basically means there's no cooling, just a tube and a nozzle that you can blow air down to remove chips. There's no liquid cooling option, which does limit what you can machine. Make say that machining steel and titanium is possible, but it's not advised for prolonged processing. What you can very realistically machine is wood, foam, plastic, carbon fiber, and softer metals like aluminium, copper, and brass. As we've discussed at length, the software Maker advise you to use is Maker Cam, which is pretty good, and it's free. However, there are other options, and it's very likely that there's a better option for fouraxis machining, but it won't be free. Other CAM software that you can use with Makeare is CNC machines includes Fusion 360, Solid Works, AutoCAD, VCarve Pro, Aspire, and Illustrator. Since I started my testing, controller software compatibility has been updated to say that it now works with iOS as well as Android, Mac OS, Windows, and Linux. So, there are a lot more options when it comes to controller devices. Now, there are also plans for a very soonto-bereleased new software called Makeer Studio, which should make it even easier for beginners. From what I've seen, it adds a 3D printer style UI to Make Cam, which should make it more familiar to 3D printing users and reduce the steepness of the learning curve for beginners. I did ask, but unfortunately, Mera Studio won't resolve all of the fourth axis issues I encountered during my testing. Those will have to be resolved in future updates. Make error also plan a ba</t>
+          <t>What's holding most men back isn't their circumstances, their age, or a lack of opportunity. It's actually their identity. Their identity being rooted in fear, insecurity, confusion, and hesitation. And these are not personality traits. They're actually symptoms of identity, not rooted in Jesus Christ. You see, the Bible says that God did not give us a spirit of fear, but of power, love, and a sound mind. So if fear is leading your decisions, it didn't come from God. And when a man doesn't know who he is, he begins second-guessing himself. He begins acting in delayed obedience. And he is waiting for confidence before taking action. And that's how potential and purpose stays locked up for years. But when identity is rebuilt, the mind is transformed. Everything begins to shift. Confidence follows, clarity follows, and even courage. You don't overcome internal battles by trying harder. You overcome them by standing on who you are in God. You were created on purpose, for a purpose, and with the purpose. An identity will always precede action.</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>How is the noise level with this machine? || Delivery to the UK is best part of 2 months.... || The spindle Power is 200W. Yeah, if you want to have an actual CNC at home, you should might be looking at the DMC 2 Mini, which has a real Spindle to do work with.Thank me later. || a 3d printer is a cnc machine. cnc is not an indication of what kind of machine it is, cnc means that it is run by a computer rather than by a human manually || I love the machine, hate the software. I bought it mainly for the 4th axis. Even though it has a surface probe, you can't make it engrave on a curved surface. Like say you have bracelet or mug, the soft ware can't work an end mill on  the surface. It can create a say a pot handle with a fancy inlay  from a raw stock, but you can't make a fancy inlay on a pot handle you already have. The machine is structure so it supposed to be "automatic" . but coming from a manual CNC with a manual z probe and manually changing end mills, the work flow doesn't make sense. I got it as a kick starter but hardly use it. I use my Woodmads much more, fast, simple to setup. So until they improve their software (or I pay for SW with true 4th axis support) it sits and waits. || metal ? Why did you not start lost PLA casting in Sand ??
-also how do you know you hit every problem from the beginner perspective, how do you know where the line is ?? || 0:20 Absolute bollocks. I've had my 3-axis Chinese desktop CNC mill for at least a decade now if not more, and it was about $500 when I got it. Not particularly great at cutting metals, but it WILL do that too for softer ones if I insist. I even cut a bunch of holes in cca. 1mm thin steel sheet with it - slowly, sure, but it did that too. There's nothing "but now..." about any of this. || Is it catproof? || The results speak for themselves. If I had a use for making my own parts at home, I'd definitely go for this over a 3d printer. || Well I cant afford this right now but I think you've sold me on buying this when I can. || Was stoked to see the same model 3D printer that I also bit the bullet on || Great video.  You talked me into both buying one and then changing my mind lol.  Seems like we are at the first stages of 3D printing…. Very slow, and very small.  I look forward to the next gen of systems. || I bet you could cut soapstone with this, I find it easier to carve than most woods. || Every single review i see of carvera is always donated or sponsored by carvera. I have not seen a single review unsponsored.... || 5,000 to more than 6,000 Euro for a machine that has been made in an anti-Western and highly oppressive authoritarian country. Not with me, sorry. || it always important to keep absolute origin in material you work on so to can rebuild the project. Estimate the location of the stop , open the gcode in notepad, paste into AI tell her something like "it stopped  1.27cm from the neck rotated 70deg from origin clockwise please rebuild gcode at this location minus few steps before" it will build an gcode image in its mind, and rebuild new gcode. open in notepad and save as gcode extension,  load the new gcode to continue. if you had absolute origin marker you tell her that your head is on the origin so it can jump to the new location without any offset errors || $2.5k - $6k for a curiosity hobby?  Yeah no....Basically, this is for people who plan to make money with it.  This is not a hobby machine in that price range.  Unlike a 3d printer. || damn.... i see the '' i want one '' but i imagine it must be way way expensive for material and the machine itself is ouuuuuuuuu || You talk too much and show too little. || Wow, basically 3000K for the model he is showing. I will stick with 3D printing. Give this tech another 5 years. || Producing the part is not the problem, get a file to send the machine is the problem. Really good 3D scanners are super expensive. || These Carvera machines are available in Australia for anywhere between 4k to 10k. If you just wanted them to print trinkets for your family and friends, I'd n never recommend it, but if you have a business like mine, that prints functional or essential parts for other businesses, like hospitals and hotels, then this is an investment. || 4:35 I have a cheap CNC machine for under $300 for more than half a year now, and it has offline controller actually.
-All I need to do is plug in a flash card with GCode file(s) and start them running.
-Actually it's my preferred way of working with the machine because it doesn't depend on my computer whether it's on or went standby etc. || "Makera has no influence on what i say"
-continues to NOT mention the price. What "real" review doesnt do that? Especially when its about an affortable product for "normal" people. || Get yourself a Milwaukee Sawzall buddy. You can put a longer hacksaw blade on it and a Sawzall is a tool you can use to cut many many things. || HGR Industrial Surplus occasionally has CNC's for a fraction of the original. (Near Cleveland, Ohio) || If you looser in precisson on 3D-printers an 0 in materials understandng - you get all the problems. It's not the problem of 3D-printers, problem is YOU. I'm 3D-printing for the 8 years and ger precise results in every print, cause I know how setup my printers by materials, calibrate and print. Thats why I say YOU"RE INCOMPITENT IN 3D-PRINTS. You're just make low-level revews that did not mean anything, cause you're bad in printing 👌 || Yet, I only want to see damn thing running.... || Not with this price || Same fails on design, but lowered price and updated software access. This is why printer was moved forward widespread. Basically.. CNC is the logic product movement of Apple mindset. "Peasants, they dont deserve it." Laughable that mess still refusing to be resolved. || Are there Linux-drivers for this? || CNC a space marines ? || its too much money and hassle with materials and tools.
-If you have the money you might have it for a professional machine. || Custom shifter knobs sell 30 machine pays for itself.  You're welcome . || This is not for the "normal" people. || Roland made their CAMM3 desktop mill almost 40 years ago || word?
-...
-I want it || I think a lot of people are missing the point. This is a very nice piece of equipment and not for the “curious consumer”. There really isn’t one that is worth a darn for the curious consumer. This is for a prosumer or a wannabe engineer. 
-If you want to CNC for $1000 you’re gonna have to build it yourself. The good news is, you can totally do that. Start with DIY CNC on the googs. || zzzzzzzzzzzzzzzzzzzzzzzzzzz || Nah, I will wait for it to get cheaper and better. || Carvera told me in an email that this machine requires an internet connection to use. Meaning that if you buy this machine YOU DO NOT OWN IT. This is unacceptable for a $3,000 piece of equipment. Carvera lost a customer due to shady enshittification tactics. Do not accept this kind of behavior. Let them know it is unacceptable || 3D printers USE CNC, it stands for computer numerical control. Youre just talking about CNC tools that work with metal. Please dont confuse the world even more. || LETS MAKE GUNS!!!  YOHOO  PEW PEW PEW || The English stopped having kids because they no longer feel at home in England. Personally i would welcome a falling population and a falling GDP. A reduced workforce makes labour more valuable and transfers money from the rich to the working and middle classes, this is why the privileged freak out at the idea of a falling GDP. || I'm not even on here to watch the video, just comment on the thumbnail. you cannot even draw a fair comparison between FDM and CNC with those result pictures because the CNC'd picture has clearly been finished and polished whereas the FDM print looks raw/unfinished. || I mean...CNC is cool, but it's not capable of even half of the complexity of 3D printing. It can't make internal bits that work together straight off the print bed. Additive manufacturing is capable of so, so much more than subtractive. A desktop CNC certainly has it's place though. Imagine if you could carve a full sized helmet with it. || this is thr best review I think i've ever seen . You haveyou've no music, no extra B. S to try and make it longer . new sub
-thanks || I would consider updating to this but I ineed to deal with far bigger dia wood than the 4th axis can cope with :| probaably 150mm with a cut depth of 60mm || If it can make detailed warhammer miniatures i will buy one. doubt it though. (ps..sarcasm) || You have a very quiet voice. || Damn, I didn't know that this was a thing obtainable by normal people. I have very few projects for it, but I want one! || Yeah, cause "normal" people can afford the price of this so casually. || @thrrax Between $2500 and $4000? Normal people spend 10x for a car. || You bought a cnc machine but are stupid enough to use chat gpt to ask technical questions tells me all I need to know how valuable your thoughts actually are. || "implying something I was doing was wrong"
-After describing that you had a power cut, and that you tried to restart a job by manually measuring/positioning restarting a print.
-I wonder if you'd just restarted it from scratch if you would have ended up with a part sooner than the futzing. || Recommended for complete beginner to 3d printing in general? || If it cant print warhammer minis it's not what i want. || Выглядит не плохо, но скорость не высокая для качества , мне кажется 3дпечать будет быстрее. 
-Зависит конечно от целей. Станок сам по себе интересный. 
-Но на практике огромное время работы, количество сломанных фрез, сделает конечную деталь крайне дорогой. На одну деталь может уйти не одна фреза каждого вида, просто из за того что они тупятся и заточке не подлежат. 
-Если речь о фигурках то себестоимость пластика намного меньше и работы 3д принтера чем ЧПУ фрезерного по металлу. 
-Уборка стружки отдельный гемор )
-И как я понимаю ограничение только  деталями вращения. 
-Для дома и прототипирования вариант очень крутой. Хотя степеней свободы не хватает, для токарной составляющей, не универсальный вариант для любых деталей. || At best you could get a wood cnc machine for the desk. They could also do plastic. || Don't you have a machine shop nearby that can cut that aluminum billet in seconds? #MakeFriends || Wow, a $2,500 CNC-machined solid metal piece that you polished by hand will look better than a 3D print from a consumer-level printer in generic gray PLA with low quality slicer settings and no sanding or post-processing of any kind??? Shocker. || Si può usare nel dentale? || Wow!!!! || Fyi...$2500 - $3000! || cuales son los precios, y serviría para mecánica dental ? || That FOOKIN NICE BUTT PLUG U MADE || I've worked with CAD, CAM, and CNC machining—using software like SurfCAM, CAMWorks, SolidWorks, Mach3, the excellent Centroid control software, and G-code itself—for many years. I started with a custom-built CNC machine and later retrofitted a Bridgeport mill with a Centroid kit (which I highly recommend, by the way).
-CNC machining is far more challenging than operating a 3D printer. It will demand a significant investment of both time and money. Make sure you have a solid business plan in place before diving in—you've been warned! || You might be able to fix your 4th axis wall issue by lying to your program about what size of tool your using in the cam for the roughing tool path. Tell it you’ve got a .270 diameter tool when using a .25 to effectively use wear offsets in software instead of at the machine. || imagine, people start making replacement car parts at home... || It’s already a thing for all the plastics. || Depends if forged metal or not... If machined part, sure absolutely provided match the performance of the original metal or material. Lots of details people could overlook. || Hot Take here: mechanical failure due to improperly made part YOU designed sends you into oncoming traffic, YOU will be found at fault. || nice video. Thanks || Good review.  I've been looking at these for some time for machining prototype parts and, as noted in other comments, the prices have really dropped while the capabilities have gone way up.  I may have missed it, but does this model rely on connecting to a remote website for operation ?
-Any make/model that relies on an internet connection I would not consider purchasing. || This needs to be $1000 || Dream on. You would like a Lamborghini for $1000 too but you are not yet in the real world.  Once you get your college degree in a good paying STEM field the $7 to $8 grand of this machine will be affordable! || @glasslinger lol you have zero vision. Stay in STEM || Four axes? Is that a new dimension??? Cause we live in the 3D world (meaning any point is defined by x, y and z coordinates). || Axis is not the same as dimension. There are 3 spatial dimensions, but there can be theoretically infinite number of axis of movement and/or rotation within those 3 dimensions. || 27:43 Well, in fairness, you did a LOT of finish work on the metal piece and NO finish work at all on the 3D printed piece....... || Would it work with Freecad?  Yeah I heard that the makeracam software was a bit buggy.  This is what happens when marketing depts drive the release dates of new products.  Engineering says 'we are not ready for production', marketing says 'but we have a full marketing and release planned for this date', and enevitatbly marketing wins because it means dollars coming in the door sooner. || Nice video || You talk way too much || I am kinda concerned about the opposite; the non-CNC machining of old.
-Should a WW3 happen, the old non CNC precision tooling will be as precise as always, while the computers controlling CNC would be no more.
-/John Titor may have wanted the IBM system for a machine cutter? || where do you buy solid blocks of material? || I’m glad there’s gonna be Linux support || As an more 'advanced' feature - would be good if it had polishing bits along with the software knowing how to apply the polishing bits to the job just cut for metals. || This just screems Try to machine mill a Warhammer 40 000 Mini. Please do it ! || Minecraft looking lines hahaha, oh man thanks for the laugh || You should be able to use the GOTO command to skip through the Gcode assuming its standard Gcode
-GOTO1
-;
-;
-;    &lt;- all this gets skipped 
-;
-;
-N1
-We use this on AMADA lasers whenever we get a trace error. || I’m a toolmaker 45 years retired…. As for your cutter issues, I would recommend carbide always and do your research because the prices of these cutters very widely, but they can be found in those ones are affordable……. But to my point…… there’s a cutter out there. You can get it in high-speed steel you can get them in carbide you can get them with a coating to make them last longer Each one has their own issues but what it does is it manages the chip in such a way or you can go faster, much faster use a water-based coolant a must so look into cutters called rough cutters you use them to machine your part usually oversize 10 or 15,000 then you go back in with a carbide  and mill and you do the finish pass cheap affordable software is called (sharp cam) an English software developer very nice software. Very easy to use you’re welcome || Make a cap shaped thing to fixture to. Run the jaws out in the cup. And whala turning full size 😊 || Please face the camera and not the ceiling || Wonder if mastercam could work with it. and nc code to g code would come out good. || Travaille le bois tu saliras moins ton environnement avec des copeaux toxiques pour tes enfants 😂😂😂😂😂😂 || Thanks for this great video.......Although I think its going to cost me.........:) || ❤ dreaming to have one || Yap..!  3D printers are not suitable for all purposes...! 
-Though metal 3D printers may be preferable but they are too expensive for small workshops...! || 4:40 well, 3D printers may have displays, but i would say that most people theese days, who for example do build their models use pc as well, especially because all modern units already have wi-fi. || Yeah, and that’s the point of the android tablet is to serve as the HMI. It’s highly recommended so not doing it as kind of weird when you can buy one for 90 bucks. Considering the cost of the machine it’s also kind of weird they don’t just include one || *Great video* - I got my Carvera-air as one of the kickstarter backers, and I did not have time over summer to start using it - Last week at XMAS, I finally started using it. Very impressive indeed. Also, the learning curve into CNC ist very steep indeed. Glad I waited until I had a couple of days to dig into this.
-About your _'air assist pump'_ (16:06): How many liters per minute does yours deliver? || One doesnt replace the other, additive manufacturing vs substractive, there are things you can 3d print that you cant cnc and vice versa, they have overlap but one machine doesnt replace the other || There's absolutely nothing I CAN (reasonably) make on a CNC mill that I would want to make on a 3D printer though. Replace? No. Trump? Yes. || You did a nice job of hiding how poor this thing mills.
-Any one familiar with milling can see this thing can barely mill plastic.
-Metals though are nothing but chatter || Should have just let it run for a couple hours milling the air. Trying to hack it was the cause of all your troubles. || The worst thing about cnc machines is cleaning metal splinters, my hands are always full of it, and i have to dig them with a needle and tweezers. 😂 || gloves? || you should be milling metal with water/oil solution and just wash them away to the deposit and then filter it || Desktop CNC machines are hardly new. Businesses usually avoid them because they compromise stiffness, accuracy, speed, vibration damping and work envelope . All things that matter if you intend to make a profit or if your hobby involves larger parts like guitars, sports equipment or furniture etc.
-If space and cash are tight my view is that you want to be able to do as much as possible on one machine. I find these tiny machines to be too limited. 
-Remember you'll lose some of your work envelope to clamps and other work holding devices. + you'll want to be able to cut down larger pieces of wood and metal even for smaller parts. 
-I never regretted having too much work space. I definitely regretted the opposite || This is great. Probably will wait for the Z1 to get one. I am very much a hobbyist so getting the Air is hard to justify. || CNC is a totally different world. It is complex in terms of how to plan your cutting path and which and when to switch tools. Esecially with cam, it is something people have a degree in cad and understanding of material and multiple runs and changing the orientation. 
-With 3D printing, you can at least create a model you can use to make mold with bentonite clay and iron cast it.
-Or, cast a rough dimensions and then let cnc finish it. || you used to need a degree to work with anything 3d, not anymore now days, no worries, it comes in cnc to. || I don't know your background, so my apologies if I am teaching you to suck eggs, but swarf removal is crucial with fine machining using small diameter cutters as it can break the tools, and mar surface finish.  This is usually done by washing the swarf away with a jet of soluble oil or similar cutting lubricant, but blowing away with air works almost as well.  Cutting lubricant is not an option in this case, and I am not sure how effective the vacuum is going to be. || How good a job can it do at making replicas of coins? || I have to be honest, it always depends on the project at hand. I own a CNC, 3 3d printers, and 2 laters. The project dictates which machine is best suited for the task. If you plan to sell things, determine what that item is first and then invest in the machine that can make it the fastest with the functionality you need. Sometimes plastic is the way to go, sometimes you need wood, sometimes you need metal. But you shouldn't  buy the machine first, you should figure out what you are building and then buy the machine that best suits the project. || It costs $2.5k. You’re welcome || $6000 || Now I am confused || Lol || Well, that answers one question I have about it. || Doesn’t seem unreasonable. About 2.5x a high end 3D printer. || Get on with it. Watching paint dry is faster || Nice review... But 5k is a LOT compared to a 3d printer + casting... || Depends on what you 3d print. Engineering grade materials to meet structural requirements and somewhat largish parts? Machine prices even out,  now it's more a question of which process works better with part geometry. || Not cheap, but still considerable.PF2026🥳🥳🥳 || Money Comes, and Money goes.
-Time... Just goes.
-Look: I have a small workshop worth of tools - It gets expensive buying tools - it really does. I have also built decks, done framing, and I wager the tools have AT LEAST broken even in value. I have made tables, and other such - At some point, when you want to do a thing, you are going to have to consider - Money vs. Time. And like I said: Time just goes.
-If you are seriously using this machine and producing 10-20 parts a week, it is very likely that the time savings PER WEEK will be in that range in hours. If you are starting to produce some one off parts, and duplicate parts - and selling them: Well: Making 100-200 parts a week, and saving yourself easily that much time in hours to go do other things - That machine will pay for itself in terms of opertunity cost within the first month of owning it. And I wager - that machine, with tuned settings, can comfortably do that much work for you.
-Look: This isn't the greatest CNC, or the fastest, or the most hands off. But this is going to be used by people like this and trust me: The value - isn't in what it does. The value is in how much bloody time of yours it free's up. || ​@formes2388You said it very wel, I will remember your phrase. 😀 || @MarekV82 Look at what you are paying for medical insurance per year. THAT is considerable! || Hola Ricky, recién encuentro tu canal, le daré seguir con mucho gusto. Pocas veces he podido disfrutar de un video tan bien explicado, además que abordas todos los temas. Considero que eres un genio y lo digo desde el respeto, es increíble todo lo que sabés de estos temas. Te envío un gran saludo desde Buenos Aires Argentina. Feliz navidad y excelente comienzo del nuevo año que está llegando. || Really good review. I have watched a ton of videos and this is one of the best for this model.
-Please post your other experiments. I have noticed that almost everyone that workes with this machine does the same test pieces included with the device. Seeing other stuff gives a better understanding of what can be expected. || Did you know that I am your second cousin and I am subscribed. I also have a YouTube channel called JWGamerKidPlayz and I have 48 subscribers 😀 || why have i never seen this advertised before?     i have been waiting for somthing like this.    i may need it to make fittings and mounts etc to build a bentley double blower, from a twin turbo w12. i want to eradicate plastic pipes and fittings.  vr6 been done. || Thanks for the detailed review 
-I feel its a first generation and its not “streamlined” like the revolution bambulab did to 3d printers. 
-I dont actually see the advantage over aliexpress cnc machines that can coat much less. || This is a good 3rd generation. Thanks to us gun nuts who want to cnc guns away from government eyes
-We had ultimaker2 s ages ago which are not bad vs bambu labs || @bobo-cc1xwtrue but bambu was so disruptive because they didn’t compromise.
-as a one who tested all generations, i think the cnc market is still far from being  “bullet proof” for creating without breaking heads and without too much of a hassle || The problem with this, as a concept, not this specific tool. Is that you can get parts printed from metal, 4 CNC machine or laser cut, in China for absolutely dirt cheap. There's no point in spending thousands of dollars on this machine when on the rare occasion you need a metal part you can just order it. Unless you just really like the idea of learning how to use a CNC machine as a hobby. || 19:29 I don't know about the software use in this but you need to watch out for the "plunge rate" (tool moving down like in 19:05) slower is better and you are correct if the tool (CNC bit) is long it is more likely to break 
-also if the RPM is slow this can also break the bit
-and in the groves of the bit if you see material stuck like it is melted this could be that the bit is not sharp and it is time to replace it or "feed rate" (cutting movement sideways) is too fast or RPM is slow for that material or both
-note: just bumping up the RPM can also break the bit if the feed is fast so it is better to slow down the feed rate first, this way you are not stressing the bit !
-(it is better to not mess with the RPM that much, it is safer to change the feed rate and always start/test with slow feed)
-with acrylic and plastic if the waste is stuck on the tool path after it is cut, then the bit has lose the sharpness but you can still use them for other stuff like soft MDF/wood (you don't have to do this with V-bits, only for flat end mill bits)  
-also keep bit's used for wood/MDF separated if you can (bit's need to be sharp to cut acrylic but not that sharp for wood but cutting wood will lower the sharpness even in a new bit but for a CNC this size i don't think you have to worry about it) 
-one last thing careful when you remove the rubber cover on the bit (the condom lol) you will cut yourself and you will bleed like the cut is about 6 times big, i don't know why but this has happen many times even when i know it, maybe get a tweezer ! || 25 years ago the cheapest CNC machines I used were £100,000 and only did something the size of your hand, might look into these || за 25 лет многое поменялось , станок из обзора слишком дорогой для его характеристик || @MORTAL666777 А что есть дешёвле из ЧПУ фрез, которые могут работать по металлу, не считая всяких Б/У станков СССР? Makera Z1 рекламируется как 900-1200 долларов. || you cannot compare your 1mil accuracy to this cheap model, they build them tuff for a reason || you would be wise to run your cutting machines through an UPS Uninterrupted power supply. I run all of my machines via one. saves you in the power out situations. || It also helps clean up dirty power which is the primary cause of power supplies burning out. || Very nice review. Thank you my friend. God bless you. || Take that 3d print now, finish it by sanding and then electroplate. ;) || yellow chromate  would look cool. || Additives manufacturing vs subtractive manufacturing. || Hmm just electro plate the 3d Printed model. || I was a machinist for 10 years, you did a fantastic job explaining a CNC machine. || Thanks for a very balanced and informative video. If I wanted to make model railway wheels in steel of around 30mm diameter do you think it would be ok? if not what do you think of making them in brass? || I'd love to be able to tell you but I'm not experienced enough to say unfortunately. I haven't tried steel yet either. It's very good for brass though. || 3D Printing was inventing to replace prototyping a casting. 3D Printing layers melted material on top of solidified material. Its mechanical properties are that of a casting.
-Don't 3D Print anything that is to take shear or torsional loading. It will snap like a cheap cast G-Clamp body.
-CNC Milling and Jig Boring have the advantage they can finish a forged component, such as a motor engine crankshaft.
-Model aircraft cranks and con-rods are from drawn alloy, which has been given a structure to withstand the stresses of operation.
-This machine would be V useful for model aircraft engine crankcases, machined from a forged billet of aluminium alloy.
-Could be used for Bicycle hub bodies. Didn't like using a dividing head to drill the spoke holes :-)
-When I did that, I cooled the job with suds oil and a paint brush. || Worse - casting is at least mostly homogenous. FDM printing comes with all the flaws that weaken castings (but turned up to 11) by default, stress concentrators as a bonus. Milling from metal is of course a completely different league! But even pastics as stock material should get you much better mechanical properties at a more moderate price. 
-Maybe considering some sort of injection molding setup to recycle scraps and shavings into workable blanks? Should work for thermoplastics at least. || And CNC has its origin in music boxes. It turned out to be useful for a great deal more than that.
-Metal printing is plenty strong, yet the machines and processes are quite expensive. Unless you have a use case that requires it, you're probably better off with CNC.
-Their real advantage is allowing for much more advanced structures compared to CNC. If you just use 3D printing to copy something that would normally have been run through a CNC, you're already doing something wrong.
-As a quick example, we use metal printed bits and drills specifically FOR CNC. While these items could be more cheaply produced conventionally, this allows us to have complex water cooling channels inside. || Machining "mess" or "machine material" is called 'swarf'. || When they taught me CNC work, we were using Apple //e's to write our tool paths on 5-1/4-inch floppies.
-This looks more current... || When I learned NC it was programmed on an MS DOS machine and then the G-code was written to punched tape - old, old school. 😂 || Its not. CNC still uses G-code / Merlin, JUST LIKE ALL PRINTERS. It's the same stuff they came up with in the 70s. || @skmail5474 yep - if it ain’t bust, don’t fix it! 😊 || Thank you! || Appreciate the video. But strange format. Have Carvera made a script for you that you are reading from? And always reefer to everything in 3`rd person || This video was made for my main audience who are 3d printer owners. I would never read a script from anyone else, my videos are always 100% my own words, good or bad. || It's 2K+ USD, too much for a hobby machine. Bummer, sucks to be poor I guess. || You don't need to be connected to the machine throughout the entire milling process. All jobs are loaded to the the machine and run locally. The App is only used to load and start the job. At least that is my experience with my Makera Carvera. Other than that, great review. || Approximately how long did the machine take to mill the chess piece? How loud is the machine? Can it be operated also in a normal apartment? || I had a CNC and it's far more messy to the workspace than a 3D printer.  But making parts that were useful that didn't easily break was nice. || but the part that you have on display you did not make with that machine did you ? || 100% || Seen few 3 in 1 machines with 3D printing + CNC + Lazer capability like the Snapmaker Artisan. Bad thing about these is that they usually can only handle aluminium and brass nothing harder.
-Also years and years ago saw the 5 axis desktop CNC that could handle hard metals called Pocket NC, but atleast back then you needed some special US government enforced license to even be able to buy it and you had to agree to all kinds of weird terms checks and such. || I think people are better of starting with analog machines and do the cutting manually to understand physical limitations of machining in general. || This is an awesome video. 
-I've been looking for something that will make vibtage watch parts that were handmade so you can't get spares.
-Do you think this could be accurate enough for it? Do you have any tolerance specs? || I just ordered one of these after this review and wondered which version of the software you are using that is gioving the 4th axis diameter issues?  To be honest, i see myself using Fusion as I have been using that for 6-7 years, but still want to keep an eye on the makera software improvements and give it a play || This is now on my shopping list, along with a descendent 3d printer. || Great review. Thanks! || A better way than epoxy to repair the damage would be to drill a hole, then plug it with aluminium that sits proud and then either repeat the finishing passes or finish by hand. || Remarkable. It looks like there is room to add a hot end (eventually) || Would really love to see someone compare this, both to the Z1, but more importantly to the NestWorks C500. But unlikely to happen before the kickstarter ends.... || 3d printers are shit compared to cnc. Toys.
-However the carvera is a terrible example. || my goal in future is make my item with raw material start(for cnc from recycling metal with fusion, for 3d print make my pellet fro</t>
+          <t>❤   Amen || Amen!</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>UCYyel9YAgwvs07rz5kugU7g</t>
+          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Ricky Impey</t>
+          <t>itsbasicbible</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>z-S0YlIrZIM</t>
+          <t>6NPZ9oRrofc</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>The REAL 3D Printing Deals This Black Friday</t>
+          <t>Breaking the Internal Battles Holding You Back as a Man</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>To learn for free on Brilliant, go to https://brilliant.org/RickyImpey/ . You’ll also get 20% off an annual premium subscription.
-Black Friday Deals can be a minefield. with fake 'deals' everywhere. I've spent the past month in discussions with all of the 3d printing manufacturers I've ever worked with to bring you genuine Black Friday Deals that will save you money AND all of my special discount codes.
-*Affiliate links (If you purchase something after clicking any of the below links I may earn a small commission at no cost to you. This is a great way to support the channel)*
-🖨️ 3D Printers
-*Flashforge*
-https://flashforge.sjv.io/XmbOOa
-Code: *XMRICKY10* &amp; *FLASH5*
-*Heygears*
-https://store.heygears.com/RICKYIMPEY
-Extra *$50 off* with code *RICKYIMPEY*
-*Anycubic*
-https://tidd.ly/4hUnhQm
-• $30 off $400+ — *ACBFCM30*
-• $25 off $300+ — *ACBFCM25*
-• $20 off $200+ — *ACBFCM20*
-• $15 off $150+ — *ACBFCM15*
-• $10 off $100+ — *ACBFCM10*
-• $5 off $50+ — *ACBFCM5*
-• $3 off $30+ — *ACBFCM3*
-*Elegoo*
-https://elegoo.sjv.io/YRJPQB
-*Bambu Lab*
-https://tidd.ly/44ltXBx
-Buy 4 → *25% off filament*
-Accessories → *20–30% off*
-*Creality*
-https://tidd.ly/3K7kV4l
-*Sovol*
-https://sovol3d.com?sca_ref=2992406.Pbdm5eiGvl&amp;sca_source=Black
- Friday
-🧪 3D Scanners
-*Creality*
-https://tidd.ly/3K7kV4l
-*3DMakerpro — Global*
-https://tidd.ly/3LMr7zc
-*Discount code - Extra15*
-*3DMakerpro — EU*
-https://tidd.ly/3JT3ep7
-*Discount code - Extra15*
-🔧 Other Machines (Laser, CNC, etc.)
-*XTool*
-https://xtool.pxf.io/DyPnOn
-*10% off* all machines • Up to *32% off* selected models
-*Sculpfun*
-https://tidd.ly/480bnzX
-Tiered discounts
-Code: *RickyImpey10off*
-*Makera*
-https://makerainc.sjv.io/e19gej
-Discount Code for $100 off - ricky100OFF
-Savings up to *$800* on Carvera Air / Carvera
-🛠️ Tools
-*Fanttik*
-E2 Ultra Precision Screwdriver
-https://amzn.to/47OyXAX
-Extra 10% code - *RIE2ULTRA* (Total 44% off)
-F2 Master Mini Cordless Rotary Tool
-https://amzn.to/4pee4oA
-Extra 8% code - *RIF2MASTER* (total 45% off)
-🎨 Filament &amp; Resin
-*Heygears (Resin)*
-https://store.heygears.com/RICKYIMPEY
-Extra *$50 off* with code *RICKYIMPEY*
-*Anycubic Filament*
-https://tidd.ly/4hUnhQm
-(same tiered codes as above)
-*Sunlu*
-https://www.sunlu.com?sca_ref=4120194.M3lnuZQl7y
-• $110 → $5 off — *SLBFCM5OFF*
-• $220 → $15 off — *SLBFCM15OFF*
-• $330 → $25 off — *SLBFCM25OFF*
-*Tinmorry*
-https://amzn.to/4i9fKNX
-*15–38% off* PETG, GF/CF PETG, TPU, ABS Pro
-*Bambu Lab Filament &amp; Accessories*
-https://tidd.ly/44ltXBx
-Filament: Buy 4 → *25% off*
-Accessories: Up to *45% off*
-*Geeetech*
-https://amzn.to/47ZjbU5
-*30–35% off* with code *AFCDKH7G*
-*Late Arrivals*
-*Insologic Filament*
-https://amzn.to/3McUBGs
-*50% discount on High Speed PLA with code INSHSPLA*
-This video was sponsored by Brilliant</t>
+          <t>Overcoming Internal Battles: Rebuilding Identity through Scripture
+In this episode of Basic Bible, we explore how most men are held back not by external factors but by internal battles such as fear, insecurity, and confusion about their identity and purpose. The video delves into Biblical guidance to help men overcome these struggles by rebuilding their identity and reshaping their thinking. Key scriptures from 2 Timothy 1:7 and Ephesians 2:10 are discussed to highlight that fear, insecurity, and confusion are not from God. Practical steps are provided to identify and replace lies with Biblical truths, act from identity rather than emotions, and understand that transformation is a continuous process. The video encourages men to immerse themselves in the Word of God, surround themselves with like-minded individuals, and consistently act from the identity that God has given them. Viewers are invited to engage by commenting with the word 'identity' and subscribing for more content focused on building men with purpose and impact.
+00:00 Introduction: The Hidden Battles Men Face
+00:40 Understanding Internal Struggles
+01:28 Biblical Insights on Identity and Fear
+04:51 Practical Steps to Overcome Internal Battles
+06:43 The Process of Transformation
+08:45 Encouragement and Call to Action
+Connect 
+https://linktr.ee/itsbasicbible
+MALTA APPAREL LINK 
+https://malta-apparel.com/?ref=BBAZ16 
+FOR 15% OFF: basicbible15 
+FREE 10 DAY DEVO BOOK 
+https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
+I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
+https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
+I WANT TO FOLLOW JESUS CHRIST
+https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
+Get vidIQ to grow your channel faster! 🚀
+https://vidiq.com/itsbasicbible</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-11-21T17:01:49Z</t>
+          <t>2025-12-27T00:00:14Z</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>5462</t>
+          <t>20</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>142</t>
+          <t>2</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0.027462</v>
+        <v>0.1</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -958,72 +824,73 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Black Friday deals can be confusing. So, I did things differently. I've spent the last month speaking directly with the manufacturers I've worked with to confirm the actual Black Friday prices, not just whatever's floating around online. These are verified straight from the source deals unless I explicitly say otherwise. And in some cases, I've even managed to negotiate extra discounts specifically for you. So, this is a fast, noonsense rundown of the deals that are genuinely worth considering. Generally through the video, I'll be quoting prices in US dollars as the USA is where most of my viewers live. And whilst it's difficult to test conclusively, all the deals should be available everywhere. Some of these deals will be very short-lived and some will be around a lot longer. And as you might expect, the description is where you can go for all the links and discount codes. So, let's quickly go through the deals that I think are worth your attention. This video is sponsored by Brilliant. So, let's start with 3D printers. This time of year is notoriously the best time to buy a 3D printer with manufacturers slashing prices everywhere. So, what are the best deals going? Now, in no particular order, we'll start with Flash Forge, who have deals on their three main models, the 5M, the 5M Pro, and the AD5X, which you can now buy for only $319, plus an extra discount if you use my discount code, Ricky10. Don't be confused by the price that you see on the website though. If you use my link and the discount code when you go through to check out that additional discount will be applied. Heygears, who are well known for their resin printers, have between 20 and 35% discounts on all their machines. Plus, you get an extra $50 off with the discount code Ricky Imp. Any Cubic have discounts on all their machines with the best deal being 38% off a Cobra S1 combo. Plus, there are additional discounts with the codes in the description, which boost that discount to over 40%. Eligu have discounts across all their machines that vary depending where you are, but you can pick up a Centuri Carbon for $279 in the US or £299 or only £240 in the UK. That is a lot of printer for the money, even though it does now seem that we won't be getting multiolor printing on this particular model as was originally hoped. However, if you're looking for a solid Corxy printer on a budget, this is probably the best you'll find right now. Check out my review of the Century Carbon if you want to know what I thought of it. Bamboo Lab traditionally slashed their prices at this time of year, and 2025 is no exception. If you're looking to buy a 3D printer as a present for someone new to 3D printing and just want something that works straight out of the box, then I have to say that for 99% of cases, buying a Bamboo Lab machine is going to be the best option. Their best discount is on the P1S combo with the AMS2 Pro where you can save 46% off the previous price. This is very likely because they're trying to run stock down on this slightly older model because of the new P2S which Bamboo Lab seem to be struggling to get on the shelves in some places. However, the P1S is still a very good printer and it's worth picking up with this bargain price. If you are buying for a beginner, then pretty much all Bamboo Lab models are beginner friendly. So, see what fits your budget. The A1 and the A1 Mini are still 3D printers that I rate very highly, and the prices keep coming down. If your budget can stretch to one of the combo models, then this will allow multiolor printing, not just one. There's roughly 30% off the A1 models right now. Creity have discounts across the board, but I can't tell you much more than what you'll find yourself on the website, as Creality don't seem to want to talk to me anymore. I don't know why, and believe me, I've tried on multiple occasions. they just don't seem to want to work with me anymore. I did get some basic information, but it doesn't seem to match what I could see on the website. So, my advice would be if you have your eye on a Creality machine, just have a look for yourself and see if the current discounts help you out. So, or so, I'm never really sure how to say that, have some small discounts. It's around 10% on their three main printer models. As I say, these are all manufacturers that I've worked with in some capacity. So, if you are thinking about a particular deal, check out my videos to see if I reviewed that particular model and see what I thought of it before buying. Don't worry, though. There won't be any links to any of the bad ones. If you do decide to pick up something in the sales, whether it's a 3D printer, a laser engraver, whatever, there's one thing that always comes with it, a whole new set of things to learn. And honestly, one of the things I like the most about getting a new machine is learning how to use it. Figuring out the quirks, understanding the tech behind it, getting better one setting at a time. That's half the fun. So, this is the perfect moment to say thank you to today's sponsor, Brilliant. Brilliant is a learning app that helps you become a better thinker and problem solver with visual interactive lessons across math, science, programming, data, and even AI. I've been going through their digital circuits and scientific thinking lessons recently, and it scratches the same itch. You learn by actually doing things. You drag components around, test ideas, and build intuition step by step. It's way more engaging than just watching a lecture. Or if you love the analytical side of dialing in a new machine, their exploring data visually course is brilliant for spotting patterns and making sense of all the little variables we deal with in 3D printing. You can start learning for free by going to brilliant.org/ ricky or by scanning the QR code you see on the screen. And Brilliant is giving my viewers 20% off an annual premium subscription, so you get unlimited access to everything. All right, speaking of learning new things, one maker tool that definitely comes with a learning curve, but can completely change your workflow is a 3D scanner. And there are actually some really good Black Friday deals on those this year. 3D Maker Pro have between 20 and 50% discounts on Moose, Seal, Mole, Lynx, Eagle, and Touan 3D scanners. My experience with 3D scanners has always been a little bit disappointing, but I'm currently discussing trying out the Tukan, which is an all-in-one scanner that doesn't need to be plugged into a high-spec PC to use it, and I'm hoping this solves most of the issues that I've had in the past. There's 30% off the Touan in the Black Friday sales, but up to 50% off some of the other models. Watch this space for a Toucan review hopefully coming soon. Creity also have some discounts on their 3D scanners, but do your research before buying any of their basic models. As I've said, I've never had a lot of joy with them, and I haven't shied away from telling you about it, which, thinking about it now, is possibly why they no longer want to talk to me. So, how about some other machines like laser engravers and now desktop CNC? You won't have seen it yet, but I've been thoroughly testing the Makeer Air desktop CNC, which I'll be reviewing in my very next video. Now, I imagine that you'll probably want to see that review before dropping a sizable chunk on a CNC machine, but spoiler alert, I absolutely love this machine, and there are massive discounts of up to $800 to be had right now, and I'm pushing hard to get that review out before the sale period ends. So, hit subscribe if you don't want to miss that one. Xol. I've reviewed a number of X tool products over the past couple of years, and without fail, I've always loved their desktop machines, including things like laser engravers. Xtool guarantee that these are their lowest prices of the year with up to 32% off in some places. If you haven't seen it yet, their brand new F2 Ultra looks great and has some heavy discounts along with their other machines. Now, alongside their 3D printers and 3D scanners, Creity have discounts on their laser engravers like the Falcon 2 Pro I reviewed last year. Again, it looks like you can save up to $800 on some Creality laser engravers, but check them out for yourself. Sculp Fun have tiered pricing depending how much you spend, plus an additional discount code just for you in the description, so check that out if you want to buy anything from Sculp Fun. If you already have a 3D printer, then Black Friday sales are a really good time to pick up raw materials like filaments and resins. Some manufacturers are only offering discounts when you bulk buy and others just have some great low prices at the moment. Any Cubic and Bamboo Lab have some good discounts if you want to bulk buy your filament. But if you want to just buy some individual rolls for some low prices, then one place to go is Sunloo who have PETG and ABS for only $8.99 with PLA at only $9.99. There are also discounts on their other filaments, but those are the headlines. And there's also additional discounts if you buy in bulk with them, too. Tinmory have discounts on all of their filament with up to 38% off their TPU and PETG, which includes their glass fiber and carbon fiber PETG. They also have discounts on their brand new ASA and ABS Pro filament. GTE have 30 to 35% discount on many different filaments which I'm currently trying out and you will need to use my discount code to get that full discount again in the description. And Hars have resin with up to 55% discount. And then in the others category we've got 3D printer accessories from companies like Mion and BQ. Mention have 10 to 20% off a lot of their 3D printing accessories, including a really useful tool kit, their Neuto Press heat insert tool, and their 3D printer filtration system, all of which they've sent to me to try out. BQ make a whole range of 3D printer upgrades and accessories. Their Panda range is specific to Bamboo Lab machines. Their discounts depend on how much you spend when you use again the codes in the description. Fantic. They make useful tools like the E2 precision screwdriver and F2 Master mini cordless rotary which I've been testing for the last couple of months and I love them. They're really useful for cleaning up things like 3D prints and more recently CNC machine parts. They have up to 45% off if you use the discount codes. So or Sovil have a small discount on their new SH03 filament dryer, but this could be the best value filament dryer available, but I need to try it out to see how it performs. Now, there are some manufacturers who didn't get back to me with their Black Friday deals in time to make the video. But if their deals look good, then I will add them to the description below. And let me and others know what the best Black Friday deals are that you found in the comments below. Also, can I please ask that you use a little caution with these Black Friday deals? We all love a bargain, but please make sure you don't overstretch yourself just because prices are lower. Make sure it's something you actually need. Thanks for watching. I hope this has been useful, and I'll see you in the next one.</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>To learn for free on Brilliant, go to https://brilliant.org/RickyImpey/ . You’ll also get 20% off an annual premium subscription. || I don't see a fantik code on the description. || Apologies, added now || Bambu lab not shipping to Mexico is legitimately infuriating || Buy two and I’ll send you one to Mexico. 😂 || "And now they [Creality] no longer want to talk to me." -- and there we have it: in a single sentence, the myth of the "this video isn't sponsored, I'm not biased, I just got this product for free" is busted. THANK YOU for being honest about the true incentives and dynamics behind free review machines. 👍 || Do you have transactions with everyone you talk to? Also do you think the companies just send him stuff to try without talking to him to find out where to send it or let him know what, where, how? Think || ​​@FuriousGriffinwhat on earth are you asking? Make sense.
-I'm thanking him for being honest. Its not that complicated</t>
-        </is>
-      </c>
+          <t>Most men are not being held back by their circumstances. Instead, they are being held back by the internal battles that no one else can see, such as fear, insecurity, doubt, overthinking, and just confusion about who they are and what they're called to do. And the dangerous part is this is that you can look fine on the outside, but quietly lose the battle on the inside. And today I want to take a moment and share why these internal battles exist and how scripture shows us as men the way out. Because freedom doesn't start with changing your environment. It begins by rebuilding your identity and reshaping your thinking. You see, most men think that the problem is really this. a lack of opportunity, a lack of money, maybe even a lack of clarity, or maybe a lack of direction and all these different things. But the Bible really shows us something deeper and different than what the world likes to communicate. See, the real internal battles are this: fear of failure, fear of people, insecurity, comparison, shame, and just confusion about who you are. You can have the talent and still be paralyzed. You can have opportunity and still hesitate. And you can even have the calling and still shrink back in fear because you don't know who you're called to be. Why is that? Because identity precedes action. And if your identity is shaky, your decisions will be shaky as well. I believe Paul tells Timothy something that every man should hear. In 2 Timothy chapter 1 verse 7, it says this, "For God has not given us a spirit of fear and timidity, but of power, love, and self-discipline." Let's break this down real quick. Fear is not from God. Insecurity is not from God. And chronic confusion is not from God. That means if fear is dominating your decisions and your thought life, it didn't come from heaven. You see, fear attacks your confidence. It attacks your obedience. It attacks your identity. It attacks your courage and your leadership and just who you are as a man. And here's the truth. Most men don't even realize they're battling fear. Fear doesn't usually tell you to stop. It tells you to delay. It tells you, "Wait a little longer. Get more ready. Make sure everything is perfect. Don't move yet. And what if I fail?" That's how men stay stuck for years. And I'm sure you've met men like that who said they're going to accomplish or pursue this vision or pursue this woman or build this, but then two years later, three years later, or even six months later, they're still in the same exact spot as they were before. Why is that? Is because fear kills more dreams than failure. And insecurity is an identity issue, not a personality issue, to be honest. And a lot of men like to say this type of stuff. I'm not an insecure person. No, insecurity is not your personality. It's a symptom of misplaced identity. It's a symptom of not knowing who you are in Christ. Because when you don't know who you are, you look to others for validation. You start comparing your life to other people. You start secondguessing your decisions and you let fear drive your decisions. You let fear make you avoid responsibility because insecurity thrives where identity is unclear. And Satan doesn't need to destroy a man. He just needs to keep him unsure of who he is. Because if a man is unsure of who he is, he is unsure on how he is supposed to be on what he is supposed to do and how he's supposed to change the world around him. Because your true identity is actually defined by God. Because here's what the Bible says in Ephesians chapter 2 verse 10. It says this, "For we are God's masterpiece. He has created us a new in Christ Jesus so we can do the good things he had planned for us long ago. I love that verse. God has planned amazing things long ago for us to accomplish. And here's what this Bible verse says. It gives us three clear things that we should look at. First, it says we are God's workmanship. That means we are not an accident. We are not a mistake. And you are not random. You were actually intentionally formed by God, by the creator to do good things. Number two, it says that you were created with a purpose. Your life has an assignment attached to it. And then here's the third thing I want you to catch. That God already prepared good works for you to do. You're not trying to invent your purpose. You're not trying to invent your calling. Instead, you're trying to discover what God has already planned for you to do. When identity is restored, direction begins to follow. That's amazing because the internal battles is the thing that's keeping you stuck. And honestly, here's how we actually conquer the internal battles that we're facing. Let me break this down practically to give you step by step so that you can ensure that you're walking with success. Step one, identify the lies that you're believing. Ask yourself this one thing. What am I afraid of? What am I afraid to do? Why do I keep telling myself this? Why am I keep telling myself that I'm not going to do that yet or that hey, not yet. This is not the right time. Also, where did this belief come from? Because most internal battles are fueled by lies we never challenge with the word of God. Number two, replace the lies with godly truth because truth will always dismantle fear. When scripture becomes your reference point, your mind begins to stabilize. That's where clarity begins. That's where vision begins. That's where the dreams begin. And you know what? That's where clarity about who you are begins. You don't fight lies with your willpower or just saying, "I'm going to stop thinking about this." No, you fight the lies by replacing it with biblical truth. Then the third thing is this. Are you ready for this one? Act from identity, not from your emotions. Because confidence isn't a feeling. It's actually a decision that you decide to make. Men grow when they act from who they are from God and who God says they are, not how they feel in the moment. A man who acts on their feelings is not a mature man at all. Because the saying that says decisions lead and feelings follow is so true. Instead, a lot of men let their feelings lead and then they let their decisions follow. Instead, be the man that decides that you're going to be this person. Decide that you're going to take action. Decide that you're going to pursue this transformation. decide that you're going to be the man that God has called you to be because all action is rooted in identity and that weakens fear and insecurity over time. And here's the other thing I want you to catch real quick, right? Is that transformation is actually a process is not a moment. And see, yes, when you become a follower of Christ, things begin to break. Your flesh begins to die and you get a new identity in Christ. Yes, those things happen in a moment, but your sanctification on who you're supposed to be and the person that God has called you to be takes time to build out. And you see, the internal battles don't just disappear overnight. Think about it like this. Let's say you just began following the Lord 10 years ago, and now you're 30. You have 20 years of junk, 20 years of the world's influence on your life. So, a course is going to take time for God to pull up all these weeds. A course is going to take time for God to reconstruct your life, to restructure your mind, to restructure your heart and your vision and who you are. So don't get upset that you're not far enough down the road as you thought you were. Instead, look to Christ. Look to him for your direction. Look for him to your scorecard. Let him be the compass on where you should go. Because if not, you're going to let your comparison, you're going to let everything else of what the world is telling you should be instead of who God has called you to be. And every time you choose truth over fear, truth over insecurity, or obedience over comfort, and decisions over feeling, and identity over your false insecurity, you grow stronger because men don't become confident overnight. They become confident by consistently acting from the identity that God has given them. They become courageous overnight from the identity that God is telling them who they are in this word. That's why guys, you can't let the world around you stop you from getting in the word. You have to let the word of God filter everything that you do. Your identity has to come from this word. And guys, truthfully, one of the reasons why you probably still have some immature things in your life, immature emotions and mindset, it's because you're not letting the word of God mature you. you're not applying the word of God and you're not surrounding yourself with other godly men who are pursuing the purpose that God has for them. So, here's my encouragement for you as we begin to close. If you've been battling fear, insecurity, or confusion, you're not weak. You're not broken. And you're not behind in life. You're just in the middle of your transformation. You're right in the middle of where you were and where you want to go. You're just right there. And I want you to know that God wants to rebuild your identity. He wants to renew your mind. He wants you to stand on truth. And he wants you to pursue the purpose that God has for you because those internal battles will no longer control you whenever you begin to submit yourself to God. Whenever you get to surrender yourself to God and say, "God, here I am. I want to be the man that you have called me to be." If this message spoke to you, if this message challenged you, I want you to go in the comment section and type in the word identity because I want to pray for you and I want to see how God is moving in your life. And also, if this video encouraged you and helped you take that next step, consider subscribing or even sharing this video with other people because on Basic Bible, I'm committed to building men with purpose and impact. So guys, see y'all next time. I love y'all. Peace.</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>UCYyel9YAgwvs07rz5kugU7g</t>
+          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Ricky Impey</t>
+          <t>itsbasicbible</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>V-Ka02Ks4fM</t>
+          <t>GmcHfaQ_C7s</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Filament Storage 2.0 - The Plan</t>
+          <t>If you want to hear God clearly watch this</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Filament Storage 2.0 continues as we turn the original single-system idea into four potential designs. In this video I break down the plan, explain each concept, and look at the pros and cons of mini dry boxes, a large drying cabinet, a vending-machine style system, and inline filament drying. Let me know which direction you think we should build next.
-*This video is sponsored by PCBWay*
-Custom PCBs, 3D printing, and CNC machining! New users can get projects started by saving $5 at PCBWay here: https://pcbway.com/g/0IW9ST
-..............................................................................................................................................................
-BUY ME A COFFEE
-If you're enjoying my content, why not consider supporting the channel by buying me a coffee? 
-Even very small amounts are greatly appreciated and re-invested into bringing you better content.
-https://www.buymeacoffee.com/rickyimpey
-You can also use the YouTube 'Thanks' button above if you prefer.</t>
+          <t>Hearing God's Voice: Silencing the Noise for Clarity
+In this episode, we delve into the struggles many face in hearing God's voice clearly. Contrary to popular belief, it's not about God not speaking, but rather about the challenge of silencing other distracting voices such as fear, doubt, and overthinking. The scripture reveals that God's voice leads us into stillness and clarity, contrasting the noise from the world. Jesus described that believers can hear His voice naturally, underscoring that confusion is not the norm. It's emphasized that a clear mind, aligned with God's word, is necessary to recognize His guidance. Transforming our minds through scripture and prayer is crucial for hearing God's direction. The importance of obeying what God has already spoken is highlighted as a step towards clarity. Viewers are encouraged to silence the worldly noise and realign themselves with God's word for a clearer connection. This episode serves as an invitation to return to scripture, prayer, and obedience for divine clarity.
+Connect 
+https://linktr.ee/itsbasicbible
+MALTA APPAREL LINK 
+https://malta-apparel.com/?ref=BBAZ16 
+FOR 15% OFF: basicbible15 
+FREE 10 DAY DEVO BOOK 
+https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
+I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
+https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
+I WANT TO FOLLOW JESUS CHRIST
+https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
+Get vidIQ to grow your channel faster! 🚀
+https://vidiq.com/itsbasicbible</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-11-16T17:00:47Z</t>
+          <t>2025-12-23T00:00:31Z</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>20836</t>
+          <t>14</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>655</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>297</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>0.04569</v>
+        <v>0.07142900000000001</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -1032,936 +899,590 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>When I asked you how you currently store your filament or how you would like to, I expected a few tips. Instead, I got a huge response, including some fantastic ideas, ranging from simple vacuum bags to highly complex vending machines and walk-in dry cabinets. So, today we're taking all of that feedback and designing filament storage 2.0 built by the 3D printing community. This video is sponsored by PCB Way. In video one of this series, I outlined some of the problems I believe we currently have with filament storage. It needs to be kept dry and clean. We need to store it in a neat, compact way. We need to keep track of what we've got. It needs to be ready to use when we want it. And we need to access everything easily. I asked you if you agreed that we had a problem that needed fixing. And what I got was a resounding yes. What I also got from your comments was a fantastic overview of what the whole 3D printing community was currently doing with their filament. And whilst there were some surprises, it was good to see that I was generally on the right track with my thinking. However, what has become very clear is that there is a much wider variety of needs than I probably realized, and I really want this project to help everyone in the community, not just people who work in a similar way to me. What I've done then is analyzed every single comment posted on that video up to this point and used it to create an outline of a road map for moving forward. In this video, I'm going to show you what people asked for and how we're going to use that information to create filament storage 2.0. So, first off, when I analyzed every comment, I found two patterns. Half of you have already hacked together your own storage systems, boxes, bags, even wine fridges. The other half are imagining what doesn't yet exist. Smart, modular, even automated ways to keep filament dry and organized. That's the gap we're going to bridge with filament storage 2.0. Of the comments telling me what you are currently doing, it was another relatively even split. 52% of you use single spool solutions like dry boxes or vacuum bags and 44% use some sort of multis-spool storage like a cabinet. I had some very long and detailed comments from some of you, which I really appreciate. One of the ones that stood out was from Mark Booth 3066, who said, "We're currently using a mix of vacuum bags and round tubs, mostly 2,000 ml with some 2500ml round tubs for those annoyingly wide spools. Each bag or tub has a desicant holder and hydrometer frame. This allows us to read humidity without opening the bag." Europa said, "I have a small collection of spools and I'm storing them in Rubbermaid cereal boxes. I have a humidistat hot glued on the inside facing out and use calcium chloride in a tea infuser bag to keep humidity around 10%." For the cabinet solution, RPM3D said, "I have an IKEA Billy wardrobe with self-made brackets and use aluminium rods and self-made name tag holders." The wardrobe is kind of sealed and has a humidity sensor with a dehumidifier machine which starts if a defined percentage has been reached. I also created a website/ app for myself to have an overview of my filament and all my spare parts. And Perkins SP or Perkins P said I have a display fridge that I got from Facebook Marketplace and put a dehydrator in the bottom. I keep around 40 filaments there. There are also a couple of comments with some of you experimenting with inline drying, which is not something I'd given a lot of thought to. However, it doesn't take much to tempt me down a rabbit hole. And after reading these comments, I spent quite a while researching if it's even possible to dry your filament as it's on the way to your printer. This would obviously solve one of the biggest problems in one go and make all of the others a lot easier to solve. And it turns out that technically it is possible and there are a couple of systems out there that you can buy right now. However, they are horrendously expensive and probably not an option for the vast majority of us. We shouldn't rule this out, though, and I think it's definitely worth some further investigation. So, we now know what a lot of people are currently doing, but I also asked for ideas on what you would want in an ideal setup. These comments were a lot of fun to read through, and there were some great ideas, some very practical and doable, and others that would be a real challenge, which could give us some great end goals for this whole project. So what was very interesting to see is that the ideas for the physical storage solutions fit into just four categories. 38% of people want a simple large mass storage solutions like a cabinet but with some of the problems of this method solved or improved. 28% want not only single small solutions like dry boxes but there was a clear message that there is a need for active dry boxes not just boxes that you put some desicant in. This was very interesting to me and really sparked some ideas for what we can do, which I'll go through shortly. 23% of the requests were for some form of automated all-in-one solution. Pretty much what I was thinking initially. This would be basically like a vending machine or jukebox where all of your filament is fully maintained and when you want it, you press a button and it's brought to you. Very cool, very complicated and massive overkill for most people. I still think we should do it though. And then finally, around 10% of people want us to look at inline drying as I mentioned a little while ago. So, you asked, let's do it. Those are our four routes for filament storage 2.0. Active single spool dry boxes, large simple cabinet storage, a fully automated vending machine, and inline drawing. With these four options, I believe there's something for everyone, no matter what scale your filament storage problem. So, those are our four directions for filament storage 2.0. And honestly, seeing how many creative ideas came from the community has been amazing. This video is sponsored by PCBway, who make it incredibly easy to turn those kinds of ideas into real engineered parts. If you've ever wanted to take your 3D printed prototype further, maybe build a custom PCB to control humidity or air flow, get precision CNC machine parts for a cabinet mechanism, or even have a housing injection molded. PCB Way can handle all of it under one roof. They offer PCB prototyping and assembly, CNC machining, 3D printing, sheet metal fabrication and injection molding. So whether you're making one prototype or a full product, you can go from idea to finished part fast and ordering is straightforward. Just upload your design files like Gerbers for PCBs or STL or step files for 3D printing and CNC. Choose your material and quantity and get an instant quote right there on the website. If you're the kind of person who loves designing clever projects like these, PCB way are also running their eighth project design contest where you can share your builds, get featured, and even win prizes. I'll leave a link in the description if you want to check it out. Now, let's start exploring how we can actually bring those four storage ideas to life. Now, we're not going to come up with solutions for all of these in one video. However, what we can do now is start brainstorming how we're going to tackle each one. Now again, I received many fantastic comments on the first video in this series, but still only around 10% of people who watched the video actually commented. So even if you don't have any particular ideas that you want to share, can I ask that you very simply let me know which of these four solutions you think you will be most interested in? That way I can gauge the wider interest and decide what to focus on first. So, if you like the active drybox option, simply comment with the number one. For a large simple cabinet, comment two. For the full-on vending machine or jukebox, comment three. And for inline drawing, comment with the number four. You can comment with more than one number if you like. I'll scoop up everything from the comments and use the feedback to guide our direction. So, as I've had a couple of weeks worth of thinking time, here are some ideas that I've had for each category so far. Number one, active dry boxes. A couple of years ago, I tried to make the simplest filament dry box I could with a Tupperware style box and some 3D printed parts. It works very well, but there have been some issues that I've learned from. Firstly, the specific system of box that I used isn't available everywhere in the world when YouTube and my channel are. I had a lot of comments from people asking for an alternative box that they could find locally. What I think we need is a way for anyone to use any kind of box that can be found where each person lives. The most common lowcost boxes are things like cereal containers, but there will be many other options that fit a filament spool. What possibly made my solution even more difficult is that I use desicant packs containing calcium chloride. These are great for keeping a very low humidity inside the box, but it means the box has to be bigger as a result. So, I want many different box styles and shapes to be usable so that it becomes a solution that anyone can use. So, what about the active part? Well, what many of you told me was that you wanted to be able to either dry the filament while it was in the dry box or at least be able to recharge the desicant. Some manufacturers have had a go at this solution. Two that spring to mind are Polymakers Poly Dryer and Sunloo's SP2. Both of these separate the filament storage box from the dryer. The idea being that once the filament's dry, you can take the box off, seal it up, and use it for storing the filament. The big problem with both of these options is that if you want more than one box for your filament, it can become very expensive as you have to buy each manufacturer's specific box. Also, what happens if you invest in one of these systems and buy multiple boxes and then a couple of years down the line, your dryer breaks and the manufacturer no longer makes them? You're left with lots of expensive storage boxes. What if we could use a very similar system, but design a universal connection method that would work on any box you can find locally? All we really need is some kind of connector in the box that allows air to pass through and then a filament dryer that has corresponding connectors. I couldn't help seeing if this idea has any legs, so I've already knocked up a very basic dry brake style connector that's cheap and easy to 3D print, which I'll be fitting to one of my dry boxes and a filament dryer so that I can experiment. Watch this space as I think we could make something that works quite quickly with this one. So, option two, the large cabinet idea. What I think we would need to be very careful to avoid is having to all use the same cabinet. Much like the dry box issue, you need to be able to use whatever you can find near to you to keep the cost down. The big problem I can see with this one is not only drawing a large volume of air inside the cabinet, but doing it quickly so that when you open the door, any moist air that enters is dried or removed quick enough to stop it being absorbed into any of your filament. Some of you use dehumidifiers inside the cabinet. Others have other solutions. I haven't given this one as much thought as some of the others, but I wonder if we could have some kind of system that uses some kind of large desicant hopper outside of the cabinet that the air can be circulated through quickly when the doors closed and then the desicant dried either automatically or manually when it gets too damp. The big downside to this one in my eyes is that it doesn't have any method for actually drying the filament specifically, only maintaining it. Need some thought. Option three for the fully automated vending machine is going to be a big project. This one's going to need a large cabinet style container, some kind of carousel style rack that rotates, mechanisms for picking and delivering the filament, and probably some kind of air lock for the spools being picked so that we don't run into the large cabinet problem of letting in damp air. I really like the challenge with this one, but it's going to take a lot more thought, and I'm not sure how many other people will actually build one themselves. I feel like we do have to do it though, just to see if we can actually solve all of the filament storage issues in a money no object project. And then finally, inline drying is technically possible, especially for the more hyroscopic filaments. Anything that absorbs moisture quickly will also give up the moisture quite quickly, too. So, it could be a good solution for materials like PA or nylon. We'd also need to find a way of doing it that costs a lot less than the commercial options, though. The basics of filament drying are that you need to excite the moisture inside the filament with heat to get it moving around and then you need to have dry air next to it to take any moisture particles away. Different filament can handle different temperatures and something like PLA can only tolerate being heated to around 55° which means that the moisture moves around less and it takes longer to draw it out of the filament. Filament like nylon can get a lot hotter, so it doesn't need to be processed for as long to remove the moisture. This makes inline drawing more practical, but there are some challenges to overcome. So, tell me your thoughts. I want ideas for each category. I want additional categories if we've missed anything. And if nothing else, a comment with a number telling me which option you're most excited about. Your feedback is what will guide this whole project. And without it, it's just me sitting in a room coming up with ideas. From here on, I imagine that I'll start making videos showing the progress of each physical storage solution. I'm fully aware that I've completely ignored the need for keeping track of each spool of filament and any kind of database. This is partly because I haven't given it too much thought and partly because it's clear that we needed to work on the physical solutions first. I will very much be looking at how we keep track of everything with each of these four options as we develop them. And I really want to know how you think we should tackle the issue with each physical solution, too. So, hit subscribe if you want to see what comes next. Thanks for watching and commenting, and I'll see you in the next one.</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>#2 with active dryer. || 2 I try to keep few open || 1 || 1 or 2 || 2 and have it be very easily visible for what spools you have available otherwise 2 and 3 || 3 and 2 use a air knife to keep the humid air out the cabinet when opening the doors || PLA goes brittle after a while, in line solutions don't work when it is already at that point for inline to be a sufficient solo solution as it can just start falling apart right on the spool || Active Dry Box - 1 || Hey, I have thought about your goals. You should look at a Barrister bookcase. I think it's the perfect place to start with the construction of this idea. Our First goal is to make a single roll dry storage box. With some 3d Printed parts, silicone calking (Type 2 would work, later in the comment, you need this type, it should be common worldwide.), and a Sheet material like Plexiglass, acrylic or any plastic sheeting. We can easily make a box capable of holding a single roll. This requires minimal tools, as you would need a drill, a straight edge, calking gun, and a utility knife. We can print corners that have slots to insert our sheets, which we secure using Silicone caulking. Most 1/4 inch or less Plastic sheeting can be scored and snapped.  Designing a 3d Printed Hinge for the door that gets pressed onto the edge like our corners do with Silicone to glue it in should work. For anyone worried that the silicone won't hold to the plastic, a little Sandpaper surface scuffing should make a solid hold. 3d printed Nerf guns hold a lot of air pressure when shooting. I'm sure silicone should hold moisture and the weight. We could further augment the design with local fasteners like M3 nuts and bolts. These are pretty common on a 3d printer, so if you have a printer, you probably can get these. As for the Door Seal, we could make a Proto-Putty Gasket. Proto-putty is simply Silicone type 2, with Cornstarch mixed in. Although Potato Starch or something similar may work as well. The King of Random YouTube Channel has a video on this. It was used to make a vacuum chamber seal and many other things. This could save a lot of people some hassle from having to use TPU if their machines can't use it. I'm sure we could print tools that would be great for making the perfect shape for protoputty seals. We may not even need to use proto putty if a design was made for the door, you could lay a bead of silicone down and, using a tool, create a shape on the door and the box to interface nicely. Latches could be added to create a better seal as well.
-Then, using the single box design, we can expand horizontally with ease. With some added supports to create a barrister's box. Create a modular back plate that we can attach brackets for holding filament inside or stands that double as support. We could add some parts inside to direct the air flow to make a convection-style heating system. Maybe the standing brackets are curved in a way to promote circulation. Using some common fans found on our printers to push the air around. Then, on either end of the case, we can include Ports on the top and the bottom to allow our heating system to draw in air and exhaust it. Then becuase it's based on a Barrister's Box, you can stack another box on top to form a bookcase and attach the Exhaust to the intake to connect the drying system and loop it back to enclose it. We could include 3d printed desiccant filters that attach to the back plate, which could be set between each roll for improved moisture absorption from increased surface area or simply before the exhaust or the intake. They could even be a dedicated door to access the desiccant, so you are not letting moist air in.  The system works well, as you can modify your system as your needs change. Have PETG and PLA? Make the Dehydator modular to attach to the end of the box or be set inside, so your PETG and PLA can be routinely dehydrated separately. 
-We could also use the Dry Break connector you designed, spaced out across the box, to let us attach to a roll without opening our box. I think this gives people the best chance at success, as filament rolls are all pretty consistent in Diameter. People can decide the length or the box they need, plus the Dehydrator. They can add modifications to the boxes, such as internal fans for convection, the drybreak, maybe a Filter box full of desicant, well recirculating air, or anything someone in the community can think of and add to an open-source set of prints. Someone could go crazy and design an automated filament driver to send any roll of filament up a bowden tube to be run to the printer. Then it can be placed on the shelves that can be locally bought and modified to accept any ducting to connect the many modular layers of the Barrister Boxes, or a system designed to interface and stack them as high as we safely can. We can also easily include an inline filament dryer at some point in the jumble of Bowden tubes that becomes possible.
-Either way, I hope this input helps you go in a direction that smooths out production on this project, as I have been thinking about similar solutions rather than plastic bags! || I am aproaching 1 year from the day I turned my first printer on.  Ive owned 17 machines since then and currently have 12 functional machines. One of those has been a 1000 plus hour project, a much larger machine project is on my horizon. Filament management has  been an issue since day one.  Here is my idea for a community project. As a self proclaimed imagineer and 20 cad user I would join this team.
-How about we take the drybox all the way. A quick change cassette style enclosure for filament. Sealed, desicant loaded,  rewind system, rfid tags for database management. Scalable dryer dock to "recharge" 1 or many cassettes. Incoperated mmu system. When you load a spool into a cassette, feed filament into a sealed drive path system thats driven from an the mmu. The configurable and scalable mmu will have dock bays that you just load cassettes into. Could even have a maintenance type dryer. From a single bay buffer feed to a 2 bay for single color auto reload, multi color cut and poop, or a tool/nozzle swapper. Loading to the mmu dock aligns the feed and rewind couplers and syncs the rfid. Loading onto the dryer syncs the rfid to tag last dry cycle. Digital humidty sensor system linked to database. Rfid system sync to klipper to manage inventory. || 1&amp;3
-1 feels most feasable to me
-3 is interesting but probably too complicated || 1 most of all, purely because of space and cost. || 2. is what I'd want if it can actually keep the filament dry enough. Simply because it'd make it easy to deal with the filament when I need it as opposed to moving stacked boxes of them around all over the place. Active single spool would be amazing too but in reality I think it'd take too much space and be far too expensive. || 2 || 1 and/or 2. I dont have many spools, thought may always increase, but having a box with active dryer seems best. One that can small to hold multiple spools is also more useful. 
-Also, 4.  I agree it may not be full-fledged now, but I think anything you do you should integrate an option for an inline dryer. Just a design element to keep on the side, optional for those who want it to add to their incarnation of the project. || A hybrid large storage box(fridge sized) with a drying compartment for say 5 spools at a time. || 1 || 1&amp;2 || you don't actually need heat to dry a filament; in fact, you shouldn't except for in an emergency situation. With every heat-based dehydration you degrade the filament and make it more brittle, especially true of nylons. Calcium chloride is great for very long storage but not for immediate use of filaments. Using clay-based desiccants I've been able to not just store nylons and be ready to use but lower the humidity to 5% RH in my filament changing boxes by using one of the spool slots for desiccant in addition to a desicant tumbler that goes in the center of the spool. Plus, I can stick the desiccant into a microwave and regenerate it. || #2
-I've been working on a dry cabinet... Not to dry my filament, I do that with a food dehydrator, but to keep it dry. This is currently only a plan, I've not started building yet, because I'm moving house soon...
-So far my design has a microcontroller (arduino), connected to a switch, humidity\heat sensor*2 and a fan.
-If the humidity in the body of the cabinet goes above 10% (needs tuning) and the door switch is closed, it'll run a fan blowing air through a desiccant cartridge. until the humidity drops again.
-There will also be a humidity sensor just past the desiccant cartridge. So if the air coming out the cartridge is too humid, it'll alert me that its time to change the cartridge and redry the desiccant. 
-My design still needs a lot of work before I'm happy with it... for example, I'm considering adding heating elements, to warm the air up to 40c to help dry filament... but not sure on that one yet. || I think 4 is a bit too much, but I think that Filament Storage 2.0 should allow any/all of 1, 2, and 3.
-I personally started building a drybox solution based heavily off of GunplaMark's "The Ultimate Cereal Container Filament Drybox - Official Remix" found on Printables. My objective is simply to have a collection that can be neatly organized against a wall. However, I can see that same wall also working for the backing of a cabinet and I can also see a robot arm vending machine selector as an over the top add on that might work better with the closed cabinet of 2, but could also work with the open wall mount system of 1. That way you have a versatile system with which anyone can build the part that they like as they go. Any combination should work. 1+2, 1+3, 2+3 and 1+2+3.
-The vending machine option 3 could also move boxes to a dryer and back to rack as needed. Though I doubt that would work with 2+3 very well. || Any way you go about it, modular vertical and horizontal options will be essential to be versatile enough for the many different needs. || I'm looking for several solutions.
-One being a large storage solution for the +60 spools I have going.
-Another being a 5-8 spool solution for the spools installed mounted on the printers.
-Currently using bags for storage and Ikea 10L 365 boxes to print from.
-How about including support for Prusas Opentags? || Microwave inline dryer ? || 2 || 1,2,3 || 2 ❤ || Option #2 please :) || 2 || I'd love a good version of 2.
-And the icing on the cake would be if all the spools are on a pole or sitting on wheels that allow them to spin and if they could all feed their filaments through small holes that I would just pull on to use them directly without ever having to open the door or pull the reel out. I'm picturing a bunch of small holes with the tip of the filament sticking out just a little either on the side or on the top around my printer sitting in the center of all those filaments. That'd be really cool. I was thinking about this because I'm about to get a Snapmaker U1 and it has no AMS like my current BL P1S so I could just pull on 4 colors I want to use and just feed them directly into the printer and when I'm done I can just push it back in and pull on another one. I'm hoping that the gap of the hole that the filament is coming out of is small enough that air wouldn't get inside. Or maybe there could be some kind of rubber of foam gasket around the opening to prevent that. || 2 :
-I currently have a single spool passive drying solution but, living in a small space, I can't stack a lot of those on shelves. I feel like a cabinet could get rid of most of the space between the spools and thus I'd be able to store them in a more efficient way. || 3 plz || I have about 30+ PolyMaker boxes and two dryers only.  That's more then I'll probably need.  They are only $21 each when on sale.   As cheap as a cereal box but very strong plastic.   And you can dry your spools without taking them out.   I've never taken them out until they run out. 
-The inlet and outlet can be easily universally adapted to other dryers of they ever stop making them.  People make too much fuss about this and make these ceral boxes that cost about $20 each anyways.  Then remove them to dry and put them back a little wet.  Go PolyMaker and focus on printing.  IMO. 😂
-I started with vacuum bags.   Unless it  is the mylar bags. But cost  $$$$.  Those plastic zip locks are junk. || 2 || i think i could use 2 || 2 || 2,3 || 1 || 3 &amp; 4 || 3 or 1 || 3.  I think this would be the way to go, but it might be more of a hassle keeping the cabinet working properly. || 2 4 || For me, 2 &amp; 3 || 3 and 4 || 4 || 1/2, multi spool active dry box || 2
-or 4 if it's compact, durable, easy to use and quick to service and has low running costs (the initial price or work is not so relevant). || 2 || 2 with 1 || 2 || 1 &amp; 2 || 1,2 I think would be ideal for the majority of people. || 2 || I have the polymaker dryer.  I use cereal containers and an adapter. It is called "the ultimate filament dry box system". It works well and the each one is only a few dollars.  They stack and they are able to print directly from the container. || 2, I think it is the most cost efficient way to store filament || 3, closely followed by 2! This is spectacular! || 2 and 4. I, personally, need a solution for storage a lot filament and to print it perdectly when needed, but I don't see any sence in vending machine. You can just put filament on your own. Or we can go on another level of automation and fully deliver filament to the printer(honestly I don't know how). Anyway keep pushing, It becomes more interesting) || 2 || I'd love to have a large cabinet with a dehumidifier built in and glass doors. Air flow is key to drying, so it would need to have fans circulating the dried air. LED lighting of course. || In order: 2, 1, 3... don't care about 4. || 2 || Polymakers drying boxes are good but expensive. And I’m not a huge fan of the seals that you can misplace; I’d love if they were more integrated into the box. || 4, to me that makes most sense || 2 and 4 || 2 and 4 || 1 || 2 || 2 with 4 || 2 || 1 || 4 || I've always loved the idea of a big cabinet. || For me, 3 in first position and 2 in second! Best regards from Italy! || 1 &amp; 2 || 3 || 1 and 2 are very practical options for Everyone. 😁👍 || 2 would be more exciting for me || I like the idea of 1 if cost and modularity can be overcome. 
-2 makes the most sense to me though. Dry the filament and then a climate controlled space to maintain it. Smaller partitions can help with not exsposing the whole space to humidity. I just dont know if maintaining smaller partitons is best done with a desicant or maybe smaller coat efficient dehumidifiers. || 2 || 2 and 3 || 2 would be great || 1 and 2 for me || 1 and 2 for me 😅 || 2 and possibly 3 || 2. I currently have two tower style storage racks in my printing room. Its kept around 40% humidity but would be nice to have storage at a lower humidity. || 1 &amp; 4.  
-Please || 2 || With some filaments (like PLA) the presence of water causes irreversible chemical changes, so drying is too late to fix the material. You can dry it, but the changes that have already taken place are not recoverable. Moisture must be managed over the life cycle of the material starting when it is received. || While I would love the big vending machine, I think 1, 4, 2, 3 is my order of interest || I have about 80 open spools that are in totes. Each tote has 5 spools and has a couple of sachets of silica. || Hi Ricky. I will go with 1 and 2 which I use now. The No1 is going back a few years ago when you adapted the legs on your drybox design for us New Zealanders who had the funny sided box's like in this video. Yup 4 years ago and I am still using them, a little bit modified but 90% the same. My No2 is a larger box that lays down with lid at top. Imagine your box on its back. It holds 5 full rolls and it is dried out with a food dehumidifier blowing in from the top down a tube to the bottom where it is directed in different directions. Only turn it on when humidity get too high which isn't often except for when I open it. Still needs a bit of work  on air flow but getting there. || 2 || Mostly 1 and 2 depending on final scope. 3 as an academic adventure that I would never go anywhere near. || 1 and 4 for me when I had the money maybe also 3 || 2 || almost 3 yrs of printing 5 days a week and have never had to fry any , || 1 and 2 || Option 2 might be the best one for me
-I'd also look into connecting ti to a computer to keep track of inventory and a scale under each spool to get the remaining grams of filament on the spool. And maybe also implement a way to read the NFC tags of the spools to automate the informations going to the computer and also putting small displays under the spools to directly see where the spool i need is || 2 || 2 and economic 1 || 1 &amp; 2. 
-I intend on pursuing a cabinet - as I was inspired by my upright freezer:  It pulls a vacuum once you close the door back.  That alone basically makes it a stasis chamber for filament.  It won't dry the filament, but included desiccant will be extremely effective on the air that does remain, as moisture can't condensate.  I just need a fridge that will be okay under slight vacuum as well as a (wireless) sensor. || So by the numbers, 1, 2, and possibly 4, while I like 3 I think it would be to involved, costly and bulky for my use. || Very interesting video, I have more than 300 spools of filament but only around 20 are opened at any one time, so I will be making shelves to hold the unopened filament and currently have, Sunlu S4, 2 Sovol 2 spool dryers, a Comgrow 2 spool dryer, several single spool cereal boxes and some plastic file boxes that hold 4 spools. Lots of vacuum bags for the rest of the opened spools, so I would be interested in a cabinet type of system that was expandable with maybe 5-10 spool wide humidity controlled storage. I would want to keep PLA, TPU, PETG and PCTG separated as for one thing they need to be dried at different temperatures and yes to the refreshing of desiccant would be nice, better than the microwave. || What the fuck??? || 1 &amp; 4 || thanks for this video .. i got enough information which i was searching online currently ..im just thinking to make a custom made Dryer  for myself .  from the list you gave i would select option 1 ( but with a  inbuilt air heater- because i dont have a oven separately  ) ... Just an idea .. need to work on it .  FYI , im a hobbist a Non Commercial user here  . || 1 &amp; 2 for me for sure. I currently have a large box I made for storage with plans for an internal dehumidifier but finding a dehumidifier sufficient enough to use has eluded me. I cannot find one that only runs when the humidity reaches a certain level so they just run 24/7 until they give out. || 1 and 2 || 3 using a dual belt carousel with cross bars to hold the line of filament. If you create positive warm dry air displacement at the top of the unit and push this to the bottom where the filament is accessed, this limits the ingress of moisture. Carousels are used in industry for part retrieval systems. So a combo using lab based positive air displacement principles and a desiccant to polish the last of the moisture out might be a good way to maintain the filament.  Then just bring out the filament when it’s require in the print queue to get out the remaining moisture. Size of the system would depend on the inventory throughout of people’s system.😂😂😂 || Like it, thanks for the input! || Wondering how MicroCenter handles moisture with their filament spool rotisserie in the store || Do you have any pictures of these? We don't have them in the UK || 1 || 1 and 2 ... maybe something integrated into a bench or under bench storage || Great video. Good community of viewers. Channel sponsorships… time for a better microphone. You sound like your mic is buried in a pile of laundry. || I'll look into it, thanks || 1 and 3 || Cant wait for the final product 🙌.  I wonder if it would be possible to have a modular base componant that we could upgrade as our needs and budget allow it. Starting with a simple box with passive dehumidifier to a shared dehumidifier and ideally active one. Also the option to add humidity sensor per unit and attach units as we go  that would be possible to be used both on a shelf or dedicated infrastructure.
-This might be a very naive view of a 3d printing newbie that want to be able to use the same parts as i grew with the ability to use existing parts || 2 then 3 || 4 || 1,2 and 4 || 2 &amp; 3 || I'm excited about this project || 2, simple and efficient || Actualmente guardo cada bobina abierta dentro de una bolsa de plástico a la que le extraigo el aire mediante una pequeña bomba y es reutilizable.
-Me gustaría un sistema que mantenga la humedad del filamento a un valor adecuado al material seleccionado y que permita de manera independiente tratar cuatro bobinas individuales, para poder secar PLA, en una, PETG en otra, TPU en otra y Nylon en otra, por ejemplo. Tendría las bobinas que uso habitualmente y siempre apunto. Para mí es importante que seque mientras imprimo y que se conecte y desconecte automáticamente cuando el material esté en los rangos óptimos. || 4 || 1 &amp; 4 is what I’ve been thinking about myself… subscribing to see what you come up with … I have a small budget and ideally wouldn’t need to store more than 10 spools at a time as I’m only got a A1 Mini… || 2 || 2😊 || Active drying would be nice, especially for things like ABS and TPU but when you say vending machine what I think of is having something controlled with something like a raspberry pie to where you can just select a color like you would on a soda machine and have the spool spit out through a receiving area lol || 1 &amp; 2 || very interested in the full vending machine idea, however would be complete overkill for me personally, still as an engineer and someone always looking for ways to improve things, I like it.  The simple active drying cabinet would be cool, but rather than having one or two big doors,  make it more like a post office box, with small doors to open just enough for the spool you want. You could hang the spools perpendicular so that the label on the spool would show, this would make it fairly skinny provided you don't have hundreds of spools you are trying to use. It would be kind of like a locker system, so each door would have a seal, but the environment inside is all shared and air inside would be circulated by fans through desiccant or even an active heater/dryer. || I like 2&amp;3. I currently have about 50 rolls in vacuum bags.And it makes it very difficult for my wife to figure out what she wants to use || 2 || 1 &amp; 2 || 1,2,3,4 || 4 || 3 and 4 +.  I am currently in development for a combination storage cabinet/MMS/in line drying system.  I have built a bench with an enclosed top for my printer.  Next step is to add a dehumidifier and racks underneath to feed multiple filaments up through the top for selection by an MMS feeding multiple tool heads.  Each tool head will have an in-feed filament dryer that consists of a direct drive extruder and filament heating block connected to 1/4-inch copper piping and compressed air injection.  I have all of the components and equipment for the first prototype sitting on the bench waiting for my attention.   I haven't done any detailed drawings yet but if it sounds interesting to you drop me an email (look at my channel for the address) and I will gladly share what I have. || 1 &amp; 3 good sir || I currently use the cereal box method with dessicant for my PETG and TPU.  There are only 4 or 5 of these boxes.  I was thinking about your vending machine.  If you have an air tight cabinet that you can see into with a carousel you could set up a pair of gloves through the wall like hospitals use with premature babies.  You could then select your spool with the gloves and place it into some type of drawer that clould then be closed inside the cabinet.  Once closed inside you remove your hands from the gloves and open the drawer from the outside and get your spool.  Air inside the cabinet doesn't change and no need for a mechanical delivery system. || Cool idea that keeps the cost down for sure! || 1 and 2 || I would like to see 1 and 2. It would be nice to have a 1 with maybe space for 3-4 rolls of filament. Or a drawer format.
-It’d be nice to see a modular solution that could exist on a set standard of space. You could then create generators similar to gridfinity. You’d have to separate the drying, desiccant, and storage into separate values. This way it could adapt to whatever containers you could fit into whatever is available. Using a generator would help keep the administrative work down while creating a successful, widely available, and logistically possible system. 
-I would love this if you could store and print from this would be best for me with a drying option being awesome. But I don’t have the technical knowledge to be able to do any of this. But it would be awesome. || I'd say 2 is a good alternative that I have been thinking about, just make it with MDF or even start out with something from IKEA, make some doors and you're done. While it's true that the open door problem is there, as in suddenlly your whole cabinet is normalized to the outside humidity (whatever that would be). I just wonder if 2 could be combined somehow with somewhat sealed drawers for each roll so that you can, even without a carousel as mentioned in 3, you can easily pick a single roll without changing much for the other rolls in the system. Obviously, 3 is even better, but it might be a bit expensive and take a long time and introduce a ton of sources to potential errors…
-roy || 4 &amp; 3 are the most interesting to me, as they provide the most obvious drying-solutions, giving the easiest use.
-If I have to watch this from the more realistic way, I must go with option 1, though I'dd defnantly would prefer option 4, 'cause  of the ease of use. || 2 || 2&gt;3 || 2 || 2 and 3 || Great Video and very good project.. I'm a Number 1 and 2 for myself. But the CFS's should have a companion dry box for all four rolls. My new K2 Pro combo is GREAT but switching filaments can be a problem. Loaded the original 4 rolls, but the WHITE went funny(wet) fast and broke off in the bottom (2) had to remove it and get the piece out. after I re-dried the spool its printing good but one part did lift the corner of a piece slightly out of 6 alike pieces, the part closest to the door(so sus) || 2&amp;3 || P.s. 2 || 1 || 2 || 1 and 2 || 1. Active Dry box. I don't have a lot of filament, so option 1 would suit my needs. If I start printing more hygroscopic filaments then 4 would be a nice option. || Option 1. Right now I have a big Rubbermaid box with an air tight gasket and a desiccant pack in it. || 2 please || Exciting ideas, and I subscribed to watch what the community comes up with, but I think many people have a requirement that's not been touched on, and that is at odds with some of the proposed goals: use of an AMS or similar system. Being able to print directly from the dry box isn't going to help when I have to move the spool to the AMS. I don't think I'll actually use whatever solution is come up with here for this reason alone. That said, I'm still highly interested in what is created here, and I may be able to "steal" some ideas for my own needs. || option 2 &amp; 3 || #4. If we can get that to work reliably, the storage becomes much less of an issue. I think that it would have to be adjustable to the filament you are printing with, and it seems like the commercial versions (that I have seen so far) don't use a long enough path over which to dry the filament. I believe some company recently introduced open-source filament RFID tags. I think these could prove themselves to be invaluable to your cause here. Obviously as a basis for keeping track of what filament you have, but also, could be read by the inline filament dryer so it knows what settings to use. || Practically speaking #1 for me.  Geek factor #3. || 2 would be awesome || 2 and 3 || 2 || 1 || Option 1 and 2 || 1 || Number 2 would be my aim. Cheers. || 2. Large Cabinet || I think I like the Active dry box (1) for single filaments the most, because it's flexible. I am pretty limited on space, so I don't really have the option for a cabinet. I think the suggestion of a dry box to dryer "adapter", so you can just put the box on the dryer instead of needing to take the filament out, is great. I am wondering if it might be possible to 3dprint the boxes, because than we wouldn't be limited by finding boxes of the right size from local sellers, but I don't know if you can make that air tight enough (Maybe with a TPU seal?) || 2 and 3 || 1,2 || 1. Because i print straight from actively heated dryers. For small print farmers like me, keeping filament dryers during long run prints is imperative. || How about one of these...
-Could we design and make something like this?
-https://www.youtube.com/shorts/8iN9AXbLbyk || 1 for me due to space || 2 and 3.
-Currently I have +200 spools all 1kg (I do have 3 or 4 3kg but I'm not stressing about those) so if there is a cabinet involved I am sure I'd need several - so.... cabinets that can be placed close to each other without impeding access to the spools would be a must.
-Thinking about the issue of opening a cabinet and allowing damp air inside.... maybe. the cabinet is actually a series of smaller cabinets, stacked and connected, so air escape/ingress is minimised.  I like the idea is stacked smaller cabinets as it could make assembly easier and cheaper.  Cabinets that have some ducting that connects via magnets and have valves that open/close as the cabinet doors are opened.  Maybe.
-This is a great project idea. || Some great ideas, thanks Ian || I think it would be good to combine option 1 with the others, so you would have an individual dry box for each spool, that would act as a cassette, or cartridge that will slot into the larger cabinet or vending machine. For storage or drying, but can be printed from directly when removed.
-Maybe then you can separate the drying and maintenance responsibilities, with the cassette holding some dessicate, but the cabinet or vending machine having a dryer that the cassettes connect to when stored || 2 || 2 || I run multiple setups focusing on pre-Dry to feed in, Sunlu S4.  I bag everything in Lowe's Husky containers that I store the vacuum packed rolls in.  Was thinking a 4-5 drawer independent sealed cabinet also. || I'm very intrigued by 4, currently I have a small 5 foot high shelf from harbor freight and I keep my filament in the boxes they come in from microcenter with small dessicant packs in the center of the spool. I use a nuwave oven to dry my filament and keep them in vacuum seal we d bags inside the boxes. But the shelf filled up immediately and I would need a second if I get more filament. But other than that it works well for me. || 4 || 1 &amp; 4 encapsulate my needs.  I am anxious to follow this channel. || I think 2 would be fine || Option 3 and Option 4 || 2 || 1 || 4 || 1 and maybe 2. || 2 || Just an idea for option 1, why not build a drier unit to a lid, then all you have to do is fit the drier lid to the box, dry the filament and then swap back to the normal lid. No need for any connectors or complication. || That’s just the Polydryer with extra steps || @spencer4hire81and significantly cheaper || @Atlas_FPV time is money, and I prefer using my printer to print prints for my projects, instead of using my printer to print prints for my printers. The filament you would need to accomplish this safely is not cheap like PLA, and you would still need off the shelf components and safety mechanisms. Buy the polydryer and modify the dry box to fit it. KISS. || @spencer4hire81none of that is true sorry, it’s extremely easy and very cheap. || @Atlas_FPVnone of it is true? Okay, ignoring the fact that you’re telling me what I prefer to print, I value my time at $20/hr. And I value my printer time at $2/hr. Show me a design that costs less than $60 in filament cost, material cost, and assembly time for a SAFE heater with at least two failsafes. Just because I’m interested in fairness, we can ignore the cost of design. And I won’t even factor in opportunity cost of the other, more lucrative projects that you could otherwise be spending those resources on. 
-For those with the resources to buy off the shelf, DIY is best reserved for where it will give you capabilities that you can’t get off the shelf, and where it can save you lots of money. I need maybe four polydryer heaters ever, but I can use doz</t>
-        </is>
-      </c>
+          <t>If you want to hear God's voice more clearly, listen to this. Most men are not struggling to hear from God. They're actually struggling to silence all the other voices that are not from him, such as fear, doubt, overthinking, pressure, people pleasing, and other people's opinions. And when everything else is loud, clarity disappears. Here's what scripture shows us. That God's voice doesn't compete with other noise. It actually leads us into stillness. That's why Jesus said, "My sheep hear my voice." That means hearing God is normal for believers. Confusion and lack of clarity is not. The real issue isn't that God stops speaking. It's that your minds have been crowded with noise. It's been crowded with the world static instead of tuning your ears to what God says. That's why the Bible says that we're transformed by the renewing of our mind. Because if your mind isn't aligned, even when God speaks, you won't be able to recognize it. Let me say this more clearly. If your Bible is closed, clarity will not be there. God is not hiding direction from you. He's actually inviting you back into alignment. So, silence the noise, create the space, and return to scripture and prayer. And also obey the last thing God already told you to do because clarity doesn't come from overthinking. It comes from aligning your life and your mind with God's</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>UCYyel9YAgwvs07rz5kugU7g</t>
+          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ricky Impey</t>
+          <t>itsbasicbible</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>y4W8Kr6shVU</t>
+          <t>BHpr16JbyqY</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>The Filament Storage Problem (and How We’re Going to Fix It)</t>
+          <t>Hearing God Clearly in EVERY LIFE SEASON</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>To learn for free on Brilliant, go to https://brilliant.org/RickyImpey/ . You’ll also get 20% off an annual premium subscription.
-Every 3D printer owner faces it sooner or later — filament storage chaos. Boxes, bags, AMS units, half-used spools everywhere.
-I’ve decided to finally do something about it.
-This video kicks off a new open-source project to design the ultimate filament storage and access system — one that actually solves moisture, organization, and usability problems once and for all.
-I don’t have all the answers, and that’s the point. I want your ideas, feedback, and experience to help shape the future of filament storage.
-This video was sponsored by Brilliant
-..............................................................................................................................................................
-BUY ME A COFFEE
-If you're enjoying my content, why not consider supporting the channel by buying me a coffee? 
-Even very small amounts are greatly appreciated and re-invested into bringing you better content.
-https://www.buymeacoffee.com/rickyimpey
-You can also use the YouTube 'Thanks' button above if you prefer.</t>
+          <t>How to Clearly Hear God's Voice in Confusing Times | Christian Guidance
+Most men are not struggling to hear God's voice; they're struggling to silence all the voices that are not from Him. If you feel confused, stuck, or unsure, this video is for you. Discover how hearing God is normal for believers, as Jesus says in John 10:27, 'My sheep listen to my voice.' Learn the importance of aligning your mind to God's Word from Romans 12:2, and understand the three primary ways God speaks: through His Word, His Holy Spirit, and through patterns and confirmations. This video emphasizes the necessity of reading scripture, the harmony between the Spirit and the Word, and recognizing God's voice amidst life's chaos. Practical steps include silencing distractions, saturating your mind with scripture, and obeying the last instruction from God. Tune in to realign your focus, deepen your faith, and hear God's voice more clearly.
+00:00 Introduction: Struggling to Hear God's Voice
+00:28 Understanding the Noise: Identifying Distractions
+00:52 Biblical Clarity: Hearing God is Normal
+01:45 Transforming Your Mind: Aligning with God's Voice
+03:06 Primary Ways God Speaks: Word, Spirit, and Patterns
+09:08 Practical Steps: Silencing the Noise and Seeking Clarity
+11:12 Conclusion: Realigning and Obeying God's Voice
+Connect 
+https://linktr.ee/itsbasicbible
+MALTA APPAREL LINK 
+https://malta-apparel.com/?ref=BBAZ16 
+FOR 15% OFF: basicbible15 
+FREE 10 DAY DEVO BOOK 
+https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
+I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
+https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
+I WANT TO FOLLOW JESUS CHRIST
+https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
+Get vidIQ to grow your channel faster! 🚀
+https://vidiq.com/itsbasicbible</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-10-26T17:01:33Z</t>
+          <t>2025-12-20T00:00:13Z</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>12681</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>510</t>
+          <t>4</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>89</t>
+          <t>5</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0.047236</v>
+        <v>0.391304</v>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t xml:space="preserve">To learn for free on Brilliant, go to https://brilliant.org/RickyImpey/ . You’ll also get 20% off an annual premium subscription. || This is one of those "that could have been a email." Type videos. || i bought 10 rolls of filament and my printer hasn't arrived yet and i want to buy more lol xD 
-but i'll probably only use four at a time in the ams, then maybe one more on the side spool. hopefully i won't keep too many open at once. || Using RFID tags on the spools might be an idea to keep up with tracking and cataloging what is being stored in the dryer. || My mom worked in the mass data storage department at IBM for over 30 years.  As a kid in the 90's, we had opportunities to see what they were doing via bring your child to work days.  At the time, almost all mass storage was either optical or magnetic.  They had some incredible machines that would store, find, transport, and read 10, 50, or even thousands of drives.  One that comes to mind of this project was a bit like the star wars data storage systems seen in various places.  It was a wall of drives on a series of conveyors that would move the drives to the reader.  It was a simple but elegant system.  Others were able to find and read multiple drives by taking them off the wall with a "claw" and putting it into one of many readers.  Others has huge robotic arms (you know the ones that build cars?) that could rapidly access thousands of drives over a huge distance.  
-I am envisioning a wall of spools with filament tubes running from each, kind of like a giant AMS.  I saw an aftermarket multi-filament adapter for my AD5M Pro that had multiple filaments connected right to the print head.  What about a MASSIVE version of that, right at the top of the printer, with 'all' of the filament in the storage box connected via tubes from the storage cabinet.  IF we are talking a full scale, print farm ready version of this thing, it could have a rewind function at every spool (or a mobile rewinder) to pull the filament back from the print head minimizing waste during filament changes.  
-Or if we want to go full sci-fi a robot that takes the filament rolls into a standard 4 spool AMS to be fed to a stock changer.  or the manual version of that, have those rubber gloves that go into the door of the cabinet allowing you to manually switch rolls without opening the cabinet. || I just store in cases. When Im ready to print something, if its important enough.. I just dry it out. Came to conclusion that its just part of the hobby at this point. || Dude, that's great that recantly we've seen a lot laying-on-the-top technologies in 3d printing , that i personally thought about too, finaly appearing, and great that you are the one of diving into it. I will track your project 'cause I wonder how far this can actually go and because I need it too)) Made it how you think it should looks like and good luck! || Large bin with silica is as far as I have gotten. However I have a server rack that outputs warm air and I have been considering putting a radiator over the exhaust and circulating that water into a bin with filament to keep it warmed slightly. Wouldn't be near as hot as say a filament heater but I feel like it would be a practical use of that warmed air. So my long term ideas basically involved scavenging and proving radiant heat into filement storage possibilities || A tad late - you have a large box - your room, you have storage - shelving - you close the door and the room is sealed - buy a dehumidifier - job done || Some food for thought: imagine a round tower much like an automated elevator storage tower for cars. Each level holds maybe six rolls. Tower is fully enclosed and connected to a dryer unit.
-Software keeps track of where any roll is at any time. Drawer at bottom (like a vending machine) accepts a roll and stores it and also presents a required roll. Towers could be made from stepping motors driving vertical threaded rods etc. Tower wall could be plastic or metal drums. You could store perhaps 50 or so rolls per vertical metre. Should work? || Im at 500ish rolls right now, I store it in different ways from soft close drawers to shelves  and even filled a 7 foot tall server rack lol || Broken wine fridges and commercial glass front fridges, combined with a reptile heat pad or lamp, some desiccant, or a small dehumidifier attached to an Inkbird IHC-200 Humidity Controller. || I’m working on something similar with a Chitu Systems 3D Printer Mini Heater and a esp that you can mark where on a 7in touch screen that’s I designed the software that looks similar to a AMS type you can pick what likely it is. || This is the exact video I was looking for. How are we all using cereal boxes and tubs with renewable dehumidifiers? There's a product gap here but this is the 3d printing community. Let's solve it. || Ok my plan for this is as follows , living in the Caribbean humidity is around 80%, in one of my rooms I have an alcove 3m wide 2,2 m high and 0.7m deep. I’m going to make a sliding track top and bottom and make 4 wooden sliding doors with plexiglass windows. On the edge of each door will have full length brushes for sealing , I already have a shelving system in the alcove so this will support 2 raise E2 , 3 A1 mini, 2 P2S and a H2S and also plenty of space to store all my filament. I found a neat dehumidifier on amazon for $59 and that will live in the alcove. This will not only look after the filament but also the machines from corrosion which is a big problem here. I’m hoping the heat generated from the machines and the dehumidifier it should work as a large dry box of 4,6m cubed
-How could we possibly upload designs to share? I think this a big problem we all face, and if we find a solution would be great👍🏽 || There’s always a place for spreadsheets🤣😂🤣😂 || Following as I'm new to the community 😊 || I’ve started building my own smart filament dry/storage box using 2080 aluminum extrusion and clear polycarbonate panels.
-This first prototype is designed to hold around 10–13 filament rolls — assuming my measurements are right 😅
-As a software engineer, I’m integrating full IoT functionality, including temperature and humidity sensors inside the enclosure to report live data. I’m also experimenting with different methods to actively dry filament while it’s being stored, aiming for consistent, low-humidity conditions.
-Once I’ve finalized the dimensions and gathered some real-world performance data, I’ll share everything here to help others build their own.
-My long-term goal is to expand this into a larger modular system featuring:
-💡 RFID or barcode tracking for each spool
-🤖 Automated spool retrieval — simply request a filament, and it rotates forward for easy access
-I’m really excited about this build and what it could evolve into — and I’m happy to help out with this community project in any way I can.
-Whether it’s sharing design files, IoT setup details, or data from my prototype tests, I’m all in on helping bring smarter filament storage to life for everyone. 💪 || Yes I own a printer, Yes I have the same problem but sorry I don't know the solution so I am right behind you watching with interest. || Looking forward to see this progress. || I use bins like the one in the video. I have 4 of them (2 are extra large). I don't know how many rolls I have and they are mixed and matched (pla with matte and multicolor, etc as long as it's pla). I keep petg and ASA in their own bin. I have dessicant bags and dessicant plug in boxes that absorb humidity and just plug them in to reset the dessicant inside. Got those on Amazon. Nfc tags scan easily with phones or a laptop. They are cheap (like $13 usd for 100). I'm thinking about a system where you pre-create nfcs info with brand, material, type, color, spool, etc. So it would hold something like Elegoo_PLA_Matte_Red_cardboard. Create one each for all of your options. Then just program the tag with one of those (which were pre-created) and stick it on the spool. Then enter a numbered location into a responsive web app that tracks filament. Would work on phone, tablet or laptop that way. If you enclose the system, I think an esp32 running ESPHome could monitor temp, humidity and control fans and/or heaters. You could hook it all up to home assistant to control it all. Esp32's are like $6 or less and home assistant and ESPHome are free.  This is just brainstorming at this point but it's one possible solution.... || I’ve got the same problem, less filaments but need a solution that stores multiple rolls efficiently and also on a shelf under a cupboard. 
-Like you I’ve got a few ideads bouncing around on how to achieve it. Skill set wise I work in biotech R&amp;D product development and could help with structuring the dev process so you make the right thing from the start (also do a bit of coding on the side). I’m also UK based, so feel free to reach out.
-FWIW I thinking something akin to the automatic prescription vending machines we have in the UK could be a workable model, possibly some kind of stackable carousel system with a single door that opens and only exposes one chamber at a time when you put in the right code (filaments are barcoded on ingestion into inventory) || Sounds like you have some great skills that could definitely help with this project! || 3dfilamentprofiles allows you to create an account - it is a library that tracks filaments, where you can purchase them, the technical details (diameter, pressure advance settings, etc) || I’m subscribed and ready to learn this, I really want a better way for my filament. At present I use bags like you, i don’t have a dryer yet as i can’t afford it, but i am saving. Can’t wait to see what comes of this, hopefully people get onboard and use them amazing minds that this community has. || My words exactly! || I don’t 3D print but I’m considering dipping a toe. A second hand frost free fridge comes to mind. They have edge seals and keep moisture levels low. They could be further hacked by replacing a section of the door with a double glazed window. Please don’t rule out spreadsheets. For a simple but flexible database, they are hard to beat, and I’d imagine a single table would do the job for most cases. || Great video hopefully it will become something awesome I would love to have a place to store my 3D printer filament and keep it dry and ready to print. Can’t wait to see what you come up with. Thanks for sharing || Cool idea I thought of would be a vending machine type filament storage  which after typing this makes me realize it would just be a giant ams. But maybe instead of dealing with super long bowden tubes, maybe a filament tool changer system  (hence vending machine reference) that's able to travel to each roll grab and dispense it. Maybe a separate head for each row. This would prevent the constant letting in moisture issue unless you're restocking it. Your thumbnail gave me the idea but that's as far as my skillset goes. || My current system is a cabinet with 6 disccantes in it...all in original or resealable vacuum bags...or air tight cereal containers....I have probably 15 (11 more on the way due to Sunlu sale....I think I have a problem) rolls of mostly PLa +, some PLu to try printing shoes for fun....and some PETG for more durability....thinking of getting into CF or Asa at some point....I already upgraded to handle it....just need to come up with a better system lol... contemplating making Swatches to hang on my rolls for easy ID or wonder if there's an aftermarket RFID system to link to a display for ease...MINi LCD display system wouldn't be horribly expensive...could probably run off a PI system easily enough || Uh just 2 years ago literally everything was manual. Got a bit spoiled with your bambu machines did you? Don’t worry bambu will first to do it in the next year or 2. And this isn’t even mentioning the whole you’re not supposed to be away from your 3-D printer while it’s printing so you don’t burn your house down fact… so you’re basically asking the cost of filaments and everything to go up and no thanks! Some of us like simple open source and low cost || Pro Tip::  Wine refrigerators make great filament cabinets. When they die, they are essentially worthless on marketplace or craigslist. They seal up nicely and with a tray of desiccant they keep your filament in great shape. As a bonus, they have glass doors and you can see all of your filament inside. || I use a large dresser for mine, along with dry bags for a lot of them || Swatches are a good way to keep track of what you've got, and not have to search through them just to remember || How about a juke box/soda dispenser type setup? 
-You load all your filament reels and have a scanner that reads the information off the reel, a mechanism loads each into a storage space in the unit, a scale determines how much is left by the weight and so on. 
-One doesn't even have to open the enclosure.  You drop in a reel, it is scanner, pushing to a available slot and unto its scale storage space. 
-Each storage space can be individually  heated or cooled. || I live in coastal South Carolina, so the humidity can be a significant factor most of the year. I started early by storing my filament in Sterilite gasket boxes. The seal isn't particularly tight, but a gentle pressure on the gasket is all that's needed to keep the humidity out.
-Eventually I started using Eva-Dry units. They are a bit expensive, but are very convenient to recharge and that worked better than printed boxes that need to be checked, emptied, recharged, and then put back into the container. If it's too onerous, then it won't get done regularly like it should and these things helped. My dry boxes would register in the teens or twenties humidity wise with these. Then I hit on another excellent desiccant.
-I started using Activated Alumina a few months ago for humidity control and it has worked very well. I pour the beads into a small metal powder shaker that can fit into the middle of most filament reels when they are in my AMS unit and can be popped into a small toaster oven to recharge at 350 Fahrenheit for a few hours.  By itself, the activated alumina will get the humidity down to about the upper twenties for humidity, but if you put an Eva-Dry unit into the box the humidity goes much lower and then the alumina alone will suffice to keep the humidity that low.
-When I open a gasket box to get a reel out, the humidity level jumps up, but quickly returns to the previous level after the box has been shut for a few minutes. I surmise that this incidental exposure to humidity does no real harm if the box is not left open for an extended time. The small volume of air trapped in the box does not contain a sufficient quantity of moisture to make a difference in the quality of filament performance during printing or significantly reduce the time between needing to recharge the desiccant.
-Edit: - I forgot to mention the best dryer idea I've seen in action. On the Samcraft youtube channel he uses a commercial food dehydrator to process a large number of filament reels at once. The Ausegia Commercial Large 12 Trays Food Dehydrator, Usable Area up to 22.67ft², 1200W Full Stainless Steel Dryer Machine, up to 190℉ Temperature, for Meat, Fruit, Veggies, Beef, Herbs, Pet Foods runs about $220 - $250 on Amazon. Not an option if space is an issue, but if it isn't this thing looks like an excellent deal. || Thanks, just found the Samcraft video. It's always interesting to see how others do things, especially people who use a lot of filament like this. || I have a ikea billy wardrobe with self made brackets and use aluminium rods and selfmade nametag holders. The wqrdrobe is kinda sealed qnd has a humidity sensor with a dehumidity machine, which starts, if a defined percentage has reached. I also created a website/app for myself to have an overview of my filament and all my spareparts. But there is no way for an "ams solution" in this case.
-I created everything my own, cause I did not like everything on the market || Maybe a section of tube that the filament goes through that dehydrates it before it's used to print? Like a "Hyper" quick drying thing. || I was afraid I was going to need to build a whole room dedicated to drying and storage. || This is a very interesting project. I have so many little ideas. But I guess there will never be a single solution that scales well for everyone.
-Reviewing what others did (like CNC Kitchen and Made with layers, among others) will help get ideas and lessons learnt rather than reinventing the wheel. Especially a follow up on CNC Kitchen's solid state dehydrator. Maybe it's cheaper/more viable now.
-A collaboration with any of them might also be a good idea. Maybe with Lost in Tech sine he might be close to you? Just a thought.
-I also have an idea that might work for people with more filament than I do: some sort of a vending machine. You don't open the whole container. You just push the one you're interested in out. I don't have an idea for how to reload conveniently though without reopening the whole thing. Alternatively, maybe tiny doors for each filament slot? I don't know.
-Another idea that might work for me is keeping everything in readily available AMS units connected to electricity only to keep filament dry, but not necessarily connected to a printer. That's provided there are cheap enough ones out there to keep this reasonable.
-My ideas aren't probably the best. Just trying to provide input. Hopefully I'm helping somehow..
-Good luck :) || Every comment is helping me refine what is actually needed by others and it's helping me sanity check my own ideas. Your ideas are very helpful. A collaboration with other creators would be very welcome. || Hope your project will became the Gridfinity of filament storage! Fingers crossed.
-Can't contribute that much because I only use two spools of black and white PLA. Don't need more 😅
-But If you make it opensource, then a community will follow! || Currently new to 3d printing  and i already have 60 spools  (I have an addiction) don't judge lol. I run a drying with 4 rolls,  most everything else in VAC bags and  4 rolls in each AMS. i have spools stored in the closest on a  rack i made  spools in heavy-duty totes lol  finding that  color i need can be a real pain unless It's something I use all the time || Just opened a huge can of very long worms. Watching with interest. || I’ve tried a few different filament catalog systems and either they aren’t very user friendly or they don’t have the right options for me. Hope to see something come out of this way more user friendly || I use the app, Spoolstock it is good for keeping track of my filament, where it is stored etc. 
-I also have a controlled room where my printers and filament reside.
-There is a dehumidifier in that room that runs 24/7. I have found this is, so far, great. However every time I enter the room I can hear the dehumidifier amp up because the air from the next room has entered. The  room is also able to be temperature controlled. (There are resin printers in this room as well)
-I also run a VOC machine in there 24/7 || Interesting project. I have a small print farm and have been playing around with ideas for this for the past year. I generally have about 300 rolls in stock with rolls being used up and replaced weekly. My current setup is far from perfect but I feel it is at least a reasonable start.
-Here’s what I currently do. First I use Sterlite air tight containers for storage (these aren’t perfect and tend to break handles after repeated use but they are easy to fix when necessary). These come in a variety of sizes and are reasonably priced with discounts available for bulk purchases. They are nice because they have a foam seal and plastic clips that push the cover into the seal to keep it fairly air tight. I’ve standardized on the larger size which holds about 20 rolls. These are nice since they are stackable with molded rides on top/bottom so they stay together when stacked. I label each with either filament type &amp; manufacturer or specific type (like Rainbow PLA or Marble PLA). I also designed desiccant holders that screw into the hub of each roll so the inside of the containers stay dry. I use 512 byte NFC tags attached to the desiccant holder and the roll to track info about each. For filament NFCs I store filament type &amp; brand, color, basic print info (nozzle temp range, bed temp range, print speed range), purchase date, price, vendor, etc.. I also store the date of the last dry session. For desiccant holders I store the date it was loaded, # of drys and last dry date (these get dried with the roll). So I can access most info about rolls &amp; desiccant holders with a quick scan of the associated NFCs. When I see desiccant has not been dried within 6 weeks, I replace it with fresh desiccant, update the NFC and put the old desiccant into a container which gets dried and the process restarts.
-I also maintain a ChatGPT filament inventory system and log new rolls when they arrive and remove rolls when they are done. I can search for rolls by filament type, color, age and a host of other ways as needed. I also store the name of the Sterlite container where it’s stored. When starting a new print I typically research my inventory and determine which rolls I’m going to use and then get the set of info for each roll so I can locate it. I check the NFC to see if it needs drying before the print and if so load into one of my 4 roll dryers before printing. I update the filament &amp; desiccant NFCs if drying is completed so all data stays current. This also allows me to calculate filament costs per print reasonably accurately since the slicer will tell me the amount used and I know the roll price from the NFCs data (I also enter this into the filament profile cost field (I use Orca &amp; Bambu Studio) so the slicer can tell me costs directly). I do multi color prints using single AMS units (max of 4 filaments per print) and studio takes care of figuring out the costs for each print based on my filament selections. 
-This works pretty well for my printing tasks but there are some downsides. First, it’s sometimes hard to locate a roll if it gets misplaced into the wrong storage container. I know where it’s supposed to be but if not found then I have to search around to find it. Obviously none of this is automatic, so I have to manually find and load rolls needed before each print. 
-Interested in what others think of this system and ways it could be improved. It’s been working fairly well for me but could certainly be improved. || Thanks for taking the time the write such a detailed description of what you do and the challenges you face. It sounds like you've put a lot of thought into this already and you have a detailed way of keeping track of everything. I hope we can come up with some ideas that give you a more automated version. || Can you share what you did with ChatGPT?  I could definitely use something similar for other items (not filaments) but also I am finding that my filament is quickly getting out of control, and I only print for our own use.  I can't imagine what it would be like to have your quantity of filament  😀 || @richardsmith3614Yes, as you start having more rolls things get harder and harder to manage. I worked with ChatGPT to create a filament inventory system. It maintains the database and I tell it to add or remove rolls as new ones come in or rolls get used up. I can tell it to search my inventory and give me color options for new prints. I log the purchase date,  seller, manufacturer, filament type, color and price. I don’t log each use of a roll but I could and then it could tell me exactly how much I have on each roll. Fairly simple and you could do it manually in an XL sheet but this is easier and you can query it using natural english language. || I keep my moisture sensitive filament in a filament dry cabinet made by eDry. It holds about 10 spools at about 7% humidity.  I also have two StatPro cabinets made by Production Automation Corporation. They hold 4 or 5 spools, cost under $250 and keep the humidity under 8% but they make bigger ones as well.  No desiccants, no fuss, just plug them in and they use very little power. maybe 10 - 15W average or less.  I also like PrintDry containers that stack. I make a label for each with the type and color so its easy to see, then I have a spreadsheet with them all so I can find them.  I probably have about 140 spools total.  Both eDry and PAC make larger filament dry cabinets but they do get pricy at the larger sizes. || what a dumb video. || I just got into 3D printing. I think there’s Polymaker boxes have been the best useable storage solution. However the more filaments I need for the prints I want to make, I realise a subscription printing service with all the machines and filaments offsite and end product posted to me is the ideal solution. My space at home and time are limited and I’d rather outsource the management and storage to someone else. || With a couple exceptions i use up my filament before I’ll order more. It only takes a day or so to order and receive a new rolls. I got my stock down to 7 rolls, i don’t care too much about color though so they’re are all material variants of black, white and gray. || We've been looking for a better solution for a while. We're currently using a mix of vacuum bags and round tubs (mostly 2000ml with some 2500ml round tubs for those annoyingly wide spools some manufacturers like). Each bag/tub has in in hub desicant holder, and a hygrometer in a frame that clips onto a spool edge and has a flat surface we can write details on. This allows us to read out what the humidity of a spool is and details of the filament (e.g. eSun PLA Green) without having to look at the side of the spool or open the bag/tub. The problem is that the tubs don't sit upright on their side, and vacuum bags have all those awkward vacced down corners that get in the way of sitting on their rims.
-I started printing some rack modules, but realised they were going to take far too much filament to do enough for all our filament, plus there wasn't enough of a height gap for the tubs, or vacuum packed filaments without those pesky corners getting stuck all of the time. So then I though about building adjustable frames using 2020 extrusion, but that would have cost far too much. What I think we need is a combination of stock material for length &amp; strength (what reprap called vitamins *8') and 3d printed parts to abstract away the complexity and fabrication hassle. Maybe the solution is a minimal 2020 frame and some sort of per spool hanger, then hanging the spools on that, like you hang clothes in a wardrobe.
-A storage system with tracking would be interesting though. If every spool and location had a QR code, they could be scanned in and out of different locations. Developing and self hosting a local database web service wouldn't be too difficult and could take a lot of drudgery out of managing a large collection. Scanning and launching those qrcodes would open a local url's to request changes to the database, for example scan the QR code for spool ESPLAGR1, it might open a webpage saying "Moving spool eSun PLA Green 1 from Rack 1 Row 2 to?" then a scan of code AMS3 and it would say "Moved spool eSun PLA Green 1 moved to AMS lite spool 3". You could even supply additional data for certain moves, such as scanning spool BLGAL1 and DRYER1's QR code it could say "Spool Bambu Labs Galaxy Purple PLA 1 moved to Elegoo Dryer, use 50°C for 8 hours" etc.
-Oh, and you're wrong about the spreadsheet, btw. Our filament storage may still be a mess, but at least we now know what we haven't got in stock as well as what's on our "never buy this again" list. *8') || Very interesting project idea. || I have felt for some time that grow tents would be perfect for using both for filament storage and for using printers in. Grow tent companies already make dehumidifiers, heaters, and carbon filters with inline fans. That's like 90% of the job, and now they can be used as a closed loop. Something like a 2'x4' tent would be perfect for storage. Maybe a 3'x3' for printers, should hold 2 or 3. I feel like it would even solve ams problems. Oh, and I forgot to mention, these grow tents also have controllers that allow you to set your desired humidity and temperature. In short, I think grow tents are an ideal solution and all you would have to figure out is the internal shelving/storage and inventory system. Look at AC Infinity, Vivosun, Spider Farmer, and Mars Hydro. || I considered this, and found a few problems, first spools are heavy, you would need additional internal frame to hold their weight. The other problem is the same one large cabinets have, that every time you open it to add or remove a spool, you're opening it up to an influx of moist air. The final problem what that there were a limited number of sizes. Given the space I have available they they were either too big, and wouldn't fit in the space without cutting down the frame, or they were soo small and left loads of space around them unused. || ​@markbooth3066I was thinking more along the lines of adding shelving or a new structure, not using the frame of the tent. I figure the opening the door problem will exist for every option, otherwise you won't be getting the filament out. But at least the grow tents can have dehumidifiers and heaters to control the environment even when the door is open, just less effectively. || That's why I went with vacuum bags and tubs for each spool @SkewToob, as you end up with a much smaller volume of air exchange. Also this allows you to individually monitor each spool (you can buy hygrometers very cheaply) and tailor the drying schedule to each filaments needs. || I thought you said that teaching course was free? || I think for advanced hobbyist use the ideal is a cabinet with decent seals around the doors, and an automated system which circulates air through large dessicant containers that's triggered either whenever the doors open or whenever the humidity gets high in the cabinet. Bonus points if it has some servo controlled louvers and a heating element that can periodically blow hot air through the dessicant outside the cabinet to regenerate it.
-For the print farm, I want to see multiplexed ams systems, where using a series of gates you can feed filament from any bank of spools to any of several printers/toolheads || Something like a Ruggard Cabinet might be a good start || I've been eyeing those walk-in humidors like a cigar aficionado's worst nightmare.
-I think/feel any solution (for me) needs to include 1k and 3k spools. Big spools are so much more economical for certain materials and colors. || for building a catalogue of filaments 3dfilamentprofiles and spoolman has the highes potential in my opinion.
-For drying its important to know, that even though PLA can be printed when wet, it needs to be stored dry for it not to go bad over long storage periods while most other filaments behave in the exact opposite way. || Spoolman runs as a docker container for tracking multiple rolls and locations. There is a plugin for octoprint for usage as well. I use it on my printers for tracking a lot of this. || I have a Display fridge that I got from FBMP and put a dehydrator at the bottom and I keep around 40 filaments there || QR codes on spools has to be the first step. Large cassette storage(jukebox) seems a non starter as it would be to bulky for most.  I currently use dozens of cereal tubs with a humidistat in each with added silica gell pouches.  Then (try) keeping main types on separate shelving. It only works when I make the effort to keep it all in order! Also now need more shelving and boxes. || -- IDK whether you're a mind reader, but I'm doing inventory of my filaments for the first time, since HT-PLA by Polymaker is out, so I'm not ordering Bambu Matte PLA anymore, that I used a lot for prototyping, along with even cheaper PLA for my Qidi Plus4(I do like my Bambu Lab A1 slightly better for quicker prints and AMS) where AMS from Qidi been promised almost a year ago, and I have not got it yet(wag finger at Qidi), so for the first time I got a transparent bin similar to what you have on your counter, pack in Creality resealable bags, again, similar to what you've got, and heading to storage to wire stowage shelf will be sitting very an accessibly, since my very roomie credenza, that I made specifically for Qidi Plus4 out of 2020 extrusion and fine particle board, around a year ago, can't store anymore filament. So, yeah, totally subscribed to your channel and ideas... || A quick Google let me to </t>
+          <t>❤    SO   GOOD  👍 
+         AMEN     ❤ || 🙏🙏 || Thank you ❤ || Welcome, God bless 🙏 || You’re welcome 🙏</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>UCYyel9YAgwvs07rz5kugU7g</t>
+          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Ricky Impey</t>
+          <t>itsbasicbible</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>ZkCviEj9v2E</t>
+          <t>GJVnq2MdWOk</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Bambu P2S vs X1 Carbon — The Knockout No One Expected</t>
+          <t>Your Purpose Has Been Waiting | Are You Ready to Receive It?</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Can this midrange 3d printer actually be better than the X1C?
-In this video, I’ll show you why it can — from the new servo-driven DynaSense extruder and eddy-current calibration to improved cooling, AI monitoring, and full AMS compatibility. If you’ve ever wanted X1C performance at a lower price, the P2S might be the one to get.
-*This video is sponsored by PCBWay*
-Custom PCBs, 3D printing, and CNC machining! New users can get projects started by saving $5 at PCBWay here: https://pcbway.com/g/0IW9ST
-*Affiliate links (If you purchase something after clicking any of the below links I may earn a small commission at no cost to you. This is a great way to support the channel)*
-*P2S*
-https://tidd.ly/4htptyp
-*H2S*
-https://tidd.ly/45LBPwc
-*H2D*
-https://tidd.ly/4lIBnEQ
-..............................................................................................................................................................
-BUY ME A COFFEE
-If you're enjoying my content, why not consider supporting the channel by buying me a coffee? 
-Even very small amounts are greatly appreciated and re-invested into bringing you better content.
-https://www.buymeacoffee.com/rickyimpey
-You can also use the YouTube 'Thanks' button above if you prefer.
-#BambuLab #P2S #3DPrinting #X1Carbon #3DPrinterReview</t>
+          <t>God's New Vision for Your Life: Embracing Change and Growth
+In this video, explore how God wants to transform your life by replacing old mindsets and beliefs with new visions and callings. The speaker delves into the biblical parable of new wine in old wineskins to illustrate the importance of embracing change in our spiritual journey. Discover how to let go of past hurts, addictions, and limited beliefs that hinder you from fulfilling your divine purpose. Learn about the significance of living with purpose, the enemy's tactics to keep you stagnant, and how true growth often involves enduring growing pains. Tune in to find out more about the upcoming Purpose and Calling Breakthrough Virtual Masterclass on December 20th, designed to help you gain clarity and confidence in your purpose for 2026.
+00:00 Introduction: God's Message for You
+00:23 Jesus and the Parable of the Wineskins
+01:17 Embracing New Beginnings
+02:03 Identifying and Letting Go of Old Patterns
+03:10 Invitation to Purpose and Call Breakthrough Masterclass
+03:57 The Enemy's Tactics to Keep You Stagnant
+05:38 The Importance of Growth and Overcoming Comfort
+06:40 Living with Purpose and Making Decisions
+12:37 Finding Purpose Through God's Word
+13:58 Conclusion and Final Invitation
+DECEMBER 20TH MASTERCLASS FORM
+https://srm.fishflow.app/widget/form/zvB4lA8lrQrYiavw5zKR
+Connect 
+https://linktr.ee/itsbasicbible
+MALTA APPAREL LINK 
+https://malta-apparel.com/?ref=BBAZ16 
+FOR 15% OFF: basicbible15 
+FREE 10 DAY DEVO BOOK 
+https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
+I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
+https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
+I WANT TO FOLLOW JESUS CHRIST
+https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
+Get vidIQ to grow your channel faster! 🚀
+https://vidiq.com/itsbasicbible</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-10-14T13:01:50Z</t>
+          <t>2025-12-13T00:00:21Z</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>62254</t>
+          <t>23</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>993</t>
+          <t>1</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>154</t>
+          <t>1</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>0.018425</v>
+        <v>0.08695700000000001</v>
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>Its funny it has the same size head frame that COULD fit a second tool head. || Keep buying Bambu's closed system devices. Very soon you'll be in a walled garden the likes of which would make Apple jealous.
-Also no filtering of outflow air? Is Bambu trying to slowly kill its customers?
-I guarantee the overwhelming majority of Bambu owners have purchased a Juul and an iPhone in the past 10 years or less. Baahhhh!! || Who wanted to see  side by side comparison? || there is a filament maker that uses the waste broski! || You forgot to put the bearing on to the extruder gear (the one that goes on to the outside of the yellow gear). || Did you also agree that you are not allowed to talk about their changes that do not allow the use of the printer offline and that each print require authorization from their server? || As far as nozzle compatibility, I took one out of my H2D and used it on my A1, and it worked fine. I did not, however, try an A1 nozzle on the H2D || I just bought the p2s combo. This is the first printer I'll ever have owned. Ships jan 22. The interesting thing if you buy the p1s combo they charge full price on the ams2 so for me in cdn funds p1s on sale 500+400 for ams2 = 900cdn or 655usd  vs p2s 799+250 for ams2 =1050cdn or 765usd. The difference is only 150cdn or 110usd, totally worth the upgrade and this vid sealed it for me thanks. || I was on the fence between the x1c and the p2s and decided on the p2s. I have never done 3d printing before and I’m hoping this will be a user friendly machine that I can grow into. || Same || I got a P2S and it's been pretty good. The prime tower has been the cause of almost every failed print for me too... They need to put some effort into addressing that. || Just got a p2s and struggling to print some of the larger ASA parts that I've been printing on the p1s for a while. Just getting more vfa's, rounded edges and some issues with rippling on a few edges between layers. Haven't fully diagnosed the problem for sure yet but just off of eyeballing the p1s and the p2s running the same print side by side my first guess is that the steel rods in the p2s are forcing it to move just a little slower and then running into layer cooling/warping. Second guess would be that the exhaust and cooling system changes are altering the consistency of the air in the chamber. Still more testing needed before I can confirm any theory if anyone else has experience on the matter I'd be curious of their thoughts. || Dual extrusion || I got my x1c year ago.  Would it be a good idea to start thinking about a p2s, or should I just hold onto my x1c. || Insane amount of waste. Ridiculous || RE: pla waste bin - melt it down, get some silicone molds. make money off the molds :) || This is an unfair comparison, as are almost all the YT videos hyping this printer.  The P2S is an enhanced P1S and is not a replacement for the X1C.  While it does have several quality-of-life improvements compared to the P1S, It lacks several more sophisticated features (lightweight carbon-rod carriage, LIDAR, etc) that the X1C has. The X1C is in an entirely different product line and there will likely be an X2C released sometime next year. Bambu Lab will not neglect that market segment. || Bambu the worst company: 1. NO customer support; 2. HORIFIC systems to mismanage order changes and cancellations; 3. Bad policies and procedures that required me to wait 7 hours on chat to communicate on an order,  and; 4. added a fraudulent charge to an order. HOW CAN THESE YOUTUBEERS RECOMMEND bAMBU? ABSOLUTELY DISGUSTING. || Puedes pasar el STL del dragon? ^^ || 가면 출력 스토리는 굉장하네요 ㅎㅎ
-한국에 3D프린터  관련 유투버들은 재미없고
-남들 따라하기 바쁨 || VFA Monster || It's close to the 4 year old flagship for a better price, but it surely isn't better. It's still the budget version.
-The Eddie current flow sensor is cheap and bad compared to LiDAR, they ditched the carbon X axis surely due to cost, making the motion system way heavier.
-The quick nozzle swap is an upgrade if you change nozzles a lot, but everything else is worse or equal.
-From what I have seen print quality is a little worse as you would expect, with the bad flow calibration and heavier motion system.
-Still awesome for the price but not better than a X1C, for the same price I would still chose the X1C over the P1S without hesitation. || They chould have called it the X2C but then Youtube reviewers and bloggers wouldn't have made these videos...  lol... marketing genius! || I did not hear a word about VFA, this is: Vertical Fine Artifacts , small, unwanted vertical lines or patterns that appear on the surface of printed objects.
-The P2S seems to perform worse than the P1S on this issue. || Multicolor printing with a single- nozzel printer is absolute nonsense and  a waste of material and money. || Just ordered the p2s. That Majora's mask is sick || the only thing missing from p2s to be a COMPLETE upgrade from x1c, is the ability to use those vision calibration plates. || think it is the perfect home 3d printer! || yup.. now you can produce much better toys, gadgets and other useless items to print!  🙂 || I’m considering buying an X1C lightly used for the same price or even less of an P2S. Would that be smart? || Personally I'd opt for a new P2S over a used X1C. The X1C was great but the new extruder and nozzles are better plus you'll have parts support for longer, not to mention a warrantee. || @RickyImpeythanks for your input || I've had my p2s for about a month now and i don't see the options for other filament manufacturers; only "bambu lab" and "generic" . what firmware is this or did it get removed? || I would imagine they don't plan to let go of the X series as they would lose out on a segment of the market. They could add an active chamber heater and increase the temp to 350°C on the nozzle to bring it up to par with the H2S just with the smaller build volume. || where do I comment to tell YouTube that their Ambient mode is the most unwelcome, unneeded and unwanted feature in the history of features? || probably a stupid question but i never had a bambu printer but if there's files that were sliced for the x1c would they work with the p2s or would they have to be sliced again for the p2s? || Technically it would probably 'work' but you are much better slicing again || I purchased the A1 printer, and now that several new printers are being released, I’m unsure which one to upgrade to. || I'm in two minds if I should go for the clearly excellent P2S when it delivers in the UK at "the end of December" or wait to see what a new X generation might deliver. My guess is it'll be  along the lines of slightly larger build volume (285 mm cubed?), finer tooth belts, quicker multi colour handling with less waste, and better emission control at a £1,200 price point. That would be worth waiting for, but will I get it? 🤔 || if you have all pla waste from the same brand. i wonder if you couldnt melt and shape it backinto a  randomize multi color filient || Semms like BambuLab controls the game, with the whole suit, but somehow Snapmaker solution for the multicolor seems unbeatable. afraid to buy and try because i'm a fan of the Bambu studio (Not Orca) || Mark my words
-The x2c will be a 305mm cubed print volume version of the p2s 😊 || Yes, but predict how much now. 💸 💸 || They should create a way for us to modify x1c into a nozzle swapper like h2c🤷‍♂️wishful thinking || I just bought the P1S 😂 || I hope they do a p2p || How do you get the nice timelaps without printerhead moving? Like at 10.54 in this movie? Thank you. || In bambu stuxio at the others tab you have timelapse moxe || Maybe, they should put a Vortek system in the X series to get a mid range printer with minimal waste for multi-color prints || Bingo.... 4 nozzle implementation of Vortek... X2C will be something really neat along those lines. || What he means is he works for Bambu labs || Nope the H2S rules the p2s is for videos || There are quite a few ways to reuse filament so you don't need to wait for someone to invent one. There are those that have already been invented and the last time I heard about one was probably 5 or 6 years ago. What I mean by that is it's been that long since I've printed anything because I had open heart surgery and other issues that I've been overcoming. However, I just acquired a Creality K1 Max. That's wonderful. || ordered my one couple days ago , can not wait to get it :) || have you played with it yet? I'm on the fence about ordering one || "I got this for free and also I benefit directly from your sales but I'm totally NOT influenced by this."  Sure dude || Looking to buy my first 3-D printer for printing car parts what do you think I should get? X1C,p2s,p1s? H2s is a bit out of my budget || Which printer eliminates poop (waste)? || The Bambu H2D eliminates most waste because it has 2 heads, so if you print dual color, the heads do not need purging. || So p2s does not have other filament makers in it. Are you sure it didn’t pull your customs from Bambu Studio? All I have is BL and Generic profiles. Fully updated on firmware and software. || How did you manage to grow your beard that fast ?!
-Yesterday I was watching your other video "Ender 3v2 - How to Calibrate E-Steps (Quick &amp; Easy)".... Without a beard ! || he used ams 2 || They should try using ink to make full rgb color printing instead of keeping the colorswaps. They did a huge leap in the 3d printing consumer industrie so now they should do it again || Please can you stop selling, show me the wasted material and time compared to the Snapmaker U1?. Affordable multicolor 3Dprinting or nothing. || He showed the waste || I was going to pull the trigger on the P2S but stopped. Not filtering exhaust air is a complete no-go. I'm waiting for an X2 instead. || I agree. I wish manufacturers took the UFP/VOC aspect much more seriously than they currently do (that is, not at all apparently) || there's already solution for this || ​@izoytmay I ask what it is? I'm about to pull trigger on P2S next week . I no idea about 3d printing but I thought this was the one to get for beginner || @Kyumilliyou can print a top panel mod for this. Or, Bambu sells an entire kit that goes on the back for this || It was communicated, that the P2S will replace all previous machines in the range of X and P series. So it's made to replace the X1C, P1P and P1S.
-Also the P1S never was a compromise for the printer part. The X1 never made much sense besides the better display for those who wanted it.. That's why the P2S is what it is. || Is there room inside the chamber for a bento box? || Asking the real questions! || Merhaba bende p2s combo aldım ama x1carbon modelinde ki karbon alaşımlı filamentleri kullanabilir miyiz? || evet basıyor || @cotyoran0652 aldığım sitede müşteri temsilcisi bana basar ama ideal değil çünkü içeride ki ısı carbon alaşım için ideal değilmiş dedi || @ALİARIÖZSOY-c2x Web sayfası bilgisi de o şekilde ama bir amerikalıdan aldığım bilgiye göre dikkat ederseniz kasanın sol duvarında birkaç monte deliği bırakmışlar, buraya harici ısıtma takılabilir gibi birşey söyledi gelecek güncellemelerle, umarım o şekilde olabilir. Genelde basabiliyor diyorsa basar, sertleştirilmiş çelik nozzle var bunda, extrüderi daha iyi x1c'ye göre, H serisi nozzle var bunda. Fakat şöyle birşey var yüksek oranlı karbon değil de belki düşük oranda yani yüzde 10 gibi katkılı filamentler rahat basılır. Tüm mühendislik malzemelerini zaten her makine basamıyor. Karbonfiber basan youtuberler gördüm bu arkadaş gibi p2s ile. || @cotyoran0652 anladım ürün henüz ön siparişte gelince deneyeceğim çok teşekkür ederim sağolun || @ALİARIÖZSOY-c2x bendeki de ön siparişte sizin gibi bekliyorum || honestly this just feels like the same old thing lol. was hoping for smth new but nah… same issues, just a new name. || Paying €730 for the 3 year old P1S AMS2 combo 1,5 week ago. Or paying €750 for the P2S combo with all the improvements it has over the P1S...
-Actually... the X1C was the better printer on a few fields over the P1S, but at a pricepoint of roughly €400 more. Now you buy a "X1C plus" for the same price as the P1S a short time ago. Can't figger out how that will be bad... || Bambu lab Delta would be cool. || Really, for a next gen X series, I guess they could just do an X1C sized H2S and price it between the P2S and H2S.
-As for the A series, there's not a whole lot that can be done; maybe just add the new nozzle/extruder system so they have nozzle compatibility across the board. || I bought the X1C just months before the H2S was released and had the same issue with the A1 mini, unfortunately this is business but, come on Bambu Lab, why do this to your followers? || Спасибо! Обзор класс!=) || just got one today, really excited || Im still waiting for november to buy without AMS :P || @justmike2916i just had to test it out, have had a prusa mk3s for years now and really missing mmu || Same here! Great machine, I’m super happy with it || Still the same closed system and the same issues, just repackaged. Real innovation seems long gone. || Free stuff review || Printer poop is so yesterday. || LOL, it is P1S all over again, no real improvement and the same security risk 😬 || china enshittification style .... RIP bambu || So nasty smell still there ?
-Disappointing || I don't smell anything, but I've only been using  PLA so far. || @chrismaidens6676 So P2S still good ? || Been looking forward to your thoughts on this new printer and it's place in the line-up going forward.
-Since the H2S came out at the same price the X1C used to be, and this seems to be the update to the X, do you think going forward we will have the H, P, and A with the X ine going away? || Lets see what the new Snapmaker sells for, it looks more appealing to me than this P2S. || Keep in mind that you have to spend an extra $150 for the U1 to be enclosed, and also it can't do more than 4 colors. I was excited for it, but I don't do multicolor printing enough for it to be a big game changer for me. || @NWGR Good points.  I'm still searching for what best fits my needs.  I mainly print with engineering filaments and will use a second filament solely for support. || @TC-hl1ws Honestly, if it were me, I'd get the H2S for engineering filaments since it has a heated chamber. I know everyone likes larger printers, but I'd be happy with an X1C sized H2S. Maybe a new X1? || @NWGRI’ll check them out thanks.  I use a Statasys at work but would like something for tinkering at home. || The multicolour prime tower was impressive as too was your dedication to holding it up for 20 minutes. LOL || Just use superglue/baking soda to glue to the bed with a couple drops.  Will scrape off. || Are the x1 getting an upgrade kit? || No. Series 1 printers will not get any upgrades. || I bought a X1C just 4 days ago. I can't decide if i should return it and get a P2S instead :( || Omg same haha || I would just keep it. It's quite an effort getting it back, end result is the same with either one you end up with. || u should || Buyer beware. If its faulty return it if its not then its what you ordered. 
-You could buy any printer and the next day another manufacturer releasses a better one for less. You made your choice and spent the money. || Depends if you're in the US and you're willing to wait until it's available here || Not one mention of the new nozzle cleaning system.. Even though you had 2771 filament changes?!? Why is not a single review talking about it. It was a huge fault on the P1S where filament poop would get thrown on to the build plate. I don't get it. || Getting the latest printer for free might have something to do with it. || I love how all the creators that got these for free are talking about how great they are but fail to mention the fact that bambu is pumping out machines 2-3 times a year. You would think..awesome. Is it though? They just put the P1S on sale and Im sure a bunch of people bought it.  Then 2 weeks weeks later they release this. The people who bought the P1S would feel ripped off. Im one of those people || While the P2S has some nice features, i'd still be happy with a P1S. But then I would say that, I run an Ender 3v2... || @faa_luke1359 I heard Ender's were pretty good. I just don't want all the tinkering around. I want to load stuff up and it just print. || That’s everything, not just Bambu. Phones, laptops, TVs etc allllll tech does this all the time. Buy something that suits what you want or wait but the manufacturer has to keep up with competitors || @notthatkindofsam It's just slimy business practices. Why not announce the new machine, THEN put the older ones on sale. It's a pretty scummy move to have a sale, knowing you have a new machine coming, THEN tell everyone about it. I already sold the machine and I will never buy anything Bambu labs every again. || Don't make judgements based on limited information. Bambu has offered multiple people who take the time to reach out to them free upgrades of gift-cards to people who bought P1S just before the release of P2S. But yes, don't ever buy anything Bambu again, I hate when stuff is sold out and I have to wait :D || What should i get now? P2S or X1C || I have the X1C and the H2S. The P2S is a smaller H2S for me, so get the P2S all day long. 
-Passive chamber heating control, all hardened steel hotend and quick change nozzle are all far superior to the X1C. 
-I can’t believe it’s so much cheaper and so much better - brilliant pricing IMO. || ⁠@garymelrose9727 How about air filter ? I sold A1 with intention to buy enclosure version of it like P2S but wonder if it actually is better at this than P1S || X2C || @juanricardopenas9274 How would they sell such a thing with these prices now?
-The P2S already has way better specs then the X1C for the price of the old P1S. When the H2S was released, which practically was a oversized X1C at release, was already cheaper then the 3 year old X1C. While being bigger, having linear rails, 3 year newer tech and many things more.
-They should make something very special then, making people not going for the cheaper P2S or for the bigger H2S. || Try to find an X1C anywhere, then ask again. || Good and informative video. Do you still have to transfer gcode via Bambu Lab's cloud or can you transfer directly via your private LAN? || It transfers through the cloud for me. || The color change is bad on bambus. I like the multinozzle tech which prusa is using || At 10x the price for poor quality and non engineering filaments? That’s what I would refer to as ‘bad’, but each to their own I suppose…SMH. || is quieter than x1c?? || I have watched 3 different videos on the P2S and not one of them mentioned printing noise! Disappointing reviews.. || ​@GTW-1807i think so || WOW this was read word for word from Bambus Script. || I got that impression as well. || thanks for this review, how would you rank the noise level? || I am also curious about the noise || About 50db when printing, no noise when not used because there's no fan whatsoever that runs during sleeping mode. || @moirbo05 Thanks! || Does this still have WAN only mode - struggling to find this info - good vid thanks || It does, i saw someone mention it in a different channel review. || @coryjay16 Thankyou!</t>
+          <t>❤   Amen  🙏 
+        It is not the  mountain 
+        we  conquer, but 
+        ourselves.   ❤</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>UCYyel9YAgwvs07rz5kugU7g</t>
+          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Ricky Impey</t>
+          <t>itsbasicbible</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Pt2j2BWcAqM</t>
+          <t>WEm0xvO7HDk</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Flexing on TPU: The Best Flexible Filament Alternatives for 3D Printing</t>
+          <t>Your Phone Is Destroying Your Focus (And You Don't Even Know It)</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>TPU has been the go-to flexible filament for years, but is it still the best choice? In this video, I put TPU head-to-head against newer alternatives like PEBA, Morphlex, and PLA-HR to see which flexible filament really performs.
-You’ll see side-by-side comparisons, bounce tests, and real-world prints to find out where TPU still shines — and where the other materials completely out-flex it.
-Whether you’re printing phone cases, gaskets, flexible hinges, or even sports gear, this guide will help you choose the right flexible filament for your 3D printing projects.
-*This video is sponsored by PCBWay*
-Custom PCBs, 3D printing, and CNC machining! New users can get projects started by saving $5 at PCBWay here: https://pcbway.com/g/0IW9ST
-*Up to 40% off TPU(FDM) extended through October*
-*Affiliate links (If you purchase something after clicking any of the below links I may earn a small commission at no cost to you. This is a great way to support the channel)*
-*Synbotron PEBA*
-https://peba-filament-the-next-gen-of-flexible.kckb.me/96226c87
-*Other PEBA Options*
-https://amzn.to/4gTJjCp
-*Morphlex*
-https://tidd.ly/4gV1qYx
-*PLA_HR*
-https://tidd.ly/3KA8o9t
-*TPU*
-https://amzn.to/3IUFEHV
-*BQ Slippers*
-https://tidd.ly/46Pd1nt
-*Fanttik F2 Master Mini Cordless Rotary Tool Kit*
-Fanttik is running a Big Prime Day promotion, offering up to 37% off on Amazon!
-Use the extra 9% off code RIE3ULTRA to save a total of 46% off the Fanttik F2 Master Mini Cordless Rotary Tool Kit: https://amzn.to/4gTJjCp
-*Durometer*
-https://amzn.to/46XrQVd
-*3D Pen*
-https://amzn.to/48cHONt
-..............................................................................................................................................................
-BUY ME A COFFEE
-If you're enjoying my content, why not consider supporting the channel by buying me a coffee? 
-Even very small amounts are greatly appreciated and re-invested into bringing you better content.
-https://www.buymeacoffee.com/rickyimpey
-You can also use the YouTube 'Thanks' button above if you prefer.</t>
+          <t>The digital age is influencing our lives more than we realize. How often is the device in your hand (smartphone) dictating your thoughts and values? Jesus warns us in Matthew 6:22-23 that "The eye is the lamp of the body." Our eyes and ears are the literal doorways to our soul (mind, heart, and emotions), and they ultimately determine the course of our life (Proverbs 4:23).
+In this powerful Christian message, we uncover the spiritual danger of distraction. Christ demands your singularity, your focus, and your undivided attention. He doesn't want to compete with Spotify artists, Instagram influencers, or Netflix. You are constantly being discipled—will you allow Christ or Culture to shape your worldview?
+We explore the profound Jewish teaching, "May you be covered in the dust of your rabbi," to understand what it means to be a truly committed disciple of Jesus. This requires us to let the Bible be our filter and the only lens by which we see the world, rather than adopting worldly ideologies. Discover the specific unholy influences (social media, music, movies) Jesus wants you to let go of to clean your soul, become His uncompromised witness, and fully step into your true purpose and calling as a man or woman of God. Learn how guarding your heart brings clarity to God's vision for your future.
+00:00 Introduction: The Power of Digital Influence
+00:53 The Spiritual Impact of What We Consume
+02:07 Guarding Your Heart and Mind
+04:37 Choosing Between Christ and Culture
+05:55 Walking Closely with Jesus
+06:39 Practical Steps to Purity
+09:31 Living as a Witness for Christ
+10:34 Conclusion and Prayer
+12:32 Final Thoughts and Resources
+Connect 
+https://linktr.ee/itsbasicbible
+MALTA APPAREL LINK 
+https://malta-apparel.com/?ref=BBAZ16 
+FOR 15% OFF: basicbible15 
+FREE 10 DAY DEVO BOOK 
+https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
+I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
+https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
+I WANT TO FOLLOW JESUS CHRIST
+https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
+Get vidIQ to grow your channel faster! 🚀
+https://vidiq.com/itsbasicbible</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-10-05T16:00:45Z</t>
+          <t>2025-12-06T00:00:43Z</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>166104</t>
+          <t>27</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>3034</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>227</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>0.019632</v>
+        <v>0.185185</v>
       </c>
       <c r="M8" t="inlineStr">
         <is>
-          <t>It's weird to call it airless balls. There's obviously air in it. 😊
-A 'non-presurized-ball' is much more pedantic 😊 || "we see the sun for 3 hours every year." hilarious || I constructed a intelligent comment, but I'll get to that later. || I have a 5m pro and never was able tô print a single piece with tpu || Build an RC Car using OPEN RC files with the PEBA. || 95A and down? Me staring at a 98A roll here || I wish you would have done the bounce test with regular PLA as well. I understand there is no flexibility, but would be interesting to see the rebounce on it. || Try using peba vs pla in compliant mechanisms like springs || great video but ditch the AI thumbnail, Just use a picture from the video or anything else. AI makes your video look like it will be low quality and like slop (it does a disservice to the effort you very obviously put into it) || I'm not going to watch the video and just want to leave the feedback that it's because the AI slop thumbnail makes me assume it's probably not worth watching. || Why does my bowden Ender5 print then soft 60A on slow to 35mm/s? TPUs are a standard material with my Ender printers😅 || так тпу нужен исключительно для гибких деталей, для остального есть TPE от Esun, он силиконоподобный || great video. one thing i think would be better test result if peba and tpu are the same collor reason diferent pigment act diferently for example black will be stronger ,harder and more riggid than other collours || 4:10 video starts. I almost didn't make it through all the babbling || "As you'll just end up with clogs".... Yes..I heard it, I even smiled. Well done. || tpu offers a wide variety of shore hardnesses. they also offer high chemical and abrasion resistance. do these new alternatives offer the same? || You only see the sun 3 hours of the year!! Must be down south. Lucky man || I think the most important question is, "Is there any 3d printing channel of any size +25K subs which ISN"T sponsored by PCBWay?" || What would you recommend for cold weather applications like tracks for an R/C vehicle? || peba sounds nice but 50 bucks a spool makes it too expensive for most. then biqu is the same. bring those prices down to 25 and its game on || 2:13 best consumer printer on the market, but can't beat a prusa Mk4 when it comes to printing soft TPU? though I suppose he doesn't mention what the hardness of the filament is, maybe it's less than the 85A that's about the limit for standard printers. || Hi Ricky, very interesting video, thank you. I do have a real time project for which I currently am using Bambu TPF 95A-HF and am so very keen to explore these alternative filaments. Do you know if they can both be bonded together with either flexible glue of solvents? || One thing I don't like about PEBA is that it costs 3x as much as TPU. || What printers use these newer flexible filaments the best? I'm about to buy a 3d Printer today and looking at the Bambu P2S || A very interesting video, thanks, always interested in flexible filaments.  F.Y.I. I have an Ender S1 Pro and after much fiddling can print Recreus' 70a TPU successfully. Makes very good 'rubber' replacement parts for old motorbikes. || We see the sun about 3h a year.... best man! || tpu para ams || my tpu 95a bals bounce way more than that lol || Outch peba 80$/kilo canadian pesos 😢 || Very interesting video. I'm thinking to try out PEBA. My idea is instead to make shoes, just to make airy soft inlets. Let's see. || Why 800g rolls instead of 1kg? To include a bit more math when comparing prices? || I just bought 10 rolls of tpu to restock!!! || Great tests, thank you. I wish you have made a compression test, i’d like to print a subwoofer feet ))) || Too long to get to the point. And... if I was interested in getting someone else like PCBWay to make my parts, I wouldn't have bought a 3D printer. I'm only at 4:03 to be fair, came here to see what replaces TPU, a known bothersome but wonderful print material. || BIQU, being Chinese would be pronounced more like beee tchu not be cue.  Cheers. || Your link to PBA options does not bring you to the right product. Great video though! || Good video. I know it's a strange question, but what material would you suggest for 4" to 5" diam. X 1" wide RC plane wheels. The plane itself weighs 40 lbs. and uses 2 main landing gear wheels. The runway landing surface is asphalt. Thanks. || Holy shit all these guys are the same on YouTube 😤 || Having options is a great things, but don't let fool ourselves by  considering only cheap 3D printers. Only who never used, for example, a Stratasys F series can describe a Bambu Lab PS2 as an high-end machine.
-This is to say that is a normal thing printing TPU 60-70 Sh.A with truly good results by using professional FDM 3D printer, so if you need certain shore hardness you need proper hardware, not snubbing very soft TPU just because our cheap hardware can't manage it.
-In the past I was able to print a lot of 60 Sh.A TPU with a custom machine with a proper feeding, cooling and extruding system (e.g. with an enhanced Flexion extruder.)
-Happy printing! || Great series of experiments and analytics. Thank you. I would lover to see the shoes you printed in TPU in PEBA and possibly and multi material print with Moreflex, PEBA and foaming PEBA. 😊❤❤ || 😂😂only get 3 hours of sunlight every year 😂😂 || Great video. Super insightful. You could also check out Filaflex 95A Foamy filament, and do some grip testing. I'm printing tires for my RC cars, and have not yet found acceptable filament. cheers! || Ping pong ball? || An excellent, informative video. Thanks for taking the time to create this 🙂 || Why did you let the balls down like that in the drop test instead of just holding against the underside of the table between two fingers and then letting go? It looks like you're releasing them differently even in the video. || Would one of these materials work well for making sewn on patches. I know a lot of the patches are injection molded but was thinking of trying 3d printing in tpu. Maybe another material would be better. More uv resistant? || 3 hours of sun a year. That was funny. || There is a slight error in the calculation of the return energy. You should take into account the center of mass (the middle) and not the lowest point.
-For the TPU tennis ball, you calculate 25/80 =~ 31%.
-The correct calculation is, assuming 6.6 cm balls, 28.3/83.3 =~ 34%.
-The difference is even bigger for the larger diameter basketball. For PLA-HR you calculate 50.5/80 =~ 63%.
-Assuming 24 cm diameter, it should be 72.5/102 = 71%.
-That said, I'm impressed with your effort, and the comparisons are relevant. A big THANK YOU! || Then, sholdn't you measure the lowest point also from the center of mass? || @nicklaich@nicklaich  Yes, maybe I wasn't 100% clear, you should evaluate the bounce using the center of mass of the ball, which, in this case, is the center of the ball. || ​@mrmariusi I mean you must also measure not from floor but from the lowest point of trajectory of center of mass || I could see PEBA and PLAHR being used for is sound or shock dampeners, like for sound studios walls. Also feet or cushion dampeners between metal parts for machinery, based on possilbe longivity of the materials. Also testing for UV you could put in a box with a UV light and let sit for a few weeks or a month and see its results || TPE || What a perfect market for pcbway to enter given their existing business. || What would be a good material to produce cassette drive belts? Unlike rubber bands, these belts usually only elongate 6-10% and should not have much rebound to them to minimize "wow and flutter". Iirc the stock  belts are about A68? Typically these belts are 5mm wide and are over 2" reels at maybe 4" center to center || Everyone is looking at TPU/PEBA wrong.  We should be looking at _HARDER_ versions of these materials, NOT softer.  Nylon's whole deal about being indestructible is it's resistance to delamination - TPU/PEBA being harder basically becomes Nylon without the stupid problems of being extra slippery and difficult to drive.  Printing softer and softer filaments makes no sense.  If you want softer, you cast. || I agree with and also strongly disagree. First, I agree that having harder versions and finding better substitutes for Nylon is really good and shouldn't be overlooked. 
-But..... Like ..... 3D printing main sales pitch is it can literally enable you to build things that are impossible to cast or make traditional. For example you can literally print TPU and PETG together in a multi-material printer, having it interlock them together (finally a feature now in some slicers). 
-Always good to look for better materials, but they should definitely look in both directions! || I can tell that's a damn good point and I just got into this hobby (addiction?) || I invented a medical accessory from 85A TPU that works great on the Bambu A1.  The spool has a basically sealed connection that takes the filament from the driver box directly to the canula to the extruder without it being exposed to the humid room.  My product was not going to possible if I had not been able to make this setup work.  That stuff absorbs water like a sponge even with a dehumidifier running in the room it still got way to wet for long print times like making 8 or 12 of this part all at once.  I have never heard of this bouncier PEBA material.  I don't think it would be right for the product I designed and am printing but it's good to know of it in case I have future needs that it would be right for! That's for the knowledge! || Which Filament has the best elastic properties so I can print elastic for clothes || I really wish you'd included NinjaFlex in your comparison || alwaays PC way || As always very informative video || A bounce, or restitution, test should be based on a smallish solid ball of the material. The honeycomb structure of the ball has its own properties that impact the test. If you want to only test the material, and not the structural dynamic component of the physical design, use a solid sample. || I like harder TPUs for their lack of flexibility. I have some camping gear and bike mounts for my truck I printed out of TPU. It’s virtually indestructible. Minor flexibility doesn’t make it the best option for everything but for objects that get slammed around or you slam stuff into it’s great. Never had much of a use for the really flexible stuff. || I just watched your KlipperScreen installation video (which as usual is awesome), and I clicked on this one and for a second I thought I was watching a Veritasium video :) || I print TPU with volumetric flow 12mm3/s with x1.1 flow rate compensation. On A1 mini printer. But it require precise tight extruder screw - one revolution more or less and max flow rate fill be smaller. 90A shore || How does annealing the printed TPU parts affect the results? || NBA Regulation is 70-78% Rebound Percentage || Would Peba be good for non-maring pads on clamp jaws?  Anything better for that?  Enjoyed video || I tried to buy via your amazon link, but it doesn't work.  It doesn't show peba but something else I bought in the past. || That's usually a sign that the item i linked to is out of stock but I'll check, thanks👍 || Ok but what about things like chemical resistance, or the ability to handle high compression pressures.  These things are where TPU really excel in my opinion.  Making weird gaskets even some for high pressure systems such a pneumatic cylinders and its chemical resistance make it an easy money maker for 3d printers.  I was able to pay for my 1st printer in a month 3d printing gaskets for a factory to allow better rebuilds of pneumatic cylinders. || it would be fun to use some flexables show us some tips and tricks || TPU's low energy return is a huge advantage when you're after vibration isolation. One such application are camera mounts for drones. || And here I am playing with peba for drone camera mounts...😅... || He mentions this near the end... || Car bushings and bump stops as well || I will have to keep this in mind! || You talk to much. Get to the point. TPU is cheap? lol || Can you mix  these materials with more "regular"  print, say PLA or PETG, say to work as softer-than-the-rest, hit prevention areas? Will they connect together? What would be the best replacement for  1.5mm dense foam layer? || Huh. Ungodly expensive Bambu printer is the most advanced out there, yet my Neptune 4 Max prints 70A TPU right out of the box. Weird. || No PEBA filament in the market to purchase whoever. || How is tpu disposed of. I have a print that didn't work out and I just have it there. I can throw it out but I wonder what happens to it. || In Australia at least, TPU is still the go-to based on price unless you need one of the others for a very specific advantage they have.  4 to 5 times the price of TPU here !!! || thanks for sharing 🙂 || I would be very interested in seeing these different filaments in a rc (remote control cars) component like suspension ie: A arms/ wishbones etc. In this the energy return would be interesting as need to be stiff enough to be used in operation but flexible enough to be able to take impacts (when hitting rock/wall/ ground from height etc) and retaining/ returning its original shape. The cold test would be invaluable also as this is where rc components are at highest risks of failure when driven at cold temperatures. Also in UK so need any help with testing then give me a shout. || I've gotten a roll from Siraya Tech on sale for even less than shown here. Symbotron is out of their mind with the pricing. || The link for PEBA is actually for the rotary toolkit || Surprised to see such a big account saying a blanket statement of “I never advise to invest in a kickstarter “ … like for 3D printing community or makers or whatnot, that’s a pretty harsh outlook on a platform that is one way many startups or people with good ideas can get their product to market. Sure many fail, but good ones with a good plan don’t. And agreed, this filament in particular seems poorly priced. Hot take though. || Fair point, I probably should have explained my statement better. I didn't mean it as a negative, only in the same way that I never tell anyone to buy a product. I think people should gather their own information and not invest in something like a kickstarter without knowing the risks.  I invest in kickstarters myself, for the right people it's a great way to get products into the market. || Hello Ricky, been following your channel for 3 years now and I have to say you changed your visuals a lot 😄, you look a lot more juvenile and your new hair style and the beard fits your face pretty well. Can you believe I randomly found this video and I only recognized you after a few minutes into the video, because of your voice and the the way you speak so articulate. Congratulations on the change. (I'm not gay, if you're wondering 😁) Keep bringing your amazing videos. Big hug from Portugal. || Ha ha, thanks man. Appreciate the positive comments. You made me smile this morning reading this. Perhaps you should subscribe so you don’t miss out on any further changes to my appearance🤣 || ​@RickyImpeyHi, I'm subscribed to your channel for the last 3 years, been following you since I bought the Ender 3 S1 Pro, you helped me a lot back then with a video about the bed leveling of the Ender 3 S1 Pro. You shared with us how to add the command "M420 S1 Z10" to the Start G-code, so it would keep the leveling data. Now I sold the very reliable Ender 3 S1 Pro, and recently bought the Creality K2 Pro, been loving this new printer. Cheers || Ricky, I'm mostly going through flexible filaments for another application: gripping arms for machinery. Imagine something like a bottle cap screwer with mechanical arms that grabs the bottle cap and twists it until its closed. TPU can be great for this, but non-related to hardness I find that the surface sometimes isnt "grippy enough" between brands. Would you be able to provide a quick note on if any of these materials you tried felt particularly grippy? || A couple of people have asked similar questions, I feel another test coming on.... || ​@RickyImpey
-Would be interesting to watch!
-So far Filaflex 60A has been the best in terms of grip - but it's extremely challenging to print with. Between the usual TPU/TPE 85-95A, it seems to be more of a issue how matte the surface is, as softer rubbers can perform worse if the surface has a slightly matte finish. Will try Filaflex SEBS soon. Maybe play around with fuzzy skin, but I suspect such techniques will be more susceptible to wear &amp; tear. || I "designed" and printed some TPU roller skate cushions/bushings from 95A TPU, and the main thing I noticed when skating on them, is they compressed during the session and I had to keep tightening my trucks - I printed them at 100% infill, but as the sides are open, they were likely just squishing. Normal cushions are urethane, so I would be curious about the feel of the higher energy returns from the PEBA. I did get the attention of the manager of the local roller rink, so printed a set for her for her derby skates, but I haven't had a chance to go back yet. (Designed is in quotes, as it is a simple cylinder with a hole in the middle - just did that in the slicer, but then made an OpenSCAD model for future use.) || I've actually been thinking about almost this exact same use case for a friend of mine. I'd like to do some experiments if I can think of a good way to measure how different filament responds🤔 || A tip for releasing tpu from the print bed is to spray some alcohol on the bed and it seperate the bond easily and has made tpu so much nicer to print || 20% lighter means you get 20% more spool length per kg which is amazing || I get you need a clickbait title but “is tpu dead” and questioning if its now all of a sudden irrelevant because some other filaments in an already niche market segment (flexibles) have gained a mild anount of traction for an already niche demographic (enthusiasts) is just a weird, hyperbolic, and unrealistic take that doesn’t really mean anything. Id wager your average Joe with an a1 they got for xmas hardly even knows what TPU is to begin with let alone peba etc
-People also for some reason like to forget about price when making such ridiculous claims and lines of questioning. Sure peba is great, but it’s also like $80 for a spool va $20-$40 for some tpu. I’ve gotten quality 95a for like $15 on sale lol || Be interested to see how it fairs in the ultimate 3d print torture test.... Robot combat || 21:21 Hehe. I wonder how many people actually got it. || 😁 || Figures, the slippers don’t go up to my size || Prusa core one prints tpu stock no problem 😂 || I wish tech monkeys stopped doing these clickbait titles ... Downvoted and don't even care about what is said. Moving on. || 5:38 BEPA ball has an unfair advantage of few extra centimeters... ;-) Balls were not dropped from the same high but I assume it doesn't effect the result significantly... || Apologies if it looks that way. I actually did at least 10 drops with each and averaged the results. I probably just picked the wrong footage in the edit. || Toxicity? || I love my fanttik, 100% recommend. They tried to do Apple design, and did ok at doing better than usual. Not Apple level, but good. || Isn’t every 3D printing video sponsored by PBnJWay now? I do believe so. || Thank you for the informative video. I may have missed it (unfortunately, my English isn't that great yet), but I'd still like to know how you processed PEBA and PLA-HR. Did you feed it through the AMS 2 Pro, and what settings did you use for your tests? If it's not too much work, I'd appreciate this information. Thanks again for your tips – best regards from Germany/Bavaria. || Sorry, perhaps I didn't explain well. All of these filaments need to be treated like a soft TPU in that you can’t run them through multi-filament systems like an AMS. You can use the TPU outlet on the AMS-HT but it can't be pushed down the PTFE tube by the AMS motors. || @RickyImpey Very kind of you to reply.
-I was afraid of something like this :-)
-Thanks again and best regards || I have been printing quite a bit with TPU lately, and it is always pretty funny to me to see that most people are looking for the softest TPU available, and I am looking for the absolute hardest.
-I have been printing several things for practical uses, PLA seems to prone to brittleness, PETG is darn near perfect for most ridged body things, however it still is too brittle when using it on very thin, or spindly prints, so I turned to TPU, I very much enjoyed it's near indestructability from impact and delamination, but it was too soft for ridged body prints, I found some sooper hard 72D TPU, and it is the definition of frustration, but the stuff is SO tough, I printed a test cube and took it to my anvil and hit it with a piece of metal, it left a mark but nothing more.
-It also will print out of an AMS, which is nice since I'm in a totally different building from my printer.
-I've heard it prints a lot like nylon, I've never printed with nylon, or most materials for that matter, I am not big into 3d printing as a hobby, instead as a means for my other hobbies.
-It's resistant to cutting, essentially impact impervious, is strong in thin parts, prints cleanly, but I've had a few troubles with layer adhesion, when printed well it has a high layer adhesion, when the print goes wrong, it can delaminate, I suspect I'm having temp troubles, I'm still getting it dialed in.
-I see TPU, as of right now, the best material to print tough parts, especially thin ones, I hate the slow extrusion, but it's a worthy tradeoff, I want a hard material yet that can bend and not break. || I’m sure you’re already aware of it, but bambu’s “tpu for ams” is fantastic and seems right up your alley. Very hard being 68d but still extremely impact resistant
-It’s a shame bambu botched how tpu for and is perceived (you mostly only see people screeching about it not being particularly flexible), by marketing it as an ams compatible alternative for flexibles (it absolutely is not that) as it’s a genuinely fantastic material. Almost all of the benefits of softer tpus (impact resistance, layer adhesion) but in a rigid, easily printed material. || What printer and ams do you use? || ​@kaisenberg161 P1P with the AMS, feeds great.
-I think the only 72D TPU on the market is from CC3D, it's what I use, it sucks to print with but it's super tough, I print at 4MM/3 and 255C nozzle temp, nearly no cooling, 70C bed temp
-If you're interested I can give you my list of changes I made to the TPU profile, it's a very unpopular filament and there's not a lot of information out there about it.
-Glue stick &lt;required&gt;
-I wish there were more options for hard TPU like this, when it's just 1 company making it, it worries me they'll discontinue it or something.
-Also, when I say it's resistant to cutting, I mean that relative to other TPU that cuts like soft rubber, this is more like cutting tire tread, hard, but not impossible. || ​​@Evanevan-v5jthanks, I wondered if 72d tpu could be used with bambus ams since their tpu for ams is rated at 62d but it doesn't behave like the usual tpus with the rubbery properties it just snaps, the 72d from cc3d sounds like it's more impact resistant. Ill try it on a p1s so any settings you can provide would be big help thank you. || @kaisenberg161 i used the generic TPU for AMS profile in orca slicer as a base
-I changed the following settings:
-Vendor: CC3D
-Price: 27/kg
-Recommended nozzle temperature: 245 (MIN) 260 (MAX)
-Nozzle: 255 (First layer) 255 (Other Layers)
-Textured PEI (My bed, not sure of others) 70C (First layer) 70C (Other layers)
-Max volumetric speed: 4 mm3/s
-Auxillary part cooling fan: 10%
-(Unchanged from base profile, however i will list it here anyway: part cooling fan, min speed 10%, layer time 40, max 50% layer 10)
-Retraction 1.2MM
-Wipe while retracting (YES) 
-Wipe distance: 3MM
-Notes: I have had very good luck with this material, I recently printed a holster out of it, I've been wearing it for 2 days and it seems to be holding up well, I have /not/ printed that much with it, your milage may vary and I am sure you'll have to tweak the settings.
-Make sure to use a glue stick, make sure to dry it VERY WELL, it seemed pretty damp out of the package.
-this TPU is also not rubbery /at all/ it is very hard and feels closer to kydex if you've ever felt of it, it does flex though, I have several items I've printed and one of my tests is a fold test. || I have some different slides in morphlex and they’re super comfortable. It’s the ones with the open sides. The issue is that there’s been some separation between the open infill and shoe sole and I’ve had to glue them || Yes, if it's the same model then I had the same issue. It's because the designer used separate models for the different parts and then set the middle sole part to have no walls. Therefore there is a gap between the parts. I added the wall back in so that the part would not separate but they don't look as good. || ⁠@RickyImpeyI’ll have to check the model to be sure, but sounds like it’s the same one. I was going to try just running it even hotter (first pair was at 245, was going up to 260) and hope for better adhesion on the next pair, but adding the wall back sounds like a better solution. I’ll have to give that a go. I’d rather have them functional than looking good and falling apart || Woah.
-I've only been watching the really old videos, so the beard caught me off guard lol. || I would like to print insoles or orthotics. Would it last more or less than regular? || That's a great idea! || What ever happened to TPR? Thermoplastic rubber. Great for chewable dog toys and much more. Very bouncy too, perfect for bouncy balls. || We only see he sun for 3 hours per year. 😂 || what is friction on these alt materials? || Since your video is quite new: Can you say something about heat resistance of the PLA-HR? At what temperature does it deform or lose its mechanical properties? Can't find a single video, test or producer spec sheet about this... too expensive to just order and test it myself. Thx! || I'd believe an actual basketball would be at 80% because the air inside acts like a wave for the impact vibration to pass through, and air taking up space inside allows for more bounce, whereas the airless one is well... airless, there is no force keeping the air in so the moment it impacts the ground the air inside it just gets pushed out through the million holes it has, and with so many holes, there is less surface area for the impact to ripple across the ball. || Now accourding to other brands:
-PEBA: 170 eur / kg
-TPU: 18 eur / kg
-So I don't think that PEBA could be a really big rival to TPU in the near future. || With the right design 95 A is soft enough for shoes. Layer adhesion or elasticity is not. PEBA has better elasticity, idk about layer adhesion. || Bambu doesn’t care about TPU, it is a side thought. It’s obviously in each printer they’ve released that it was an after thought. It’s obvious in their TPU profiles that are just wrong and slow for no reason, using profiles from when the X1 first released. There are many other printers that can easily handle 80 A TPU at speed, Bambu has held back  awareness of TPU || totally agree with this, my roll of bambu branded tpu 95 printed horribly using the stock profile, dried prepped as required. The sunlu profile i downloaded and used gave me near perfect results. || 7:00 .... and what was the result of the elongation test?? || IF you get over 85 on an A durometer, then you need to go up to D as you're outside the proper, accurate, test range of A. This is the most annoying thing about flexible, they're never labled with a valid durometer rating. Might as well just guess when you're above 95. All those "96A" tpu's are not 96A, their missmeasured. Try testing 4 different brands on a D durometer and they'll likely all be different. It's like putting a 250Killo and a 300killo man on a scale that goes to 180kilo's and declaring them the same weight. || Some good info there, thanks. That's not something I knew. || @RickyImpey Official Durrometers use a physical spring, near max compression and near zero compression things get non-linear and other issues make it ill advised to use springs in those regions for precision measurment. This is why the Shore scales overlap so much.
-For most TPU's out there they should be using the D scale. The rating would be in the 20's IIRC. || PEBA tears much easier than TPU || Do airless balls really not have any air? Nope, they don't have any pressure. || Love the clog joke! :D || Sorry to sound like that guy but testing TPU hardness right on the edge gives false low readings — the material flexes instead of resisting the probe. Always measure at least 12 mm from any edge on a flat, solid section (ideally 100 % infill, 6 mm thick). If the part’s thin, back it with a rigid plate for support. Edge readings don’t reflect true Shore hardness. || Thanks, that might explain why I was getting such varied readings across each part. || I was going to say that all those readings seemed suspect to me. || Thanks for saving me 20 minutes of watching incorrect testing and analysis based on those results. || ​@jonathannguyen9425that was only a small part of the analysis, there was a lot of valid (and arguably more useful) data still || @WhatDennisDoes Thanks for the heads up.  I'm back in! || What about using PEBA for cell phone covers ? || I'll probably stick with TPU for most projects, but it's nice to have options, especially where they have such different properties.  TPU is both cheap and quite cheerful and it's pretty predictable, so once you're used to it, you don't need lots of test prints.  I particularly like the foaming TPU, which allows you to vary the shore hardness by changing the nozzle temperature.  This allows you to do things like print progressive rate buffers for end-stops, or you can create feet for equipment with relatively hard soles but a spongy interior to absorb impacts.
-What would be interesting to know, is the bonding strength of these materials with other filament.  For instance, Functional Print Friday (FPF) has found that using PLA as support for TPU prints can work well, but its adhesion seems to be temperature dependent.  On small test prints it works like a charm, but on larger prints it fails because the PLA or TPU has cooled down too much by the time the next layer is laid down.  PETG seems to have a similar property, but at different temperatures, so it may work where PLA fails.
-FPF also found that the bond strength of TPU on PLA was not the same as PLA on TPU.  This might also boil down to temperature.  If PLA is printed much faster than TPU, you have hot PLA being laid onto cool TPU, then hot TPU laid onto still-warm PLA, creating different bond strengths between the layers.  With enough information, we would be able to tune which materials to use based on print size and temperatures.
-I think it's great that so much development is going into filament composition.  It's not that long since we only had PLA or ABS as viable options.  Now, we have a huge range of possibilities and our printers are capable of printing exotic materials too.  3d-printing has matured a lot in the last decade.  It's no longer the preserve of congenital tweakers, who manage to get a good print on the sixth attempt.  Now "normal" people can get good results on their first attempt.  I can't wait to see what the next decade has in store for us. || Love this👍 I'm also really interested in all of the questions you raise. Combining different materials could offer so many more opportunities for 3d printing. I've done some successful experimentation with TPU and PETG and used PLA as supports for the Morphlex shoes in this video. But I've had very mixed results with using PLA as PETG supports and vice versa. The experimentation continues! || What are these people talking about😂 i regularly push TPU and any other filament at 30-35 mm/s^2 with immaculate results. Why everyone is listing their max flow as like.. 7mms like the tech is still 15 years old baffles me. Even CHEAP printers can easily do much higher flow on any of these filaments perfectly fine || Creality rigs were pushing 35mm/s tpu, Bambu going 150mm/s || I wonder if this would be a quieter replacement for pickleballs if you can match the rebound force || The bounce test to calculate energy recovery has one major flaw; it ignores the aerodynamic drag. When comparing equally sized objects,</t>
+          <t>❤     God   Bless   you    ❤ || God bless you 🙏</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>UCYyel9YAgwvs07rz5kugU7g</t>
+          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Ricky Impey</t>
+          <t>itsbasicbible</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>w0AW1hXOaWg</t>
+          <t>7E57K6D-ztc</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Bambu Lab H2S: $800 Cheaper… But What's Missing?</t>
+          <t>Your BREAKTHROUGH Is Around The Corner‼️</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Bambu Lab has just released the H2S — and it’s a massive *$800* cheaper than the H2D. But what’s missing, and is it still worth it? In this quick first look, I’ll cover the key features, the differences from the H2D, and whether Bambu has cut too much to bring the price down.
-*This video is sponsored by PCBWay*
-Custom PCBs, 3D printing, and CNC machining! New users can get projects started by saving $5 at PCBWay here: https://pcbway.com/g/0IW9ST
-*Affiliate links (If you purchase something after clicking any of the below links I may earn a small commission at no cost to you. This is a great way to support the channel)*
-*H2S*
-https://tidd.ly/45LBPwc
-*H2D*
-https://tidd.ly/4lIBnEQ
-*A1 Mini*
-https://tidd.ly/3ULWyuQ
-*A1*
-https://tidd.ly/4mK9zBa
-..............................................................................................................................................................
-BUY ME A COFFEE
-If you're enjoying my content, why not consider supporting the channel by buying me a coffee? 
-Even very small amounts are greatly appreciated and re-invested into bringing you better content.
-https://www.buymeacoffee.com/rickyimpey
-You can also use the YouTube 'Thanks' button above if you prefer.</t>
+          <t>Hope is NOT A STRATEGY precise action is. Don’t be the person that waits. Begin now, because your purpose can’t wait on you. The people you’re called to influence and impact can’t wait they need what you only have. Trust God and move 
+Your Procrastination is the enemy to your breakthrough 
+Comment and I’ll personal message you 🤙</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-08-26T13:00:20Z</t>
+          <t>2025-12-05T21:44:07Z</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>9385</t>
+          <t>553</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>226</t>
+          <t>6</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>3</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>0.026851</v>
+        <v>0.016275</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>The H2S is finally here — $800 cheaper than the H2D! 👀
-But is it the smarter buy, or has Bambu cut too much to bring the price down?
-👉 Check the current prices in your region here (affiliate links, helps support the channel 🙏):
-🔗 H2S https://tidd.ly/45LBPwc
-🔗 H2D https://tidd.ly/4lIBnEQ
-What do YOU think — is the bigger build volume worth losing the dual hotends?
-Drop your thoughts below 👇 || This doesn't seen to be a very complete list. The H2S has a different nozzle wiper and some rumours have it that it is also missing the nozzle type check. This last part is very hard to confirm, which is why I clicked on a video purportibg to break down the differences. || The H2 Series from Bambu will cater for all needs, far better than the previous X, P and A Series. It appears that:
-1: H2S is ideal for those, like me, who rarely do multi colour, never do multi material and for whom the X1C was good…but not big enough and not ideal for engineering filaments. 
-2: H2D is ideal for those who need to use engineering filaments and require multi-material prints. It also allows fast 2 colour printing, but is limited in terms of multi colour printing above 2 colours. 
-3: H2C will be for those who require fast multicolour prints, multi material prints and engineering filaments. I suspect this will also be followed up with a ‘professional’ model for the industrial sector, larger print farms with copyright concerns and the ‘never cloud’ conspiracy theorists. 
-H2S all the way for me. Mines hasn’t been idle since I got it at launch in the UK and my X1C has been relegated to secondary PLA/PETG prints which it excels at. || I’ve seen some Youtubers that lost their ability to get bamboo products because they did not give it a good review. But I guess if I was bamboo labs, I would probably go to users that are happy with it. || I just ordered the H2 S and now I see the H2C is coming. I feel like maybe I should’ve waited but then again I’m sure the price is going to be astronomically high on that printer. They say you can update but it’s going to take some time. I think when my H2 S comes out of warranty. I will probably do that upgrade, even though they’re saying it’s a lengthyproject. I wish they’d be a little bit more specific about the cost of the upgrade for these printers. || Yes, the H2C announcement was a surprise to all of us. I'm glad an upgrade will be an option. The H2S is a fantastic printer, I'm sure you'll love it. || I love how these YouTubers tell us they get items from the company for free BUT it doesn't taint their opinions.... I mean come on guys.... If u accept "GIFTS" for free on the item your reviewing it does impact your opinion.... To say otherwise is just bs.... || I appreciate your opinion but you obviously haven't seen the reviews where I don't like products. || ​@RickyImpeyhe's still right though. Like it or not. || How do you think the camera on this unit is compared to the X1C? Is the video quality better? || Excellent Video! Bambu also announced another new printer to be available before the end of the year, the H2C.  So many choices, do I wait for it? || Well, I can't offer an opinion on that until I've got my hands on one...... || H2D słabo się sprzedawała chyba...
-Ta H2S jest ok i ma to co powinna mieć drukarka.
-Poczekam do wiosny i kupie sobie za pewnie 700$.
-To będzie już 3 Bambu w moim domu. || this feels more like an XL version of the X1C than an actual H2 line printer || My P1P has a super easy hot end change. A few minutes and I have a different nozzle size. Is the H2 the same or do I need a whole tool head assembly? || Its same as A1 || Even easier to change than the P1S and P1P || I added the Revo hot end on my P1 andX1C and it is super easy to change. But I am looking forward to my H2 S, which should be here in a couple of days. || ​@nmfireman very easy hot end change. Noticed they added a cold pull option to the tools menu too || @nmfiremanhow is it going hoss?? || Had a little double take for a moment here when your video popped up, then I remembered your videos were the ones I always looked up when I was having troubles leveling my ender 3, the beard threw me for a moment! , glad to see you are still making really informative videos, id love one of these modern printers that seemingly take all those old troubles away! || Yep, still here Mark🙂 Glad you found me again. These new machines are incredible and the tech will filter down into more affordable machines in time. The A1 models are still some of my favourite for what they do for the price. || Great review - thanks!  I have the H2D which I love - this new model will give me larger print capabilities so it will be my 2nd printer from BL. || An excellent point about "the best printer for...". Every printer that is excellent at something needs to make trade offs. || Completely agree. There will never be a perfect 3d printer for everyone. However, everyone may be able to find their perfect printer if they know what they want to do with it.</t>
+          <t>Hope is NOT A STRATEGY precise action is. Don’t be the person that waits. Begin now, because your purpose can’t wait on you. The people you’re called to influence and impact can’t wait they need what you only have. Trust God and move 
+Your Procrastination is the enemy to your breakthrough 
+Comment and I’ll personal message you 🤙 || Amen God bless u || Thanks for the comment! I would love to have the conversation with you. Please email me so we can begin! Itsbasicbible@gmail.com</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>UCYyel9YAgwvs07rz5kugU7g</t>
+          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ricky Impey</t>
+          <t>itsbasicbible</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>rNMW-fXrZYo</t>
+          <t>DG7HhphSyG0</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Why This $350 Filament Dryer Might Actually Be Worth It…</t>
+          <t>God Is SPEAKING To You</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>This is the most expensive filament dryer I’ve ever seen. It costs more than some 3D printers. So naturally, I had one big question…
-*What makes this thing worth over $350?*
-*This video is sponsored by PCBWay*
-Custom PCBs, 3D printing, and CNC machining! New users can get projects started by saving $5 at PCBWay here: https://pcbway.com/g/0IW9ST
-*Affiliate links (If you purchase something after clicking any of the below links I may earn a small commission at no cost to you. This is a great way to support the channel)*
-*Sunlu E2*
-https://rebrand.ly/yhi0ueo
-*Sunlu S4*
-https://rebrand.ly/x8p33g8
-..............................................................................................................................................................
-BUY ME A COFFEE
-If you're enjoying my content, why not consider supporting the channel by buying me a coffee? 
-Even very small amounts are greatly appreciated and re-invested into bringing you better content.
-https://www.buymeacoffee.com/rickyimpey
-You can also use the YouTube 'Thanks' button above if you prefer.</t>
+          <t>Connect 
+https://linktr.ee/itsbasicbible
+MALTA APPAREL LINK 
+https://malta-apparel.com/?ref=BBAZ16 
+FOR 15% OFF: basicbible15 
+FREE 10 DAY DEVO BOOK 
+https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
+I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
+https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
+I WANT TO FOLLOW JESUS CHRIST
+https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
+Get vidIQ to grow your channel faster! 🚀
+https://vidiq.com/itsbasicbible</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-07-13T16:01:18Z</t>
+          <t>2025-12-04T21:30:04Z</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>4884</t>
+          <t>229</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>124</t>
+          <t>3</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>2</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>0.033579</v>
+        <v>0.021834</v>
       </c>
       <c r="M10" t="inlineStr">
         <is>
-          <t>I’m going to comment as someone who bought one of these for business use. 
-I print almost exclusively nylon PAHT-CF, PA12-CF, PA6-CF and PA12 Support (PA12 without any infill so far as I can tell) and I need to be able to anneal the parts to prevent warping and provide adequate dimensional stability for the entire service life of the part, where it will be exposed to varying levels of humidity. 
-This is the only dryer I was able to find that allows me to dry these materials at their suggested temperatures, print from the dryer for longer production runs without worry of filament re-wetting over the course of a print, and also provide an annealing solution that doesn’t require manual control of an oven. 
-For everyone who is saying this is over priced, you are not the target audience. If you’re primarily printing PLA and PETG, there is no reason to get one of these, it’s complete overkill and would be downright idiotic when you have so many cheaper solutions that will be just fine for you. If you’re dealing with more hygroscopic filaments that require drying temperatures over 70c, this is one of very few options on the market from a trusted brand capable of getting the job done. || Thanks for making a good review! I've used the E2 extensively for drying most of my filaments and desiccant and annealing parts printed in PETG, PA6 and PA12-CF and it has worked beautifully. 
-My only gripe is that I think it heats up a bit too quickly for annealing, so I usually start the process on a lower temperature and ramp it up manually over time and also put the parts in fine sand to work as a kind of heat sink to distribute the heat more evenly and to reduce warping.
-To me the asking price is worth not dealing with the headaches of using the kitchen oven and microwave and having to clean them constantly. A specialized tool to do the job properly is always a good way to go. || Well for that price i will just use the oven lol
-Plastic box isnt worth 350 bucks. || Good review. Assuming you have the retail version, does it have the lid warping issue other reviewers with prototypes saw? || No issues so far, yes I do have the retail version. || @RickyImpeyThanks. I took a shot and ended up ordering just after I saw your review. Did have an issue with one of the rails for the feet being bent incorrectly from the factory (so the dryer would rock if you touched it ) but that was sorted out. No regrets at all. || Get the Chitu Filipartner E1 $139 and don't look back 👍 || Only goes to 70C || You're not drying laundry. || @Mcsandwhich Whats that have to do with filament?
-Many filaments take a lot higher temperatures to dry. fine if your making Barbie dolls with PLA || ​@McsandwhichYou missed the point of the video. 
-This is for those who use higher end filament. He says that like twice in the video. 
-ABS, PA12, etc.
-Not filaments that can dry under 80c.
-This video is not for you. It's not even for me but that's why you got the response you got.
-🤷🏻‍♂️🖖🏻 || At first I thought this video was claiming the S4 was $350, which confused me. It was recently $118 at Amazon, which is when I bought mine. But then I saw this was a different model. I'm sure it's nice to have for nylon and other expensive filaments, but my needs top out at PETG and ABS. I have zero reason to drop nylon money on filament because I don't tend to need aerospace precision in my garage || Fascinating! Are there any other videos describing items that you don't have need for? I'm sure your comments on those would be just as compelling as your comment here. || @steveh8724 Of course. They can be found in large quantity in the comments sections of YouTube videos on every hardware topic || Does it vent air while drying, does it rotate the spool while drying? These are basic questions that should have been addressed in a competent review. || Each of the filament ports can also serve as a vent. || Does it have a method to automatically vent out the most air it pulls from the filament?  Both of Bambu's new AMS units have vents that open and close as necessary.  The vents open periodically when actively drying, but are otherwise closed to serve as a drybox.  
-Dryers without automatic venting require users to remove filament from the dryer as soon as drying is completed.  If not, the filament can rapidly regain the moisture that was just removed. || having a display that looks like that for 350 is a joke || WAY, WAY overpriced compared to dozens of other options. || Name 1? || Yeah, if you count dozens of other options NONE of which offer the features of this one. What's your favorite other dryer that offers 100+ degree C temps AND costs less than this one?
-As mentioned in another comment, if you're just printing with PLA and other filaments that DON'T NEED high temp drying, then DON'T BUY THIS. || @steveh8724 Also let's not forget the E2 has an annealing mode || ​​@steveh8724 Yeah. I noticed a lot of people have comprehension issues.
-"I use my insert ghetto rig here&gt;".  
-Cool. This video isn't for you. And as I told someone else, it's not even for me! LOL But GD are people dense.
-Watch the video. Like or don't and move on if it's not for you! Ffs. 
-Nothing better to do than bark on someone's video while you wait for your PLA to dry in your Ninja Foodie dehydrator I guess. 🙄🤦🏻‍♂️🤣 || Have a single spool Creality and a Sunlu S4 both do exactly what I require for PLA( silks included ) TPU and PETG.  When I move into ASA, ABS etc I will get an appropriate tool to deliver the results. || How are you finding the S4? I'm considering buying it atm from Amazon on Prime day as it's on a ridiculous discount for $169 AUD. I've been looking around for air fryers and dehydrators on marketplace to not overspend though I'm tired of searching and just need a good solution. || ⁠@YaNeK92it had worked flawlessly everyday.   I put it through a bit of rougher treatment as it is in my semi. Engine vibration all night. Bouncing down the road ( 300-680) miles 6 days a week.   
-I would say you will not be sorry to get it.     Worth every penny. || ​@PrintedTrucker I appreciate your prompt reply bro! I think I might just pull the trigger and go ahead with it, since it does support 4 spools and I have the AMS so it will be future proofed if I ever want to print something in colour and won't have to wait for individual rolls to dry. 
-Wait, are you saying that you've taken the 3D printing hobby on the road with you whilst trucking (if I understand that correctly)? 😅
-How do you deal with the fumes and VOCs? 
-I had the A1 Mini on my main desk in my small office and I could only last a day or so with it before getting watery eyes, itchy throat and a small cough which was all early signs of the microplastics having a negative effect on my body, so unfortunately (even though the printer is cool to look at whilst it prints), I had to move the whole operation into the garage. || @YaNeK92built a BENTO BOX. Carbon and Hepa filter. No problems at all.   Still when I do ASA I put in a fan and open the windows.  
-Yes. In my 389 peterbilt truck.    
-And my trucking channel thistruckerslife || I have a SUNLU S1. And love it.  $350.  No thank you || If the S1 is adequate, then you most certainly don't need something with these capabilities. So  thank you for confirming that people, like you, who don't need this, probably should not spend $350 to buy it! Also people who don't have 3D printers should not buy this either. So there you have it, if you don't need it, don't buy it! Who would have thought it would turn out to be so simple... || I use my food dehydrator!! 😂 || It goes to 110 C?
-What model || It goes up to 71 C and works well to dry out the spools❤ || @mellow_mel1313 Ok this model does 110C, that's the point, different tool altogether || I use an Air Fryer.  1/3 the price and if you shop around you can find ones with the temp. range you need. Just watch out, with all these solutions the spool can melt.  Mine has a "dehydrate" setting which can go to 170F (76C). Then the regular setting goes up from there. Up to 204C if you need it. It works great, just shop around because specs and sizes vary.  And it makes great french fries. Lets see your dry do that. || I love microplastics in my food! || ​@mossy5127 You use your filament dryer for food? || Better yet, get an actual food dehydrator. There are many circular ones that can house a 3kg spool if that's of any interest to some and they're a cost effective solution. || you know, a screwdriver makes a decent chisel, but I would still want to use a chisel. || ​@Keyan9 Great point!</t>
+          <t>❤    Amen   🙏 || Hi you now</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UCYyel9YAgwvs07rz5kugU7g</t>
+          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Ricky Impey</t>
+          <t>itsbasicbible</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Casciq9ehTk</t>
+          <t>e2gSSVkbeaI</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3D Printing for Beginners: From Model to Print with Orca Slicer</t>
+          <t>Daughter Nearly Killed by Parents Over Family Honor #DomesticAbuse #NewsTrending</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Just got a 3D printer and have no idea what to do next—or what half the technical jargon even means? I get it—I’ve been there. That’s why this video breaks everything down, step-by-step. No confusing terms, no techy overwhelm and no fluff,—just exactly what you need to go from downloading your first 3D model through to slicing it like a pro and getting it running on your printer. If you're brand new, this is the perfect place to start. Let’s get into it!
-*This video is sponsored by PCBWay*
-Custom PCBs, 3D printing, and CNC machining! New users can get projects started by saving $5 at PCBWay here: https://pcbway.com/g/0IW9ST
-*Orca Slicer Download*
-https://github.com/SoftFever/OrcaSlicer/releases/tag/v2.3.1
-*Print Files*
-Calibration Cube - https://www.thingiverse.com/thing:1278865
-Cute Octo - https://www.printables.com/model/178035-cute-mini-octopus
-Cali Cat - https://www.thingiverse.com/thing:1545913
-*3d Printing Glossary*
-*3D Model*
-A digital file that represents the shape of an object. Common formats include .STL, .3MF, or .OBJ.
-*G-code*
-The set of instructions your printer follows to build a model—telling it where to move, how fast, what temperature to use, and how much filament to extrude.
-*Slicer Software*
-A program that converts your 3D model into G-code. It slices the model into thin layers and calculates the exact printer movements. Examples: Orca Slicer, Bambu Studio, Cura.
-*Print Profile*
-A saved group of slicer settings for a specific printer, material, or quality level.
-*Layer Height*
-The thickness of each printed layer. Smaller layers mean more detail but longer print times.
-*Infill*
-The internal structure of a 3D print. You can control the density and pattern. More infill makes a part stronger.
-*Supports*
-Temporary structures that help hold up parts of your model that overhang or would otherwise print in mid-air.
-*Overhang*
-Any part of a model that extends outward beyond the layers below it. Steep overhangs often need supports.
-*Bridge*
-A horizontal section of filament printed across a gap. Many printers can handle short bridges without needing support.
-*Z Seam*
-The vertical line where each new layer starts. Its position affects the look of your final print.
-*Skirt*
-A line printed around your model to help prime the nozzle before the print begins.
-*Brim*
-A flat ring printed at the base of your model to help it stick better to the bed and avoid warping.
-*Extrude / Extruder*
-To push filament through the printer's hot nozzle. The extruder is the part that feeds the filament.
-*Calibration Print*
-A test print used to fine-tune printer settings like temperature, retraction, and flow.
-*PLA / PETG*
-Types of 3D printing filament.
-PLA: Easy to use and great for beginners.
-PETG: Stronger and more flexible, but slightly trickier to print.
-*Print Bed*
-The flat surface on which your printer builds your model. Often heated to improve adhesion.
-*Print Plate (Orca Slicer)*
-A virtual workspace in the slicer where you arrange your models before slicing. You can use multiple plates for larger or multi-part projects.
-*Retraction*
-Pulling filament back slightly between movements to prevent stringing or blobs.
-*Firmware*
-The internal software that controls how your printer operates and responds to commands.
-*IP Address*
-A network address that allows slicer software to connect to and control your printer over Wi-Fi.
-..............................................................................................................................................................
-BUY ME A COFFEE
-If you're enjoying my content, why not consider supporting the channel by buying me a coffee? 
-Even very small amounts are greatly appreciated and re-invested into bringing you better content.
-https://www.buymeacoffee.com/rickyimpey
-You can also use the YouTube 'Thanks' button above if you prefer.</t>
+          <t>Listen closely 
+Ephesians 6:4 
+4 Fathers,[c] do not provoke your children to anger by the way you treat them. Rather, bring them up with the discipline and instruction that comes from the Lord.
+Connect 
+https://linktr.ee/itsbasicbible
+MALTA APPAREL LINK 
+https://malta-apparel.com/?ref=BBAZ16 
+FOR 15% OFF: basicbible15 
+FREE 10 DAY DEVO BOOK 
+https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
+I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
+https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
+I WANT TO FOLLOW JESUS CHRIST
+https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
+Get vidIQ to grow your channel faster! 🚀
+https://vidiq.com/itsbasicbible</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-06-29T16:00:15Z</t>
+          <t>2025-12-03T21:30:09Z</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>10210</t>
+          <t>1283</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>360</t>
+          <t>96</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>7</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>0.036337</v>
+        <v>0.08028100000000001</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Hi. How can I print a jpg file on the Orca Slicer? I can do it with ultimaker cura, but there is no option for the "jpg" file in the orca. || This is excellent, thanks! || Are you able to control the ad5x remotely that you spoke about on this video? || You’re pointing to a fake website!!!! Orca slicer condeem ths site on their official website || I've learned a lot from your clear and understandable explanations since I bought my FDM printer three years ago. Thank you. || Grazie , spero che farai altri video che riguardino Orca Slicer  , avendo delle stampanti Prusa  uso  Prusa Slicer  ma Orca lo trovo più interessante 😁 || Hi this is not about  the slicer  but i have  found  things  about  it  i only  used it once or twice  i have  learn  loads of  things  off your  videos  about problems  I have had i have an ender3 v3 se  printer  it has worked  well since  I got it new it won't extruded filment  I have cleaned it all out put a new nozzle on it but still no joy i have got a new hotend when it is apart  the extruder extrudes  the filment  and u can push the filment  out of the hotend  all OK put it all back together  and  you can push the filment  through OK but when u go to print  it works OK for about  3 mins  the the filment  stops  coming out and if u try to pull the filment out its like it is jammed  but when u take it apart it isn't hope u  can help me as tired  everything I can think of || Thanks Ricky. It was your videos that got me into 3d printing and hepled me setting up my E3v2 almost 3 years ago. But for all the time I was stuck with Cura and thinking of switching. Thanks to this vid, now I'm  finally switching to Orca. || Thanks for this;  I would like a video about using Orca Slicer with Sonic Pad || Good stuff. I'm well past this point in my printing history, but since I'm largely self-taught, it is valuable to see your explanation. I didn't know I could paint in support exclusions! || Thank you for the video. I am brand new to printing and still watching and learning so this one is useful to me. I particularly like you covering the settings and instructions. I will save the transcript and the video. I have enjoyed your other videos as well.</t>
+          <t>Get them out of your country before he poisons your communities. || Open a secret shelter for young ladies who have to run from thier own Parents due to the different religious beliefs that may get them killed. Someone has to step in to help these young ladies from the unhinged parents. || This is awesome, thank you for sharing your thoughts! || Assimilate || Or better yet don’t enforce your beliefs and rights on others when you live in a land of freedom and opportunity so presumably your children can live a better life. || Thanks for the comment! || Good thoughts, thank you for sharing!</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UCYyel9YAgwvs07rz5kugU7g</t>
+          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Ricky Impey</t>
+          <t>itsbasicbible</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>kW8Jy09-ns4</t>
+          <t>2jMryl3y3Ts</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3D Printer Nobody Noticed – Flashforge AD5X Is Doing Things Differently</t>
+          <t>Your SUCCESS DEPENDS On This</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>The Flashforge AD5X is a budget 3D printer with some surprisingly clever features — multi-material printing, a solid build, and a few thoughtful design choices you don’t usually see at this price point. But is it all good news?
-In this hands-on review, I test the Flashforge AD5X to find out if it’s an underrated gem or if there's a reason nobody’s talking about it. From multi-color printing to minor flaws (and one major dealbreaker), I cover everything you need to know before buying.
-*This video is sponsored by PCBWay*
-Custom PCBs, 3D printing, and CNC machining! New users can get projects started by saving $5 at PCBWay here: https://pcbway.com/g/0IW9ST
-*Affiliate links (If you purchase something after clicking any of the below links I may earn a small commission at no cost to you. This is a great way to support the channel)*
-*Flashforge AD5X with $10 Discount for a limited time*
-https://flashforge.sjv.io/3J3P7v
-UK: https://flashforge.sjv.io/N9VKNO
-Discount Code: XMRICKY10
-Further Discount With: FLASH5
-*Metmo Multi-drive*
-http://shrsl.com/4wt98
-*Stick on eyes*
-https://amzn.to/4ku9wsh
-*Print files used*
-Poker Chip - https://makerworld.com/en/models/13936-dual-color-poker-chips?from=search#profileId-14302
-Owl - https://cults3d.com/en/3d-model/art/flexi-factory-owl
-Drago-Rex - https://cults3d.com/en/3d-model/game/drago-rex
-Airless Tennis Ball - https://makerworld.com/en/models/253687-airless-tennis-ball-2-0-pickleball-wiffle?from=search#profileId-272027
-Banana Holder - https://www.thingiverse.com/thing:3577644
-..............................................................................................................................................................
-BUY ME A COFFEE
-If you're enjoying my content, why not consider supporting the channel by buying me a coffee? 
-Even very small amounts are greatly appreciated and re-invested into bringing you better content.
-https://www.buymeacoffee.com/rickyimpey
-You can also use the YouTube 'Thanks' button above if you prefer.</t>
+          <t>Connect 
+https://linktr.ee/itsbasicbible
+MALTA APPAREL LINK 
+https://malta-apparel.com/?ref=BBAZ16 
+FOR 15% OFF: basicbible15 
+FREE 10 DAY DEVO BOOK 
+https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
+I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
+https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
+I WANT TO FOLLOW JESUS CHRIST
+https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
+Get vidIQ to grow your channel faster! 🚀
+https://vidiq.com/itsbasicbible</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-06-10T16:01:17Z</t>
+          <t>2025-12-02T21:30:00Z</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>45572</t>
+          <t>896</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>616</t>
+          <t>57</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>133</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>0.016436</v>
+        <v>0.06808</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>Online cloud account?  I have an AD5X. There is no need to create a cloud account.  The spool holders are great, they are spring-loaded and retract filament just fine.  Ahh, just noticed this video is 6 months old.  Thanks helping us all out by letting Flashforge know all their shortcomings.  Looks like they fixed some of the design flaws in the preprod model.  Happy printing. || Camera module and light kit are available for the AD5X but sold separately. || For me, three things. 
-1 locked into flashforge's slicer for full functionality
-2 build plate too small
-3 still too much filament waste.
-I am willing to wait and see who is going to try to compete with Snapmaker and their U1 Multi-toolhead machine. if there's no competition by March of 2026 I will more than likely go with Snapmaker. It supports Orca slicer, is 270 cubed and has only purge tower waste which can be cut down by purging into the print. As it stands right now it's in a class all by itself for the price. Thanks for the video Ricky. || Own one. Prints just as well and faster than my P2S. || You can use regular OrcaSlicer with this printer. However, to use the filament changer, you must upload (but not print) and select the multi-filament checkbox on the printer. Aside from trying to lockdown the software options, this printer is reliable and the best bang for the buck. However, Flashforge really needs to stop the requirements to "call home" like even light bulbs want to do, and just use OrcaSlicer as is and support that open source project. Note to Flashforge - you are only hurting yourself. This is the ultimate hobbyist printer, but the software issue is restricting your market reach into that segment. || The touch-screen is resistive, not capacitive. So use your fingernail or a hard stylus, not your fingertip or a rubber-tipped stylus, and you'll find the rouch-screen works fine || AUD69 for a compatible camera from Amazon. || I've had mine for a couple of weeks and so far no major issues. I bought the camera and it works well enough to monitor the print. I'm not a professional  so I haven't been able to try everything but so far everything I've printed has done very well. It's not the largest printer but for a hobbyist like myself, it's big enough. I can't argue with the price I paid, $306! For a printer this size with multi-color/material in a compact size, there's not much to complain about. It is strange that the only way to load a print is by Flashdrive. || You can do it via online. I do. I have to wake up my printer each time but still you can send it over the net via the orca software || Great video.   One question.  Can the IFS be mounted behind the printer to sit an dryer box in the back?   Thanks || So far my ad5x haven’t given me problem || Can you do an update since it has been four months? || Had mine 2 weeks the orca flashforge is unstable and crashes often. The filament presets are incredibly limited. Bed adhesion with petg seems poor but this may be my problem as ive not cleaned it yet. The jury is out but at £252 delivered im prepared to do a little tuning untill flashforge sort the software and firmware || I cannot see the advantage over the Bambu A1 Combo other than taking up less space. || hey im getting it what does it have to print || The only thing I give a crap about is if it runs OPEN SOURCE klipper or if they stole other peoples work without following the license. || Just sent mine back after two weeks, Constantly fails any print around a hour or two into the print. || Sorry to hear you had issues, I hope the return process was straightforward. || ​I think i just got a faulty heating system and wasn't the machine itself or the manufacturer, i have a adventurer 5M that has been close to flawless so i guess i just expected same results
-Amazon shipped it back free and easy but only gave back amazon credit || 15:54 How can you say that? The bed can reach up to 110C and the nozzle up to 300C, So the printer IS also made for materials like ABS and ASA. Those materials benefit from an enclosed chamber. Wouldn't be hard at al to DIY something for that.
-Furthermore ; It is a compact printer, so the chamber would be very easy to heat up || why does no one ever bounce the balls they make with TPU prints on video? || I'm in Saudi Arabia and I would like to get my first 3D Printer and use it for business. My budget is $800. However, prices here are really high. I can get a Flashforge AD5X for $625 or a Creality Hi Combo for $730. 
-Other printers are unavailable or more expensive, so these 2 are my only options. Which one is better and why? || This was my front runner right up to the login account.
-Nope.
-Locked firmware?
-Nope || 8:31 || You can send gcode directly to the printer via its IP.
-You might need to unregister it by resetting the firmware first. || I just an AD5X a couple weeks ago and I'm printing with no account. LAN only is an option. You can also change temps and add a USB camera or the FlashForge Camera so you can view whats printing. || cuz its too small || good review || The ad5x has too many issues, it’s noisy it’s small, the ifs doesn’t work properly the extruder gets stuck with filament. If that’s not enough flashforge wants you to reverse engineer their machine to fix their issues. I told them heck no it’s your machine you fix it. Sent mines back for full refund. Anyone out there we hi buys wants don’t mess around past the 30 days or you’ll regret it. You’ve been warned. || I do believe the latest version of orca has this machine in its lineup, so whether it's usable is still to be seen I did watch one review where the guy was using proper orca with some caviates. I've taken a punt on buying one as it is available on amazon for £315.00 at the time of writing this. For what I want it for it should be okay. Mostly 2 colour work. I do know the colour change isn't good when you run out, goes to the next roll.
-Still looking forward to using it as its my fist core xy rather than a slinger. || Just a note, the covers are available now on the FlashForge site.  They're $49 , plus $15 from China. Just ordered them yesterday.  I hope someone comes up with a good minimalist version of it soon. This is certainly the way to go with the AD5M. || That’s just the acrylic. You still have to print everything else || @ClappinCheex Acrylic and hardware.  Customization is a benefit (to some).  Some I've seen are incredible (ugly).  
-It is a printer.  
-I did put mine together.  It's OK, though not anywhere close to being sealed.  The Bowden Tubes need a big hole in the upper side panel.  There is also a second story to fit them.
-It does knock down some of the high pitched noise and the clanging (some).  I think it's worth the time and money but it would be a good idea to try to find a picture  before buying. || There is a LAN only access mode (that bypasses the cloud service) but it's clunky. || Is it improved at this moment ? || just one question though are you experiencing extremely long multicolor print times? the koi fish model that came with the printer takes me 8 hours to print || Just got mine 2 weeks ago, they have changed the spool holder design and they now have a built in rewinder as long as the inner diameter of your spool isn't too large for the spool holder to grip it. || I printed out adapters for spools that are too large || I could maybe live with the Orca-fork, but no LAN-mode? Using an USB-stick? Hahaha, for sure, not. Too bad, this printer would be ideal to print from dry-boxes, like the A1 mini.
-It’s incredible how printer vendors repeat the same mistakes again, and again, and again. There’s always a dealbreaker on any printer. Good for me, saves me a lot of money. 🙂 || AD5X got lan mode and can work with original orca slicer... || I have had mine for a week.
-No bed adhesion.2-3 prints fail. My #3 feeder tangles.
-Have sent Flashforge s detailed account of yhe issues and documented them in video.
-Its s $400 paperweight right now.
-Ladt failed it blew the cover off the print head.
-Love my 5M
-The 5X not so much.
-Makes me sad || Once someone hacks this, it might be a good deal. || Just got the AD5X in today and I can confirm there is NOT an online/cloud requirement. Not sure if they changed something since he got his machine, but mine is not tied to any account and it's working just fine over my network with regular Orca or the Flashforge version. Though you do need to use the Flashforge version of Orca for use of the IFS, but regular Orca works fine for single color. || @Mindless_One That's great news.  My AD5X is still in the box.  I haven't found a suitable place to put it. || current orca works with ifs, but as with the flashforge version you have to tick ifs localy on each print before starting || Can you use USB ports on it || I like how it has 104 five star reviews in their shop but if you go to the reviews there are none || a lot of people will tick off a star rating but not bother with a written review.
-That's what I usually do unless the experience was extremely good/bad || Thanks for the review. I will go for a multi upgrade on my K1 max as I am now used to the way it works. Looks like an interesting low cost option for a starter. || Its expensive and terrible. Gee i wander why no one cares about it lol || Which 4 color printer is less expensive? $370 is not an expensive printer. Had mine for a month only 1 failed print. Only complaint I have is the filament waste. Print quality has been phenomenal. || 3D Printer Nobody Notice they did notice it was due last year 
-NEW Flashforge Adventurer 5M Will Be A Multicolor 3D Printer
-Figure Feedback•
-5.2K views
-7 months ago
-Flashforge AD5X Enclosure &amp; More Questions Answered!
-Figure Feedback•
-6.7K views
-6 months ago || I was looking at this printer a couple months ago, but that build volume is too small for my needs. || I love my flashforge Adventurer 5m pro. I had an issue the first time i tried switching heads and it dug into the plate (probably user error) and the company was pretty prompt at emailing me back and within a week or 2 i had a replacement head and plate free of charge, they keep emailing me for updates, will answer any question I ask, and keep offering to help with any other questions i might have. || The FlashForge cloud server recently crashed.  There is an ability to use the AD5X in LAN mode without being logged into the cloud server.  Jeremy @FigureFeedback showed how to do it in a video that he released today.  However, there shouldn't be a cloud service.  I don't do anything in the cloud and I definitely don't want any part of 3D printing through someone's cloud.  Ditto for the proprietary re-skinned OrcaSlicer.  I'm not doing that, either.
-I was initially very impressed with the IFS and the general design of the AD5X.  I print a lot of TPU for my business so I was initially impressed by the claim that the AD5X would allow multi-color 95A durometer TPU printing.  FlashForge backed off that claim but it still does mostly work and would probably work well for my applications that swap filaments only rarely per part.
-The AD5X is the best hardware implementation I've seen of using multiple filaments multiplexed into a single print head, but I'm not a fan of those poopy designs.  I'm waiting to see how the Bondtech INDX syatem works in reality.  Having a single extruder and swapping the heater and nozzle allows printing with incompatible filaments rather than simply changing colors of PLA, and there is no poop.  Print a small purge tower and that's all you need. || I wish they were not stuck on the 220x220 build plate also.  It's a shame || you clearly like a particular brand and no others will do brand snob || you can fit a camera to it it just doesnt come with it || you are very hard to please you totaly ripped it apart i just bought this i have the 5m it works perfect with orca and you can send a print directly to it via wifi you shouldnt expect 5 grand quality on a £340 printer || No cloud bricks the machine, account required, hard pass, nope. || Just buy a Bambu || It is very cheap for a 4 colour printer || tldr; An inferior attempt to clone the Bambu A1 into a cheap Core-XY. Not recommended when there are better alternatives.
-Great review. Glad you didn't hold back on the many issues this printer has as many other reviews I've seen are glossing over these issues. I pre-orderd by in November and have had my unit since February and have experience many of the same problems. I view this printer as a worse in every way A1 with a price to match that inferiority. The IFS itself isn't anything revolutionary and is less capable than the feeders on the AMS Lite often having trouble pulling filaments with even the slightest amount of resistance.
-The build volume is 220x220, but it uses a 235x235 build plate so you can use any Ender sized bild plate, you just can't use all of it.
-I do not recommend using 95A TPU through the IFS. It will have frequent feeding issues and jams in the extruder especially on multi-color prints. I only got a couple Multi-Material TPU prints to finish successfully and even single color TPU prints failed over 50% of the time.
-Be very careful unplugging the extruder. It connects to very tiny pins on the extruder board and can easily rip those out if you pull too hard or at an angle. I'm still waiting on a replacement board nearly a month after submitting my service request.
-You can use other slicers (standard Orca, etc), but there is no way to control the IFS for multi-color prints so it just uses slot 1 of the IFS. If you want to do multi-color, at least for now, you have to use their slicer. My biggest issue there is that they don't display the flush amount when slicing, just a total material usage.
-I got the FlashForge camera and it's terrible especially when there is no light on the bed. It doesn't even point at the bed correctly so you can't see half the plate. Maybe this is because it was designed for the AD5M and the mounting point is different on the AD5X?
-One of my biggest issues with this printer is whenever I opened a 3mf created with BambuSlicer it would ignore any filament selections it carried and just print as a single color print from the most recently used IFS slot. It would not recognize the filament types as being valid, even if I changed them, so would just panic and pick a random slot and start printing, ignoring any color changes.
-I also had problems after the last firmware update where the printer would just stop mid-print as if it experienced a power failure, then it would report that the print was finished and fail to resume printing. This happened so many times in a row and at different points in the print, that I just stopped using it entirely, until they release a firmware update fixing this issue.
-Flashforge has released plans to print a full enclosure for the AD5X including the top, but they are not selling the hardware kit yet. I just used a 3rd party "tent" enclosure though and it worked pretty good. It was designed for the A1 and had holes in the side to run the PTFE through. I tried running lines out the side to my Sunlu S4 and got mediocre results, the holes are a bit too high on the side causing a very poor filament path which creates a lot of resistance especially with very full spools. There is just enough room to run the filaments on the side spool holders though.
-The AD5X is much louder than either my A1 or P1 printers, by a fair margin. Both the fans and movements cause more noise. Also I started getting rough patches on my X and Y rails after only a couple months of light use. Likely because like you said it lacks proper lubrication. Another build quality issue is the little flap that holds the hot end in is very thin and weak. It bent the very first time I tried to remove the hot and and feels very flimsy, unlike the one on the A1.
-There are some things to like about this printer. For example, it uses an A1 style poop try and flings the poop out the back of a short, open poop shoot. This avoids the main issue I have with my P1s where it dumps directly into the shoot and often gets stuck on the flap, eventually building up and overflowing into the machine. I don't see this being an issue with the AD5X, and I praise them for that design. The filament change times are also roughy 20 seconds faster than the A1 and almost a minute faster than the P1, which can add up to a lot of time savings on prints with lots of color changes.
-I listed my printer for sale trying to offload it before the full launch, but then a potential buyer asked to see it running which is when I ran into the jammed extruder and broke the extruder board. Now I'm stuck with a paperweight that I can't sell for anything close to what I paid for and still waiting on FF support to ship me the parts I need to fix it.
-As it stands currently, until they can fix their issues, I do not recommend this printer when the A1 Mini combo is the same price (slightly smaller build area) or for a little more you can get the A1 combo with a larger build volume. If you don't like Bambu, the Creality Hi or the Anycubic Kobra 3 combo are better alternatives (Kobra 3 is currently $349 for the combo). || No one noticed it because its flashforge. A company with less quality, and more locked down than bambu. Its trash || "Trash" seems pretty harsh tbh.  It clearly has some significant negatives but there is nothing directly comparable in the market for this price (that isn't a bed slinger). || Yeah but if you can get the same or better quality with a bedslinger what does it matter if you have a core XY. Especially if it's for similar or same price or in some cases less. ​@ferrumignis || ​@ferrumignisbecause remember you're putting up with a super closed source, bad slicer and a bunch of proprietary parts. I think that's sort of a negative for bambu too but they provide parts affordably and their slicer is not hot garbage. And if you really want to, you can use third-party stuff just locally || Too small || Print area is a bit small by comparison to it's direct competitors I agree, but on the flip side that gives it a very compact footprint which may be appealing to people with limited space.  If this was available when the Q1 Pro was released I'd have been very tempted as the Q1 barely sits on the desk in my workspace.  I'm less than impressed with the custom slicer and cloud account shenanigans though. || Nozzle is/was almost direct copy of Bambu Lab A1 nozzle, but without heatsink - and it is much more expensive (if one can get them from anywhere).
-It seems nobody knows what the updated nozzle looks like and how it is different from the old...
-FlashForge needs to step up their game with this printer. || Found a couple on amazon at £22 for a 0.4 nozzle and a 0.6 at an eye watering £77.
-I'm sure someone will bring a set of aftermarket cheaper soon. || It's not open source - so not for me. || When I first started watching this, I was like, well drug, its too humid here, thanks for showing us the sunlu bring hooked up to it, that is the same dryer I have and it helps so much in the humid area I live in. So that would be a better fix for my use than the ones mounted on the side. I seen another video where the guy pulls his each day and puts it back into the dryer, I actually print a lot all night long trying to keep up and that would be a huge pain for me. I mostly print PETG for my production stuff, and or ABS some as well. 
-Thanks for taking the time to make this video, maybe I will get to try one of these soon and be able to compair it to some of the other options for a small print shop. 
-Thanks agian and have a blessed week
-dale || The regular M5 is incredible. Orcaslicer is fully compatible and the printheadsystem is superb. It's the ultimate Ender3 upgrade (same printarea) || Custom slicers and required logins are terrible. JUST USE ORCA! || You can use Orca, but not for multi-color prints. There is no way to communicate with the IFS or slice a file for multi-color prints without using their slicer. || @donnyriggz That's my point though. I mean the brand should just use Orca. All of the features for multi-color printing are already there. They need to just integrate with an existing popular slicer instead of modifying it and releasing an inferior less frequently updated product instead. They can add all of their code to Orca so that when you select their printer it works properly. If they did it, the open source community wouldn't have to later instead. || I would have bought one if it had been available when they said it would be, but it just kept being delayed. Now I have two more machines and no need for this. During this time there have been a litany of issues. 
-It’s not that nobody noticed it, they sold out the presale. They also got a lot of loyal fans made by the 5M series annoyed with them. They have some work to do in order to get that confidence back. || I just got one a month ago, and wasn't worried about that baggage. It's a great printer now that it's out. || I don't care about multi-color or material (in their current form).  But people do sleep on Flashforge printers.
-I'm the type the doesn't really care what others do or if they can even understand why something is good or is not good.  I don't know about this particular printer (see my first line) but I know people make the same complaints about the AD5M.  And guess what?  You can use any slicer you want, run Klipper, add Bambu-style hotends and make them into the best printers for the money to a point that it's almost sad that people are so blinded by the tribalism. || How do you work around the requirement for cloud log in to get LAN access if you don't use the Flashforge custom version of Orca? || My 5M pro messed up device binding on the 1st day 2nd test. It ran into an error, corrupted, factory reset, can't bind again, serial number if abcdefg. So I gave up flashforge orca slicer. Used original orca slicer. It was very easy. Just pick the model from devices, set the correct IP (I used both WiFi and LAN, both worked perfectly). I'm thinking of installing Klipper CFW to minimize waste. After all done, I tried their flexible PLA, it made the extruder stuck (my mistake when switching from petg to pla I've selected PLA as the new filament which wasn't hot enough to remove old PETG), I had to completely disassemble the whole extruder unit to fix this (it went deep in). This was my very first time ever learning about 3D printing and starting it. But I've managed to get everything done by myself without ever needing anyone's help and learned everything in hard way. I specifically choose 5M pro above any other printer is because the built in HEPA filter which is very important to as I'm concerned about health effects. I haven't found this feature in any other printer (I have no problem affording high end printers but non of them had feature). I know I should've been pissed at flashforge for giving me such a hard time but it was very well built and if you're resourceful, you can tackle all those things and get behind this well made printer. The software is messed up but as a software engineer, I didn't had any problem with switching from vendor locking sw. As a person who never even watched a single video of 3D printing before trying it by myself, I can assure this printer is very beginner friendly. 
-It's been a week now and I made so many flawless prints with different materials and switching materials in between prints, switching different nozzles, etc and not a single print failed even when I brought cheap petg for testing. || Why doesn't the changing weight of the filament spools affect the quality of prints, i.e. resonances, no matter what printer that has filament hanging off the frame? || Because it was a major fail the first time it came out and most of its competitors  are fully enclosed || BOOO to FLASHFORGE on the software login. I won't be buying your PRODUCT!!! @FLASHFORGE #FLASHFORGE || Because it's a piece of shit, bro. Maybe stop advertising crap and actually make something instead? || These manufacturers have to stop with the software lockdowns || AD5X is not software locked... || orca slicer works on linux, orca-flashforge only does windows and mac. (it will run in wine but not well) || ​@johnwhitney3436tysm, been looking all around for an answer to this specifically lol
-other vendors have appimages for their flavors of orca, so I wasn't sure || I wish reviewers reported on the (lack of) quality of the SBC and electronics on the back. Those are the parts most likely to fail, but they are covered up, and 3D printer reviewers don't usually have enough know-how to review what is essentially a part-computer. The Flashforge AD5* backplates are shockingly poor in terms of PSU, SBC, and cooling quality. There are even long threads on how to make sure the cables are connected properly, because they can come undone from the pure shaking of the printer. You'd think they would have tested that! || Is this one from the batch releasing now or the first edition back in January? || Based on spool holders, seems to be from the first edition 🤔 || The proprietary slicer and cloud access requirement are  a deal-breaker for sure! || I've been using it with OrcaSlicer since they first introduced it... there's nothing proprietary about it. || @williamsteele Does networking, either LAN or WiFi, work? If so, I'll switch from OrcaFlashforge, though neither of those work for me either.  
-I can't long into FlashForge anymore.  I can change the password, but no-go. It refuses to send me acknowledgment emails, likely because I have an oddball email address (personal server).   Their login process has always been a mess. Even when I could log in, the success rate was 50/50.  I just use the Sneaker-Net now.  
-I've also had some component failures with my AD5M Pro.  It's down now because I think the motherboard is bad.  On the positive side, parts are readily available, even on Amazon, and they're relatively inexpensive. || There is no cloud access requirement. 
-The LAN Only mode does not require any Internet access at all. || @VladimirPutin-p3t All you have to be is smart enough to set up a LAN.  I've failed every time I've tried. I have better things to do that fight computers for hours at a time. || If I can't print over the local network without a cloud connection, from a standard slicer, I'm not interested. || I just an AD5X a couple weeks ago and I'm printing with no account. LAN only is an option. You can also change temps and add a USB camera or the FlashForge Camera so you can view whats printing. || You only need the account if you're using their cloud software.
-Just tell orca slicer the IP, and it'll upload the gcode to the printer. || This is the only multicolor printer that allows you to use TPU .  The version 1 did it without any issues, It actually can even mix TPU and other filaments in 1 print.  Thats actually ground breaking.  Btw your dellusional saying Bambus AMS can use "all spools well".  That is COMPLETELY FALSE.  So much so people have to use makeshift adapters on several brands not named Bambu || You absolutely cannot run TPU through this printer and expect it to work every time. I've tried it and I've had more failed than successful prints. It "can" work, but you're likely going to need several attempts and may have to clear an extruder jam a couple times. Not worth the headache. 
-The spool holders this printer shipped with the early release models absolutely cannot use all spools well. Cardboard spools sit at a weird angle and the edges of the spool rub against the holder, if it's one of the top spools it drops ground bits of cardboard onto the spools below it. This also causes a lot of resistance which the IFS doesn't handle well at all throwing out frequent errors because it can't feed the filament. Also most mini-spools also do not fit. You would also need different spool adapters for this printer as well and the new spool holders are basically copying the A1 style and will also likely not fit all spools. || A locked down firmware and a printer that only working with an online account is a hard pass for me and many others 😢 || maybe this is why no one is mentioning it 😭 || Its a sponsored video, so guess that is why. Maybe someone will sell a klipper board for this in the future || As far as I know their other printers can easily be turned into open source kliper, I believe the same will soon be true for this one. However, having a different premade printer than anybody else comes with its own set of challenges: spare parts and accessories are more difficult to find, software is being developed slower as less people are working on it, any possible issue that you have with the printer is experienced by less other people hence it is less likely to be resolved already etc...
-Overall I really like this printer but I don't expect to be getting it, especially as it isn't being sold in my country || Yup.  Bambu burned that bridge with the gaslighting.  In the future, I wont even consider a printer thats not open source || If you want to print via wifi, yes you have to have an online account. But you can use a usb flash drive. Which I don’t mind and I don’t have to worry about network/wifi hiccups. || Bondtech INDX will solve all these problems || for printer builders maybe..not everyone wants to build printers lol || Got my brother an AD5 but it broke within a few days. I would have fixed it if I lived closer. FlashForge has been around forever but their attention to detail has always been a bit lacking. || Too much monetization, takes forever to start. || So this company wants people to buy their printer, fix it for them, and be caged by them................mmmmmmmmm..........NO! 😂 || Meh || This fixed income retired hobby guy won’t be buying one.   Sorry || Copy/Paste design. || Well ... that is what brings prices down.
-If everyone guarded their designs like Apple, you and I wouldn't be able to afford anything. || Like every other company. Oh nooooooo lol || @RandomPickles yeah, its the new Ender 3. || ​@user-lx9jm1wo3h Its the new every company ever.</t>
+          <t>❤    Amen   🙏 
+        Only  as  high  as 
+        I  reach  can
+           I  grow || Amen! || The victor is not victorious if the vanquished does not consider himself so || Thanks for the comment!</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>UCYyel9YAgwvs07rz5kugU7g</t>
+          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Ricky Impey</t>
+          <t>itsbasicbible</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>-icvl_M33iQ</t>
+          <t>UU7TLaOj8qY</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3D Printing Finally Catches Up With My Ambition! – Bambu Lab H2D Review</t>
+          <t>Is Trump going to heaven? #jesuslovesyou #jesuschrist #shorts</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>For their new flagship printer, Bambu Lab’s mission was simple. Just build a bigger X1C and everyone would be happy.
-That’s not the Bambu Lab way though and instead of giving us the 3d printer that we were asking for, they surprised everyone by releasing the H2D, a dual-nozzle, heated-chamber powerhouse that makes the idea of just a 'bigger X1C' look quaint.
-Finally, 3d Printing can be what I always wanted it to be!
-*This video is sponsored by PCBWay*
-Custom PCBs, 3D printing, and CNC machining! New users can get projects started by saving $5 at PCBWay here: https://pcbway.com/g/0IW9ST
-*Affiliate links (If you purchase something after clicking any of the below links I may earn a small commission at no cost to you. This is a great way to support the channel)*
-*Bambu Lab H2D*
-https://shareasale.com/r.cfm?b=2750409&amp;u=3409153&amp;m=138211&amp;urllink=&amp;afftrack=H2D_Review
-*Biqu Cryogrip Bed*
-https://tinyurl.com/5n6ry2fk
-*Print Files Used*
-*Shoes* - https://makerworld.com/en/models/1236494-bubbleberry-a-3d-printed-round-toe-casual-shoe#profileId-1268724
-*Flip Flops* - https://makerworld.com/en/models/579530-flip-flops-fully-3d-printed#profileId-500330
-*Oni Mask* - https://makerworld.com/en/models/1062398-oni-mask-samurai-mask-3#profileId-1355727
-*Mando Helmet* - https://makerworld.com/en/models/1024154-tribal-mandalorian-helmet#profileId-1006043
-*F1 Tracks* - https://makerworld.com/en/collections/450282-motorsport-f1-miniatures
-*Xbox Controller Holder* - https://makerworld.com/en/models/1191431-xbox-controller-stand-crystal#profileId-1203276
-*Videos Referenced*
-https://www.youtube.com/watch?v=dGP-pr3tEts&amp;t=112s
-https://www.youtube.com/watch?v=2JChLLMpJ00&amp;t=4452s
-https://www.youtube.com/watch?v=oA5eGO3VCNA
-https://www.youtube.com/watch?v=8d99KvGiynA&amp;t=391s
-https://www.youtube.com/watch?v=dGDzf6ZwwI4
-..............................................................................................................................................................
-BUY ME A COFFEE
-If you're enjoying my content, why not consider supporting the channel by buying me a coffee? 
-Even very small amounts are greatly appreciated and re-invested into bringing you better content.
-https://www.buymeacoffee.com/rickyimpey
-You can also use the YouTube 'Thanks' button above if you prefer.
-00:00 Intro
-04:22 Quality
-08:25 Reliability
-12:22 Reduced Waste/Speed
-22:55 Compatible Materials
-26:59 Material Control &amp; Care</t>
+          <t>Here's what the Bible says, it will SHOCK YOU!
+1 Peter 2:13-17
+13 Submit yourselves for the Lord’s sake to every human authority: whether to the emperor, as the supreme authority, 14 or to governors, who are sent by him to punish those who do wrong and to commend those who do right. 15 For it is God’s will that by doing good you should silence the ignorant talk of foolish people. 16 Live as free people, but do not use your freedom as a cover-up for evil; live as God’s slaves. 17 Show proper respect to everyone, love the family of believers, fear God, honor the emperor.
+1 Timothy 2:1-4
+I urge, then, first of all, that petitions, prayers, intercession and thanksgiving be made for all people— 2 for kings and all those in authority, that we may live peaceful and quiet lives in all godliness and holiness. 3 This is good, and pleases God our Savior, 4 who wants all people to be saved and to come to a knowledge of the truth.
+Romans 13:1-7
+Let everyone be subject to the governing authorities, for there is no authority except that which God has established. The authorities that exist have been established by God. 2 Consequently, whoever rebels against the authority is rebelling against what God has instituted, and those who do so will bring judgment on themselves. 3 For rulers hold no terror for those who do right, but for those who do wrong. Do you want to be free from fear of the one in authority? Then do what is right and you will be commended. 4 For the one in authority is God’s servant for your good. But if you do wrong, be afraid, for rulers do not bear the sword for no reason. They are God’s servants, agents of wrath to bring punishment on the wrongdoer. 5 Therefore, it is necessary to submit to the authorities, not only because of possible punishment but also as a matter of conscience.
+6 This is also why you pay taxes, for the authorities are God’s servants, who give their full time to governing. 7 Give to everyone what you owe them: If you owe taxes, pay taxes; if revenue, then revenue; if respect, then respect; if honor, then honor.
+Also, I mixed up Peter with Paul. I meant to say Paul.
+Connect 
+https://linktr.ee/itsbasicbible
+MALTA APPAREL LINK 
+https://malta-apparel.com/?ref=BBAZ16 
+FOR 15% OFF: basicbible15 
+FREE 10 DAY DEVO BOOK 
+https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
+I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
+https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
+I WANT TO FOLLOW JESUS CHRIST
+https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
+Get vidIQ to grow your channel faster! 🚀
+https://vidiq.com/itsbasicbible</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-06-01T16:00:00Z</t>
+          <t>2025-12-01T21:30:09Z</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>33188</t>
+          <t>1172</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>846</t>
+          <t>65</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>114</t>
+          <t>5</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>0.028926</v>
+        <v>0.059727</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>Good review, at 9:46 no brim on those supports?   I wouldnt call that bed adhesion issues, but improper support management.  Buti never blame the user,  the slicer should of caught that i believe, it should know better to have all that support above concentrated to one little spot on the bed was asking for trouble without a brim.   The one that held you could see was more verticle then the one that fell which started to angle quickly from the bottom, giviing it the side forces needed to knock it off easily.  I wish we didnt  have to catch all these edge cases and more intelligent slicers could figure this stuff out, but at leaste we dont have to mess with the mechanics anymore.  AI slicers next please. || The opening minutes are too long winded. Got to find another video that's more concise into the point without wasting my time || Aich. AICH!!! || I’m really leaning towards this printer vs H2S. Yes the H2S has a bigger build plate, but only by 15mm wide (4.4%) when using only the H2D right nozzle, so the benefit is negligible. As some concerns with power, I use an EcoFlow Delta 2 Max for my UPS for my network/NVR along with my 2 current printers (X1C &amp; P1S). If I switch out my current printers for 2x H2Ds, then I’ll just get a Delta 3 Ultra while still plugged into a 15A outlet. This will allow 3,600W to be drawn easily, so 2x H2D will have a max combined draw of 2880W, and unit will still charge at 1,800W. I’m sure both printers won’t sustain 2,880 draw the whole time they’re running, so it powerstation should be able to keep up 😊 || I almost stopped this video due to the incredibly annoying subtitles! || Sold my Prusa XL's and have made offers on Ebay for $500 less for the ones for sale and now have 3 H2D's and am not looking back, the H2D is fantastic and love there ability to print ASA and ABS.  I also have a few K2's and they are work horses for my industrial prints but something about the H2d's that give me a smile while it works, and for only $300 more then a new K2 the H2D is a better unit. || I’m tired and going to bed.  I’ve committed my evening to watching all these reviews with their FREE H2D printers.  I bought one 2 month ago and suspect I got a lemon as I’ve invested in 3 parts thus far, that I payed for, and yet to get one print.  This guy promotes a printer that he has received for Nothing and requires him to tickle the tip of Bambu.  Stay away.  This thing is junk. || Then buy something else... no one's stopping you.. but your mouth || An excellent comprehensive review that does a great job of describing pros and cons of the H2D which ticks most boxes.
-One of the best I have seen and as a prospective buyer provides some confidence in the purchase of the machine.
-One area that needs more explanation is the need for  a sacrificial tower using multi  filament colours to avoid carryover.
-This also wastes a LOT of filament (!)   Why can't this be solved by extending hot end changeover time?
-Does this requirement only apply to printing more than two colours?
-I haven't seen the sacrificial tower requirement mentioned in H2S reviews - presumably this version also needs a sacrificial tower as well?
-Did you find the print quality improved over say the X1C? || The simple explanation that I have seen is that the nozzle pressure needs to be primed before it starts printing again. Therefore the prime tower is always needed for any filament or nozzle changes to avoid spots of under or over extrusion on your print as the filament begins to extrude. || Seeing you next to this printer, I am building a desk not that's going to hold it. I targeted 36 inches to get some usable height out of the counter top, But also did not want the thing as high off set as that one there. They are tall!! || Haha, yes they are tall, you'll be glad you measured! || great video , you gave great details regarding   the printer, just subbed || Best and more complete review on H2D i have seen so far, thank you! || For your football goal replacment part. If you use infill "Gyroid" You dont have the best Z Bonding, use CUBIC 30-60% for overall best XYZ Tensile Strength within printed parts. Gyroid is only good for large scale objects to be fastly infilled but has nothing to do with strength. || Excelente y muy explicativo video! Después de 5 años estar con mis 2 Ender 2 Pro. Me decidí por la H2D y todo lo que veo me hace reforzar mi idea de que es una compra muy buena. Todas las posibilidades que tiene me encantan y los contra que veo mencionar una y otra vez son algo que no me molestan para nada. || what's a "lido pane" pretty sure you mean litho-phane || Cosplay helmets as a primary reason for the size choice says a lot about who the target market is. It’s insanely disappointing for a manufacturer that needs a 500mm cube machine for the majority of their projects. || Hi, I would like your feedback, for normal prints PLA/PETG max for doing min items (scale) 2 colors maybe 3 or 4 would it be faster in H2D and filament saving than in others? I had a P1S and sold it hoping h2d would be way faster than others, like instead of buying 2 P1S , H2D would print the same amount of items in less time than same amount of items in 2 P1S in multy color || iso9001? || ...no comment || One of the best videos I’ve seen on the H2D Ricky. Thank you so much! || my biggest issues is power, my entire farm is 220v and they refuse sell me a 220v parts.  They told me to return it and buy the 220v from oversea....  Just design it with both voltages in mind!   Even the A1 supports this! || Have you checked that the 120v in the US version isn't switchable to 220v? Most modern PSU have an input switch || I bought the ‘smoke purifier’ here in Thailand and they sent me one with a manual that claims 220v 50hz but the data plate on the machine says 100-110v 60hz. They are yearly making it as difficult as possible to exchange it. The email trail is now two months long and they will not send me a return shipping label as yet. || Great video,  thanks || You really glossed over the connectivity options.  Didn't even mention how being forced into these options prevents you from using the most popular slicer on the market Orca Slicer which is just a flat out better, more feature rich slicer than Bambu Slicer.  This is on top of breaking many other integrations that were available before.  Seems really dishonest not mention it and make it sound like they have all these different connectivity to suit everyone.  They do not || Yet another paid sponsored bambu lab "review"
-The H2D is a beta product with more flaws than an 8 year old ender 3. Nobody buys these things, the only people who have them were given them for free in return for a positive review. || tell me you're not a hater, without telling me you're a hater  || Another Prusa AI bot. They definitely don't know how to save their bankrupt company. || @MrlegendOr I wasn't aware that selling 11k printers a month and having a 25% YoY grown was  "gOiNg bAnkRupT".
-But at least prusa isn't out here manipulating consumer reviews like bambu lab. They just added over 2600 5 star bot reviews in the last 7 days on trust pilot. Becasue that's totally natural.. || another paid for biased review. never trust paid reviewers || Hello! Thanks for the great video! Could you make the files available for the NAS damper? || I love my H2D just printed a full size stormtrooper came out amazing blows my X1-C away || I keep getting an Extrusion Motor Overloaded error on my H2D, and no one seems to know why. I’ve been 3D printing for a while, so I’m not new to this. I’ve checked the basics, but the issue persists. I’m starting to think there may be a problem with the printer itself. Their US support has been really unhelpful so far. Has anyone here run into this or know what could be causing it? Would appreciate any advice! || The H2D has only a maximum chamber temperature of 65°C. This is simply not enough for many technical filaments. Even with the P1S, 50°C is possible. Also, the heating bed of the H2D is simply a joke. If you want to talk yourself into it, go ahead, it is and remains a joke. The H2D is also very technically complicated in many aspects, and maintenance work is hell with it. The H2D wants to be everything, but unfortunately it can only do everything very mediocrely and at a very high purchase price. || I can only agree about the chamber temperature. That's just not enough for a flagship 3D printer. They should have left out all the laser stuff or never developed it, but used better components for a higher chamber temperature. || @Oz1111 I don't recommend anything. Everyone has to decide for themselves what is important to them. There are plenty of tests on YT for all 3D printers available on the market, so you're sure to find your personal favorite. || I’m a bit pissed off with having to change the studio filament list each time I switch it on. There is probably a box to tick to just show me what I have in my AMS and no others but I haven’t found it yet || Agreed, it's very annoying || Nah, I am not impressed by the H2D. In my opinion,  developed past the market.  However, have fun with it... || 😂 || I'm hoping that they update the firmware for the AMS 2 Pro and AMS HT to not rotate the filament and be able to print with the dryer going as well. Anothet setting just for maintaining humidity, not drying. Have it run at a lower temp or a custom temp user input, and the humidity will still go down without warping the filament in the feeder. Luckily, it's just software. But it would be a huge miss if they don't fix something so simple. Knowing Bambu Lab, I'm still optimistic about that feature rolling out in a future firmware update. || I love how clear your content is, really appreciate it. My H2D is coming in a couple of days! || Excelente video !!👏 || At 25.26 you say the exhaust is filtered from and nasty particulates. Thats not the case, the top area behind the filter grill isnt covered by the included filter and the exhausted air is completely unfiltered. This is something banbu themselves dont mention. || Just ordered the H2D. I hope it is as great as everyone is saying. I already have ideas for projects bubbling up in fevered brain. I had a tough time getting the order made until I worked with Bamboo Labs and not another seller. || Ricky.. While Im impressed with the aspects of the H2D vs the Plus4, I find your comparison of the "big 3" between the 2 printers a bit off-putting. The BASE H2D is nearly 3x the cost of the Plus4. And even with some of its flaws, the PLUS4 outperforms the H2D for its price point.
-Lets stop playing word games shall we? || It's a paid sponsored bambu "review"...what did you expect? Bambu wont send anyone a $4k printer without them promising to glaze it and crap on the competition. Even when the competition is far superior. || I bought a plus4 it CNCd its own print bed
-Had to return it || this can't be serious 🤣 || I had an H2D for anout a month... As I generally tend to print mostly high-detail stuff (D&amp;D minis, etc), I was quite excited for the multi-material capabilities. Unfortunately, my machine was never up to the level, quality-wise, as my X1c was. I couldn't get minis to reliably print well, never got the multi-material stuff to work well &amp; the quality that came out of the printer varied widely.
-All in all, I've traded it back in for an X1c. We'll see what the future will bring us. I'll be keeping my eyes on what printers will be released. || 🤣🤣🤣🤣no se te cree nada … 😢 || trust me bro. || I see a lot of similar comments about FDM printers and mini figurines but I thought that was why people tend to buy resin printers for such things? || @PaddyFromPaddistan Not me. I don't like the chemicals &amp; the post-processing of resin, from what I've seen on YT. Plus, my lungs are far from "in working order", so the fumes are probably very very bad for me specifically.
-That said, there's, for me, also the "1 meter rule". Any detail you can't see from 1 meter, is useless.
-Hence, FDM minis are the way to go for me. || ​@mctazman407Ahh that makes sense mate, I did wonder what drew people to want to make figurines via FDM printers. I'm definitely in agreement with the fumes and post processing! || Bigger build volume… I think is already quite big maybe they can release an XL version but is not for everyone. || On the Bambulab forum, users are discussing serious issues with PETG printing on H2D models. They mention problems such as inconsistent print results, frequent layer adhesion issues, excessive stringing, and unreliable filament flow. Some posts point out the need to adjust the PETG profile settings, highlighting that printing this material on the H2D is not stable without additional tweaks. Overall, there’s a sense of frustration over the lack of support and inconsistent PETG print quality. || Interesting, my PETG prints have been very good overall. I will see if I can find the discussion you're talking about. || Siempre es mejor ajustar los perfiles || Did you have chatGPT write this for you, sounds just like a bot || Can say, I am mostly printing PETG and even if my H2D hast only around 250 hours on it. 200 of those are probalby PETG, with no issue at all. SUNLU PETG, Bambu HF PETG, Prusa PETG, and some other brands are used. I just try to keep em dry, cause that leads to some stringing and overall less quality in printing... but that is also true for other printers i use, or have used. || Petg hasnt been an issue in my h2d || Bambulab actually put this issue on their wiki and explained why this happens for the heatbed || Uneven bed heating, nozzle blobs of death, VFA issues, odd print bed sizing.  This thing is rubbish. || I have none of these issues except "odd print bed sizing" which is not a real issue. || @CL-gq3noI haven’t had the blob of death but I see a lot of posts on FB and some YT videos with people having issues.  The bed heating shows up if you use a thermography camera.  You can see the uneven heating while printing.  VFA is hit our miss depending on the printer quality control when it was assembled but it is not consistent. || ​@ericb9328For the heatbed Just let it heat for a few mins 
-Nozzle blobs of death happend when people dissabled nozzle cam (I saw one vid where one dissabled AI detection and it got clogged)
-VFA havent heard abt it || Excellent, comprehensive review!
-I don't understand why the print times didn't decrease a lot more when using larger nozzles, given that you can print wider and thicker layers proportional to the increase in nozzle size. || It's probably hitting the volumetric flow rate limit setting which will depend on the filament/profile and nozzle temp.  With tweaking of the profile/temp or high flow nozzles the 0.8 nozzle advantages could be fully realized. || @CL-gq3no Oh right, that refreshes my memory of what I read at the Bambu's H2 D forum when I was last there several weeks ago.
-As far as I can remember, there were various discussions about the higher flow capabilities and how they might be achieved with different settings, but had apparently not yet been realized by anyone. || On a US 15A circuit, that 15 Amp value is the absolute maximum allowed short peak current draw. Any sustained current draw has to be a maximum of 80% of the abs max - in this case 12A. So the max sustained power draw for a 15A circuit is then 120v x 12A = 1440W. Thus, basically, the H2D must be the only device on that 15A circuit. || Thats a issue only during the initial 30 seconds when is doing the initial bed heating after that the power draw should be similar to any other printer || @lotsad1234, It's not even an issue during bed heating.  It is the active chamber heater that uses ~1000 watts, but as you said that is only initially.  After that, it cycles on and off and only for filaments that need it.  I found this out while trying to run it from a UPS.  Only used a few hundred watts for low temp filaments during initial heating, but for ABS it overloaded the UPS while heating the chamber. || @CL-gq3no what wattage ups did you use? || I am going to have to get another 200 amps run to my house. I have 3 kids and our computers are already drawing already drawing 6 amps each. || @kdw75BS - computers do not draw much power. 6 amps?! No way. Maybe your wife should turn off the high powered vibrational motors. 😅😊 || Idk where you got your h2d but mine is horrendous. VFA out of whazoooo, wherever you have a hole in a print I get either a layer shift of over extrusion, something wrong with the left tool head that the support is trying to fix for 2 weeks(temp won't go lower than 78 degrees and the fan is always on even after replacing the heating element) and the list of issues I have makes me want to throw it out the window and try a Prusa. I wish I would have kept my x1c but I made the dumb decision to sell it and get the h2d. Big big mistake || 😂😂😂😂 otro que se crea sus propias películas!!! 🤣🤣🤣 ¡ cuánto darías por tenerla ! || @AndresDuque-qs9zz i don't need to dream boy i have it and i'm not here to prove you anything. keep scrolling till you grow a pair, and stop being a fan boy! || hes paid thats why || odd mine is flawless. You should call customer support and get it replaced. || @unitymind i did and they don't want to replace it but they are bamboozling me around asking me to disassemble half of the printer take videos of that and that than tell me they can;t see video number "whatever' and send it again. and in between each email is about 4-5 days || If they just came out with a bigger X1-C, people would be complaining. They can’t win as the hobby crowd is after them. Fortunately, they are losing influence over the industry. I’m impressed with my H2D. I use the left nozzle for the AMS 2 and the right for the AMS HT. The plan is to use the right for TPU as that’s recommended as it doesn’t move up and down. I’d rather disconnect the AMS HT than the AMS 2. It works just fine.standard “mains” in the USA is 120v (actually 123 v), 20 A, which is 2,400 watts. Old homes would be 15 amps. But they would have to be older than about 60 plus years. || The haych 2 d lmao || The size is just perfect imho, the footprint would be too much if it was larger. Was wearing some shoes I printed on it earlier, they came out really well. || I love your review but am really impressed with your nas sound dampening ! I have the same issue, and the sound carries via the wall. Now I have it sitting on foam, but I would love to print your design! Could you share your model? || Thanks so much for this review.  Seems very unbiased to me :).   I would love to learn more about combining tpu and other materials.  Strength testing.  Printers that can do it? || it's big , you are NOT joking the printer is big and the printer's box is massive , "don't dispose of this box" where do you store a box which could fit a family of 4 ? , I don't think they could make it any bigger without making it a industrial product. 
-I've only had it a few days but I think the print quality is better than the X1C , someone said you need a steady table etc , but I think that table need to fasten to the walls too. || I’ve had to put the box in my shed, couldn’t get it through the loft hatch 😂 || I'd have been a customer if they hadn't locked it to their cloud system. || Just print in lan mode 🤦‍♂️ || @iainhay2823 Except it periodically demands to call home, doesn't it?
-What happens if the company goes out of business, or they start charging for accounts? || @iainhay2823LAN mode using the Ethernet plug on the back, oh wait…. || They didn't lock it to their cloud.  They just locked unapproved 3rd parties from their cloud which really should have been done from day 1. || Great review, I love my H2D, next level printing from everything else on the market, including X1C. FYI you don't need external power to the AMS pro 2, that dries fine on the normal cable from printer. Only the AMS HT needs external power as it can dry higher temp materials. || True, what I meant was that I wanted to dry filament in the AMS pro 2 while I was printing from another source. For this you need the additional power supply. || Great review, I don't regret my H2D at all.  It has successfully completed every project I've thrown at it. || Great video! Really up in the air as to whether to buy one of these or not. Currently have two A1s and a Flashforge 5MPro. The price is just pretty much up there to justify for mostly printing PLA and PETG.  By the way could you please increase the volume of your videos? They are a lot quieter than other YouTube videos and almost have to crank volume up to max on my PC to hear. Thanks, Gerry || It is a lot of money and there are other printers that will give you basically the same results with PLA &amp; PETG. I would only buy the H2D if you think you'll use the heated chamber &amp; dual nozzles. Whilst it is great, I don't think I'd buy it if I wasn't interested in more engineering style printing. I will look at the volume issue. I always set it to recommended levels but perhaps there is something else going on. || Recuerda que detrás de cada impresora Bambulab … hay una gran compañía que te da mucho respaldo ! || Ricky do you prefer bambuu over creality? || also, would love the nas damper files if you can share them somewhere :D || best review I saw so far on the H2D.
-Good job || Too mush $$$$$ 😥 || Find another 2 nozzle printer with better experience
-They don't exist... || @mostlymessingabout Lmao probably becasue dual nozzle printers suck and nobody want to get tied up bothering with outdated tech. The H2D is a flop.</t>
+          <t>❤    Amen  🙏   ❤ || Amen! || AMEN || Amen! || Nobody is going to heaven. If God is real, then its not the any God we know. Thats what disinformation does. Its like a big game of telephone</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update API keys and scraper logic
</commit_message>
<xml_diff>
--- a/output/master.xlsx
+++ b/output/master.xlsx
@@ -453,40 +453,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
+          <t>UCXS90ukmtQo2kg3Ydf-cj3A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>itsbasicbible</t>
+          <t>Stay Ready To 3D Print</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Welcome to the channel.
-I help young men build lives of purpose, clarity, confidence, and conviction through biblical truth and practical leadership teaching.
-Most men feel stuck because they lack three things: Bible clarity, purpose clarity, and calling clarity.
-This channel gives you all three.
-Here, you’ll learn how to:
-• Understand Scripture with simplicity and truth
-• Discover your God-given purpose and calling
-• Renew your mind and rebuild your identity
-• Grow in biblical masculinity, strength, and discipline
-• Lead your life with confidence and conviction
-• Overcome insecurity, confusion, and internal limitations
-• Become a man of impact, influence, and Kingdom leadership without limitations
-If you're ready to stop drifting and make an impact, subscribe and join a community of men becoming who God created them to be.
+          <t xml:space="preserve">Hey, I'm Lawrence - Welcome to Stay Ready To 3D Print 👋
+I've tested tons of printers and logged thousands of hours troubleshooting, tuning, and
+figuring out what actually works in 3D printing.
+Now I run my own 3D printing business while helping you avoid the expensive lessons I learned the hard way.
+Here’s what you’ll actually learn here:
+✅ Tutorials - from first print to advanced tuning
+✅ Printer mods that actually make a difference
+✅ Honest gear reviews 
+✅ Step-by-step project builds you can follow
+✅ Side hustle lessons from running my own 3D printing business
+✅ Regular live streams solving print problems together and live giveaways! 
+Subscribe and join the community. 
+Email Chris (Production Manager) at stayreadyto3dprint@gmail.com for all business, brands, reviews, and collaboration inquiries. 
+ Visit our website to check out our products at 
+www.stayreadyto3dprint.com
 </t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>17200</t>
+          <t>47700</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>868</t>
+          <t>240</t>
         </is>
       </c>
     </row>
@@ -579,78 +581,56 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
+          <t>UCXS90ukmtQo2kg3Ydf-cj3A</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>itsbasicbible</t>
+          <t>Stay Ready To 3D Print</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>TO_COKkK6Pw</t>
+          <t>MQ2Cb2a8hJQ</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Is Your Faith SABOTAGING Your IMPACT? | Middle Ground Christian</t>
+          <t>Slicer Ninja is launching soon on kickstarter! Don’t miss out! #3dprinter #3dprinted  #trending</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>The problem with lukewarm Christianity is that you blend in with everyone and you impact no one." Are you following Jesus just enough to be called a disciple, but still betraying Him with your lifestyle? As we move into 2026, it’s time to stop repping the "Christian jersey" on the sidelines and actually get on the field. Remember: You may be the only Bible someone ever reads.
-In this powerful message, we dive deep into the spiritual danger of the "middle ground." Using the warning to the church of Laodicea in Revelation 3, we explore how becoming "comfortable" makes us ineffective for the Kingdom of God.
-Just like the lukewarm water in the ancient aqueducts of Laodicea, a faith without heat is worthless to a world in need of a savior. We break down the betrayal of Judas, the choice of Joshua (Joshua 24:15), and the sobering reality of Titus 1:16—where people claim to know God but deny Him by the way they live.
-If you feel like your impact has been sabotaged by compromise, this video is your wake-up call to stop looking back like Lot's wife and start pursuing your purpose with undivided attention. Don't waste 2026 like you did 2025. It’s time to choose: Christ or Culture?
-00:00 The Problem with Lukewarm Christianity
-00:47 A Message from God
-00:53 Understanding Revelation 3
-02:02 The Call to Make a Difference
-02:20 Reflecting on 2025 and Looking Ahead
-03:00 Living a Committed Christian Life
-03:46 The Consequences of Lukewarm Faith
-05:57 Choosing to Follow Christ Fully
-08:33 The Importance of Loving God and Others
-11:40 A Prayer for Dedication
-13:08 Final Encouragement and Farewell
-Connect 
-https://linktr.ee/itsbasicbible
-MALTA APPAREL LINK 
-https://malta-apparel.com/?ref=BBAZ16 
-FOR 15% OFF: basicbible15 
-FREE 10 DAY DEVO BOOK 
-https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
-I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
-https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
-I WANT TO FOLLOW JESUS CHRIST
-https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
-Get vidIQ to grow your channel faster! 🚀
-https://vidiq.com/itsbasicbible</t>
+          <t>Sign up for free here:  http://kickstarter.com/projects/slicerninja/slicer-ninja-ai-3d-print-file-optimizer
+What Is Slicer Ninja?
+Slicer Ninja is a web-based tool designed to take the guesswork out of slicer settings.
+Instead of digging through menus, forums, and trial-and-error prints, Slicer Ninja analyzes your model, your printer, and your filament, then recommends optimized slicer settings automatically. The goal is simple: better prints, less waste, and less time spent fighting your slicer.
+You upload a model, select your printer and material, and Slicer Ninja helps optimize things like orientation, layer height, walls, infill, flow, and speed—based on real-world printing logic, not generic presets. It’s built to work with your existing slicer, not replace it.
+Whether you’re new to 3D printing or you’ve been doing this for years, Slicer Ninja is meant to save time, reduce failed prints, and help you get consistent results without overthinking every setting.</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>2026-01-03T00:00:39Z</t>
+          <t>2026-02-02T17:06:08Z</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>1113</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>28</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="J2" t="n">
-        <v>0.173913</v>
+        <v>0.02965</v>
       </c>
       <c r="K2" t="inlineStr">
         <is>
@@ -659,78 +639,76 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>The problem with lukewarm Christianity is that you blend [music] in with everyone and you impact no one. And also another problem with lukewarm Christianity is that you can follow [music] Christ enough to be called a disciple but then still betray Jesus. And that's what [music] Judas did. He followed Jesus enough to be counted as one of the 12, but then when [music] the time came to it, when his life was on the line, when he was desperate, where his commitment [music] was there, his choice, he betrayed Jesus. And that's what happens with lukewarm Christianity is that you end up betraying Jesus. You don't have [music] time to be a lukewarm Christian. And ultimately, God doesn't have time for you to be a lukewarm Christian. You know, people's lives mistake because of the way that [music] we live because you may be literally the only Bible that someone reads. Hear that? You literally may be the only Bible that someone reads. Hey guys, I truly believe that God is speaking to you right now and he wants you to hear this. Today as I was reading the Bible, this particular verse stuck out to me. And it's not the first time that I read it, but it's something that just hit me a little differently, if that makes sense. And that was in Revelations chapter 3 where God was talking to the church of Leodysia. And he was talking about how I don't want you to be lukewarm. You're neither hot nor cold. And he's like, I just wish that you would choose one or the other. And as I began to think about that, I did some research just to get a better understanding of what that particular Bible verse was saying. And in case you didn't know that the church of Philadelphia, that city had an aqueduct that was six miles long and it was taking in water from a hot spring. So whenever it reached the city, it was lukewarm and people just got used to it. And I think that as believers, if we're not careful, the more we are hanging hanging around with the world or hanging out with believers who are not pursuing their purpose and really living the life that God has called them to, we can we can become comfortable. And because of that, we become ineffective for the kingdom of God. And I believe that Jesus wants us to make a difference in this world around us. He doesn't want us just to have the label Christian and really not make an impact. Instead, he wants us to live the Christian life so that we can actually make a difference. And I just began to think about how many of us, including myself, a little bit in 2025, we wasted time because we wasn't pursuing our purpose or we lived in compromise and we wasn't fully dedicated and being in alignment with what God has for us. And it just got me thinking that guys, God doesn't want you to waste your 2026 like you did in 2025. He doesn't want you to be the Christian that has the label Christian, but your life doesn't reflect Christ. Come on. You know what I'm talking about, right? You have Christian all over your Instagram bio. You you you you call yourself a believer. You go to church, but then on Saturdays and Friday nights, you're not really living for the Lord. Or even in the things that you're watching or even listening to, you know, it's not good for your soul, but you're still listening to it. And I believe that God is really trying to help the church, help the believers to really draw a separation because honestly guys, the time for middle Christianity being in the middle ground, those days are over. And to be honest, that should have never been a time, but it has been a time. And really, I believe God is really trying to extract and draw out people and believers who are truly committed to following the Lord. Because Jesus even said it that if you are a lukewarm person, you are worthless to me. I'm going to spit you out my mouth. And that's what's happening to some of us because we are not committed to God. Because we are not desperately dedicating our life to God. We're worthless to God. We can't even make an impact. We can't even make a difference in the world around us. And maybe that could be the reason why some of our family members are not saved still or even some of our friends or even our co-workers. Maybe that could be one of the reasons why we actually don't see transformation in our life is because we're not fully de dedicated and submitted to God. And because of that, God is just going to spit us out. You know what's so interesting? When Jesus said, "I I I wish you was just hot or cold." It made me think about being allin, right? Jesus is looking for committed followers of Christ. He's looking for people who are truly seeking after him and not just playing the middle ground or just happy that they're on the team and they got the jersey, but they really don't want to get in. They don't really want to get on the field and play. And guys, Jesus will spit you out his mouth. The person that is lukewarm, you see, I I would say this, the problem with lukewarm Christianity is that is that you blend in with everyone and you impact no one. Think about that for a moment. Lukewarm Christianity, you blend in with everyone, but you impact no one. That means your life looks the same as everyone else. Your speech looks the same. Your lifestyle, your your dress, the way you carry yourself, the way you even treat other people. It looks like the world around you, but you impact no one. You're not being a light. You look just like the darkness. And also, another problem with lukewarm Christianity is that you can follow Christ enough to be called a disciple, but then still betray Jesus. And that's what Judas did. He followed Jesus enough to be counted as one of the 12. But then when the time came to it, when his life was on the line, when he was desperate, where his commitment was there, his choice, he betrayed Jesus. And that's what happens with lukewarm Christianity is that you end up betraying Jesus. Even though you follow Jesus, you end up betraying Jesus in your commitments, your values, your theology, your your beliefs, your ideology, and all these different things. how you raise your family, the the type of people that you vote for in office, the the ways that you conduct your business, the way that you treat other people, your friendships, all these different things, your personal life. Lukewarm Christianity will eventually cause you to betray Jesus. And Jesus doesn't want that. Jesus wants you to be fully committed. That's why in Joshua 24:15, Joshua looks at the people and says, "Look, you can follow the people across the Euphrates River. You can follow these guides. you can follow these people, but he said, "As for me in my house, I will serve the Lord. As for me in my house, I will follow God in." And guys, as believers, some of you haven't made a commitment yet on who you're going to follow. You want to follow Jesus because you like what he gives, but then you still tampering around and playing with the world. You still want to drink a little bit. You still want to get drunk. You still want to smoke weed. You still want to watch seductive movies. You still want to uh read books that that spur the desire of lust in your life. You think it's all okay, but what you really don't know is that because you became comfortable with it, you don't realize that is toxic to your life. See, the issue with lukewarm Christianity as well is that you can get so used to toxicity that you are unfamiliar with what health looks like. And guys, God doesn't want that for you in 2026. He wants you to be a man and a woman that's fully passionate, that's fully surrendered, and that's fully committed to him. He doesn't want you to pursue the other things. He doesn't want you to be like Lot's wife who was running away from danger. But because she loved the cities of of Sodom and Gomorrah so much, she turned and she she looked back at the city and became a pillar of salt. Guys, God doesn't want you to look back anymore. He wants you to let go. That's why he says just uh the person who follows me and puts the hand to the plow and then looks back is is unfit for my kingdom. God doesn't want people who's constantly looking back and looking at what they missed out. Instead, God wants you to focus on the things that you can get for him from him because you are pursuing his his purpose that he has for you, you are pursuing the kingdom. And guys, I just believe that if you really want to make an impact in the world around you, if you really want to make a difference in this world that Jesus Christ has for you, guys, you got to be committed. You got to be fully surrendered and committed to God. Because even in Titus 1:16, man, guys, this verse always hits at home and and and to be honest, it always checks me. It says this, "People claim that they know God, but by the way that they live, they deny him. And because of that, they are detestable and they are disobedient and worthless for doing anything good." hear that people claim that they know God, but by the way that they live, they deny Jesus. And because of that, they are detestable and disobedient before God and they are worthless to him. Guys, that's the Bible. That's strong. That's not Renee Mallet. That is the Bible. That's what Jesus is saying is that you have to ensure that you're not just a person that has the label of Christianity, but your life actually reflects Christ. Does your lifestyle, does your deeds, does your thoughts, does your actions, does the way you treat people? Because Jesus also said this when they asked him, "What is the greatest commandment?" And he said, "Love the Lord your God with all your heart, mind, soul, and strength. And then love your neighbor as yourself." He says, "This sums up the law and all the ten commandments." Says, "Loving God with everything and then love your neighbor as yourself." You got to love your neighbor. You got to love people. You got to love God ultimately because the way that you love God reflects how you're going to love people. And the way that you love people is a reflection on how you love yourself and also God. And guys, I just believe that God is stirring up the church. He is stirring up the believers say, "Look, there's no time for lukewarm Christianity anymore. There's no more time to be on the sidelines and not on the field playing it. there. There's no more time just to say you have the Christian jersey on just so that you can be part of the team, but you don't want to contribute to the team. And Jesus is saying if you want to be that, if you want to be that type of follower, if you want to be a fan of Christ, but not a follower, then I'm going to spit you out my mouth. See, what I noticed whenever I played football is that the players who played and who who got reps and everything was the ones that were good, right? It was the ones that were really good. But this is what I've noticed through the the training and offseason is that you had a lot of people that wanted the jersey of the football team, but they didn't really want the commitment. They they always looked nice. They always had their bands, the sleeves, and all the gloves. They always looked pretty, right? They always looked pretty cuz they were part of the team, but they never really played. And it was because some of them just wanted the jersey so much that they didn't really care if they played or not. They were just happy that they rep the jersey. And Jesus doesn't want that. He doesn't just want you to rep the jersey of Christ. He wants you to be on the field playing the plays that he's given you, the assignments that he's called you to so that you can go out and really make a difference. And guys, I just want to say that God does not want lukewarm Christianity. You have to choose today whom you're going to serve. Is it going to be God? Are you going to follow Christ? Are you going to follow culture? Are you going to follow your carnal nature and your flesh? But guys, that that day of Christianity, that time is over. God doesn't want you to do that anymore. That day of Christianity is over because your family is counting on it. Your children, your businesses, the industry that you're in, the schools that you're in, the people around you don't have time for you to be a lukewarm Christian. And ultimately, God doesn't have time for you to be a lukewarm Christian. You know, people's lives are at stake because of the way that we live. Because you may be literally the only Bible that someone reads. Hear that? You literally may be the only Bible that someone reads. And if you're not living out the life how God has for you, man, you're giving them a false narrative of the gospel. And God doesn't want that. So, look, I just want to pray for you. If you just feel like this really touched home for you and you really want to submit and you just want to get back in alignment with Christ so that you can be fully dedicated to him, then I want to pray this prayer for you so that you can start off 2026 on the right foot. You can start off strong so that you can also end well. So let me pray for you real quick. All right. Lord, I thank you for my friend right now that's watching this video. And I just pray that as they are just [music] seeking your face. I pray that my friend would just repent from all of their sins right now. [music] Repent from being lukewarm and instead, God, that they would choose [music] to be fully dedicated to you. I pray that you forgive my friend right now. And Lord, as they are surrendering their mind and their heart back to you to get in alignment to you, [music] that you're just flooding their heart and their mind with peace and that they would just feel that you are closer than a [music] brother. God, you're closer than anyone else, God, because your word says that you're [music] standing at the door and knock. And God, you're knocking right now. And I pray that they will let you in. I pray for my friends right now [music] that they will just start off strong, God, and that they will end well and be the light and salt of the earth, God. That they won't compromise. instead that they will [music] emit your rays, God. They will be your lighthouse, God. And when people [music] look at them, they know, man, that man and that woman is a Christ follower in Jesus name. [music] Amen. Well, guys, hope this video really blessed you. Um, thank you so [music] much for tuning in and I just pray that, man, why don't you just encourage somebody with this video as well? If you're not a subscriber, man, [music] please consider subscribing because, man, I would love for you to be a part of the family here so that we can continue to grow [music] together. But ultimately, man, I love y'all. Thank y'all so much for tuning in and y'all have a great day. Peace.</t>
+          <t>running into problems like this, they get old really fast when you're 3D printing, especially when you're new. Because let's face it, in slicers, there are a ton of settings and some of which I still to this day don't know exactly what they do. So, I created a software, it's called Slicer Ninja, and it's launching on Kickstarter here pretty soon. And it basically allows anyone to 3D print without even knowing a single thing about the slicer. You can simply upload your STL file, give it to Slicer Ninja, it'll optimize it, give it back to you with all the settings set, all your supports, everything is done for you. Even if you're not a beginner like myself, it'll save you a ton of time. But the only way it's ever going to make it is with the community support, and that's you. Now, Slicer Ninja is fully functioning. It just needs some finishing touches from actual developers. My plan is to bring in a dev team to finish out Slicer Ninja and make it the best software possible. With your help, I think we can do it. No problem. If you want to get a really good deal on Slicer Ninja and stay in touch with what's going on with it, check out the link in the description. I'll pin it in the comments so you won't miss a</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>❤   Amen  🙏 
-        ALL  IN
-        💯    ❤ || Yes!</t>
+          <t>http://kickstarter.com/projects/slicerninja/slicer-ninja-ai-3d-print-file-optimizer || what is the cost to back this project?  I am a teacher, and a slice like this could be a great alternative for my younger students.  we us Mac M1, M2 and M4 computers, will this software be Mac Compatible?  thanks || It’s going to be several methods of backing as low as $10 on up to a few hundred. It’s a web based software so it’ll work as long as you have internet and a browser. || If it’s fully functioning, what does the dev team need to do? || Make it better. We want to add features such as filament management, batch optimization, and more. I’m not a developer so I need help to finish it and make sure it’s going to work as expected when thousands of people are using it. It’s not as simple as it may seem.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
+          <t>UCXS90ukmtQo2kg3Ydf-cj3A</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>itsbasicbible</t>
+          <t>Stay Ready To 3D Print</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>hb9G_3dqr9I</t>
+          <t>YiMevD99WKE</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Men Don't LEAVE 2025 WITHOUT HEARING This</t>
+          <t>The Truth: Bambu Lab Finally Clears The Air</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>This Video delves into the core issues holding many men back: a flawed identity rooted in fear, insecurity, confusion, and hesitation. These symptoms arise when one's identity is not anchored in Jesus Christ. The Bible teaches that God has given us a spirit of power, love, and a sound mind, not of fear. When a man is unsure of his identity in God, he hesitates and operates in delayed obedience, waiting for confidence. This hinders his potential and purpose. The key to overcoming these internal battles is not trying harder but standing firm in one's identity in God. When this identity is rebuilt, it transforms the mind, leading to shifts in confidence, clarity, and courage. Every man is created on purpose, for a purpose, and action must stem from a strong sense of identity in Christ.
-Connect 
-https://linktr.ee/itsbasicbible
-MALTA APPAREL LINK 
-https://malta-apparel.com/?ref=BBAZ16 
-FOR 15% OFF: basicbible15 
-FREE 10 DAY DEVO BOOK 
-https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
-I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
-https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
-I WANT TO FOLLOW JESUS CHRIST
-https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
-Get vidIQ to grow your channel faster! 🚀
-https://vidiq.com/itsbasicbible</t>
+          <t>🎉 PROMO ALERT
+Use PROMO CODE: STAY20 and get 20% OFF our all-new MorphX TPU filament.
+⏰ Offer ends 2-10-26 — limited supply available, so don’t wait.
+In this video, I directly question Bambu Lab about recent changes to their Terms &amp; Conditions and Terms of Use, and what those updates really mean for everyday users. Link to Bambu lab ToS Document's.....https://bambulab.com/en-us/policies/terms
+Specifically, we break down:
+How the new software and firmware terms affect Bambu Lab 3D printers
+Whether enabling Developer Mode can impact warranty coverage
+If refusing firmware updates could void your warranty
+Concerns around data collection and user privacy
+Claims of hidden changes and whether anything was intentionally buried
+Allegations of unethical business practices — fact vs rumor
+The goal of this video is to clear the air, separate truth from speculation, and provide on-the-record answers so the community can make informed decisions instead of reacting to misinformation.
+If you’ve been confused by the recent controversy, worried about losing warranty protection, or unsure how these updates affect the way you use your printer — this video is for you.
+If this video helped you, consider liking, subscribing, and sharing it with other makers who may still be confused by the situation. My goal is transparency — not hype.</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>2025-12-30T00:01:01Z</t>
+          <t>2026-01-28T10:30:19Z</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>19689</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>608</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>317</t>
         </is>
       </c>
       <c r="J3" t="n">
-        <v>0.142857</v>
+        <v>0.046981</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
@@ -739,83 +717,83 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>What's holding most men back isn't their circumstances, their age, or a lack of opportunity. It's actually their identity. Their identity being rooted in fear, insecurity, confusion, and hesitation. And these are not personality traits. They're actually symptoms of identity, not rooted in Jesus Christ. You see, the Bible says that God did not give us a spirit of fear, but of power, love, and a sound mind. So if fear is leading your decisions, it didn't come from God. And when a man doesn't know who he is, he begins second-guessing himself. He begins acting in delayed obedience. And he is waiting for confidence before taking action. And that's how potential and purpose stays locked up for years. But when identity is rebuilt, the mind is transformed. Everything begins to shift. Confidence follows, clarity follows, and even courage. You don't overcome internal battles by trying harder. You overcome them by standing on who you are in God. You were created on purpose, for a purpose, and with the purpose. An identity will always precede action.</t>
+          <t>So, let's stop right there. We all know who they're talking about. What? So, you knew about this over a year? You were selling paper weights? Premium paper weights is what you were doing. Not cool. As a business owner, I would never do that. So, in this video, we'll cover some of the questions that I asked Bamboo and the answers that I got. Like, why'd you change your terms of service? Did you try to hide it? And if I don't update to the latest firmware, will I lose warranty or will I lose warranty if I stay on developer mode or LAN mode? There was a ton of questions that were floating around the internet. A lot of them just left everybody confused, not knowing what to believe, including me. And come to find out, some of the stuff that I believe it was actually not even true. So, I'm going to cover several different topics around this whole controversy of firmware, the ecosystem, locking out third-party softwares, and oh, speaking of thirdparty software, there's another company in this whole thing that deserves your attention way more than Bamboo Lab does. I can't wait to tell you about that. So, real quick, let me tell you about today's sponsor, and it's me. Stay Ready to 3D Print has come out with Morphex TPU. We launched it a couple of weeks ago, and the sales have been absolutely nuts. Everybody loves this stuff. It's a super easy to print TPU. So, it makes printing shoes like these a breeze. And they're super comfortable, too. I was so tired of dealing with TPUs and being forced to print with a super stiff 95A TPU just to get the 3D printer to print the TPU. And what's the point in printing a shoe in 95A? It'll be so stiff that you won't even be able to wear it comfortably. But with Morphex, all those problems are over. It's the best of both worlds. It starts out as a 90A, so it's easy to print, and then after it's heated and extruded, it morphs into a 70A, so it's super soft. I mean, you can take this whole shoe right here that's done in 15% infill and you can bend it everywhere. It's soft. I wore these exact shoes to BitSummit 2025 and let me tell you, they were great. So, if you want to get Morphex TPU, go to stay readyto3dprint.com and check it out. And I'll leave a promo code in the description to give you 20% off. So, go check them out because that code will only be good for a limited time. So, real quick, let's go back a little bit so I can explain how we got here today. So, some of you might remember I went to Rapid TCT up in Detroit a few months ago. I built Creality's 11th anniversary motorcycle. I took it up to Detroit and I actually went around all of Rapid TCT and I interviewed several different brands, Bamboo being one of them. And while I was at their booth, I was asking about their new H2D machine. And one of the Bamboo reps, he was just going on and on and explaining all about the H2D machine. And then towards the end of the interview, he brought up software. And so I thought it was a great opportunity to actually ask some follow-up questions and that is when this happened. &gt;&gt; So speaking of developer mode, I think some people were worried about with Huh. &gt;&gt; Do you chat with &gt;&gt; I'm sorry. &gt;&gt; Are you asking about authorization stuff? &gt;&gt; The the land mode &gt;&gt; land developer mode. &gt;&gt; The developer mode. Yeah. Huntington has also. &gt;&gt; Now, keep in mind, this happened right in the middle of that whole controversy thing, right after they had announced the terms of service changes and all that good stuff. So, this didn't look good at all. And to me, it looked like, what are you hiding, right? Why would you abruptly stop an interview like that and do it so rudely? That was the main problem that I had with the whole thing. It wasn't that you didn't want us to talk about software, cuz I get it. you want to do that in a controlled way, especially with all the controversy bouncing around. So, I understood that. But for me, it was just the way that they went about doing it. It rubbed me the wrong way, especially when I was there to talk about their H2D machine and I was promoting it on my channel for free. &gt;&gt; Oh, okay. Okay. We'll cut that out. Don't worry about it. &gt;&gt; Yeah. &gt;&gt; So, I know in the video I said, "Okay, don't worry. I won't post it." But honestly, when I got back home, I thought long and hard and I had decided, you know what? No, I need to post this and let people make their own decision. I didn't try to influence anybody's decision in that video. I simply posted it and just gave the facts. Now, if you look at some of the comments, people got pretty heated about that whole thing, and that video got over 10,000 views in the first few hours. But if you look at it as a whole, like I do, when I look at my analytics, it was over 75% likes and only like 25% dislikes. So, the video resonated with most people. So, about a week after the video had been out on YouTube, I got an email and it was Bamboo actually replying to an email that I sent them asking to review a machine. And needless to say, they were a bit confused. They were wondering, "Hey, we see you want to review one of our machines, but we're a little confused cuz now we see this video." I'm glad that they did because if they wouldn't have reached out, this video never would have happened and I would never have been able to bring you guys the actual truth. And I think that's what everybody needs. And honestly, it's kind of sad because a lot of those people made decisions just like I did based on rumors that mostly weren't true. And a lot of those rumors, they were just simply misconstrued and baseless. So, after a few emails back and forth with the Bamboo Lab rep, we came to an agreement. He sent out an X1C and he gave me a $400 Bamboo Lab gift card where I could go on their store and buy pretty much everything I needed to basically test out their printer over the next couple of months. And that's exactly what I did. So, needless to say, me and Bamboo Lab started off on a really good foot considering the video I had just posted. I was a little confused at this point and I was definitely on my guard because I was like, "Wait a minute. I just posted this video basically bashing you and you reply to an email and at first you're confused and at the end of a couple of emails now you're sending me a $1,000 printer and giving me a $400 gift card. So I was wondering, okay, wait a minute. Are they trying to buy my opinion or like what's going on here? And I've had the printer several months now and I've been using it pretty much almost every day. I just got busy and I couldn't just jump on the video right away. But honestly, it's been a good thing because it's allowed me to use the printer over a long period of time and really get to know the Bamboo ecosystem and test out all the stuff that everyone's saying to see for myself, is it true? And then the things that I wasn't sure about, I reached out to Bamboo Lab directly with a whole laundry list of questions and they answered them. All right, so I'm not even going to pretend like I memorized this whole email because I didn't. So, I got my phone here. I'm going to go over with you the questions that I presented to Bamboo and then as you'll see on the screen here, my questions will be in white and their answers will be in red. So, the first question I asked was what support and warranty coverage do you get if you're using the cloud on the latest firmware, if you're in LAN mode with no internet, if you're in developer mode, or even if you're on an older firmware. And here's what they said. Support and warranty are provided for all publicly released models and firmware. Naturally, if a user requests support for a bug or feature that has already been fixed, the only recommendation support can provide is to update to the version where that fix was implemented. So, that was their answer on that. Pretty much you've got support and you've got warranty. So, the second question was about terms of service and updates. So, my question was, if a user declines an update, can functionality, support, or warranty be reduced or blocked under the current terms of service? and they basically said please read above basically refer me to the answer for the first question. So in other words no you won't be blocked and it won't be reduced you will have warranty and they will provide support. So number three is authorization control and thirdparty tools and this is where it gets interesting. This next question is Bigtree Tech/Panda Touch support. And my question was, Bigtree Tech has publicly stated that some of their devices, including Panda Touch, will lose functionality after recent Bamboo updates. What is Bamboo's position on this? And is there a plan to maintain compatibility or provide an alternative? Here's the answer they gave. Once again, this is old news. They had over a year's notice. In fact, their release of Touch was one of the triggers for us to be transparent about closing these exploits. We don't want people purchasing something without knowing it won't work in the future. Outside of developer mode, we will not allow this functionality as it involves an unauthorized device. And again, the reason why Bamboo is doing this is to protect you. And Big Tree Tech is only concerned about selling you a third party device. That's the only reason they care if Bamboo patches some of these security exploits. And Bamboo has pretty much said that if it means compromising security that they're going to patch it and they're not really worried about what Big Tree Tech thinks about it. They let them know about this a long time ago and they chose to continually sell these third-party devices. Blows my mind. My question was, will Bamboo provide an official pathway API program for thirdparty controllers like Home Assistant or Panda Touch to retain full functionality? And if so, what is the plan or timeline? And here's what they said. API access will only be allowed through authorized license partners. Now, for the community, the available option is developer mode. As mentioned in my previous emails, we gave more than a year and a half of advanced warning about this change. In Panda Touch's case, we cannot take responsibility if a manufacturer chose to rely on a known exploit and still decided to sell hardware that was bound to stop functioning at some point. So, let's stop right there. I want you to think about this. Who are they talking about? We all know who they're talking about. They're talking about Big Tree Tech who makes all the panda stuff. And here's where a lot of this controversy came into play. Because guess who played dumb? Whenever this whole controversy came about, Big Tree Tech, they acted surprised. Oh, I can't believe this. Oh, this doesn't work now. What? So, you knew about this over a year? You knew Bamboo was going to push out an update that basically rendered your product useless and you continued to sell those products to the public? I don't understand that. Now, I could get if you announced like, "Hey, these products might be coming useless. Here's what we're going to do with products that we already have manufactured in stock. We're going to go ahead and reduce the price down to basically build price and push them out at super low prices just to get rid of them and stop manufacturing them." But that's not what they did. They continued to build these products for Bamboo Lab machines knowing that at some point a firmware update was coming out that would render their products useless. So, like I said earlier, I think there's a company here that deserves our attention way more than Bamboo Lab does at this point. Yeah, it just blew my mind when I heard that. Now, you might be thinking like, "Oh man, Bamboo Lab is throwing Big Tree under the bus." But really, they're not. Bamboo Lab is covering theirelves at this point. and really big tree tech threw them under the bus. By continually selling these products, you set users expectations that they'll be able to use these products. So, of course, these users got mad when Bamboo Lab did this that everybody looked at Bamboo Lab like, "Hey, what's going on here?" Right? when in all actuality, Big Tree Tech should have put out something along with Bamboo Lab when they found that out, letting people know, hey, you might not want to buy these devices because they probably won't work here in the next 6 months to a year. So, Big Tree Tech, if you're watching, I think you owe everybody an apology for one, acting surprised when you already knew what the game was, and for two, for continuing to sell a product that you knew was going to be useless. you were selling paper weights. Premium paper weights is what you were doing. So yeah, to me not cool as a business owner I would never do that. So for my question number four is about LAN only mode. Now my question was will LAN via Bamboo connect always work without internet or an account? Which features differ from cloud mode and is any telemetry collected in LAN mode? And the answer was yes. On current hardware, there will be no changes to how things work. As always, I can't speak to future hardware or software. Those remain unknowns, which is, and that's fair. Developer mode. Now, here's one that I heard all the time from various different people. And honestly, somewhere along the line, I adopted it and I actually believed it, too. So trust me, if you got caught up in this whole controversy, you're not alone because there's a lot of stuff that I believed and now looking back, I didn't even do my homework and I just adopted certain things. And I don't typically do that. I'm a very, very curious and investigated person, but I heard it from a reliable source, so I didn't even think about it. So, on to developer mode. I asked, "Does enabling developer mode affect support or warranty by itself or only if issues are directly caused by changes made while using that mode?" And the answer was, as stated above, running this mode does not void warranty or support. They're basically saying that you can use developer mode and you're not going to lose support or warranty, as a lot of people believe before, including myself. So, question number six I asked was about firmware roll back. And the question I asked was, will Bamboo provide a supported roll back option to older firmware that keeps first-party apps functional for users who need compatibility? So basically, will they offer a firmware roll back that allows you to continue using those big tree tech products? And the answer was yes, unless stated otherwise in release notes. So that's kind of left open. It it's like yeah, unless we decide not to. So, that one, I mean, I wouldn't bank on it. I really wouldn't bank on it. Cuz let me tell you this, a lot of the reason why Bamboo Lab did the whole terms of service thing boils down to their new machine. And here's why. They released the H2D. And in the H2D, there's a laser inside that machine. And what the bamboo rep had explained to me during an email was that we're basically putting a laser inside people's living rooms, inside their bedrooms, inside their garages, and we have to do everything that we can to protect those people and not allow some person with ill intentions to hack into their system using an exploit that, let's say, Big Tree Tech used in order for that Panda Touch to work. Someone else can use that same exploit to get into your machine and do nefarious things such as turning on your laser in the middle of the night or while you're away on vacation or get access to your camera and be able to, you know, look around or whatever. But the biggest thing was was safety. You don't want someone to be able to get into your machine and turn on that laser in the middle of the night and burn down your whole dang house. And honestly, big props to Bamboo Labs for not caving in to those companies, those third party companies that, you know, out of selfish reasons, they wanted those accesses to be left open. They wanted those exploits to not be patched. That way, they could continue selling you their little third-party products. And Bamboo Lab decided to choose their customer and their customer safety over all of those companies. And that's kind of how this whole thing started. So, I just want to give props to Bamboo Lab for that. And I see why they did it now and honestly it was the right move 100%. So we're going to move on to question number seven and that is future gating of core functions. So my question here was can you confirm that core printer operation start stop jogging temps job uploads etc will not be gated behind proprietary authorization except where necessary for documented security reasons. And that kind of plays to what I just said. Can you confirm that you're going to allow us basically allow us freedom unless security reasons require you to shut it down basically is what I was asking and he said nothing will change with current hardware but to be clear the only mode that currently allows this is developer mode and that's something we already knew and that's great. So in developer mode you have a lot more freedom. All right now moving on to number nine public documentation. So my question on this was, "Can you point me to the official pages covering terms of service, authorization, control, land mode, developer mode, and warranty so I can cite them directly in my video?" Their answer was, "Once again, since all of these modes are supported, I can only refer you to our terms of service." And then he gave me the link. And so I'll include that link in the description for you guys to go check out for yourself. Okay. Now, next, it's kind of a paragraph, so bear with me. I asked the Bamboo rep. I said, "Hey, I'm not sure if you've seen Lewis Rossman's video about this a few months back." I'm asking some of the questions he brought up as well, but one thing I'd like to know is, did Bamboo delete the web archives of the terms of service changes made? If so, why? Why not just tell everyone they made changes versus trying to hide it? Was it just to avoid confusion? I'm curious because if that truly happened, then it just seems odd without a logical explanation. and his answer was, "Please refer back to my original email." And then he reiterated, "The only change was a minor clarification regarding forced updates. We would only ever apply or force an update if a public safety issue arose from a firmware version. That's the simple fact. Despite how some may want to portray it otherwise, we openly reported this change, but after being accused of gaslighting, we chose not to make further comment. In my opinion, that was probably not the greatest choice, but hey, that's a choice that Bamboo Lab made, and honestly, I think they'll be okay. So, my response was, "Well, I'm sure you have some very logical explanations for a lot of this, and I look forward to hearing them." And he went on to say that we had hoped that clear-minded users would understand why these changes became necessary once we began integrating features like a laser into the printer. Unauthorized 3D print commands are one thing, but triggering a laser unattended could put lives at risk. So, like I had explained earlier, Bamboo instituted a lot of these changes due to the fact that they're putting a laser in people's living room. So, just let that sink in and maybe some of this will make sense now because before to me, yeah, I was with you guys. A lot of it didn't make sense. And I'm an avid Creity user up until recently. Of course, I will be selling off all my Create machines and changing brands. I don't know if that's going to be Bamboo or Prussa, but it will be one of the two. And that has nothing to do with this video. It just happens to be that I'm no longer promoting Create as a brand. So, he goes on to say, "As a company, we have a responsibility to protect not only the best interest of our customer, but also the best interest of the company itself." With that said, most if not all of the accusations made back in January have proven untrue. We were not hiding anything. We were simply closing a known protocol exploit. Even then, we provided our user base with options and continue to support developer mode. At this point, it's baseless for anyone to continue pushing this narrative. So, yeah, there you have it. A lot of the hard questions were asked and every single time they came back with a solid answer. Now, I didn't take these as just straight up fact. When I got the machine, I've tested the machine over a period of several months. Now, let me give you my thoughts on the machine, right? I've always thought that Bamboo Lab had a great product from day one. I just never used a machine for the simple fact that previously I enjoyed modding my machines and to a degree that you just couldn't do it on a bamboo machine. And now a few years down the road, I'm just not at that point anymore where I want to do mods like that. Honestly, now I just want to be able to print with a printer that works 9 out of 10. And yeah, I like to add the occasional light kit, the occasional flowtech hotend, uh different extruder gears, minor stuff like that, but I'm not doing those in-depth mods that I was doing before. I'm just not doing them anymore. And that was one of the biggest things holding me back from using bamboo. And of course, now that they've clarified this, it really has put my mind at ease. And I feel 100% okay going out and just buying bamboo machines if that's the brand that I decide to go with. I'm not sure yet. It might be Prussa or who knows, it might be another brand, but those are the two brands that are, you know, number one and number two. I'm just not sure which one it'll be just yet. But I can tell you with the X1C, my experience with the X1C, it was basically just like any other printer that I've had. I always put all these printers basically in the same category pretty much. Nine out of 10 printers, they just work and they all have little minor issues. Like my X1C, it's been phenomenal until recently whenever the extruder stopped working and it just kept jamming after jam after jam. I didn't know what was wrong with it. I reached out to the rep like, "Hey," he was on vacation, but like he went and made sure the next day I had an extruder in the mail and I got the extruder. it solved the problem. I don't know what happened and maybe it's something I did. I'm not sure. But honestly, I mean, I don't get upset at those things because those are simple 3D printing issues that from time to time, you're going to have them even with the best machine. And I think the sooner people realize that and stop putting certain brands on these pedestals that they really don't belong. I mean, after all, these are robots. They only do what you tell them to do. And very very rarely do they just up and do something on their own that they weren't told to do. So n out of 10 if your machine is messing up or it's printing bad. It's usually something you're doing and that's just the raw truth. It's usually usually something you're doing you're doing. But overall the X1C has been a good machine and honestly the print quality is actually phenomenal. And I really love the way that you can basically just use your Bamboo Handy app and you don't even have to connect to a PC. That's been my biggest thing with the X1C is it's kind of how I use the X1C. Now, I have a bunch of other printers, but the X1C, it's kind of like my running gun machine. I'll be on Bamboo Handy and I find something that I want to print real quick. I'll just pull it up, hit start print, and and there it goes. So, I leave that machine on pretty much 24/7 and I'll just shut off the lights from my phone or whatever the case may be. So, that's one of the biggest things that I like about the Bamboo whole ecosystem thing is the way they require people to upload their files basically in a 3MF format to where someone's already printed that file. It's ready to go. All I have to do is hit print and make sure that I have that filament in my printer. And honestly, you don't even have to make sure you have that filament in your printer. You can select, let's say it's a PLA model and you all you have is PET G in your printer. You can actually select Pet G and it'll actually print it in Pet G for you. All the settings are already pre-done. You don't have to do anything. And as far as print profiles, oh, I haven't done any of that with the Bamboo machine. It's been great. And really, Bamboo has really been innovating here lately. So, obviously, they're coming out with the H2S, which has already hit, and then they're coming out with the H2C. And from what I understand, it's going to be six tool head changer. And that thing is going to be absolutely phenomenal. I mean, wireless induction hotends, it's got some high-tech stuff in there, and it's going to change the way we do color printing. And the future is tool changers. So, if you're thinking about buying a machine, you need to consider, if you want to do multicolor, you need to highly consider getting a tool changer. Whether it's the Bamboo H2D with the upgrade or the Bamboo H2C or even the Snapmaker U1. There's several brands coming out with multi-tool head machines. I even heard that Creity is finally thinking about doing one after I decide to get rid of all my Creity machines. Now, I'll make a video on that later on why I'm leaving Creity and I'm no longer promoting their brand. They didn't treat us very nicely and they allowed some stuff to happen that I'm just not okay with as a human being and I have to do what's best for the channel. And at the same time, they weren't innovating like other brands were. Other brands were coming out with tool changers and all this new stuff. And it seemed to me that Creality was basically just slapping another letter on on a printer and saying, "Oh, here's our new printer." Like the K1 Max and then they released the K2 and then the K2 Plus and then the K2 Pro and the K2. And honestly, the only thing different in the whole K2 lineup is size. They didn't change much of anything. If anything, they just took away features and put out another printer. And so that is part of the reason why I left Creity was lack of innovation. Well, now they're coming out with the multi-tool head supposedly. I guess we'll see. But one thing in this game, I'm always open ears to anything new. If it's a new brand or a new product, I'm not married to anybody. And I go where the innovation is and where we're being treated fairly. One thing I can say about the Bamboo community is that their users are dieh hard. Because when I made that rapid TCT video, man, were they in the comments. They were in the comments bashing me and talking all kinds of smack and saying that I was a Creity fanboy and all this stuff. Well, what do you have to say now? I own a bamboo machine and I'm even considering bringing bamboo products throughout my whole studio. They're in my top two as two brands that I'm considering of bringing into my studio. So, now I know what they'll say. They'll probably say, "Oh, you're just riding on bamboo or whatever the case may be." So, I know what to do with all that. I just don't listen to it. I know at the end of the day, I just want a solid brand in my studio and Bamboo is a solid brand and I really respect what they've done with the terms of service, how they handled it, how they answered all these questions and it just really opened up my eyes about them and so yeah, I really appreciate that. Thank you, Bamboo. And with that, until next time, stay ready to 3D</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>❤   Amen || Amen!</t>
+          <t xml:space="preserve">Win A Laser! Anyone who purchases MorphX TPU will be entered into a giveaway for an ACMER 7w Diode Laser! We will announce the giveaway on Discord so be sure to join our server here. 
+https://discord.gg/ZGgcwk7eWt || says this link has expired? || @TheGhinishok let me refresh it. || https://discord.gg/ZGgcwk7eWt || So, they did not lock the printer, but rather their cloud. As long as they stay out of their cloud, anybody can use do whatever they want with the printer. || OMG, dude get to the point…..could have made a 2 minute video… || $11.50 for standard shipping for one roll of TPU? IDK bro, seems pretty steep. || BTT had a disclaimer on the product description well before the controversy began.. They were not trying to pull a fast one on anybody. And to your point of "they should have sold at cost and quit manufacturing". Why?? Their product is still useable. || They def did not.  There are tools that allow you to look at the internet from the past. They def did not. || @stayreadyto3dprint  Do let me know if you post the CFS for sale anywhere. I need a second one. || Not the first time an update or firmware update screwed over people. Cough nvidia, samsung, apple, sony, even LG etc. || True || The security excuse is fiction. The issue was all in their cloud. Nobody was connecting to your printer, except Bambu. They did have that in ident where THEY sent reprint commands that cause people problems. 
+My fix, printer no net access. Delete Bambu handy and slicer. Install Orca slicer and use home assistant for secure remote.  Turn on LAN mode and it is on a version before they crippled the printer. || We knew ALL this except the future laser, at the time - if you bothered to read and listen instead of jumping on a Reddit/YouTube bandwagon. || PUBLIC SAFETY ISSUE MEANS COMPLYING TO THE GOVERNMENTS NEW RULES AND REGULATIONS! ALL FOR YOUR SAFETY TRUST US. || How about contacting Luke from BigTreeTech for their side of the situation, not doing so is showing your bias. Luke is on record refuting the slant you present. There is more to it than you make out. || What record is he on refuting it? And I did reach out. They stopped replying to my emails a long time ago. So I don’t owe them anything at this point. They’ve done other things that inspired them of mentioning publicly. Let’s just say they aren’t very ethically motivated as a brand. That’s all I’ll say on that. || Wtf is that sh1t on your head?
+so stupid ape try to look bada$$ || this whole situation just confirms why i’m stepping away from bambu. the printers might be great on the hardware side, but locking things down after the sale and calling it “security” really doesnt sit right with me. if firmware updates can sudenly take away tools or limit how i use a machine i paid for, thats a hard no... || I understand that completely || Bambulab never more! Not gonna lie, I’m more disappointed than satisfied with Bambu. || where can i find  the stl for those shoes? || Go to my website and the TPU sale will pop up. Tap Get MorphX.  Scroll to the bottom and I included a few files for free. Those are the whaleberry sport shoes. 
+www.stayreadyto3dprint.com || Are you bias on Bambu? What brand should I go with chat? I need support and freedom here. Coming from an ender 3 years ago! || I think Bambu or Prusa would be great options. Prusa has a better customer service. Price is higher but you pay for the customer service and quality of the build. The Nextruder system is why those machines are so rock solid. Depends on your needs really. || The issue for me at least is 3d printing was built on open source.  Bambu has gone closed source with all the Intellectual Property many brilliant engineers and tinkers have given to the community to bring it where it is today. Bambu took all of that and started a business and doesn't give back to the community which build their business.  Then hides behind our security as the reasons to go closed.  Even when it is an obvious rip off of open source projects. || Yeah I don’t agree with how they did that for sure. One of the reasons I don’t own bambu machines. But I think I’m over it now. Cause I really want the H2C lol😅 || this video sounds really one sided + they make claims but you don't verify or explain why it could be like that yes or no. Don't get me wrong here, you might be right, but I feel it lacks a bit of rigor :) || Maybe so. Hindsight is always 20/20. I tried to just provide facts I found and allow viewers to form their own opinions || They just want to be able to not let you print “prohibited items” later on… || Hope not || @stayreadyto3dprint lol that's like pulling your pants down. Putting your head in the sand and your ass up in the air and saying "i hope no one is gonna fuck my ah" || Bullshit. I had the shittiest experience in my first two weeks and they ran me around in circles with "What did you do?" "Can you send me 5 MORE photos of the same 5 photos you sent". I've ran mine offline since I heard about the firmware update and since then I have scanned my printer with an ESP32 Marauder I built and guess what it gives off wifi and bluetooth - I hate that BBL marketing suckered me and now I am the wiser for having made that mistake, one I won't make again. American or Canadian made and wifi as an option. || Duly noted. I’m wanting to come out with a us made printer brand. We will see if I can pull it off. With actual customer service as well. I think it’s high time || 😂😂😂"customer safety". Fucking shill. 😂😂😂 || The answer to question 6 is just No, with extra words. 😅😅 || About the answer to Question 3. 🤦 Using a protocol/API as intended is in no way an EXPLOIT! I don't buy that Bambu warned BTT. According to Bambu, they also allegedly reached out to the makers of Orca, but no one from the Orca slicer dev team had been contacted by Bambu. Not to forget how Bambu kept insisting that MQTT was turned off for safety reasons, and it was an exploit, and unless you know what it was and how it worked, you don't know if that is a lie. Also, remember that the security of YOUR local network is YOUR responsibility, not Bambu Labs. Even if you have a fully open Wi-Fi, it’s still not Bambu’s responsibility what happens on your network. The only responsibility of Bambu Labs is that I can’t access your printer over the internet, and that's it! || BTT was using more than just api access. FYI || About the answer to Question 2, in my book beeing forced to update firmware to get support is the same as no or limited support. For example, Lidar is having trouble scanning the QR code, bambu see i dont run the latest firmware, they will not assist me in any way before that is fixed! || To be clear, they said you would receive support no matter if you’re using dev mode or what firmware you’re running, but sometimes updating firmware is a fix for some things. They made it very clear. They weren’t abandoning users who decide not to upgrade or use dev mode because that was one of my biggest issues with them before and they did clarify that for me. || Brother this is bullshit. They could have made a new TOS for the new machines and left the old ones alone. This is the dumbest take in the world. Oh they put in a laser. So fucking what? Change the TOS for that machine leave the rest alone. The older machines dont need those updates. || Good video but just a shame he couldn't spell Bambu correctly 😂 || The biggest reason I went to bambu, as an engineer, I hated messing with my printer before I could use them, tweak them, etc... I wanted a printer to just work. || Do you have your BL machine air gapped? || I grabbed my A1 Mini about a year ago as a hobbyist due to recommendations on ease of use.  Since then, I grabbed a Comgrow T300 secondhand to print larger items.
+Suffice to say, my tax refund is going to a P2S.  HOPEFULLY, it'll work with OrcaSlicer out of the box, if not, than in Dev Mode. || They bought off another influencer 😢 || Well that was cheap! Lol a printer buys a guy who has a ton of them and give stuff away all the time? I’m still not a full blown bambu user. Just sharing what I discovered. Nothing more || so why didn't bambu labs design the own 5inch screen for the p1s etc || They did now. It’s the p2S. || Bigtree's animated LCD screen adds more mass to the A1's toolhead - that accelerates wear over the warrany period. The Panda Touch is not using an API that Bambu provided for devs, it's using a clever hack, that inevitably would be patched. I don't blame Bambu for locking them out, but I don't see why they need to lock out 3rd-party slicers. I think they could have developed the secured communications protocol to enable the laser cutting functionality while leaving the 3d printing alone. || I think you’re the first one that actually realizes that BTT is not using just an API authorized by Bambu. They’re also using as you stated, clever, hacks, and exploits to gain access. Obviously, if they were only using an API, there would be no patching and their device devices would just work. || So, then why didn’t they just make those changes for the H2D? || Maybe it was easier to make a blanket change versus just the H2d. Idk? || Короче Крупная фирма с своей экосистемой агрессивно ее навязывают, перекрывая доступ к любым сторонним улучшениям говоря нам: "Это для вашей безопасности". Ничто не ново под луной. || Big Tree did the expedient thing... "We're getting ours!" || so....you sold out? || No. I’m still not a bambu user. Wdym? I’m a prusa user just stating facts here to share with the community. || ​@stayreadyto3dprintk || Talking too much, saying little.
+Anyway, when Bambu decided to close its system, I didn't update my printers. I disconnected them from the internet and use them with a memory card. I don't mind. I started with an Ender 3 and I'm fine with it. What I am very clear about is that when they reach the end of their useful life, I will replace them with another brand. No more Bambu for me. || better to have the option than not. let people decide what security options to enable. no conspiracy about it. I'm looking elsewhere || I was almost tempted to pick up a Bambu just to see if it lives up to the hype. I'm so glad I went with my gut and decided it'd be more sensible to stick with Creality. I have to say it's disappointing that your video is awfully disingenuous when you're effectivly saying that if the manufacturer of your car makes it impossible to use after market  parts or modifications, the fault lies totally on the producers of the parts. Personally, if I bought a Toyota Corolla and for some dumb reason I want a chrome skull as a shifter knob, Toyota doesn't get to to veto my poor life choices. I really regret having purchased from your site. || Well Ferrari and big brands do it do it all the time. I never said I liked it. I was simply explaining why they did it and that if they truly did things for security reasons they I can see why and if it was to protect their customer I think it was the right move. Note if they had ill intentions then obviously I don’t agree with it. I’m sorry you regret purchasing from me just because our opinions don’t align. I’m more than happy to offer you a refund if you’d like to send back whatever it is you bought. Unlike other brands I actually care about my customers and I pride myself on excellent customer service. || It is a bunch of lies! (not you Bambu Labs) Bambu Labs had tons of sales for Christmas the year before last then right after the return window closed in the new year pushed out new terms of service quietly and new firmware that then required you to sign in to their cloud server but they got caught and it became a huge deal and they walked it back and made the lan mode thing AFTER they got caught. I was one of the ones burned by this crap. They set it up this way so that they can approve or disallow your prints. It may not currently be being used, but it was the ground work for it. The Biden White House and Alvin Bragg was also part of this because they where pushing 3D printer companies about 3d printed guns at the same time this happened. (Look up Alvin Bragg 3d print letter) They are still not done look at the 3d printer ban laws that are currently being proposed across the country. They are trying to pose it as a safety issue but it is really going to be about control and DRM on 3d printers.  The so called exploits were written into the firmware and were a feature until they needed to be able to control who used your printer and how. As other have said if it really was about security, local authentication using industry standards would have been far superior than trying to develop a whole new cloud system that now involved user name and password being sent across the internet and stored in databases in the cloud waiting to be compromised. || Yes, Biqu/BTT DID know the touch MIGHT be locked down, they released a specific video about it and that they were in talks with Bambu.  They was posted here on youtube and it does have the option to flash your Touch to a Klipper Touch IF it happened.  
+Bambu needs to be clear IF behind the scenes PARTNERED with BIQU after the talks between them happened about the Panda Touch.  BIQU somehow has more than 10x the amount of PANDA gear as it did before "talks" between them happened.  Just food for thought. || But once they found out stuff was going south they didn’t announce that part I don’t think. If they did I didn’t find it. Bambu told me that they gave them plenty of warning. About a year to be exact and they just kept selling products. To be fair they now have a disclaimer on their website. But they didn’t have it before. lol
+Nice to see you stopped by. Haven’t seen your vids lately bud. Idk if the algorithm just stopped showing me or if you’re not posting. Say hi to the misses. Hope you all ate doing well || Just bought 2 rolls of the tpu. Running a bbl p1s. Any idea on what profile would be best to run on it? It's gonna ask what filament type. I'm guessing generic tpu settings? || I wouldn’t use tpu settings. It’ll work but be a lot slower than it has to be. I would import the Prusa Flex profile. It works great. No changes needed. But I also recommend doing material calibrations for your specific machine. Thanks for the support by the way! || ​@stayreadyto3dprintI'm really new to the 3d printing world. Only had my machine about a month now. Don't know how i would import the settings you are talking about. Any help in that area would be greatly appreciated. And did i order a day too early to be entered in the drawing?! || @westsidecracker1nope you’re good to go. Anyone who orders will be entered. 
+As for the profile goes if you don’t know how. Just get prusa slicer and look at the flex profile and take photos. Then go to your slicer of choice and make the changes. Or join discord and I can get on and help you personally. Just tag me in the chat somewhere. https://mee6.xyz/i/4YMcjZjNO6 || ​@stayreadyto3dprintsounds good. Thanks for the help. This will be my first try with tpu. Hoping for the best! Lol || Try this link if the other one’s broken. https://discord.gg/ZGgcwk7eWt || First ever video of you that I've watched coz I was interested in buying a bambulab printer. And you were in my recommendeds. Well. Not anymore. I have NO idea what big tech is or does or did but what I DID notice is that you're tryna sweet talk us like they sweet talked you. They paid you off with a printer &amp; gift card first to sweeten you up, since you (apparently) dissed them after the in person interview at (wherever you were, which was really REALLy rude of that guy btw. I'd hate for someone to represent MY company like that!). .. anyway....... free printer, free filament, email worded to protect their company. I read other comments and have to agree. This is a paid ad for a company who's printer I'm no longer interested in. I guess I can thank you for that. I'll stick with the current brand I'm using. Stay offline and hope for the best 😂 || So the first video someone makes you don’t agree with they are shunned huh? lol can’t please everyone all the time. Impossible. But thanks for insinuating I have no morals and I’m a piece of shit bribe taker. Thats awesome. Nice to meet you too || At the end of the day, it comes down to this. If I don't control it (root) I don't OWN it. It's not mine and can be modified or taken away at any time by the manufacturer. This is an intolerable situation when I still am expected to pay full price. 
+If they want to provide me with the hardware and I only pay for filament, maybe. But probably not. Frankly, if Bambu decides to shut down or similar, you own a paperweight. And outside of replacing the control board, nothing you can do about it. This is why my X1C has X1Plus installed, and is completely blocked from the internet. And I can still monitor it, and my other printers, thanks to Octoanywhere. 
+My other issue with this, is that they modified the device AFTER THE SALE. I bought it knowing I could use various tools. They forced those tools to break. They can call it security, but there are other ways to secure things. Again, unreasonable. If they wanted to do it for new machines only, and were very clear about the change, fine. But that's not what happened.
+I think you are legit trying to be objective. This has a LOT of backstory that you aren't going to get from Bambu. As for BTT, they could be letting potential customers know about the issues a bit more clearly. But it's also not unreasonable for them to be irritated at Bambu.
+As a result, I don't recommend Bambu to people anymore. I used to suggest them to people all the time. It sucks, but I won't put my reputation on the line for backstabbers.
+As a programmer who has custom built printers and modified the software. There are better ways to handle security that would work and still allow users to use their printers. This, like most so-called safety restrictions are not about safety. They are about control. || Well put. Thanks for your insight. Also, we’re looking for people who can build printers because I think it’s high time we have a USA made printer with USA style customer service. So if you’re interested send us an email. || you got the shore hardness backwards bro. 95A is super flexible  and harder to print || lol def not. 95a is pretty stiff and if you print shoes with it you’ll see it sucks for shoes. 70a is much softer. As is 60a and so on and so forth. || So, you can only access the API via developer mode. However if your licenced you can use the API with out your user needing to use turn on developer. So they closed a 'bug/security'. TBF they allow you to roll firmware back, which seems ok. With that said, there is no reason to stop Bambu from 'pair' API's like alot of other software (looking at EvE Online API access) , so you only allow API's the customer has chosen. I think I am still on the fence for both companys. || I honestly don’t feel that BL has any ill intent in doing what they are doing. I truly believe they’re doing it to cover their own butts in case of an accident or something. || Love the explanation. I agree IF they had the heads up that's pretty slimey for them to roll the dice. Really wanna try the morph flex but it's first time I've seen it here...any samples or anything? 50$+ is a bit steep for me for something I haven't tested (no shade meant) || I wish we could afford to send out samples like these big companies. But if you go on my page, there’s a few videos that I posted of shoes that I printed. It prints flawlessly using the Prusa slicer flex profile. With the 20% off it comes out to around 40 bucks. It was 49. I dropped it down to 44 and added 20% off of that. || ​@stayreadyto3dprinthonestly it beats many of the other filaments of this style, think I'm gonna cop a roll! Ty sir || Ty as well || I'm with you, thats why i buy Bambu printers i'm tired of working on and modding then fixing, i just want to fill orders and keep my farm running || I used to enjoy modding my machines, but I’m just kind of over it I guess lol || I've never seen a video of yours. This would be the first. My general impression is that you're not very professional. || That would be correct. I’m just a guy who enjoys 3d printing and I make videos. I’m not a professional videographer. I provide my opinion on things and review machines and do giveaways when I can. Def not a professional at this. Just having fun and giving away as much stuff from brands that I can and always replying to comments unlike most YouTubers. Thanks for watching though. || BTT should certainly be transparent regarding on what firmware their devices function and in what modes.  From what I understand all of BTT's products that have been developed for bambu lab printers still function correctly on the latest firmware in developer mode.  Personally I own a p1s, and I run it in lan mode with developer mode enabled.  I keep my printer on my iot vlan and block external network access to all of my printers (the rest of the printers that I have run klipper (voron v2, voron v0, creality k1 max)) just like I do for the rest of the IOT devices that run on my network (because I don't trust anything these days to not phone home, and it limits remote attack surface). while still allowing me to do anything that a printer is capable of just by using an authorized computer on my network.  if someone wanted to access my printers and iot devices they would either have to gain access via the administrative vpn that I run (which would require my username, password, AND a key file (so reasonably unlikely) or they would have to be inside my house using one of the computers that i've authorized to talk to said devices OR i suppose they could manage to get on my user lan and then either hack my network switch or my firewall to allow access (pretty unlikely... i'm not that sweet of a target).  so even if I were to buy a network enabled laser machine (I honesly just might at some point), I trust that if I configured it that same as my printers network-wise that I'm pretty safe regarding the network security aspects.  but it should NOT be up to my device manufacturers to tell me that I can't use a device that I purchased and own with other equipment or software in any manner that I like.  THAT'S the part that I find obscene.  equipment that I own should be made to work in any manner that I see fit that is technically doable.  my klipper machines do exactly what they're told when they're told, my marlin machines (when I ran them) used to do the same (with a little help from some raspberry pis for wifi and frontend administration in that case), my bambu labs printer needs to do what I want when I want, and when it doesn't, I'll resell it and buy something new and tell everybody exactly why I did so.  it's NOT an exploit to use undocumented APIs to gather data end control a product if that's the owner's intent.  that's not a bug, that's a feature, and removing features (even untentional ones) because bambu simply doesn't want users to be able to inexpensively expand capabilities and undercut bambu's more expensive models doesn't mean that they should be able to get away with locking down their ecosystem.  at this point I don't care how well they work, I am *MUCH* happier with my creality k1 max than my p1s because of the direction bambu is going with their firmware. - with the k1 max, I can go right on the front panel and if I want (and only if I want) enable the root account of the computer that drives the thing and do literally anything that I want with the printer's underlying operating system... creality CLEARLY will not warrant any changes I choose to make, but they'll still honor the warranty of the hardware (assuming I didn't cause physical damage through modifying the software or hardware) and they'll still support me (so long as I didn't create the problem at hand via my modifications).  it enabled me to use shaketune (which is advanced belt tensioning and resonance compensation), KAMP so I can choose to do finer meshing in just the print area and have more control over purging as well, I can add various hardware and other software components, directly live stream from the printer if I want to, added a bunch of macros for various bits of calibration, etc.  does anyone have to do these things to enjoy their k1 max? no.  does is significantly add value to that machine for me and other hobbiests? absolutely!
+right now I'm mostly happy with my p1s in lan only + developer mode. it does mostly what I tell it to do. if they choose to remove or cripple that functionality, that'll be the day that I no longer own a bambu machine.  Prusa is a bit more open, but still pretty expensive for what you get... the core one is a nice printer but I can't stand factory unenclosed printers, and the enclosure design for the prusa xl is pretty terrible overall.  these closed printers are trouble though (bambu, elegoo centauri carbon, etc.)... I really wish more brands would just use klipper and call it a day. || Someone sounds like the got pissed off and then just complains and waffles back and forth. The point is lost somewhere. || Will maybe you can find it lol let me know if you do 😅 || This video blows MY mind... you obviously have zero knowledge about cybersecurity and what constitutes and exploit. At the very least try to understand what you're talking about and verify facts before making broad statements and reading Bambu's response word for word. You're getting played.  I hope to see a video in the future on your channel where you take an objective approach to this topic. Its a very serious issue especially with US States starting to introduce Bills that would force all of your prints to be scanned by AI and tracked forever. Off grid printing is about to become very important and this video helps push a dangerous narrative cloaked, per usual, as being for your safety when its really about control and influence. || I’m sure there will be more videos on this topic. This video was simply to ask Bambu questions and provide the community with their answers verbatim in order for people to form their own opinions. I’m not really taking sides. I also recently posted a video about what Washington lawmakers are doing, and trying to force printer companies to alter their software to scan for gun models. I don’t know if you saw that it’s in my short videos. || For the record, I do not agree with them trying to dictate what we can and can’t print, but thankfully printing off-line is an option and they can never ever control that || I'm like you.  I've been printing for years, and I've worked through my tinkering phase and I'm sick of it.  Now, I just want a printer that works.  Since I got my H2D in December, I've done lots of printing, and only one was less than perfect.  That one turned out to be a problem with the model and the designer's profile, not the printer.
+I bought the printer in full knowledge that it is a closed-source printer.  I would prefer open-source, but not one other commodity item in my house is open source.  My central heating, my microwave, my coffee maker, washing machine, TV, none of my music hardware like keyboards, effects pedals, electronic drums, none of my workshop tools, or my car, nothing.  Why do we demand our printers and only our printers are open source?  It's because until Bambu Labs came along, they weren't good enough.  We needed to mod them endlessly to get them to perform well.  Bambu Labs made the first printers that were good enough out of the box to get great prints.
+My only reservation is that, if a time comes when Bambu decide it's not economical to continue to support the product, that they should then open source the product.  I've spent a lot on this printer, I don't want to be left with a brick, or have to downgrade it in order to continue using it.  If by such a time they still have IP worth protecting, then they can open source most of the product, but continue to support the library containing their secret sauce.  Open source code can call the API for the library without knowing what magic it's doing.  If Bambu don't do this, and I am left with a useless printer, I will never buy from Bambu again, and I dare say most others would say the same, so it's in their own commercial interest to look after their customers. || Well said. I agree. I don’t think it will come to that though. || Exactly! || WTF is land mode? Its LAN mode... . || It’s a typo from the editors. Geez. 😅 || screw warranties, I'll take open source and physical ownership over warranty any day of the week. || Honestly, wtf security issue is a hardware device plugged into it? If you have physical access to a printer, what are they afraid of - stealing files from the onboard memory? They literally have a secure model of printer for this stuff. It should not apply to general consumer printers. This is seriously one of the reasons I am not buying Bambu for my first printer. I do not want to buy into a closed ecosystem. || wonder why it needs to connect to the internet at all.  Do you really believe that they wont shut down printing certain "models"  I prefer being able to print what i want without being monitored. || I do believe they are trying to shut down being able to print certain models. I recently posted a short video talking about this showing a US law maker talking about how doing that is basic common sense if you look at my recent videos, you’ll see it. For the record, I do not agree with that at all. || Bull. All they had to do was add a level of security to the “exploit “ so it could still be used by you and third party but secure it from those scary “hackers”. This is not about security. It’s about protecting their walled garden and their ability to stop you from using your machine how you want || Wait, so this whole video is basically saying "We have 100% irrefutable proof that BambuLabs was acting in bad faith and lied repeatedly, but trust me bro, they said it wasn't their fault it was BTT." That's a weird take. I hope the free machine was worth it lol. MQTT isn't an exploit. || It was actually me just sharing questions I asked bambu lab directly. To clear the air and all the misinformation out there from people who haven’t even spoken to a bambu lab rep. And to allow ppl to form their own opinion after that based on remarks from bambu themselves. That’s all. || For me, this clarifies nothing. I'm still not buying it. Bambu Lab have offered NO assurance that they won't remove developer mode at a later date. Then we're into things like loss of our IP and having to pay a subscription to use our own hardware! This whole issue of trust (because we don't trust them) could have been avoided if they had put ethernet ports on their H series machines and made the use of the Laser LAN mode only. Personally I'm still a bit pissed that a simple ethernet port is still missing from nearly all of their machines.  Thanks for trying on our behalf. I still believe that we are the ones being exploited though. || Hey I tried. I just wanted to get some questions answered directly from Bambu because I know a lot of people, including myself or relying on information from other people on the Internet and even I was wrong on some of it. || Just got into this hobby and am finding more and more how much I dislike Bambu and am glad I didn't go with them. That interview bullshit just sealed the deal with me. But it's good to see Bambu can fight negative press one free machine at a time.. I guess. || Just bought a roll of the TPU. || Nice!!! You will love it. The best starting point for a profile is Prusa’s flex profile. It prints MorphX perfectly. || Just to be clear here, they only restrict API touch functions of these panda screens right?
+My panda knomi will still work? || It all depends on what firmware you are running, and if that firmware is blocking key things, your device needs to function. From what I was told basically at any point if they find a Security reason to patch it, they will do so without warning. But they aren’t doing it just to render those devices useless they would only do that if needed for security reasons so it’s kind of up in the air I guess. || ​@stayreadyto3dprintoh I thought that it was safe because it's just displays information and it doesn't have any input/ touch screen like the regular knomi v2 || @anthonyrossetti7509it may be. I’m not 100% sure what allows it to function tbh. || Ok so what is driving the dropping creality? || Coming soon. They suck that’s why. Lol and they treated us pretty shitty. Details coming soon. Plus they aren’t innovating. They keep coming out with machines, basically changing a few things and </t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
+          <t>UCXS90ukmtQo2kg3Ydf-cj3A</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>itsbasicbible</t>
+          <t>Stay Ready To 3D Print</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>6NPZ9oRrofc</t>
+          <t>OReSdBUIe3A</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Breaking the Internal Battles Holding You Back as a Man</t>
+          <t>Is 3D Printing About To Take a Dive?</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Overcoming Internal Battles: Rebuilding Identity through Scripture
-In this episode of Basic Bible, we explore how most men are held back not by external factors but by internal battles such as fear, insecurity, and confusion about their identity and purpose. The video delves into Biblical guidance to help men overcome these struggles by rebuilding their identity and reshaping their thinking. Key scriptures from 2 Timothy 1:7 and Ephesians 2:10 are discussed to highlight that fear, insecurity, and confusion are not from God. Practical steps are provided to identify and replace lies with Biblical truths, act from identity rather than emotions, and understand that transformation is a continuous process. The video encourages men to immerse themselves in the Word of God, surround themselves with like-minded individuals, and consistently act from the identity that God has given them. Viewers are invited to engage by commenting with the word 'identity' and subscribing for more content focused on building men with purpose and impact.
-00:00 Introduction: The Hidden Battles Men Face
-00:40 Understanding Internal Struggles
-01:28 Biblical Insights on Identity and Fear
-04:51 Practical Steps to Overcome Internal Battles
-06:43 The Process of Transformation
-08:45 Encouragement and Call to Action
-Connect 
-https://linktr.ee/itsbasicbible
-MALTA APPAREL LINK 
-https://malta-apparel.com/?ref=BBAZ16 
-FOR 15% OFF: basicbible15 
-FREE 10 DAY DEVO BOOK 
-https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
-I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
-https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
-I WANT TO FOLLOW JESUS CHRIST
-https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
-Get vidIQ to grow your channel faster! 🚀
-https://vidiq.com/itsbasicbible</t>
+          <t>Lawmakers are trying to invade makers privacy and dictate what we can and cannot 3-D print on a machine that we bought and paid for in a home that we own as a free American. 
+Make it illegal, but you don’t get to install software that spies on me. 
+What’s next? Will they install cameras in our house to make sure we’re not committing a crime?</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>2025-12-27T00:00:14Z</t>
+          <t>2026-01-23T22:37:10Z</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>1293</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>46</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>21</t>
         </is>
       </c>
       <c r="J4" t="n">
-        <v>0.1</v>
+        <v>0.051817</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -824,73 +802,69 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>Most men are not being held back by their circumstances. Instead, they are being held back by the internal battles that no one else can see, such as fear, insecurity, doubt, overthinking, and just confusion about who they are and what they're called to do. And the dangerous part is this is that you can look fine on the outside, but quietly lose the battle on the inside. And today I want to take a moment and share why these internal battles exist and how scripture shows us as men the way out. Because freedom doesn't start with changing your environment. It begins by rebuilding your identity and reshaping your thinking. You see, most men think that the problem is really this. a lack of opportunity, a lack of money, maybe even a lack of clarity, or maybe a lack of direction and all these different things. But the Bible really shows us something deeper and different than what the world likes to communicate. See, the real internal battles are this: fear of failure, fear of people, insecurity, comparison, shame, and just confusion about who you are. You can have the talent and still be paralyzed. You can have opportunity and still hesitate. And you can even have the calling and still shrink back in fear because you don't know who you're called to be. Why is that? Because identity precedes action. And if your identity is shaky, your decisions will be shaky as well. I believe Paul tells Timothy something that every man should hear. In 2 Timothy chapter 1 verse 7, it says this, "For God has not given us a spirit of fear and timidity, but of power, love, and self-discipline." Let's break this down real quick. Fear is not from God. Insecurity is not from God. And chronic confusion is not from God. That means if fear is dominating your decisions and your thought life, it didn't come from heaven. You see, fear attacks your confidence. It attacks your obedience. It attacks your identity. It attacks your courage and your leadership and just who you are as a man. And here's the truth. Most men don't even realize they're battling fear. Fear doesn't usually tell you to stop. It tells you to delay. It tells you, "Wait a little longer. Get more ready. Make sure everything is perfect. Don't move yet. And what if I fail?" That's how men stay stuck for years. And I'm sure you've met men like that who said they're going to accomplish or pursue this vision or pursue this woman or build this, but then two years later, three years later, or even six months later, they're still in the same exact spot as they were before. Why is that? Is because fear kills more dreams than failure. And insecurity is an identity issue, not a personality issue, to be honest. And a lot of men like to say this type of stuff. I'm not an insecure person. No, insecurity is not your personality. It's a symptom of misplaced identity. It's a symptom of not knowing who you are in Christ. Because when you don't know who you are, you look to others for validation. You start comparing your life to other people. You start secondguessing your decisions and you let fear drive your decisions. You let fear make you avoid responsibility because insecurity thrives where identity is unclear. And Satan doesn't need to destroy a man. He just needs to keep him unsure of who he is. Because if a man is unsure of who he is, he is unsure on how he is supposed to be on what he is supposed to do and how he's supposed to change the world around him. Because your true identity is actually defined by God. Because here's what the Bible says in Ephesians chapter 2 verse 10. It says this, "For we are God's masterpiece. He has created us a new in Christ Jesus so we can do the good things he had planned for us long ago. I love that verse. God has planned amazing things long ago for us to accomplish. And here's what this Bible verse says. It gives us three clear things that we should look at. First, it says we are God's workmanship. That means we are not an accident. We are not a mistake. And you are not random. You were actually intentionally formed by God, by the creator to do good things. Number two, it says that you were created with a purpose. Your life has an assignment attached to it. And then here's the third thing I want you to catch. That God already prepared good works for you to do. You're not trying to invent your purpose. You're not trying to invent your calling. Instead, you're trying to discover what God has already planned for you to do. When identity is restored, direction begins to follow. That's amazing because the internal battles is the thing that's keeping you stuck. And honestly, here's how we actually conquer the internal battles that we're facing. Let me break this down practically to give you step by step so that you can ensure that you're walking with success. Step one, identify the lies that you're believing. Ask yourself this one thing. What am I afraid of? What am I afraid to do? Why do I keep telling myself this? Why am I keep telling myself that I'm not going to do that yet or that hey, not yet. This is not the right time. Also, where did this belief come from? Because most internal battles are fueled by lies we never challenge with the word of God. Number two, replace the lies with godly truth because truth will always dismantle fear. When scripture becomes your reference point, your mind begins to stabilize. That's where clarity begins. That's where vision begins. That's where the dreams begin. And you know what? That's where clarity about who you are begins. You don't fight lies with your willpower or just saying, "I'm going to stop thinking about this." No, you fight the lies by replacing it with biblical truth. Then the third thing is this. Are you ready for this one? Act from identity, not from your emotions. Because confidence isn't a feeling. It's actually a decision that you decide to make. Men grow when they act from who they are from God and who God says they are, not how they feel in the moment. A man who acts on their feelings is not a mature man at all. Because the saying that says decisions lead and feelings follow is so true. Instead, a lot of men let their feelings lead and then they let their decisions follow. Instead, be the man that decides that you're going to be this person. Decide that you're going to take action. Decide that you're going to pursue this transformation. decide that you're going to be the man that God has called you to be because all action is rooted in identity and that weakens fear and insecurity over time. And here's the other thing I want you to catch real quick, right? Is that transformation is actually a process is not a moment. And see, yes, when you become a follower of Christ, things begin to break. Your flesh begins to die and you get a new identity in Christ. Yes, those things happen in a moment, but your sanctification on who you're supposed to be and the person that God has called you to be takes time to build out. And you see, the internal battles don't just disappear overnight. Think about it like this. Let's say you just began following the Lord 10 years ago, and now you're 30. You have 20 years of junk, 20 years of the world's influence on your life. So, a course is going to take time for God to pull up all these weeds. A course is going to take time for God to reconstruct your life, to restructure your mind, to restructure your heart and your vision and who you are. So don't get upset that you're not far enough down the road as you thought you were. Instead, look to Christ. Look to him for your direction. Look for him to your scorecard. Let him be the compass on where you should go. Because if not, you're going to let your comparison, you're going to let everything else of what the world is telling you should be instead of who God has called you to be. And every time you choose truth over fear, truth over insecurity, or obedience over comfort, and decisions over feeling, and identity over your false insecurity, you grow stronger because men don't become confident overnight. They become confident by consistently acting from the identity that God has given them. They become courageous overnight from the identity that God is telling them who they are in this word. That's why guys, you can't let the world around you stop you from getting in the word. You have to let the word of God filter everything that you do. Your identity has to come from this word. And guys, truthfully, one of the reasons why you probably still have some immature things in your life, immature emotions and mindset, it's because you're not letting the word of God mature you. you're not applying the word of God and you're not surrounding yourself with other godly men who are pursuing the purpose that God has for them. So, here's my encouragement for you as we begin to close. If you've been battling fear, insecurity, or confusion, you're not weak. You're not broken. And you're not behind in life. You're just in the middle of your transformation. You're right in the middle of where you were and where you want to go. You're just right there. And I want you to know that God wants to rebuild your identity. He wants to renew your mind. He wants you to stand on truth. And he wants you to pursue the purpose that God has for you because those internal battles will no longer control you whenever you begin to submit yourself to God. Whenever you get to surrender yourself to God and say, "God, here I am. I want to be the man that you have called me to be." If this message spoke to you, if this message challenged you, I want you to go in the comment section and type in the word identity because I want to pray for you and I want to see how God is moving in your life. And also, if this video encouraged you and helped you take that next step, consider subscribing or even sharing this video with other people because on Basic Bible, I'm committed to building men with purpose and impact. So guys, see y'all next time. I love y'all. Peace.</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr"/>
+          <t>Well, this is going to blow your mind. And honestly, I can't believe this is where we're at in life. But check this out. &gt;&gt; I'm proposing the first in the nation law requiring all 3D printers sold in the state of New York to include software that blocks the printer from creating a gun. It's just common sense. Just common sense. &gt;&gt; Common sense. It's funny they mentioned that. So, if you're using common sense, common sense would say to go after the real guns that's had millions of cases in the past 5 years versus 3D printed weapons that's had in the hundreds in the past 5 years. I mean, come on. Do you really think that criminals are going to buy a 3D printer, sitting down, taking the time to learn the software, figure out how to 3D print, how to get a print to come out good, and do all of that to get a 3D printed weapon when they could just go on the street and buy a weapon on the black market or steal one or do whatever they do to get unregistered firearms or illegal weapons, whatever it is. So, this stuff about 3D printed weapons and all that, they're they're going after this. To me, that is not common sense. To me, there there's an underlying agenda here, and I'm pretty sure you guys can see through it. So, what do you think about this? Do you think they should continue to do this and basically invade our privacy by watching our 3D printers and dictating what we can 3D</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>How would ai even be able to correctly identify a part and what it’s intended for? BTW I support gun restrictions, but this is just Looney Tunes. || Yeah I agree. || Open source software/hardware wins again || Yup. They can’t stop
+That. It’s a waste of time. We all know that. All smoke and mirrors || GOP is proposing a bill to fine women $17 thousand dollars if they aren’t married by 30 years of age. || Oh nice. How about that. LOL || I'd outlaw home depot selling pipe bomb components... Idiots || Why not just outlaw installing those components (a.k.a water pipes) into any politician's home? They would surely enjoy the pre-industrial lifestyle without running water. || Yesh what about that? Geez. || Umm. Yeah. And how are you going to identify that....
+And this is what you're going for? Oh dear gods. || Right? How will they? By invading our privacy is how. Ugh || Look, I'm not in favor of 3D printing guns, and I'm no 2A advocate, but I am a certified drafter, and I worked 20 years in silicon Valley, and I have NO IDEA how this "software" could be written. 
+I don't think it's possible. || I think if they do it’s way more to do with spying on citizens of interest versus caring about guns. || hi Lawrence why was my comment taken down ? Or not showing up cheers mate || Yeah I do not know. I didn’t do it. Probably YouTube pushing a narrative or blocking one. 😝 || @debraSam2012strange. Not surprised || Its LEGAL for american citizens to manufacture their own firearms for personal use without an FFL. It's the states that are illegally taking their rights away.
+But what if they sell it? Theres already a law for that.
+But what if a falon makes a gun? Theres already a law for that.
+What if its used in a crime? ..... really?.... || Exactly. Make a law. If they break it lock them up. Simple. But they don’t get to dictate what a machine we bought does or doesn’t do. Thats bs. || I was just watching videos about it so dumb || Crazy huh? What do you think will happen ? || Knowing the way things are they'll probably do it but i hope not</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
+          <t>UCXS90ukmtQo2kg3Ydf-cj3A</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>itsbasicbible</t>
+          <t>Stay Ready To 3D Print</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>GmcHfaQ_C7s</t>
+          <t>5ipo5Vlc7tU</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>If you want to hear God clearly watch this</t>
+          <t>My Fav’s From CES 2026 #3dprinter #tech #ces #laser @xToollaser</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Hearing God's Voice: Silencing the Noise for Clarity
-In this episode, we delve into the struggles many face in hearing God's voice clearly. Contrary to popular belief, it's not about God not speaking, but rather about the challenge of silencing other distracting voices such as fear, doubt, and overthinking. The scripture reveals that God's voice leads us into stillness and clarity, contrasting the noise from the world. Jesus described that believers can hear His voice naturally, underscoring that confusion is not the norm. It's emphasized that a clear mind, aligned with God's word, is necessary to recognize His guidance. Transforming our minds through scripture and prayer is crucial for hearing God's direction. The importance of obeying what God has already spoken is highlighted as a step towards clarity. Viewers are encouraged to silence the worldly noise and realign themselves with God's word for a clearer connection. This episode serves as an invitation to return to scripture, prayer, and obedience for divine clarity.
-Connect 
-https://linktr.ee/itsbasicbible
-MALTA APPAREL LINK 
-https://malta-apparel.com/?ref=BBAZ16 
-FOR 15% OFF: basicbible15 
-FREE 10 DAY DEVO BOOK 
-https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
-I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
-https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
-I WANT TO FOLLOW JESUS CHRIST
-https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
-Get vidIQ to grow your channel faster! 🚀
-https://vidiq.com/itsbasicbible</t>
+          <t>I went to the world’s largest tech event, CES 2026 in Las Vegas where I found some of the newest tech to come in the 3d printing world in 2026. Enjoy!!!</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>2025-12-23T00:00:31Z</t>
+          <t>2026-01-15T20:02:50Z</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>1859</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>63</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J5" t="n">
-        <v>0.07142900000000001</v>
+        <v>0.036041</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -899,590 +873,527 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>If you want to hear God's voice more clearly, listen to this. Most men are not struggling to hear from God. They're actually struggling to silence all the other voices that are not from him, such as fear, doubt, overthinking, pressure, people pleasing, and other people's opinions. And when everything else is loud, clarity disappears. Here's what scripture shows us. That God's voice doesn't compete with other noise. It actually leads us into stillness. That's why Jesus said, "My sheep hear my voice." That means hearing God is normal for believers. Confusion and lack of clarity is not. The real issue isn't that God stops speaking. It's that your minds have been crowded with noise. It's been crowded with the world static instead of tuning your ears to what God says. That's why the Bible says that we're transformed by the renewing of our mind. Because if your mind isn't aligned, even when God speaks, you won't be able to recognize it. Let me say this more clearly. If your Bible is closed, clarity will not be there. God is not hiding direction from you. He's actually inviting you back into alignment. So, silence the noise, create the space, and return to scripture and prayer. And also obey the last thing God already told you to do because clarity doesn't come from overthinking. It comes from aligning your life and your mind with God's</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr"/>
+          <t>Here's some of the coolest things that I found at CES 2026, [music] like this circuit board printer. It prints a conductive liquid directly on the PCB board. Very cool. [music] But check out this metal 3D printer. It takes liquid cartridges and turns it into hard metal. Depending on which cartridge you put into it, whether it be aluminum, copper, steel, nickel, and as you can see, it can print intricate designs. But check out how you load this thing. I've never seen one like [music] this. It takes these liquid filled syringes full of liquid metal, and you just simply load it up and go. Now, I did a video on this one already, but this is the Atom Form Pallet 300 made by MOA. It's a 12 nozzle changer with [music] 36 colors. Pretty cool, and it's coming soon. Now, this isn't a printer. This is a software [music] from AF Research where they basically took machine learning and jammed it into a printer. It takes a $5 webcam and some high-tech software where it can basically [music] teach itself how to print quality prints from nothing. So, no more programming filament profiles. XL had a humongous booth. This is their apparel printer. It's a DTF printer that prints on [music] these plastic films here and it prints super vibrant color and then you just hit it with a heat press. But they're really known for their lasers and they brought [music] the F2 Ultra again with the rotary attachment and the passer attachment on the UV model. Now, the UV model is the one that can actually laser inside of crystal blocks and do the glass and [music] clear stuff. It's really nice, and so is the M1 Ultra. It's not brand new, but it's [music] still awesome. It's a laser that actually has a inkjet printer built into it that can print on top of the wood, which [music] creates endless possibilities. But this one was the talk of the show. This is their all-new UV additive printer. Unlike a UV laser that subtracts [music] material, this one adds material and it's full color. I mean, it looks absolutely wonderful. All of these were done on the new machine, and [music] I can't wait for it to launch. Then we have Create, who brought the Create High and disguised it as the allnew Sparks i7 and kind of made a new CFS. And I don't know, but the Falcon team is still on my good side because they're actually innovating and making new products. [music] And this is the allnew T1 5 in1 laser. And this is the Falcon A1C 20 watt desktop.</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>Liquid metal? This is T2 stuff. || That metal 3d printer is sweet || It’s like 30k though ughhhhh😢 || Dang ​@stayreadyto3dprint</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
+          <t>UCXS90ukmtQo2kg3Ydf-cj3A</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>itsbasicbible</t>
+          <t>Stay Ready To 3D Print</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>BHpr16JbyqY</t>
+          <t>Lwi_rKRQx54</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Hearing God Clearly in EVERY LIFE SEASON</t>
+          <t>Uniformation GK3 PRO Printer Giveaway! 1/11/26 @6  pm CST</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>How to Clearly Hear God's Voice in Confusing Times | Christian Guidance
-Most men are not struggling to hear God's voice; they're struggling to silence all the voices that are not from Him. If you feel confused, stuck, or unsure, this video is for you. Discover how hearing God is normal for believers, as Jesus says in John 10:27, 'My sheep listen to my voice.' Learn the importance of aligning your mind to God's Word from Romans 12:2, and understand the three primary ways God speaks: through His Word, His Holy Spirit, and through patterns and confirmations. This video emphasizes the necessity of reading scripture, the harmony between the Spirit and the Word, and recognizing God's voice amidst life's chaos. Practical steps include silencing distractions, saturating your mind with scripture, and obeying the last instruction from God. Tune in to realign your focus, deepen your faith, and hear God's voice more clearly.
-00:00 Introduction: Struggling to Hear God's Voice
-00:28 Understanding the Noise: Identifying Distractions
-00:52 Biblical Clarity: Hearing God is Normal
-01:45 Transforming Your Mind: Aligning with God's Voice
-03:06 Primary Ways God Speaks: Word, Spirit, and Patterns
-09:08 Practical Steps: Silencing the Noise and Seeking Clarity
-11:12 Conclusion: Realigning and Obeying God's Voice
-Connect 
-https://linktr.ee/itsbasicbible
-MALTA APPAREL LINK 
-https://malta-apparel.com/?ref=BBAZ16 
-FOR 15% OFF: basicbible15 
-FREE 10 DAY DEVO BOOK 
-https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
-I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
-https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
-I WANT TO FOLLOW JESUS CHRIST
-https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
-Get vidIQ to grow your channel faster! 🚀
-https://vidiq.com/itsbasicbible</t>
+          <t>FILL THE FORM HERE
+https://forms.gle/7BDED7YRwbos1wwdA
+https://uniformation3d.com/
+follow on instagram here
+https://www.instagram.com/uniformation3dprinter?utm_source=ig_web_button_share_sheet&amp;igsh=ZDNlZDc0MzIxNw==
+Stay Ready To 3D Print Instagram
+www.instagram.com/stayreadyto3dprint
+Check out the NEW AXI Pro here
+https://em-smart.com/?gad_source=1&amp;gad_campaignid=23334198655&amp;gbraid=0AAAABBeSBMzBKNbys7Q5YRsV_Mx_DoqiQ&amp;gclid=CjwKCAiAjojLBhAlEiwAcjhrDmiUXCBi4unFPA7GTY3ovx0MtKBwaBHXN3y40NVDE3SR-j0xSN-WAxoC69wQAvD_BwE
+Thanks for watching! If you're into 3D printing, whether it’s tuning your slicer settings, upgrading your Creality, Bambu Lab, or Elegoo printer, or experimenting with TPU, PLA, PETG, or custom filaments, you’ll feel right at home here.
+Join our Discord server to connect with one of the most active and supportive 3D printing communities online. We share printer mods, filament reviews, print profiles, and behind-the-scenes looks at our latest projects — plus, we run regular giveaways, offer support, and drop early news on upcoming content.
+Stay ready, stay printing — and be sure to check out our latest builds and experiments using today’s top 3D printer brands and materials.
+Join Discord here!  https://discord.gg/E5gPc8C2cs
+🌐 **Facebook Page**  
+📘 https://www.facebook.com/profile.php?id=61565872940311
+👥 **Facebook Group – “Stay Ready To 3D Print”**  
+📘 https://www.facebook.com/share/g/196GC85xxo/?mibextid=wwXIfr  
+📸 **Instagram**  
+https://www.instagram.com/@stayreadyto3dprint
+🎵 **TikTok**  
+https://www.tiktok.com/@stayreadyto3dprint
+🎁 **Patreon** – Get early access &amp; exclusive content  
+https://www.patreon.com/stayreadyfans
+📬 **Business inquiries / sponsorships**  
+Email: stayreadychat@gmail.com</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>2025-12-20T00:00:13Z</t>
+          <t>2026-01-12T13:10:43Z</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>280</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>28</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J6" t="n">
-        <v>0.391304</v>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>❤    SO   GOOD  👍 
-         AMEN     ❤ || 🙏🙏 || Thank you ❤ || Welcome, God bless 🙏 || You’re welcome 🙏</t>
-        </is>
-      </c>
+        <v>0.1</v>
+      </c>
+      <c r="M6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
+          <t>UCXS90ukmtQo2kg3Ydf-cj3A</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>itsbasicbible</t>
+          <t>Stay Ready To 3D Print</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>GJVnq2MdWOk</t>
+          <t>Vk2MosCyQdM</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Your Purpose Has Been Waiting | Are You Ready to Receive It?</t>
+          <t>Uniformation 3D Printer Live Giveaway! 1/10/26 11pm CST</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>God's New Vision for Your Life: Embracing Change and Growth
-In this video, explore how God wants to transform your life by replacing old mindsets and beliefs with new visions and callings. The speaker delves into the biblical parable of new wine in old wineskins to illustrate the importance of embracing change in our spiritual journey. Discover how to let go of past hurts, addictions, and limited beliefs that hinder you from fulfilling your divine purpose. Learn about the significance of living with purpose, the enemy's tactics to keep you stagnant, and how true growth often involves enduring growing pains. Tune in to find out more about the upcoming Purpose and Calling Breakthrough Virtual Masterclass on December 20th, designed to help you gain clarity and confidence in your purpose for 2026.
-00:00 Introduction: God's Message for You
-00:23 Jesus and the Parable of the Wineskins
-01:17 Embracing New Beginnings
-02:03 Identifying and Letting Go of Old Patterns
-03:10 Invitation to Purpose and Call Breakthrough Masterclass
-03:57 The Enemy's Tactics to Keep You Stagnant
-05:38 The Importance of Growth and Overcoming Comfort
-06:40 Living with Purpose and Making Decisions
-12:37 Finding Purpose Through God's Word
-13:58 Conclusion and Final Invitation
-DECEMBER 20TH MASTERCLASS FORM
-https://srm.fishflow.app/widget/form/zvB4lA8lrQrYiavw5zKR
-Connect 
-https://linktr.ee/itsbasicbible
-MALTA APPAREL LINK 
-https://malta-apparel.com/?ref=BBAZ16 
-FOR 15% OFF: basicbible15 
-FREE 10 DAY DEVO BOOK 
-https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
-I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
-https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
-I WANT TO FOLLOW JESUS CHRIST
-https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
-Get vidIQ to grow your channel faster! 🚀
-https://vidiq.com/itsbasicbible</t>
+          <t>https://uniformation3d.com/
+follow on instagram here
+https://www.instagram.com/uniformation3dprinter?utm_source=ig_web_button_share_sheet&amp;igsh=ZDNlZDc0MzIxNw==
+check out the new AXI Pro here
+https://em-smart.com/?gad_source=1&amp;gad_campaignid=23334198655&amp;gbraid=0AAAABBeSBMzBKNbys7Q5YRsV_Mx_DoqiQ&amp;gclid=CjwKCAiAjojLBhAlEiwAcjhrDmiUXCBi4unFPA7GTY3ovx0MtKBwaBHXN3y40NVDE3SR-j0xSN-WAxoC69wQAvD_BwE
+GOOGLE FORM LINK WILL BE POSTED IN THE CHAT! TO ENTER GIVEAWAYS
+Thanks for watching! If you're into 3D printing, whether it’s tuning your slicer settings, upgrading your Creality, Bambu Lab, or Elegoo printer, or experimenting with TPU, PLA, PETG, or custom filaments, you’ll feel right at home here.
+Join our Discord server to connect with one of the most active and supportive 3D printing communities online. We share printer mods, filament reviews, print profiles, and behind-the-scenes looks at our latest projects — plus, we run regular giveaways, offer support, and drop early news on upcoming content.
+Stay ready, stay printing — and be sure to check out our latest builds and experiments using today’s top 3D printer brands and materials.
+Join Discord here!  https://discord.gg/E5gPc8C2cs
+🌐 **Facebook Page**  
+📘 https://www.facebook.com/profile.php?id=61565872940311
+👥 **Facebook Group – “Stay Ready To 3D Print”**  
+📘 https://www.facebook.com/share/g/196GC85xxo/?mibextid=wwXIfr  
+📸 **Instagram**  
+https://www.instagram.com/@stayreadyto3dprint
+🎵 **TikTok**  
+https://www.tiktok.com/@stayreadyto3dprint
+🎁 **Patreon** – Get early access &amp; exclusive content  
+https://www.patreon.com/stayreadyfans
+📬 **Business inquiries / sponsorships**  
+Email: stayreadychat@gmail.com</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>2025-12-13T00:00:21Z</t>
+          <t>2026-01-11T18:57:46Z</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>240</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>35</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J7" t="n">
-        <v>0.08695700000000001</v>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>❤   Amen  🙏 
-        It is not the  mountain 
-        we  conquer, but 
-        ourselves.   ❤</t>
-        </is>
-      </c>
+        <v>0.145833</v>
+      </c>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
+          <t>UCXS90ukmtQo2kg3Ydf-cj3A</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>itsbasicbible</t>
+          <t>Stay Ready To 3D Print</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>WEm0xvO7HDk</t>
+          <t>P3ik_UAA9u4</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Your Phone Is Destroying Your Focus (And You Don't Even Know It)</t>
+          <t>Live at CES 2026!</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>The digital age is influencing our lives more than we realize. How often is the device in your hand (smartphone) dictating your thoughts and values? Jesus warns us in Matthew 6:22-23 that "The eye is the lamp of the body." Our eyes and ears are the literal doorways to our soul (mind, heart, and emotions), and they ultimately determine the course of our life (Proverbs 4:23).
-In this powerful Christian message, we uncover the spiritual danger of distraction. Christ demands your singularity, your focus, and your undivided attention. He doesn't want to compete with Spotify artists, Instagram influencers, or Netflix. You are constantly being discipled—will you allow Christ or Culture to shape your worldview?
-We explore the profound Jewish teaching, "May you be covered in the dust of your rabbi," to understand what it means to be a truly committed disciple of Jesus. This requires us to let the Bible be our filter and the only lens by which we see the world, rather than adopting worldly ideologies. Discover the specific unholy influences (social media, music, movies) Jesus wants you to let go of to clean your soul, become His uncompromised witness, and fully step into your true purpose and calling as a man or woman of God. Learn how guarding your heart brings clarity to God's vision for your future.
-00:00 Introduction: The Power of Digital Influence
-00:53 The Spiritual Impact of What We Consume
-02:07 Guarding Your Heart and Mind
-04:37 Choosing Between Christ and Culture
-05:55 Walking Closely with Jesus
-06:39 Practical Steps to Purity
-09:31 Living as a Witness for Christ
-10:34 Conclusion and Prayer
-12:32 Final Thoughts and Resources
-Connect 
-https://linktr.ee/itsbasicbible
-MALTA APPAREL LINK 
-https://malta-apparel.com/?ref=BBAZ16 
-FOR 15% OFF: basicbible15 
-FREE 10 DAY DEVO BOOK 
-https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
-I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
-https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
-I WANT TO FOLLOW JESUS CHRIST
-https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
-Get vidIQ to grow your channel faster! 🚀
-https://vidiq.com/itsbasicbible</t>
+          <t>Check out the all new AXI Pro from EM Smart,  it’s coming soon, so don’t miss out 
+￼www.em-smart.com 
+Thanks for watching! If you're into 3D printing, whether it’s tuning your slicer settings, upgrading your Creality, Bambu Lab, or Elegoo printer, or experimenting with TPU, PLA, PETG, or custom filaments, you’ll feel right at home here.
+Join our Discord server to connect with one of the most active and supportive 3D printing communities online. We share printer mods, filament reviews, print profiles, and behind-the-scenes looks at our latest projects — plus, we run regular giveaways, offer support, and drop early news on upcoming content.
+Stay ready, stay printing — and be sure to check out our latest builds and experiments using today’s top 3D printer brands and materials.
+Join Discord here!  https://discord.gg/E5gPc8C2cs
+🌐 **Facebook Page**  
+📘 https://www.facebook.com/profile.php?id=61565872940311
+👥 **Facebook Group – “Stay Ready To 3D Print”**  
+📘 https://www.facebook.com/share/g/196GC85xxo/?mibextid=wwXIfr  
+📸 **Instagram**  
+https://www.instagram.com/@stayreadyto3dprint
+🎵 **TikTok**  
+https://www.tiktok.com/@stayreadyto3dprint
+🎁 **Patreon** – Get early access &amp; exclusive content  
+https://www.patreon.com/stayreadyfans
+📬 **Business inquiries / sponsorships**  
+Email: stayreadychat@gmail.com</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>2025-12-06T00:00:43Z</t>
+          <t>2026-01-09T23:55:44Z</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>290</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>14</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J8" t="n">
-        <v>0.185185</v>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>❤     God   Bless   you    ❤ || God bless you 🙏</t>
-        </is>
-      </c>
+        <v>0.048276</v>
+      </c>
+      <c r="M8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
+          <t>UCXS90ukmtQo2kg3Ydf-cj3A</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>itsbasicbible</t>
+          <t>Stay Ready To 3D Print</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>7E57K6D-ztc</t>
+          <t>xzJKWf8-hKQ</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Your BREAKTHROUGH Is Around The Corner‼️</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Hope is NOT A STRATEGY precise action is. Don’t be the person that waits. Begin now, because your purpose can’t wait on you. The people you’re called to influence and impact can’t wait they need what you only have. Trust God and move 
-Your Procrastination is the enemy to your breakthrough 
-Comment and I’ll personal message you 🤙</t>
-        </is>
-      </c>
+          <t>The Atomform Palette 300 Is Almost Here! #3dprinter #3dprinting #ces2026 #ces</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr">
         <is>
-          <t>2025-12-05T21:44:07Z</t>
+          <t>2026-01-09T04:52:40Z</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>553</t>
+          <t>11589</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>365</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>66</t>
         </is>
       </c>
       <c r="J9" t="n">
-        <v>0.016275</v>
+        <v>0.03719</v>
       </c>
       <c r="M9" t="inlineStr">
         <is>
-          <t>Hope is NOT A STRATEGY precise action is. Don’t be the person that waits. Begin now, because your purpose can’t wait on you. The people you’re called to influence and impact can’t wait they need what you only have. Trust God and move 
-Your Procrastination is the enemy to your breakthrough 
-Comment and I’ll personal message you 🤙 || Amen God bless u || Thanks for the comment! I would love to have the conversation with you. Please email me so we can begin! Itsbasicbible@gmail.com</t>
+          <t>Show me just ONE shot of it actually printing and I'll place a deposit! Well no? So Atomform, that's how you ruin your business ... || Be patient. Don’t buy it now. Wait till it’s released and full price if you’re unsure. || @stayreadyto3dprintall I want to know is if this is real! Prices are out as far as I know, starting at 999 for the solo machine all the way up to about 1800 for the fully configured combo. But they never showed an actual working machine or even a prototype which seems a bit fishy… || I saw AI and a login menu, so it's not open source? || I’m not sure. I should’ve asked. Dang. || Ive been following this for a while and pretty excited to see it running. || Same
+Here || Can you say "amazing" any fucking more ? I dont see it printing or doing shit. This is a cash grab || Again, I have yet to see this thing run in action. || while I'm subscribing to 'updates' on their website, Imma go ahead and order a few more Bambu printers. They work juss fine. || Great idea lol || An AI assistant that will eventually not allow you to print a thousands of files || Let’s hope not. lol || Is the belt 2mm? It’s dealbreaking. VFAs will be dramatic. || You mean like 10 mm... and yes, I agree with you. My SVO8 has 5.7 mm belts and it is horrible with the VFA's || @treyduval5399I am talking about the teeth. Width of the belt itself is not that important. || @SpectraLzz so you think that going from 2 mm teeth to like 1.5 on the belts is way better VFA? I'm asking this because I'm modding my SVO8 as we speak. || @treyduval5399 Yes. Bambu H series uses 1.5 and is way better than P series which uses 2.0. || @SpectraLzz well how hard is this to do? Would it require replacing motors or stepper drivers or is it just plug and play with a belt and pulleys? || I’ve placed a deposit on it already || @DukeGaGa what does the deposit get you || Nice || @njv.rooyen5353lower backer price || It whould bena lot better when they print something. || I’ll have one soon. So I can show it all. I’m due time || Putting an "AI" button in the menu sounds like a gimmick and is being overused. Can't say if this printer is good or bad without seeing it in action and looking at a finished print. || Yeah I don’t think anyone can form a valid opinion just yet. In theory it’s cool. That’s all. || But if you feel like an AI button is a gimmick then you should prepare yourself because pretty soon. Everything will have AI buttons lol || I need to see how it handles multicolor and I'd be sold. || Same. How much do you think it’ll cost? || @stayreadyto3dprint What I would pay is like $1200. What it probably will be is $1500-$2k lol || 2k for a kick starter scam || @andrewroy9263 $999 for just printer. $1299 with filament box || Kickstarter price anyways. || would love to see it swapping nozzles. || Soon my friend. Lol || Anybody can put a cute box on display, I'd want to see it actually printing and nozzle switching before I believed it was "amazing". || Well, it’s from a reputable company and they’re not gonna tarnish their whole brand name by putting a fake product out that doesn’t work || @stayreadyto3dprint Reputable means having a good reputation. This is their first product; they don't have a reputation yet.
+If you go to their website, you see a computer rendering of the product working, not a video of the actual product working. That suggests the product isn't running yet.  And it's a kickstarter, which means you can send your money and get nothing, not even a box of bricks. || @stayreadyto3dprint reputable my ahh first product they "made" no one has seen it working wasn't even working ces26 because of "technical difficulties"  they're going to take the kick starter money and run || Mova is a huge company. Do some homework before totally knocking them. It’s def not their first product. || So Mova is going to bankrupt their multimillion dollar company over a 3d printer scam? Got it. That makes zero sense. lol || Wow! I have not heard of this company yet. I’m impressed by the nozzle switching tech. || You and me both! || How are you impressed with the nozzle switching tech that no one has seen working or seen the machine printing at all || @Og_paine I guess we will find out whenever a demo occurs lol I am just impressed on the fact they took their ambition and produced a machine ready for CES haha
+But I get your point of view too || So you’ve never seen a concept car and thought it was cool? Or a drawing of something someone was going to build? You gotta see it working to envision the end result? It’s a cool concept is what ppl are saying. Note we wait to see if they release it as they say they are. If they don’t then you don’t lose anything. But Mova is a huge company. Highly doubt they are scamming people just for a few bucks from a printer. Think about it. How dumb that would be for a successful multi million dollar company. || Finally a video! Thanks! Does it look promising? I feel bad not backing the U1. 😢 But looking at it, the swap time will be the same as the H2C as there is only 1 tube going into the tool head. Hopefully it's worth backing. || I think it’s great for a single tool printer. But I do believe multi tool head machines are making single tool printers alot less of a viable option in 2026. Why wouldn’t someone buy a multi tool machine if they could? || @dyops  it pre-stages the next filament right upto end of the ptfe tube inside the chamber. As soon as the current filament retracts passed the pre-staged filament, the next color starts feeding. Don't think the BL machines do that. || Yeah true. || It's Alive!!! been waiting to see a floor model. ;) || Yeah it’s def real! I was a little skeptical myself tbh</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
+          <t>UCXS90ukmtQo2kg3Ydf-cj3A</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>itsbasicbible</t>
+          <t>Stay Ready To 3D Print</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>DG7HhphSyG0</t>
+          <t>_qWzooEmzBo</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>God Is SPEAKING To You</t>
+          <t>Walk With Me @CES 2026</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Connect 
-https://linktr.ee/itsbasicbible
-MALTA APPAREL LINK 
-https://malta-apparel.com/?ref=BBAZ16 
-FOR 15% OFF: basicbible15 
-FREE 10 DAY DEVO BOOK 
-https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
-I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
-https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
-I WANT TO FOLLOW JESUS CHRIST
-https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
-Get vidIQ to grow your channel faster! 🚀
-https://vidiq.com/itsbasicbible</t>
+          <t>Check out the em smart AXI Pro laser here https://em-smart.com 
+Thanks for watching! If you're into 3D printing, whether it’s tuning your slicer settings, upgrading your Creality, Bambu Lab, or Elegoo printer, or experimenting with TPU, PLA, PETG, or custom filaments, you’ll feel right at home here.
+Join our Discord server to connect with one of the most active and supportive 3D printing communities online. We share printer mods, filament reviews, print profiles, and behind-the-scenes looks at our latest projects — plus, we run regular giveaways, offer support, and drop early news on upcoming content.
+Stay ready, stay printing — and be sure to check out our latest builds and experiments using today’s top 3D printer brands and materials.
+Join Discord here!  https://discord.gg/E5gPc8C2cs
+🌐 **Facebook Page**  
+📘 https://www.facebook.com/profile.php?id=61565872940311
+👥 **Facebook Group – “Stay Ready To 3D Print”**  
+📘 https://www.facebook.com/share/g/196GC85xxo/?mibextid=wwXIfr  
+📸 **Instagram**  
+https://www.instagram.com/@stayreadyto3dprint
+🎵 **TikTok**  
+https://www.tiktok.com/@stayreadyto3dprint
+🎁 **Patreon** – Get early access &amp; exclusive content  
+https://www.patreon.com/stayreadyfans
+📬 **Business inquiries / sponsorships**  
+Email: stayreadychat@gmail.com</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>2025-12-04T21:30:04Z</t>
+          <t>2026-01-08T08:04:57Z</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>229</t>
+          <t>312</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>15</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0</t>
         </is>
       </c>
       <c r="J10" t="n">
-        <v>0.021834</v>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>❤    Amen   🙏 || Hi you now</t>
-        </is>
-      </c>
+        <v>0.048077</v>
+      </c>
+      <c r="M10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
+          <t>UCXS90ukmtQo2kg3Ydf-cj3A</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>itsbasicbible</t>
+          <t>Stay Ready To 3D Print</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>e2gSSVkbeaI</t>
+          <t>_8WnWYPrRS0</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Daughter Nearly Killed by Parents Over Family Honor #DomesticAbuse #NewsTrending</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Listen closely 
-Ephesians 6:4 
-4 Fathers,[c] do not provoke your children to anger by the way you treat them. Rather, bring them up with the discipline and instruction that comes from the Lord.
-Connect 
-https://linktr.ee/itsbasicbible
-MALTA APPAREL LINK 
-https://malta-apparel.com/?ref=BBAZ16 
-FOR 15% OFF: basicbible15 
-FREE 10 DAY DEVO BOOK 
-https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
-I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
-https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
-I WANT TO FOLLOW JESUS CHRIST
-https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
-Get vidIQ to grow your channel faster! 🚀
-https://vidiq.com/itsbasicbible</t>
-        </is>
-      </c>
+          <t>New Printer or another Creality remake? Ender 3 v100 😂</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr">
         <is>
-          <t>2025-12-03T21:30:09Z</t>
+          <t>2026-01-07T06:03:49Z</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>1283</t>
+          <t>2204</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>96</t>
+          <t>23</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>4</t>
         </is>
       </c>
       <c r="J11" t="n">
-        <v>0.08028100000000001</v>
+        <v>0.01225</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>Get them out of your country before he poisons your communities. || Open a secret shelter for young ladies who have to run from thier own Parents due to the different religious beliefs that may get them killed. Someone has to step in to help these young ladies from the unhinged parents. || This is awesome, thank you for sharing your thoughts! || Assimilate || Or better yet don’t enforce your beliefs and rights on others when you live in a land of freedom and opportunity so presumably your children can live a better life. || Thanks for the comment! || Good thoughts, thank you for sharing!</t>
+          <t>I want more video's, lol || I’m trying lmao. 😅 || Pretty cool man. Yeah, I was wanting to get a scanner. || There are better options out there for less money.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
+          <t>UCXS90ukmtQo2kg3Ydf-cj3A</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>itsbasicbible</t>
+          <t>Stay Ready To 3D Print</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>2jMryl3y3Ts</t>
+          <t>kT19HFqeApc</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Your SUCCESS DEPENDS On This</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Connect 
-https://linktr.ee/itsbasicbible
-MALTA APPAREL LINK 
-https://malta-apparel.com/?ref=BBAZ16 
-FOR 15% OFF: basicbible15 
-FREE 10 DAY DEVO BOOK 
-https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
-I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
-https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
-I WANT TO FOLLOW JESUS CHRIST
-https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
-Get vidIQ to grow your channel faster! 🚀
-https://vidiq.com/itsbasicbible</t>
-        </is>
-      </c>
+          <t>The Most Useful Thing I’ve Done All Year! #3dprinter #3dprinted</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr">
         <is>
-          <t>2025-12-02T21:30:00Z</t>
+          <t>2026-01-04T23:00:38Z</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>896</t>
+          <t>7460</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>106</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>23</t>
         </is>
       </c>
       <c r="J12" t="n">
-        <v>0.06808</v>
+        <v>0.017292</v>
       </c>
       <c r="M12" t="inlineStr">
         <is>
-          <t>❤    Amen   🙏 
-        Only  as  high  as 
-        I  reach  can
-           I  grow || Amen! || The victor is not victorious if the vanquished does not consider himself so || Thanks for the comment!</t>
+          <t>I love how it looks kinda OEM next to the actual machine, Very nice 👍🏽 || Same. Thanks || what kind of pens did you use to paint? || They are the Just art from my website. Here’s a link. 
+https://www.stayreadyto3dprint.com/products/72-colors-acrylic-paint-markers-set-with-canvas-bag-dual-tips-with-brush-tip-fine-tip-no-bleed-waterproof-non-toxic-odorless-paint-pens-for-rock-egg-wood-fabric-glass-ceramic-diy?_pos=1&amp;_psq=paint&amp;_ss=e&amp;_v=1.0 || First problem is you use k cups - literally drinking hot plastic 😂 || Taste good to me lol. || What printers || Used the k2 plus and the Bambu x1c for this one. I gotta say the quality from the k2 wasn’t near as good as the x1c this time. || ​@stayreadyto3dprint oh nice i think they both came out good || Thank you !! || The carousel is 100 times better than being forced to randomly remove K-cups until you get the flavor you want. || You just add another box. They’re magnetic. I’d say you can add 3 boxes before it starts looking wild. lol. || I can’t do that awful cluttered look. That’s just me. Plus I only drink one flavor anyways. I may add one more box with another flavor for quest. || That’s significantly worse. I don’t want random flavors. Surprise pumpkin flavored coffee, or decaf, or dark roast when I want light roast would be a terrible surprise. || I loaded mine with one flavor lol. I should have showed random flavors in the video I guess. It’s confusing. If you want more flavors just add another box. They stick together. Although more than 2-3 wouldnt look very good. So if you’re a big flavor drinker this isn’t for you. I’m not. || Only now you can't choose flavor || You just add another box. They’re magnetic. I’d say you can add 3 boxes before it starts looking wild. lol. || @stayreadyto3dprint lol seems counterproductive || I like it. I hate the clutter look of the carousel. That’s just my preference. || bro i am so going to print this tonight for my K-cups, thanks || You can add boxes. They have a place for magnets on the side. But I’d say only add up to 3 or you won’t have any more counter space lol || Sweet || Thanks</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>UChWSdSRhJWUpq82L2LsVJSA</t>
+          <t>UCXS90ukmtQo2kg3Ydf-cj3A</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>itsbasicbible</t>
+          <t>Stay Ready To 3D Print</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>UU7TLaOj8qY</t>
+          <t>vsVbjtoe-g8</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Is Trump going to heaven? #jesuslovesyou #jesuschrist #shorts</t>
+          <t>Prusa Keeps The Pressure On Competitors with THIS!</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Here's what the Bible says, it will SHOCK YOU!
-1 Peter 2:13-17
-13 Submit yourselves for the Lord’s sake to every human authority: whether to the emperor, as the supreme authority, 14 or to governors, who are sent by him to punish those who do wrong and to commend those who do right. 15 For it is God’s will that by doing good you should silence the ignorant talk of foolish people. 16 Live as free people, but do not use your freedom as a cover-up for evil; live as God’s slaves. 17 Show proper respect to everyone, love the family of believers, fear God, honor the emperor.
-1 Timothy 2:1-4
-I urge, then, first of all, that petitions, prayers, intercession and thanksgiving be made for all people— 2 for kings and all those in authority, that we may live peaceful and quiet lives in all godliness and holiness. 3 This is good, and pleases God our Savior, 4 who wants all people to be saved and to come to a knowledge of the truth.
-Romans 13:1-7
-Let everyone be subject to the governing authorities, for there is no authority except that which God has established. The authorities that exist have been established by God. 2 Consequently, whoever rebels against the authority is rebelling against what God has instituted, and those who do so will bring judgment on themselves. 3 For rulers hold no terror for those who do right, but for those who do wrong. Do you want to be free from fear of the one in authority? Then do what is right and you will be commended. 4 For the one in authority is God’s servant for your good. But if you do wrong, be afraid, for rulers do not bear the sword for no reason. They are God’s servants, agents of wrath to bring punishment on the wrongdoer. 5 Therefore, it is necessary to submit to the authorities, not only because of possible punishment but also as a matter of conscience.
-6 This is also why you pay taxes, for the authorities are God’s servants, who give their full time to governing. 7 Give to everyone what you owe them: If you owe taxes, pay taxes; if revenue, then revenue; if respect, then respect; if honor, then honor.
-Also, I mixed up Peter with Paul. I meant to say Paul.
-Connect 
-https://linktr.ee/itsbasicbible
-MALTA APPAREL LINK 
-https://malta-apparel.com/?ref=BBAZ16 
-FOR 15% OFF: basicbible15 
-FREE 10 DAY DEVO BOOK 
-https://srm.fishflow.app/widget/form/unvJSsn9MrPIOVqf5b14 
-I DECIDED TO FOLLOW JESUS AND WANT TO TAKE MY NEXT STEP
-https://srm.fishflow.app/widget/form/Uz07h4LYU0k5f0b4aTPG
-I WANT TO FOLLOW JESUS CHRIST
-https://srm.fishflow.app/widget/form/AsbicSxZteiove5fAonq
-Get vidIQ to grow your channel faster! 🚀
-https://vidiq.com/itsbasicbible</t>
+          <t>The 3D printing market is moving fast right now — and instead of slowing down, Prusa Research is doubling down on meaningful innovation.
+In this video, I break down Prusa’s latest move, including a major new add-on release that pushes the Prusa CORE One platform forward and keeps it competitive as other brands roll out similar ideas. Rather than chasing trends, Prusa continues to refine what actually matters: reliability, expandability, and long-term usability.
+I also share my honest thoughts on the CORE One — where it shines, where it could improve, and how it stacks up in an increasingly crowded field. This isn’t hype or brand loyalty — it’s a real discussion about innovation, pacing, and what keeps a company relevant as the industry accelerates.
+🎁 UPCOMING LIVE GIVEAWAY
+I’m also hosting a LIVE giveaway you won’t want to miss:
+🏆 Prize:
+• Uniformation GK3 Pro Resin Printer
+• 6 bottles of resin
+There will be 4 winners. 1 winner getting the printer and 3 winners getting 2 bottles of resin each!
+🗓 Date: January 10, 2026
+⏰ Time: 9:00 PM CST
+📍 Where: Live right here on my YouTube channel
+How to Enter:
+✅ You must be present live to win
+✅ You must follow Uniformation on Instagram
+https://www.instagram.com/uniformation3dprinter/
+Join our Discord for any questions aboutgiveaways you may have.
+https://mee6.xyz/i/4YMcjZjNO6
+Winners will be selected live on stream, so don’t be late.</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>2025-12-01T21:30:09Z</t>
+          <t>2026-01-04T00:38:13Z</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>1172</t>
+          <t>27443</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>79</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>24</t>
         </is>
       </c>
       <c r="J13" t="n">
-        <v>0.059727</v>
+        <v>0.003753</v>
       </c>
       <c r="M13" t="inlineStr">
         <is>
-          <t>❤    Amen  🙏   ❤ || Amen! || AMEN || Amen! || Nobody is going to heaven. If God is real, then its not the any God we know. Thats what disinformation does. Its like a big game of telephone</t>
+          <t>i treyed the MK4S and it was so bad! i sendet it back to Prusa exactly like they told me and better, Prusa aproved it, after inspection the told me shiping damage, -130€ and after 11 weeks in the return progress i still wait to get my money!!! stay away from Prusa!!! || I highly doubt that. They’re one of the best companies out there. I can msg one of my reps to help you but are you sure you’re sharing the whole story here? || @stayreadyto3dprint when they are one of the best, why are they than like that? i even looked up the internet and i am not alone with this kind of support. but i have to say the are better than Nathan Stone. still waiting on my printer 1 year later :D its the Nextruder guy || great take. this is exactly why prusa still matters in the market. they’re not chasing hype features, but building solid platforms that keep evolving. real upgrades, long-term support, and stuff that actually works in practice. you can tell they’re thinking years ahead, not just the next launch || Exactly right. Couldnt agree more. || totally agree. Prusa is top tier, no doubt. The video turned out great and the printer itself is an awesome example of how far 3D printing has come. || Thank you kind sir ! 😊 || I’m personally keen on seeing how the INDX will handle TPU’s on the Core One machines.
+I’m waiting till probably the end of 2026 to either get a Snapmaker U1 or Core One with INDX (or some other brand shows up in 2026 with a new machine)
+Bambu has locked down standard rigid filaments but the H2’s were not deigned with the moving left nozzle to handle flexible cutting out multi colour options on their machines. || I’m def excited for the INDX option for the prusa machines. || Great video 😊 Clearly explained and it all makes sense 👍 You can see that Prusa focuses on honest quality and long term value 💪 That’s why people trust this brand just like I do 🚀 || Thank you. I agree. They are def invested here. They do things that let you know they are listening. And they actually have customer service. Lol || I got the K2 and I am thinking of selling it and buy the core one soon. I understand your point about using the manufacturers slicer but man is the Creality slicer a pain. Curious to know more about why you kick Creality though. For me it is that the K2 wasn't particularly precise or reliable. When it works it's great but when it's clogged it's hell. I've gone through 3 nozzles with this thing. || I can tell you it was about 20% due to machinery. The rest was due to things they did as a brand. Which I’ll be releasing a video about. || Curious to hear more on why you're kicking Creality to the curb. || same || Oh trust me. There’s a video coming soon ! You won’t wanna miss it. I’ll be revealing it all. || LOL, Prusa not putting any pressure on ANY 3D printer manufacturer.  Prusa can't make their old stuff work, let alone the new stuff.  Bondtech stepped in to try and save Josef.  If they can't get this right out of the box, Prusa will be filing for bankruptcy in 2026. || You must not own any of their machines. lol || ​@stayreadyto3dprintNot any more.  Not interested in being Josef's guinea pig cuck.  No amount of toxic gummies will get my money.  IF, when, or ever the INDX hits the consumer market and actually works out of the box, and Josef provides a gummy delete option, I will consider.  However, if the train wreck XL is $5k, what will the INDX be? Only diehard Prusa cucks will buy it. || That’s the cool thing about 3d printing. 10 different people will have 10 different opinions on what brand they like. And none of them are wrong. You gotta use the brand you enjoy most. Whatever brand that may be. These are just MY opinions and preference. That’s all. 
+What brand do you prefer? || Great video 👍 || Ty! || pretty cool stuff, glad the streams are back. oh and its 8 tools for the INDX. either way its going to be an exciting year. || I think so too!!!! Stay tuned for live footage from CES 2026 next week</t>
         </is>
       </c>
     </row>

</xml_diff>